<commit_message>
Added Scania and Guy articulated trucks
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Vehicle</t>
   </si>
@@ -95,12 +95,39 @@
   </si>
   <si>
     <t>Foden Alpha</t>
+  </si>
+  <si>
+    <t>Scania 3 Series</t>
+  </si>
+  <si>
+    <t>Scania 4 Series</t>
+  </si>
+  <si>
+    <t>Scania R Series</t>
+  </si>
+  <si>
+    <t>Guy Big J4T</t>
+  </si>
+  <si>
+    <t>Guy Big J6</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>170hp</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -455,12 +482,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -473,9 +498,10 @@
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -483,7 +509,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,8 +537,14 @@
       <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -543,8 +575,11 @@
         <f>H4*0.9</f>
         <v>56.920997883030836</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -568,15 +603,18 @@
         <v>20</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" ref="H5:H13" si="0">SQRT(F5*G5)/$B$1</f>
+        <f t="shared" ref="H5:H14" si="0">SQRT(F5*G5)/$B$1</f>
         <v>81.649658092772611</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" ref="I5:I13" si="1">H5*0.9</f>
+        <f t="shared" ref="I5:I14" si="1">H5*0.9</f>
         <v>73.484692283495349</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -607,8 +645,11 @@
         <f t="shared" si="1"/>
         <v>92.466210044534662</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -639,8 +680,11 @@
         <f t="shared" si="1"/>
         <v>88.02840450672727</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -671,8 +715,11 @@
         <f t="shared" si="1"/>
         <v>97.488460855631544</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -703,8 +750,11 @@
         <f t="shared" si="1"/>
         <v>135.8970198348735</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -735,8 +785,11 @@
         <f t="shared" si="1"/>
         <v>148.43180252223578</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -767,8 +820,11 @@
         <f t="shared" si="1"/>
         <v>153.08820986607688</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -799,8 +855,11 @@
         <f t="shared" si="1"/>
         <v>50.911688245431421</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -830,6 +889,185 @@
       <c r="I13" s="2">
         <f t="shared" si="1"/>
         <v>141.98591479439079</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>1987</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <f>IF(B14 &gt; 1900, ((B14-1900)*10)+400+C14, ((B14-1730)*2)+C14)+VLOOKUP(D14,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>4871</v>
+      </c>
+      <c r="F14">
+        <v>65</v>
+      </c>
+      <c r="G14">
+        <v>44</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>178.26322609494585</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>160.43690348545127</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>1995</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15">
+        <f>IF(B15 &gt; 1900, ((B15-1900)*10)+400+C15, ((B15-1730)*2)+C15)+VLOOKUP(D15,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>4951</v>
+      </c>
+      <c r="F15">
+        <v>68</v>
+      </c>
+      <c r="G15">
+        <v>48</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" ref="H15" si="2">SQRT(F15*G15)/$B$1</f>
+        <v>190.43809142780935</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" ref="I15" si="3">H15*0.9</f>
+        <v>171.39428228502842</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>2004</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16">
+        <f>IF(B16 &gt; 1900, ((B16-1900)*10)+400+C16, ((B16-1730)*2)+C16)+VLOOKUP(D16,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>5041</v>
+      </c>
+      <c r="F16">
+        <v>72</v>
+      </c>
+      <c r="G16">
+        <v>54</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" ref="H16" si="4">SQRT(F16*G16)/$B$1</f>
+        <v>207.84609690826528</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" ref="I16" si="5">H16*0.9</f>
+        <v>187.06148721743875</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>1964</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17">
+        <f>IF(B17 &gt; 1900, ((B17-1900)*10)+400+C17, ((B17-1730)*2)+C17)+VLOOKUP(D17,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>4641</v>
+      </c>
+      <c r="F17">
+        <v>54</v>
+      </c>
+      <c r="G17">
+        <v>36</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" ref="H17:H18" si="6">SQRT(F17*G17)/$B$1</f>
+        <v>146.9693845669907</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" ref="I17:I18" si="7">H17*0.9</f>
+        <v>132.27244611029164</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>1964</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <f>IF(B18 &gt; 1900, ((B18-1900)*10)+400+C18, ((B18-1730)*2)+C18)+VLOOKUP(D18,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>4642</v>
+      </c>
+      <c r="F18">
+        <v>54</v>
+      </c>
+      <c r="G18">
+        <v>22</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="6"/>
+        <v>114.89125293076057</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="7"/>
+        <v>103.40212763768452</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -841,7 +1079,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'ID Scheme'!$A$2:$A$4</xm:f>
           </x14:formula1>
@@ -854,7 +1092,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Added Leyland X Type
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
   <si>
     <t>Vehicle</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Leyland X Type</t>
   </si>
 </sst>
 </file>
@@ -483,9 +486,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -562,18 +567,18 @@
         <v>4131</v>
       </c>
       <c r="F4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G4">
         <v>18</v>
       </c>
       <c r="H4" s="2">
         <f>SQRT(F4*G4)/$B$1</f>
-        <v>63.245553203367592</v>
+        <v>66.332495807108003</v>
       </c>
       <c r="I4" s="2">
         <f>H4*0.9</f>
-        <v>56.920997883030836</v>
+        <v>59.699246226397207</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>33</v>
@@ -581,10 +586,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="B5">
-        <v>1936</v>
+        <v>1907</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -594,21 +599,21 @@
       </c>
       <c r="E5">
         <f>IF(B5 &gt; 1900, ((B5-1900)*10)+400+C5, ((B5-1730)*2)+C5)+VLOOKUP(D5,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>4361</v>
+        <v>4071</v>
       </c>
       <c r="F5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" ref="H5:H14" si="0">SQRT(F5*G5)/$B$1</f>
-        <v>81.649658092772611</v>
+        <f>SQRT(F5*G5)/$B$1</f>
+        <v>63.245553203367592</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" ref="I5:I14" si="1">H5*0.9</f>
-        <v>73.484692283495349</v>
+        <f>H5*0.9</f>
+        <v>56.920997883030836</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>33</v>
@@ -616,10 +621,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>1952</v>
+        <v>1936</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -629,347 +634,347 @@
       </c>
       <c r="E6">
         <f>IF(B6 &gt; 1900, ((B6-1900)*10)+400+C6, ((B6-1730)*2)+C6)+VLOOKUP(D6,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>4361</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" ref="H6:H15" si="0">SQRT(F6*G6)/$B$1</f>
+        <v>81.649658092772611</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" ref="I6:I15" si="1">H6*0.9</f>
+        <v>73.484692283495349</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1952</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <f>IF(B7 &gt; 1900, ((B7-1900)*10)+400+C7, ((B7-1730)*2)+C7)+VLOOKUP(D7,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4521</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>38</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <v>25</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H7" s="2">
         <f t="shared" si="0"/>
         <v>102.74023338281629</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I7" s="2">
         <f t="shared" si="1"/>
         <v>92.466210044534662</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="J7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>1957</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7">
-        <f>IF(B7 &gt; 1900, ((B7-1900)*10)+400+C7, ((B7-1730)*2)+C7)+VLOOKUP(D7,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <f>IF(B8 &gt; 1900, ((B8-1900)*10)+400+C8, ((B8-1730)*2)+C8)+VLOOKUP(D8,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4571</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>41</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>21</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H8" s="2">
         <f t="shared" si="0"/>
         <v>97.809338340808068</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I8" s="2">
         <f t="shared" si="1"/>
         <v>88.02840450672727</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="J8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>1963</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8">
-        <f>IF(B8 &gt; 1900, ((B8-1900)*10)+400+C8, ((B8-1730)*2)+C8)+VLOOKUP(D8,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <f>IF(B9 &gt; 1900, ((B9-1900)*10)+400+C9, ((B9-1730)*2)+C9)+VLOOKUP(D9,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4631</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>44</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>24</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H9" s="2">
         <f t="shared" si="0"/>
         <v>108.32051206181282</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I9" s="2">
         <f t="shared" si="1"/>
         <v>97.488460855631544</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="J9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>1965</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <f>IF(B9 &gt; 1900, ((B9-1900)*10)+400+C9, ((B9-1730)*2)+C9)+VLOOKUP(D9,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <f>IF(B10 &gt; 1900, ((B10-1900)*10)+400+C10, ((B10-1730)*2)+C10)+VLOOKUP(D10,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4651</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>57</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>36</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H10" s="2">
         <f t="shared" si="0"/>
         <v>150.99668870541501</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I10" s="2">
         <f t="shared" si="1"/>
         <v>135.8970198348735</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="J10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>1968</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10">
-        <f>IF(B10 &gt; 1900, ((B10-1900)*10)+400+C10, ((B10-1730)*2)+C10)+VLOOKUP(D10,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <f>IF(B11 &gt; 1900, ((B11-1900)*10)+400+C11, ((B11-1730)*2)+C11)+VLOOKUP(D11,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4681</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>68</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <v>36</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H11" s="2">
         <f t="shared" si="0"/>
         <v>164.92422502470643</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I11" s="2">
         <f t="shared" si="1"/>
         <v>148.43180252223578</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="J11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>1980</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11">
-        <f>IF(B11 &gt; 1900, ((B11-1900)*10)+400+C11, ((B11-1730)*2)+C11)+VLOOKUP(D11,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <f>IF(B12 &gt; 1900, ((B12-1900)*10)+400+C12, ((B12-1730)*2)+C12)+VLOOKUP(D12,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4801</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>62</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>42</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H12" s="2">
         <f t="shared" si="0"/>
         <v>170.09801096230765</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I12" s="2">
         <f t="shared" si="1"/>
         <v>153.08820986607688</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="J12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>1902</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12">
-        <f>IF(B12 &gt; 1900, ((B12-1900)*10)+400+C12, ((B12-1730)*2)+C12)+VLOOKUP(D12,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <f>IF(B13 &gt; 1900, ((B13-1900)*10)+400+C13, ((B13-1730)*2)+C13)+VLOOKUP(D13,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4021</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>18</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>16</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H13" s="2">
         <f t="shared" si="0"/>
         <v>56.568542494923797</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I13" s="2">
         <f t="shared" si="1"/>
         <v>50.911688245431421</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="J13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>1997</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13">
-        <f>IF(B13 &gt; 1900, ((B13-1900)*10)+400+C13, ((B13-1730)*2)+C13)+VLOOKUP(D13,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <f>IF(B14 &gt; 1900, ((B14-1900)*10)+400+C14, ((B14-1730)*2)+C14)+VLOOKUP(D14,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4971</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>70</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>32</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H14" s="2">
         <f t="shared" si="0"/>
         <v>157.76212754932311</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I14" s="2">
         <f t="shared" si="1"/>
         <v>141.98591479439079</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="J14" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>1987</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14">
-        <f>IF(B14 &gt; 1900, ((B14-1900)*10)+400+C14, ((B14-1730)*2)+C14)+VLOOKUP(D14,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15">
+        <f>IF(B15 &gt; 1900, ((B15-1900)*10)+400+C15, ((B15-1730)*2)+C15)+VLOOKUP(D15,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4871</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>65</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>44</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H15" s="2">
         <f t="shared" si="0"/>
         <v>178.26322609494585</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I15" s="2">
         <f t="shared" si="1"/>
         <v>160.43690348545127</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15">
-        <v>1995</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15">
-        <f>IF(B15 &gt; 1900, ((B15-1900)*10)+400+C15, ((B15-1730)*2)+C15)+VLOOKUP(D15,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>4951</v>
-      </c>
-      <c r="F15">
-        <v>68</v>
-      </c>
-      <c r="G15">
-        <v>48</v>
-      </c>
-      <c r="H15" s="2">
-        <f t="shared" ref="H15" si="2">SQRT(F15*G15)/$B$1</f>
-        <v>190.43809142780935</v>
-      </c>
-      <c r="I15" s="2">
-        <f t="shared" ref="I15" si="3">H15*0.9</f>
-        <v>171.39428228502842</v>
-      </c>
       <c r="J15" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16">
-        <v>2004</v>
+        <v>1995</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -979,21 +984,21 @@
       </c>
       <c r="E16">
         <f>IF(B16 &gt; 1900, ((B16-1900)*10)+400+C16, ((B16-1730)*2)+C16)+VLOOKUP(D16,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>5041</v>
+        <v>4951</v>
       </c>
       <c r="F16">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G16">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" ref="H16" si="4">SQRT(F16*G16)/$B$1</f>
-        <v>207.84609690826528</v>
+        <f t="shared" ref="H16" si="2">SQRT(F16*G16)/$B$1</f>
+        <v>190.43809142780935</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" ref="I16" si="5">H16*0.9</f>
-        <v>187.06148721743875</v>
+        <f t="shared" ref="I16" si="3">H16*0.9</f>
+        <v>171.39428228502842</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>33</v>
@@ -1001,10 +1006,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17">
-        <v>1964</v>
+        <v>2004</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1014,21 +1019,21 @@
       </c>
       <c r="E17">
         <f>IF(B17 &gt; 1900, ((B17-1900)*10)+400+C17, ((B17-1730)*2)+C17)+VLOOKUP(D17,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>4641</v>
+        <v>5041</v>
       </c>
       <c r="F17">
+        <v>72</v>
+      </c>
+      <c r="G17">
         <v>54</v>
       </c>
-      <c r="G17">
-        <v>36</v>
-      </c>
       <c r="H17" s="2">
-        <f t="shared" ref="H17:H18" si="6">SQRT(F17*G17)/$B$1</f>
-        <v>146.9693845669907</v>
+        <f t="shared" ref="H17" si="4">SQRT(F17*G17)/$B$1</f>
+        <v>207.84609690826528</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" ref="I17:I18" si="7">H17*0.9</f>
-        <v>132.27244611029164</v>
+        <f t="shared" ref="I17" si="5">H17*0.9</f>
+        <v>187.06148721743875</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>33</v>
@@ -1036,43 +1041,78 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>1964</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
       </c>
       <c r="E18">
         <f>IF(B18 &gt; 1900, ((B18-1900)*10)+400+C18, ((B18-1730)*2)+C18)+VLOOKUP(D18,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>4642</v>
+        <v>4641</v>
       </c>
       <c r="F18">
         <v>54</v>
       </c>
       <c r="G18">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="H18" s="2">
+        <f t="shared" ref="H18:H19" si="6">SQRT(F18*G18)/$B$1</f>
+        <v>146.9693845669907</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" ref="I18:I19" si="7">H18*0.9</f>
+        <v>132.27244611029164</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19">
+        <v>1964</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <f>IF(B19 &gt; 1900, ((B19-1900)*10)+400+C19, ((B19-1730)*2)+C19)+VLOOKUP(D19,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>4642</v>
+      </c>
+      <c r="F19">
+        <v>54</v>
+      </c>
+      <c r="G19">
+        <v>22</v>
+      </c>
+      <c r="H19" s="2">
         <f t="shared" si="6"/>
         <v>114.89125293076057</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I19" s="2">
         <f t="shared" si="7"/>
         <v>103.40212763768452</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" t="s">
+      <c r="J19" s="2"/>
+      <c r="K19" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B9">
-    <sortCondition ref="B5"/>
+  <sortState ref="A2:B10">
+    <sortCondition ref="B6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Dray and Stagecoach
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5897BF6-5E34-41AC-BBB2-2FFDD5476BC7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ID Scheme" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>Vehicle</t>
   </si>
@@ -125,6 +126,9 @@
   </si>
   <si>
     <t>Leyland X Type</t>
+  </si>
+  <si>
+    <t>Horse-Drawn Dray</t>
   </si>
 </sst>
 </file>
@@ -486,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,10 +555,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B4">
-        <v>1913</v>
+        <v>1800</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -564,21 +568,21 @@
       </c>
       <c r="E4">
         <f>IF(B4 &gt; 1900, ((B4-1900)*10)+400+C4, ((B4-1730)*2)+C4)+VLOOKUP(D4,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>4131</v>
+        <v>3741</v>
       </c>
       <c r="F4">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G4">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H4" s="2">
         <f>SQRT(F4*G4)/$B$1</f>
-        <v>66.332495807108003</v>
+        <v>46.188021535170058</v>
       </c>
       <c r="I4" s="2">
         <f>H4*0.9</f>
-        <v>59.699246226397207</v>
+        <v>41.569219381653056</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>33</v>
@@ -586,10 +590,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>1907</v>
+        <v>1913</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -599,21 +603,21 @@
       </c>
       <c r="E5">
         <f>IF(B5 &gt; 1900, ((B5-1900)*10)+400+C5, ((B5-1730)*2)+C5)+VLOOKUP(D5,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>4071</v>
+        <v>4131</v>
       </c>
       <c r="F5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G5">
         <v>18</v>
       </c>
       <c r="H5" s="2">
         <f>SQRT(F5*G5)/$B$1</f>
-        <v>63.245553203367592</v>
+        <v>66.332495807108003</v>
       </c>
       <c r="I5" s="2">
         <f>H5*0.9</f>
-        <v>56.920997883030836</v>
+        <v>59.699246226397207</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>33</v>
@@ -621,10 +625,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="B6">
-        <v>1936</v>
+        <v>1907</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -634,21 +638,21 @@
       </c>
       <c r="E6">
         <f>IF(B6 &gt; 1900, ((B6-1900)*10)+400+C6, ((B6-1730)*2)+C6)+VLOOKUP(D6,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>4361</v>
+        <v>4071</v>
       </c>
       <c r="F6">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" ref="H6:H15" si="0">SQRT(F6*G6)/$B$1</f>
-        <v>81.649658092772611</v>
+        <f>SQRT(F6*G6)/$B$1</f>
+        <v>63.245553203367592</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" ref="I6:I15" si="1">H6*0.9</f>
-        <v>73.484692283495349</v>
+        <f>H6*0.9</f>
+        <v>56.920997883030836</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>33</v>
@@ -656,10 +660,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>1952</v>
+        <v>1936</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -669,347 +673,347 @@
       </c>
       <c r="E7">
         <f>IF(B7 &gt; 1900, ((B7-1900)*10)+400+C7, ((B7-1730)*2)+C7)+VLOOKUP(D7,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>4361</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" ref="H7:H16" si="0">SQRT(F7*G7)/$B$1</f>
+        <v>81.649658092772611</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" ref="I7:I16" si="1">H7*0.9</f>
+        <v>73.484692283495349</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>1952</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <f>IF(B8 &gt; 1900, ((B8-1900)*10)+400+C8, ((B8-1730)*2)+C8)+VLOOKUP(D8,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4521</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>38</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>25</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H8" s="2">
         <f t="shared" si="0"/>
         <v>102.74023338281629</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I8" s="2">
         <f t="shared" si="1"/>
         <v>92.466210044534662</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="J8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>1957</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8">
-        <f>IF(B8 &gt; 1900, ((B8-1900)*10)+400+C8, ((B8-1730)*2)+C8)+VLOOKUP(D8,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <f>IF(B9 &gt; 1900, ((B9-1900)*10)+400+C9, ((B9-1730)*2)+C9)+VLOOKUP(D9,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4571</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>41</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>21</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H9" s="2">
         <f t="shared" si="0"/>
         <v>97.809338340808068</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I9" s="2">
         <f t="shared" si="1"/>
         <v>88.02840450672727</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="J9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>1963</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <f>IF(B9 &gt; 1900, ((B9-1900)*10)+400+C9, ((B9-1730)*2)+C9)+VLOOKUP(D9,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <f>IF(B10 &gt; 1900, ((B10-1900)*10)+400+C10, ((B10-1730)*2)+C10)+VLOOKUP(D10,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4631</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>44</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>24</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H10" s="2">
         <f t="shared" si="0"/>
         <v>108.32051206181282</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I10" s="2">
         <f t="shared" si="1"/>
         <v>97.488460855631544</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="J10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>1965</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10">
-        <f>IF(B10 &gt; 1900, ((B10-1900)*10)+400+C10, ((B10-1730)*2)+C10)+VLOOKUP(D10,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <f>IF(B11 &gt; 1900, ((B11-1900)*10)+400+C11, ((B11-1730)*2)+C11)+VLOOKUP(D11,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4651</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>57</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <v>36</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H11" s="2">
         <f t="shared" si="0"/>
         <v>150.99668870541501</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I11" s="2">
         <f t="shared" si="1"/>
         <v>135.8970198348735</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="J11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>1968</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11">
-        <f>IF(B11 &gt; 1900, ((B11-1900)*10)+400+C11, ((B11-1730)*2)+C11)+VLOOKUP(D11,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <f>IF(B12 &gt; 1900, ((B12-1900)*10)+400+C12, ((B12-1730)*2)+C12)+VLOOKUP(D12,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4681</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>68</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>36</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H12" s="2">
         <f t="shared" si="0"/>
         <v>164.92422502470643</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I12" s="2">
         <f t="shared" si="1"/>
         <v>148.43180252223578</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="J12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>1980</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12">
-        <f>IF(B12 &gt; 1900, ((B12-1900)*10)+400+C12, ((B12-1730)*2)+C12)+VLOOKUP(D12,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <f>IF(B13 &gt; 1900, ((B13-1900)*10)+400+C13, ((B13-1730)*2)+C13)+VLOOKUP(D13,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4801</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>62</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>42</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H13" s="2">
         <f t="shared" si="0"/>
         <v>170.09801096230765</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I13" s="2">
         <f t="shared" si="1"/>
         <v>153.08820986607688</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="J13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>1902</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13">
-        <f>IF(B13 &gt; 1900, ((B13-1900)*10)+400+C13, ((B13-1730)*2)+C13)+VLOOKUP(D13,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <f>IF(B14 &gt; 1900, ((B14-1900)*10)+400+C14, ((B14-1730)*2)+C14)+VLOOKUP(D14,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4021</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>18</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>16</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H14" s="2">
         <f t="shared" si="0"/>
         <v>56.568542494923797</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I14" s="2">
         <f t="shared" si="1"/>
         <v>50.911688245431421</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="J14" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>1997</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14">
-        <f>IF(B14 &gt; 1900, ((B14-1900)*10)+400+C14, ((B14-1730)*2)+C14)+VLOOKUP(D14,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15">
+        <f>IF(B15 &gt; 1900, ((B15-1900)*10)+400+C15, ((B15-1730)*2)+C15)+VLOOKUP(D15,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4971</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>70</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>32</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H15" s="2">
         <f t="shared" si="0"/>
         <v>157.76212754932311</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I15" s="2">
         <f t="shared" si="1"/>
         <v>141.98591479439079</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="J15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>1987</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15">
-        <f>IF(B15 &gt; 1900, ((B15-1900)*10)+400+C15, ((B15-1730)*2)+C15)+VLOOKUP(D15,'ID Scheme'!$A$2:$B$4,2)</f>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16">
+        <f>IF(B16 &gt; 1900, ((B16-1900)*10)+400+C16, ((B16-1730)*2)+C16)+VLOOKUP(D16,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>4871</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>65</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>44</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H16" s="2">
         <f t="shared" si="0"/>
         <v>178.26322609494585</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I16" s="2">
         <f t="shared" si="1"/>
         <v>160.43690348545127</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16">
-        <v>1995</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16">
-        <f>IF(B16 &gt; 1900, ((B16-1900)*10)+400+C16, ((B16-1730)*2)+C16)+VLOOKUP(D16,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>4951</v>
-      </c>
-      <c r="F16">
-        <v>68</v>
-      </c>
-      <c r="G16">
-        <v>48</v>
-      </c>
-      <c r="H16" s="2">
-        <f t="shared" ref="H16" si="2">SQRT(F16*G16)/$B$1</f>
-        <v>190.43809142780935</v>
-      </c>
-      <c r="I16" s="2">
-        <f t="shared" ref="I16" si="3">H16*0.9</f>
-        <v>171.39428228502842</v>
-      </c>
       <c r="J16" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17">
-        <v>2004</v>
+        <v>1995</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1019,21 +1023,21 @@
       </c>
       <c r="E17">
         <f>IF(B17 &gt; 1900, ((B17-1900)*10)+400+C17, ((B17-1730)*2)+C17)+VLOOKUP(D17,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>5041</v>
+        <v>4951</v>
       </c>
       <c r="F17">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G17">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" ref="H17" si="4">SQRT(F17*G17)/$B$1</f>
-        <v>207.84609690826528</v>
+        <f t="shared" ref="H17" si="2">SQRT(F17*G17)/$B$1</f>
+        <v>190.43809142780935</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" ref="I17" si="5">H17*0.9</f>
-        <v>187.06148721743875</v>
+        <f t="shared" ref="I17" si="3">H17*0.9</f>
+        <v>171.39428228502842</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>33</v>
@@ -1041,10 +1045,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18">
-        <v>1964</v>
+        <v>2004</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1054,21 +1058,21 @@
       </c>
       <c r="E18">
         <f>IF(B18 &gt; 1900, ((B18-1900)*10)+400+C18, ((B18-1730)*2)+C18)+VLOOKUP(D18,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>4641</v>
+        <v>5041</v>
       </c>
       <c r="F18">
+        <v>72</v>
+      </c>
+      <c r="G18">
         <v>54</v>
       </c>
-      <c r="G18">
-        <v>36</v>
-      </c>
       <c r="H18" s="2">
-        <f t="shared" ref="H18:H19" si="6">SQRT(F18*G18)/$B$1</f>
-        <v>146.9693845669907</v>
+        <f t="shared" ref="H18" si="4">SQRT(F18*G18)/$B$1</f>
+        <v>207.84609690826528</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" ref="I18:I19" si="7">H18*0.9</f>
-        <v>132.27244611029164</v>
+        <f t="shared" ref="I18" si="5">H18*0.9</f>
+        <v>187.06148721743875</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>33</v>
@@ -1076,43 +1080,78 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19">
         <v>1964</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
       </c>
       <c r="E19">
         <f>IF(B19 &gt; 1900, ((B19-1900)*10)+400+C19, ((B19-1730)*2)+C19)+VLOOKUP(D19,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>4642</v>
+        <v>4641</v>
       </c>
       <c r="F19">
         <v>54</v>
       </c>
       <c r="G19">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="H19" s="2">
+        <f t="shared" ref="H19:H20" si="6">SQRT(F19*G19)/$B$1</f>
+        <v>146.9693845669907</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" ref="I19:I20" si="7">H19*0.9</f>
+        <v>132.27244611029164</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>1964</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20">
+        <f>IF(B20 &gt; 1900, ((B20-1900)*10)+400+C20, ((B20-1730)*2)+C20)+VLOOKUP(D20,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>4642</v>
+      </c>
+      <c r="F20">
+        <v>54</v>
+      </c>
+      <c r="G20">
+        <v>22</v>
+      </c>
+      <c r="H20" s="2">
         <f t="shared" si="6"/>
         <v>114.89125293076057</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I20" s="2">
         <f t="shared" si="7"/>
         <v>103.40212763768452</v>
       </c>
-      <c r="J19" s="2"/>
-      <c r="K19" t="s">
+      <c r="J20" s="2"/>
+      <c r="K20" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B10">
-    <sortCondition ref="B6"/>
+  <sortState ref="A2:B11">
+    <sortCondition ref="B7"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added AEC Regent (I and II) and AEC Routemaster
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5540AA39-0AE0-4FD4-B6F5-7522F4F685E1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E82747-7E42-4EDB-B74F-489DAED432C8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
   <si>
     <t>Vehicle</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>Bedford VAL</t>
+  </si>
+  <si>
+    <t>AEC Regent I</t>
+  </si>
+  <si>
+    <t>AEC Regent II</t>
+  </si>
+  <si>
+    <t>AEC Routemaster</t>
   </si>
 </sst>
 </file>
@@ -499,11 +508,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -702,7 +709,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1262,6 +1269,111 @@
         <v>160.43690348545127</v>
       </c>
       <c r="J23" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24">
+        <v>1929</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24">
+        <f>IF(B24 &gt; 1900, ((B24-1900)*10)+400+C24, ((B24-1730)*2)+C24)+VLOOKUP(D24,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>1291</v>
+      </c>
+      <c r="F24">
+        <v>29</v>
+      </c>
+      <c r="G24">
+        <v>50</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" ref="H24:H25" si="14">SQRT(F24*G24)/$B$1</f>
+        <v>126.92955176439848</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" ref="I24:I25" si="15">H24*0.9</f>
+        <v>114.23659658795863</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>1945</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25">
+        <f>IF(B25 &gt; 1900, ((B25-1900)*10)+400+C25, ((B25-1730)*2)+C25)+VLOOKUP(D25,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>1451</v>
+      </c>
+      <c r="F25">
+        <v>38</v>
+      </c>
+      <c r="G25">
+        <v>57</v>
+      </c>
+      <c r="H25" s="2">
+        <f>SQRT(F25*G25)/$B$1</f>
+        <v>155.13435037626795</v>
+      </c>
+      <c r="I25" s="2">
+        <f>H25*0.9</f>
+        <v>139.62091533864117</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26">
+        <v>1954</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26">
+        <f>IF(B26 &gt; 1900, ((B26-1900)*10)+400+C26, ((B26-1730)*2)+C26)+VLOOKUP(D26,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>1541</v>
+      </c>
+      <c r="F26">
+        <v>40</v>
+      </c>
+      <c r="G26">
+        <v>72</v>
+      </c>
+      <c r="H26" s="2">
+        <f>SQRT(F26*G26)/$B$1</f>
+        <v>178.88543819998318</v>
+      </c>
+      <c r="I26" s="2">
+        <f>H26*0.9</f>
+        <v>160.99689437998487</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add BMMO CM5T, ERF C and E series, and tweak model lifetimes
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E82747-7E42-4EDB-B74F-489DAED432C8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B451C148-2822-412D-89BC-F7E215104899}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
   <si>
     <t>Vehicle</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>AEC Routemaster</t>
+  </si>
+  <si>
+    <t>BMMO CM5T</t>
+  </si>
+  <si>
+    <t>ERF C-Series</t>
+  </si>
+  <si>
+    <t>ERF E-Series</t>
   </si>
 </sst>
 </file>
@@ -508,9 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1169,80 +1180,74 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B21">
-        <v>1800</v>
+        <v>1982</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E21">
         <f>IF(B21 &gt; 1900, ((B21-1900)*10)+400+C21, ((B21-1730)*2)+C21)+VLOOKUP(D21,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>741</v>
+        <v>4821</v>
       </c>
       <c r="F21">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="G21">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" ref="H21" si="8">SQRT(F21*G21)/$B$1</f>
-        <v>52.915026221291818</v>
+        <f t="shared" ref="H21:H22" si="8">SQRT(F21*G21)/$B$1</f>
+        <v>136.62601021279465</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" ref="I21" si="9">H21*0.9</f>
-        <v>47.623523599162638</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>33</v>
+        <f t="shared" ref="I21:I22" si="9">H21*0.9</f>
+        <v>122.9634091915152</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B22">
-        <v>1911</v>
+        <v>1986</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E22">
         <f>IF(B22 &gt; 1900, ((B22-1900)*10)+400+C22, ((B22-1730)*2)+C22)+VLOOKUP(D22,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>1111</v>
+        <v>4861</v>
       </c>
       <c r="F22">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="G22">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" ref="H22" si="10">SQRT(F22*G22)/$B$1</f>
-        <v>89.442719099991592</v>
+        <f t="shared" si="8"/>
+        <v>143.75905768565215</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" ref="I22" si="11">H22*0.9</f>
-        <v>80.498447189992433</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>33</v>
+        <f t="shared" si="9"/>
+        <v>129.38315191708693</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B23">
-        <v>1963</v>
+        <v>1800</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1252,21 +1257,21 @@
       </c>
       <c r="E23">
         <f>IF(B23 &gt; 1900, ((B23-1900)*10)+400+C23, ((B23-1730)*2)+C23)+VLOOKUP(D23,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>1631</v>
+        <v>741</v>
       </c>
       <c r="F23">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="G23">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" ref="H23" si="12">SQRT(F23*G23)/$B$1</f>
-        <v>178.26322609494585</v>
+        <f t="shared" ref="H23" si="10">SQRT(F23*G23)/$B$1</f>
+        <v>52.915026221291818</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" ref="I23" si="13">H23*0.9</f>
-        <v>160.43690348545127</v>
+        <f t="shared" ref="I23" si="11">H23*0.9</f>
+        <v>47.623523599162638</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>33</v>
@@ -1274,10 +1279,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24">
-        <v>1929</v>
+        <v>1911</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1287,21 +1292,21 @@
       </c>
       <c r="E24">
         <f>IF(B24 &gt; 1900, ((B24-1900)*10)+400+C24, ((B24-1730)*2)+C24)+VLOOKUP(D24,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>1291</v>
+        <v>1111</v>
       </c>
       <c r="F24">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G24">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" ref="H24:H25" si="14">SQRT(F24*G24)/$B$1</f>
-        <v>126.92955176439848</v>
+        <f t="shared" ref="H24" si="12">SQRT(F24*G24)/$B$1</f>
+        <v>89.442719099991592</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" ref="I24:I25" si="15">H24*0.9</f>
-        <v>114.23659658795863</v>
+        <f t="shared" ref="I24" si="13">H24*0.9</f>
+        <v>80.498447189992433</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>33</v>
@@ -1309,10 +1314,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25">
-        <v>1945</v>
+        <v>1963</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1322,21 +1327,21 @@
       </c>
       <c r="E25">
         <f>IF(B25 &gt; 1900, ((B25-1900)*10)+400+C25, ((B25-1730)*2)+C25)+VLOOKUP(D25,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>1451</v>
+        <v>1631</v>
       </c>
       <c r="F25">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="G25">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H25" s="2">
-        <f>SQRT(F25*G25)/$B$1</f>
-        <v>155.13435037626795</v>
+        <f t="shared" ref="H25" si="14">SQRT(F25*G25)/$B$1</f>
+        <v>178.26322609494585</v>
       </c>
       <c r="I25" s="2">
-        <f>H25*0.9</f>
-        <v>139.62091533864117</v>
+        <f t="shared" ref="I25" si="15">H25*0.9</f>
+        <v>160.43690348545127</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>33</v>
@@ -1344,10 +1349,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26">
-        <v>1954</v>
+        <v>1929</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1357,23 +1362,128 @@
       </c>
       <c r="E26">
         <f>IF(B26 &gt; 1900, ((B26-1900)*10)+400+C26, ((B26-1730)*2)+C26)+VLOOKUP(D26,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>1291</v>
+      </c>
+      <c r="F26">
+        <v>29</v>
+      </c>
+      <c r="G26">
+        <v>50</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" ref="H26" si="16">SQRT(F26*G26)/$B$1</f>
+        <v>126.92955176439848</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" ref="I26" si="17">H26*0.9</f>
+        <v>114.23659658795863</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>1945</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27">
+        <f>IF(B27 &gt; 1900, ((B27-1900)*10)+400+C27, ((B27-1730)*2)+C27)+VLOOKUP(D27,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>1451</v>
+      </c>
+      <c r="F27">
+        <v>38</v>
+      </c>
+      <c r="G27">
+        <v>57</v>
+      </c>
+      <c r="H27" s="2">
+        <f>SQRT(F27*G27)/$B$1</f>
+        <v>155.13435037626795</v>
+      </c>
+      <c r="I27" s="2">
+        <f>H27*0.9</f>
+        <v>139.62091533864117</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28">
+        <v>1954</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28">
+        <f>IF(B28 &gt; 1900, ((B28-1900)*10)+400+C28, ((B28-1730)*2)+C28)+VLOOKUP(D28,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>1541</v>
       </c>
-      <c r="F26">
+      <c r="F28">
         <v>40</v>
       </c>
-      <c r="G26">
+      <c r="G28">
         <v>72</v>
       </c>
-      <c r="H26" s="2">
-        <f>SQRT(F26*G26)/$B$1</f>
+      <c r="H28" s="2">
+        <f>SQRT(F28*G28)/$B$1</f>
         <v>178.88543819998318</v>
       </c>
-      <c r="I26" s="2">
-        <f>H26*0.9</f>
+      <c r="I28" s="2">
+        <f>H28*0.9</f>
         <v>160.99689437998487</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J28" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <v>1958</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29">
+        <f>IF(B29 &gt; 1900, ((B29-1900)*10)+400+C29, ((B29-1730)*2)+C29)+VLOOKUP(D29,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>1581</v>
+      </c>
+      <c r="F29">
+        <v>76</v>
+      </c>
+      <c r="G29">
+        <v>34</v>
+      </c>
+      <c r="H29" s="2">
+        <f>SQRT(F29*G29)/$B$1</f>
+        <v>169.44353369518447</v>
+      </c>
+      <c r="I29" s="2">
+        <f>H29*0.9</f>
+        <v>152.49918032566603</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 32bpp graphics, Volvo B10M and Volvo B12M
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0518EC-03B6-4530-9CE5-260D48E65552}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAE9B30-12D2-458A-B676-2D4518DDEFC2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
   <si>
     <t>Vehicle</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>Leyland Olympian</t>
+  </si>
+  <si>
+    <t>Dennis Enviro400</t>
+  </si>
+  <si>
+    <t>Volvo B10M</t>
+  </si>
+  <si>
+    <t>Volvo B12M</t>
   </si>
 </sst>
 </file>
@@ -520,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1528,6 +1537,111 @@
         <v>175.72421574728963</v>
       </c>
       <c r="J30" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31">
+        <v>2005</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31">
+        <f>IF(B31 &gt; 1900, ((B31-1900)*10)+400+C31, ((B31-1730)*2)+C31)+VLOOKUP(D31,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>2051</v>
+      </c>
+      <c r="F31">
+        <v>60</v>
+      </c>
+      <c r="G31">
+        <v>90</v>
+      </c>
+      <c r="H31" s="2">
+        <f>SQRT(F31*G31)/$B$1</f>
+        <v>244.94897427831785</v>
+      </c>
+      <c r="I31" s="2">
+        <f>H31*0.9</f>
+        <v>220.45407685048608</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32">
+        <v>1978</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32">
+        <f>IF(B32 &gt; 1900, ((B32-1900)*10)+400+C32, ((B32-1730)*2)+C32)+VLOOKUP(D32,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>1781</v>
+      </c>
+      <c r="F32">
+        <v>62</v>
+      </c>
+      <c r="G32">
+        <v>55</v>
+      </c>
+      <c r="H32" s="2">
+        <f>SQRT(F32*G32)/$B$1</f>
+        <v>194.65068427541911</v>
+      </c>
+      <c r="I32" s="2">
+        <f>H32*0.9</f>
+        <v>175.18561584787722</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33">
+        <v>2001</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33">
+        <f>IF(B33 &gt; 1900, ((B33-1900)*10)+400+C33, ((B33-1730)*2)+C33)+VLOOKUP(D33,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>2011</v>
+      </c>
+      <c r="F33">
+        <v>70</v>
+      </c>
+      <c r="G33">
+        <v>58</v>
+      </c>
+      <c r="H33" s="2">
+        <f>SQRT(F33*G33)/$B$1</f>
+        <v>212.39376429431988</v>
+      </c>
+      <c r="I33" s="2">
+        <f>H33*0.9</f>
+        <v>191.15438786488789</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Leyland Steam Van and several small vans
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FFD9B8-A01A-4F22-BE5E-82338FF8C7C1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6966146A-0421-4A5F-AE5C-898DE1086205}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="57">
   <si>
     <t>Vehicle</t>
   </si>
@@ -171,6 +171,27 @@
   </si>
   <si>
     <t>Hancock Enterprise</t>
+  </si>
+  <si>
+    <t>Ford Transit Mk1</t>
+  </si>
+  <si>
+    <t>Ford Transit Mk3</t>
+  </si>
+  <si>
+    <t>Leyland Steam Van</t>
+  </si>
+  <si>
+    <t>Bedford Rascal</t>
+  </si>
+  <si>
+    <t>Ford Transit Custom</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz Sprinter</t>
+  </si>
+  <si>
+    <t>Ford Thames</t>
   </si>
 </sst>
 </file>
@@ -532,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,20 +1286,20 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B23">
-        <v>1800</v>
+        <v>1897</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E23">
         <f>IF(B23 &gt; 1900, ((B23-1900)*10)+400+C23, ((B23-1730)*2)+C23)+VLOOKUP(D23,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>741</v>
+        <v>3935</v>
       </c>
       <c r="F23">
         <v>18</v>
@@ -1300,10 +1321,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B24">
-        <v>1911</v>
+        <v>1800</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1313,21 +1334,21 @@
       </c>
       <c r="E24">
         <f>IF(B24 &gt; 1900, ((B24-1900)*10)+400+C24, ((B24-1730)*2)+C24)+VLOOKUP(D24,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>1111</v>
+        <v>741</v>
       </c>
       <c r="F24">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G24">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" ref="H24" si="12">SQRT(F24*G24)/$B$1</f>
-        <v>89.442719099991592</v>
+        <v>52.915026221291818</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" ref="I24" si="13">H24*0.9</f>
-        <v>80.498447189992433</v>
+        <v>47.623523599162638</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>33</v>
@@ -1335,10 +1356,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25">
-        <v>1963</v>
+        <v>1911</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1348,21 +1369,21 @@
       </c>
       <c r="E25">
         <f>IF(B25 &gt; 1900, ((B25-1900)*10)+400+C25, ((B25-1730)*2)+C25)+VLOOKUP(D25,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>1631</v>
+        <v>1111</v>
       </c>
       <c r="F25">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="G25">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" ref="H25" si="14">SQRT(F25*G25)/$B$1</f>
-        <v>178.26322609494585</v>
+        <v>89.442719099991592</v>
       </c>
       <c r="I25" s="2">
         <f t="shared" ref="I25" si="15">H25*0.9</f>
-        <v>160.43690348545127</v>
+        <v>80.498447189992433</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>33</v>
@@ -1370,10 +1391,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26">
-        <v>1929</v>
+        <v>1963</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1383,21 +1404,21 @@
       </c>
       <c r="E26">
         <f>IF(B26 &gt; 1900, ((B26-1900)*10)+400+C26, ((B26-1730)*2)+C26)+VLOOKUP(D26,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>1291</v>
+        <v>1631</v>
       </c>
       <c r="F26">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="G26">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" ref="H26" si="16">SQRT(F26*G26)/$B$1</f>
-        <v>126.92955176439848</v>
+        <v>178.26322609494585</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" ref="I26" si="17">H26*0.9</f>
-        <v>114.23659658795863</v>
+        <v>160.43690348545127</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>33</v>
@@ -1405,10 +1426,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27">
-        <v>1945</v>
+        <v>1929</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1418,21 +1439,21 @@
       </c>
       <c r="E27">
         <f>IF(B27 &gt; 1900, ((B27-1900)*10)+400+C27, ((B27-1730)*2)+C27)+VLOOKUP(D27,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>1451</v>
+        <v>1291</v>
       </c>
       <c r="F27">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G27">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" ref="H27:H33" si="18">SQRT(F27*G27)/$B$1</f>
-        <v>155.13435037626795</v>
+        <f t="shared" ref="H27" si="18">SQRT(F27*G27)/$B$1</f>
+        <v>126.92955176439848</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" ref="I27:I34" si="19">H27*0.9</f>
-        <v>139.62091533864117</v>
+        <f t="shared" ref="I27" si="19">H27*0.9</f>
+        <v>114.23659658795863</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>33</v>
@@ -1440,10 +1461,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28">
-        <v>1954</v>
+        <v>1945</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1453,21 +1474,21 @@
       </c>
       <c r="E28">
         <f>IF(B28 &gt; 1900, ((B28-1900)*10)+400+C28, ((B28-1730)*2)+C28)+VLOOKUP(D28,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>1541</v>
+        <v>1451</v>
       </c>
       <c r="F28">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G28">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="18"/>
-        <v>178.88543819998318</v>
+        <f t="shared" ref="H28:H34" si="20">SQRT(F28*G28)/$B$1</f>
+        <v>155.13435037626795</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="19"/>
-        <v>160.99689437998487</v>
+        <f t="shared" ref="I28:I35" si="21">H28*0.9</f>
+        <v>139.62091533864117</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>33</v>
@@ -1475,10 +1496,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29">
-        <v>1958</v>
+        <v>1954</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1488,21 +1509,21 @@
       </c>
       <c r="E29">
         <f>IF(B29 &gt; 1900, ((B29-1900)*10)+400+C29, ((B29-1730)*2)+C29)+VLOOKUP(D29,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>1581</v>
+        <v>1541</v>
       </c>
       <c r="F29">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="G29">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" si="18"/>
-        <v>169.44353369518447</v>
+        <f t="shared" si="20"/>
+        <v>178.88543819998318</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="19"/>
-        <v>152.49918032566603</v>
+        <f t="shared" si="21"/>
+        <v>160.99689437998487</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>33</v>
@@ -1510,10 +1531,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B30">
-        <v>1980</v>
+        <v>1958</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1523,21 +1544,21 @@
       </c>
       <c r="E30">
         <f>IF(B30 &gt; 1900, ((B30-1900)*10)+400+C30, ((B30-1730)*2)+C30)+VLOOKUP(D30,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>1801</v>
+        <v>1581</v>
       </c>
       <c r="F30">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="G30">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="18"/>
-        <v>195.2491286080996</v>
+        <f t="shared" si="20"/>
+        <v>169.44353369518447</v>
       </c>
       <c r="I30" s="2">
-        <f t="shared" si="19"/>
-        <v>175.72421574728963</v>
+        <f t="shared" si="21"/>
+        <v>152.49918032566603</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>33</v>
@@ -1545,10 +1566,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31">
-        <v>2005</v>
+        <v>1980</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1558,21 +1579,21 @@
       </c>
       <c r="E31">
         <f>IF(B31 &gt; 1900, ((B31-1900)*10)+400+C31, ((B31-1730)*2)+C31)+VLOOKUP(D31,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>2051</v>
+        <v>1801</v>
       </c>
       <c r="F31">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G31">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="18"/>
-        <v>244.94897427831785</v>
+        <f t="shared" si="20"/>
+        <v>195.2491286080996</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="19"/>
-        <v>220.45407685048608</v>
+        <f t="shared" si="21"/>
+        <v>175.72421574728963</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>33</v>
@@ -1580,10 +1601,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32">
-        <v>1978</v>
+        <v>2005</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1593,21 +1614,21 @@
       </c>
       <c r="E32">
         <f>IF(B32 &gt; 1900, ((B32-1900)*10)+400+C32, ((B32-1730)*2)+C32)+VLOOKUP(D32,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>1781</v>
+        <v>2051</v>
       </c>
       <c r="F32">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G32">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="18"/>
-        <v>194.65068427541911</v>
+        <f t="shared" si="20"/>
+        <v>244.94897427831785</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="19"/>
-        <v>175.18561584787722</v>
+        <f t="shared" si="21"/>
+        <v>220.45407685048608</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>33</v>
@@ -1615,10 +1636,10 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33">
-        <v>2001</v>
+        <v>1978</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1628,21 +1649,21 @@
       </c>
       <c r="E33">
         <f>IF(B33 &gt; 1900, ((B33-1900)*10)+400+C33, ((B33-1730)*2)+C33)+VLOOKUP(D33,'ID Scheme'!$A$2:$B$4,2)</f>
-        <v>2011</v>
+        <v>1781</v>
       </c>
       <c r="F33">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G33">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="18"/>
-        <v>212.39376429431988</v>
+        <f t="shared" si="20"/>
+        <v>194.65068427541911</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="19"/>
-        <v>191.15438786488789</v>
+        <f t="shared" si="21"/>
+        <v>175.18561584787722</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>33</v>
@@ -1650,10 +1671,10 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34">
-        <v>1833</v>
+        <v>2001</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -1663,23 +1684,268 @@
       </c>
       <c r="E34">
         <f>IF(B34 &gt; 1900, ((B34-1900)*10)+400+C34, ((B34-1730)*2)+C34)+VLOOKUP(D34,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>2011</v>
+      </c>
+      <c r="F34">
+        <v>70</v>
+      </c>
+      <c r="G34">
+        <v>58</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="20"/>
+        <v>212.39376429431988</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="21"/>
+        <v>191.15438786488789</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35">
+        <v>1833</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35">
+        <f>IF(B35 &gt; 1900, ((B35-1900)*10)+400+C35, ((B35-1730)*2)+C35)+VLOOKUP(D35,'ID Scheme'!$A$2:$B$4,2)</f>
         <v>807</v>
       </c>
-      <c r="F34">
+      <c r="F35">
         <v>18</v>
       </c>
-      <c r="G34">
-        <v>22</v>
-      </c>
-      <c r="H34" s="2">
-        <f t="shared" ref="H34" si="20">SQRT(F34*G34)/$B$1</f>
+      <c r="G35">
+        <v>22</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" ref="H35" si="22">SQRT(F35*G35)/$B$1</f>
         <v>66.332495807108003</v>
       </c>
-      <c r="I34" s="2">
-        <f t="shared" si="19"/>
+      <c r="I35" s="2">
+        <f t="shared" si="21"/>
         <v>59.699246226397207</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J35" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36">
+        <v>1965</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36">
+        <f>IF(B36 &gt; 1900, ((B36-1900)*10)+400+C36, ((B36-1730)*2)+C36)+VLOOKUP(D36,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>7651</v>
+      </c>
+      <c r="F36">
+        <v>65</v>
+      </c>
+      <c r="G36">
+        <v>8</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" ref="H36" si="23">SQRT(F36*G36)/$B$1</f>
+        <v>76.011695006609202</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" ref="I36" si="24">H36*0.9</f>
+        <v>68.410525505948286</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37">
+        <v>1986</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37">
+        <f>IF(B37 &gt; 1900, ((B37-1900)*10)+400+C37, ((B37-1730)*2)+C37)+VLOOKUP(D37,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>7861</v>
+      </c>
+      <c r="F37">
+        <v>80</v>
+      </c>
+      <c r="G37">
+        <v>10</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" ref="H37" si="25">SQRT(F37*G37)/$B$1</f>
+        <v>94.28090415820634</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" ref="I37" si="26">H37*0.9</f>
+        <v>84.852813742385706</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38">
+        <v>1986</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38">
+        <f>IF(B38 &gt; 1900, ((B38-1900)*10)+400+C38, ((B38-1730)*2)+C38)+VLOOKUP(D38,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>7862</v>
+      </c>
+      <c r="F38">
+        <v>65</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" ref="H38:H39" si="27">SQRT(F38*G38)/$B$1</f>
+        <v>53.748384988656994</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" ref="I38:I39" si="28">H38*0.9</f>
+        <v>48.373546489791295</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39">
+        <v>2012</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39">
+        <f>IF(B39 &gt; 1900, ((B39-1900)*10)+400+C39, ((B39-1730)*2)+C39)+VLOOKUP(D39,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>8121</v>
+      </c>
+      <c r="F39">
+        <v>92</v>
+      </c>
+      <c r="G39">
+        <v>10</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="27"/>
+        <v>101.10500592068735</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="28"/>
+        <v>90.994505328618615</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40">
+        <v>2006</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40">
+        <f>IF(B40 &gt; 1900, ((B40-1900)*10)+400+C40, ((B40-1730)*2)+C40)+VLOOKUP(D40,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>8061</v>
+      </c>
+      <c r="F40">
+        <v>85</v>
+      </c>
+      <c r="G40">
+        <v>12</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" ref="H40" si="29">SQRT(F40*G40)/$B$1</f>
+        <v>106.45812948447541</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" ref="I40" si="30">H40*0.9</f>
+        <v>95.812316536027865</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41">
+        <v>1957</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41">
+        <f>IF(B41 &gt; 1900, ((B41-1900)*10)+400+C41, ((B41-1730)*2)+C41)+VLOOKUP(D41,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>7571</v>
+      </c>
+      <c r="F41">
+        <v>60</v>
+      </c>
+      <c r="G41">
+        <v>6</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" ref="H41" si="31">SQRT(F41*G41)/$B$1</f>
+        <v>63.245553203367592</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" ref="I41" si="32">H41*0.9</f>
+        <v>56.920997883030836</v>
+      </c>
+      <c r="J41" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added single deck buses and removed the Bob-compatibility parameter
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6966146A-0421-4A5F-AE5C-898DE1086205}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B38784-F2CD-4932-B7BE-170CF9DD013E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="62">
   <si>
     <t>Vehicle</t>
   </si>
@@ -192,6 +192,21 @@
   </si>
   <si>
     <t>Ford Thames</t>
+  </si>
+  <si>
+    <t>Northern General SE6</t>
+  </si>
+  <si>
+    <t>Leyland Tiger TS</t>
+  </si>
+  <si>
+    <t>Leyland National</t>
+  </si>
+  <si>
+    <t>Dennis Dart</t>
+  </si>
+  <si>
+    <t>Sentinel Steam Bus</t>
   </si>
 </sst>
 </file>
@@ -553,10 +568,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,6 +1962,181 @@
         <v>56.920997883030836</v>
       </c>
       <c r="J41" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42">
+        <v>1933</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42">
+        <f>IF(B42 &gt; 1900, ((B42-1900)*10)+400+C42, ((B42-1730)*2)+C42)+VLOOKUP(D42,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>1331</v>
+      </c>
+      <c r="F42">
+        <v>40</v>
+      </c>
+      <c r="G42">
+        <v>44</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" ref="H42" si="33">SQRT(F42*G42)/$B$1</f>
+        <v>139.84117975602021</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" ref="I42" si="34">H42*0.9</f>
+        <v>125.85706178041819</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43">
+        <v>1927</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43">
+        <f>IF(B43 &gt; 1900, ((B43-1900)*10)+400+C43, ((B43-1730)*2)+C43)+VLOOKUP(D43,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>1271</v>
+      </c>
+      <c r="F43">
+        <v>42</v>
+      </c>
+      <c r="G43">
+        <v>35</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" ref="H43" si="35">SQRT(F43*G43)/$B$1</f>
+        <v>127.80193008453877</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" ref="I43" si="36">H43*0.9</f>
+        <v>115.02173707608489</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44">
+        <v>1972</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44">
+        <f>IF(B44 &gt; 1900, ((B44-1900)*10)+400+C44, ((B44-1730)*2)+C44)+VLOOKUP(D44,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>1721</v>
+      </c>
+      <c r="F44">
+        <v>52</v>
+      </c>
+      <c r="G44">
+        <v>58</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" ref="H44" si="37">SQRT(F44*G44)/$B$1</f>
+        <v>183.06040290327977</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" ref="I44" si="38">H44*0.9</f>
+        <v>164.75436261295178</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45">
+        <v>1989</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45">
+        <f>IF(B45 &gt; 1900, ((B45-1900)*10)+400+C45, ((B45-1730)*2)+C45)+VLOOKUP(D45,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>1891</v>
+      </c>
+      <c r="F45">
+        <v>56</v>
+      </c>
+      <c r="G45">
+        <v>50</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" ref="H45" si="39">SQRT(F45*G45)/$B$1</f>
+        <v>176.38342073763937</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" ref="I45" si="40">H45*0.9</f>
+        <v>158.74507866387543</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46">
+        <v>1924</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46">
+        <f>IF(B46 &gt; 1900, ((B46-1900)*10)+400+C46, ((B46-1730)*2)+C46)+VLOOKUP(D46,'ID Scheme'!$A$2:$B$4,2)</f>
+        <v>1241</v>
+      </c>
+      <c r="F46">
+        <v>36</v>
+      </c>
+      <c r="G46">
+        <v>32</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" ref="H46" si="41">SQRT(F46*G46)/$B$1</f>
+        <v>113.13708498984759</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" ref="I46" si="42">H46*0.9</f>
+        <v>101.82337649086284</v>
+      </c>
+      <c r="J46" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added cabs and minicabs, plus parameters to switch on/off vehicle classes
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B38784-F2CD-4932-B7BE-170CF9DD013E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308D7107-4A2B-441B-95D5-5600B6F91802}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
   <si>
     <t>Vehicle</t>
   </si>
@@ -207,6 +207,33 @@
   </si>
   <si>
     <t>Sentinel Steam Bus</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Austin FX4</t>
+  </si>
+  <si>
+    <t>LTI TX1</t>
+  </si>
+  <si>
+    <t>Ford Cortina</t>
+  </si>
+  <si>
+    <t>Vauxhall Omega</t>
+  </si>
+  <si>
+    <t>Toyota Prius</t>
+  </si>
+  <si>
+    <t>Volvo S40 T5</t>
+  </si>
+  <si>
+    <t>68hp</t>
+  </si>
+  <si>
+    <t>88hp</t>
   </si>
 </sst>
 </file>
@@ -568,11 +595,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
+      <pane ySplit="3" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +673,7 @@
         <v>22</v>
       </c>
       <c r="E4">
-        <f>IF(B4 &gt; 1900, ((B4-1900)*10)+400+C4, ((B4-1730)*2)+C4)+VLOOKUP(D4,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B4 &gt; 1900, ((B4-1900)*10)+400+C4, ((B4-1730)*2)+C4)+VLOOKUP(D4,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>3741</v>
       </c>
       <c r="F4">
@@ -681,7 +708,7 @@
         <v>22</v>
       </c>
       <c r="E5">
-        <f>IF(B5 &gt; 1900, ((B5-1900)*10)+400+C5, ((B5-1730)*2)+C5)+VLOOKUP(D5,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B5 &gt; 1900, ((B5-1900)*10)+400+C5, ((B5-1730)*2)+C5)+VLOOKUP(D5,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4131</v>
       </c>
       <c r="F5">
@@ -716,7 +743,7 @@
         <v>22</v>
       </c>
       <c r="E6">
-        <f>IF(B6 &gt; 1900, ((B6-1900)*10)+400+C6, ((B6-1730)*2)+C6)+VLOOKUP(D6,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B6 &gt; 1900, ((B6-1900)*10)+400+C6, ((B6-1730)*2)+C6)+VLOOKUP(D6,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4071</v>
       </c>
       <c r="F6">
@@ -751,7 +778,7 @@
         <v>22</v>
       </c>
       <c r="E7">
-        <f>IF(B7 &gt; 1900, ((B7-1900)*10)+400+C7, ((B7-1730)*2)+C7)+VLOOKUP(D7,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B7 &gt; 1900, ((B7-1900)*10)+400+C7, ((B7-1730)*2)+C7)+VLOOKUP(D7,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4361</v>
       </c>
       <c r="F7">
@@ -786,7 +813,7 @@
         <v>22</v>
       </c>
       <c r="E8">
-        <f>IF(B8 &gt; 1900, ((B8-1900)*10)+400+C8, ((B8-1730)*2)+C8)+VLOOKUP(D8,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B8 &gt; 1900, ((B8-1900)*10)+400+C8, ((B8-1730)*2)+C8)+VLOOKUP(D8,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4521</v>
       </c>
       <c r="F8">
@@ -821,7 +848,7 @@
         <v>22</v>
       </c>
       <c r="E9">
-        <f>IF(B9 &gt; 1900, ((B9-1900)*10)+400+C9, ((B9-1730)*2)+C9)+VLOOKUP(D9,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B9 &gt; 1900, ((B9-1900)*10)+400+C9, ((B9-1730)*2)+C9)+VLOOKUP(D9,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4571</v>
       </c>
       <c r="F9">
@@ -856,7 +883,7 @@
         <v>22</v>
       </c>
       <c r="E10">
-        <f>IF(B10 &gt; 1900, ((B10-1900)*10)+400+C10, ((B10-1730)*2)+C10)+VLOOKUP(D10,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B10 &gt; 1900, ((B10-1900)*10)+400+C10, ((B10-1730)*2)+C10)+VLOOKUP(D10,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4631</v>
       </c>
       <c r="F10">
@@ -891,7 +918,7 @@
         <v>22</v>
       </c>
       <c r="E11">
-        <f>IF(B11 &gt; 1900, ((B11-1900)*10)+400+C11, ((B11-1730)*2)+C11)+VLOOKUP(D11,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B11 &gt; 1900, ((B11-1900)*10)+400+C11, ((B11-1730)*2)+C11)+VLOOKUP(D11,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4651</v>
       </c>
       <c r="F11">
@@ -926,7 +953,7 @@
         <v>22</v>
       </c>
       <c r="E12">
-        <f>IF(B12 &gt; 1900, ((B12-1900)*10)+400+C12, ((B12-1730)*2)+C12)+VLOOKUP(D12,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B12 &gt; 1900, ((B12-1900)*10)+400+C12, ((B12-1730)*2)+C12)+VLOOKUP(D12,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4681</v>
       </c>
       <c r="F12">
@@ -961,7 +988,7 @@
         <v>22</v>
       </c>
       <c r="E13">
-        <f>IF(B13 &gt; 1900, ((B13-1900)*10)+400+C13, ((B13-1730)*2)+C13)+VLOOKUP(D13,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B13 &gt; 1900, ((B13-1900)*10)+400+C13, ((B13-1730)*2)+C13)+VLOOKUP(D13,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4801</v>
       </c>
       <c r="F13">
@@ -996,7 +1023,7 @@
         <v>22</v>
       </c>
       <c r="E14">
-        <f>IF(B14 &gt; 1900, ((B14-1900)*10)+400+C14, ((B14-1730)*2)+C14)+VLOOKUP(D14,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B14 &gt; 1900, ((B14-1900)*10)+400+C14, ((B14-1730)*2)+C14)+VLOOKUP(D14,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4021</v>
       </c>
       <c r="F14">
@@ -1031,7 +1058,7 @@
         <v>22</v>
       </c>
       <c r="E15">
-        <f>IF(B15 &gt; 1900, ((B15-1900)*10)+400+C15, ((B15-1730)*2)+C15)+VLOOKUP(D15,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B15 &gt; 1900, ((B15-1900)*10)+400+C15, ((B15-1730)*2)+C15)+VLOOKUP(D15,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4971</v>
       </c>
       <c r="F15">
@@ -1066,7 +1093,7 @@
         <v>22</v>
       </c>
       <c r="E16">
-        <f>IF(B16 &gt; 1900, ((B16-1900)*10)+400+C16, ((B16-1730)*2)+C16)+VLOOKUP(D16,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B16 &gt; 1900, ((B16-1900)*10)+400+C16, ((B16-1730)*2)+C16)+VLOOKUP(D16,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4871</v>
       </c>
       <c r="F16">
@@ -1101,7 +1128,7 @@
         <v>22</v>
       </c>
       <c r="E17">
-        <f>IF(B17 &gt; 1900, ((B17-1900)*10)+400+C17, ((B17-1730)*2)+C17)+VLOOKUP(D17,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B17 &gt; 1900, ((B17-1900)*10)+400+C17, ((B17-1730)*2)+C17)+VLOOKUP(D17,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4951</v>
       </c>
       <c r="F17">
@@ -1136,7 +1163,7 @@
         <v>22</v>
       </c>
       <c r="E18">
-        <f>IF(B18 &gt; 1900, ((B18-1900)*10)+400+C18, ((B18-1730)*2)+C18)+VLOOKUP(D18,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B18 &gt; 1900, ((B18-1900)*10)+400+C18, ((B18-1730)*2)+C18)+VLOOKUP(D18,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>5041</v>
       </c>
       <c r="F18">
@@ -1171,7 +1198,7 @@
         <v>22</v>
       </c>
       <c r="E19">
-        <f>IF(B19 &gt; 1900, ((B19-1900)*10)+400+C19, ((B19-1730)*2)+C19)+VLOOKUP(D19,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B19 &gt; 1900, ((B19-1900)*10)+400+C19, ((B19-1730)*2)+C19)+VLOOKUP(D19,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4641</v>
       </c>
       <c r="F19">
@@ -1206,7 +1233,7 @@
         <v>22</v>
       </c>
       <c r="E20">
-        <f>IF(B20 &gt; 1900, ((B20-1900)*10)+400+C20, ((B20-1730)*2)+C20)+VLOOKUP(D20,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B20 &gt; 1900, ((B20-1900)*10)+400+C20, ((B20-1730)*2)+C20)+VLOOKUP(D20,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4642</v>
       </c>
       <c r="F20">
@@ -1244,7 +1271,7 @@
         <v>22</v>
       </c>
       <c r="E21">
-        <f>IF(B21 &gt; 1900, ((B21-1900)*10)+400+C21, ((B21-1730)*2)+C21)+VLOOKUP(D21,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B21 &gt; 1900, ((B21-1900)*10)+400+C21, ((B21-1730)*2)+C21)+VLOOKUP(D21,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4821</v>
       </c>
       <c r="F21">
@@ -1279,7 +1306,7 @@
         <v>22</v>
       </c>
       <c r="E22">
-        <f>IF(B22 &gt; 1900, ((B22-1900)*10)+400+C22, ((B22-1730)*2)+C22)+VLOOKUP(D22,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B22 &gt; 1900, ((B22-1900)*10)+400+C22, ((B22-1730)*2)+C22)+VLOOKUP(D22,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>4861</v>
       </c>
       <c r="F22">
@@ -1314,7 +1341,7 @@
         <v>22</v>
       </c>
       <c r="E23">
-        <f>IF(B23 &gt; 1900, ((B23-1900)*10)+400+C23, ((B23-1730)*2)+C23)+VLOOKUP(D23,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B23 &gt; 1900, ((B23-1900)*10)+400+C23, ((B23-1730)*2)+C23)+VLOOKUP(D23,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>3935</v>
       </c>
       <c r="F23">
@@ -1349,7 +1376,7 @@
         <v>21</v>
       </c>
       <c r="E24">
-        <f>IF(B24 &gt; 1900, ((B24-1900)*10)+400+C24, ((B24-1730)*2)+C24)+VLOOKUP(D24,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B24 &gt; 1900, ((B24-1900)*10)+400+C24, ((B24-1730)*2)+C24)+VLOOKUP(D24,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>741</v>
       </c>
       <c r="F24">
@@ -1384,7 +1411,7 @@
         <v>21</v>
       </c>
       <c r="E25">
-        <f>IF(B25 &gt; 1900, ((B25-1900)*10)+400+C25, ((B25-1730)*2)+C25)+VLOOKUP(D25,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B25 &gt; 1900, ((B25-1900)*10)+400+C25, ((B25-1730)*2)+C25)+VLOOKUP(D25,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1111</v>
       </c>
       <c r="F25">
@@ -1419,7 +1446,7 @@
         <v>21</v>
       </c>
       <c r="E26">
-        <f>IF(B26 &gt; 1900, ((B26-1900)*10)+400+C26, ((B26-1730)*2)+C26)+VLOOKUP(D26,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B26 &gt; 1900, ((B26-1900)*10)+400+C26, ((B26-1730)*2)+C26)+VLOOKUP(D26,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1631</v>
       </c>
       <c r="F26">
@@ -1454,7 +1481,7 @@
         <v>21</v>
       </c>
       <c r="E27">
-        <f>IF(B27 &gt; 1900, ((B27-1900)*10)+400+C27, ((B27-1730)*2)+C27)+VLOOKUP(D27,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B27 &gt; 1900, ((B27-1900)*10)+400+C27, ((B27-1730)*2)+C27)+VLOOKUP(D27,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1291</v>
       </c>
       <c r="F27">
@@ -1489,7 +1516,7 @@
         <v>21</v>
       </c>
       <c r="E28">
-        <f>IF(B28 &gt; 1900, ((B28-1900)*10)+400+C28, ((B28-1730)*2)+C28)+VLOOKUP(D28,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B28 &gt; 1900, ((B28-1900)*10)+400+C28, ((B28-1730)*2)+C28)+VLOOKUP(D28,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1451</v>
       </c>
       <c r="F28">
@@ -1524,7 +1551,7 @@
         <v>21</v>
       </c>
       <c r="E29">
-        <f>IF(B29 &gt; 1900, ((B29-1900)*10)+400+C29, ((B29-1730)*2)+C29)+VLOOKUP(D29,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B29 &gt; 1900, ((B29-1900)*10)+400+C29, ((B29-1730)*2)+C29)+VLOOKUP(D29,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1541</v>
       </c>
       <c r="F29">
@@ -1559,7 +1586,7 @@
         <v>21</v>
       </c>
       <c r="E30">
-        <f>IF(B30 &gt; 1900, ((B30-1900)*10)+400+C30, ((B30-1730)*2)+C30)+VLOOKUP(D30,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B30 &gt; 1900, ((B30-1900)*10)+400+C30, ((B30-1730)*2)+C30)+VLOOKUP(D30,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1581</v>
       </c>
       <c r="F30">
@@ -1594,7 +1621,7 @@
         <v>21</v>
       </c>
       <c r="E31">
-        <f>IF(B31 &gt; 1900, ((B31-1900)*10)+400+C31, ((B31-1730)*2)+C31)+VLOOKUP(D31,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B31 &gt; 1900, ((B31-1900)*10)+400+C31, ((B31-1730)*2)+C31)+VLOOKUP(D31,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1801</v>
       </c>
       <c r="F31">
@@ -1629,7 +1656,7 @@
         <v>21</v>
       </c>
       <c r="E32">
-        <f>IF(B32 &gt; 1900, ((B32-1900)*10)+400+C32, ((B32-1730)*2)+C32)+VLOOKUP(D32,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B32 &gt; 1900, ((B32-1900)*10)+400+C32, ((B32-1730)*2)+C32)+VLOOKUP(D32,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>2051</v>
       </c>
       <c r="F32">
@@ -1650,7 +1677,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -1664,7 +1691,7 @@
         <v>21</v>
       </c>
       <c r="E33">
-        <f>IF(B33 &gt; 1900, ((B33-1900)*10)+400+C33, ((B33-1730)*2)+C33)+VLOOKUP(D33,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B33 &gt; 1900, ((B33-1900)*10)+400+C33, ((B33-1730)*2)+C33)+VLOOKUP(D33,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1781</v>
       </c>
       <c r="F33">
@@ -1685,7 +1712,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -1699,7 +1726,7 @@
         <v>21</v>
       </c>
       <c r="E34">
-        <f>IF(B34 &gt; 1900, ((B34-1900)*10)+400+C34, ((B34-1730)*2)+C34)+VLOOKUP(D34,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B34 &gt; 1900, ((B34-1900)*10)+400+C34, ((B34-1730)*2)+C34)+VLOOKUP(D34,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>2011</v>
       </c>
       <c r="F34">
@@ -1720,7 +1747,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -1734,7 +1761,7 @@
         <v>21</v>
       </c>
       <c r="E35">
-        <f>IF(B35 &gt; 1900, ((B35-1900)*10)+400+C35, ((B35-1730)*2)+C35)+VLOOKUP(D35,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B35 &gt; 1900, ((B35-1900)*10)+400+C35, ((B35-1730)*2)+C35)+VLOOKUP(D35,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>807</v>
       </c>
       <c r="F35">
@@ -1755,7 +1782,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -1769,7 +1796,7 @@
         <v>23</v>
       </c>
       <c r="E36">
-        <f>IF(B36 &gt; 1900, ((B36-1900)*10)+400+C36, ((B36-1730)*2)+C36)+VLOOKUP(D36,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B36 &gt; 1900, ((B36-1900)*10)+400+C36, ((B36-1730)*2)+C36)+VLOOKUP(D36,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>7651</v>
       </c>
       <c r="F36">
@@ -1790,7 +1817,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -1804,7 +1831,7 @@
         <v>23</v>
       </c>
       <c r="E37">
-        <f>IF(B37 &gt; 1900, ((B37-1900)*10)+400+C37, ((B37-1730)*2)+C37)+VLOOKUP(D37,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B37 &gt; 1900, ((B37-1900)*10)+400+C37, ((B37-1730)*2)+C37)+VLOOKUP(D37,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>7861</v>
       </c>
       <c r="F37">
@@ -1825,7 +1852,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -1839,7 +1866,7 @@
         <v>23</v>
       </c>
       <c r="E38">
-        <f>IF(B38 &gt; 1900, ((B38-1900)*10)+400+C38, ((B38-1730)*2)+C38)+VLOOKUP(D38,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B38 &gt; 1900, ((B38-1900)*10)+400+C38, ((B38-1730)*2)+C38)+VLOOKUP(D38,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>7862</v>
       </c>
       <c r="F38">
@@ -1860,7 +1887,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -1874,7 +1901,7 @@
         <v>23</v>
       </c>
       <c r="E39">
-        <f>IF(B39 &gt; 1900, ((B39-1900)*10)+400+C39, ((B39-1730)*2)+C39)+VLOOKUP(D39,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B39 &gt; 1900, ((B39-1900)*10)+400+C39, ((B39-1730)*2)+C39)+VLOOKUP(D39,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>8121</v>
       </c>
       <c r="F39">
@@ -1895,7 +1922,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -1909,7 +1936,7 @@
         <v>23</v>
       </c>
       <c r="E40">
-        <f>IF(B40 &gt; 1900, ((B40-1900)*10)+400+C40, ((B40-1730)*2)+C40)+VLOOKUP(D40,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B40 &gt; 1900, ((B40-1900)*10)+400+C40, ((B40-1730)*2)+C40)+VLOOKUP(D40,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>8061</v>
       </c>
       <c r="F40">
@@ -1930,7 +1957,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -1944,7 +1971,7 @@
         <v>23</v>
       </c>
       <c r="E41">
-        <f>IF(B41 &gt; 1900, ((B41-1900)*10)+400+C41, ((B41-1730)*2)+C41)+VLOOKUP(D41,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B41 &gt; 1900, ((B41-1900)*10)+400+C41, ((B41-1730)*2)+C41)+VLOOKUP(D41,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>7571</v>
       </c>
       <c r="F41">
@@ -1965,7 +1992,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -1979,7 +2006,7 @@
         <v>21</v>
       </c>
       <c r="E42">
-        <f>IF(B42 &gt; 1900, ((B42-1900)*10)+400+C42, ((B42-1730)*2)+C42)+VLOOKUP(D42,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B42 &gt; 1900, ((B42-1900)*10)+400+C42, ((B42-1730)*2)+C42)+VLOOKUP(D42,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1331</v>
       </c>
       <c r="F42">
@@ -2000,7 +2027,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2014,7 +2041,7 @@
         <v>21</v>
       </c>
       <c r="E43">
-        <f>IF(B43 &gt; 1900, ((B43-1900)*10)+400+C43, ((B43-1730)*2)+C43)+VLOOKUP(D43,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B43 &gt; 1900, ((B43-1900)*10)+400+C43, ((B43-1730)*2)+C43)+VLOOKUP(D43,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1271</v>
       </c>
       <c r="F43">
@@ -2035,7 +2062,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -2049,7 +2076,7 @@
         <v>21</v>
       </c>
       <c r="E44">
-        <f>IF(B44 &gt; 1900, ((B44-1900)*10)+400+C44, ((B44-1730)*2)+C44)+VLOOKUP(D44,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B44 &gt; 1900, ((B44-1900)*10)+400+C44, ((B44-1730)*2)+C44)+VLOOKUP(D44,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1721</v>
       </c>
       <c r="F44">
@@ -2070,7 +2097,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -2084,7 +2111,7 @@
         <v>21</v>
       </c>
       <c r="E45">
-        <f>IF(B45 &gt; 1900, ((B45-1900)*10)+400+C45, ((B45-1730)*2)+C45)+VLOOKUP(D45,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B45 &gt; 1900, ((B45-1900)*10)+400+C45, ((B45-1730)*2)+C45)+VLOOKUP(D45,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1891</v>
       </c>
       <c r="F45">
@@ -2105,7 +2132,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -2119,7 +2146,7 @@
         <v>21</v>
       </c>
       <c r="E46">
-        <f>IF(B46 &gt; 1900, ((B46-1900)*10)+400+C46, ((B46-1730)*2)+C46)+VLOOKUP(D46,'ID Scheme'!$A$2:$B$4,2)</f>
+        <f>IF(B46 &gt; 1900, ((B46-1900)*10)+400+C46, ((B46-1730)*2)+C46)+VLOOKUP(D46,'ID Scheme'!$A$2:$B$5,2)</f>
         <v>1241</v>
       </c>
       <c r="F46">
@@ -2137,6 +2164,222 @@
         <v>101.82337649086284</v>
       </c>
       <c r="J46" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47">
+        <v>1958</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47">
+        <f>IF(B47 &gt; 1900, ((B47-1900)*10)+400+C47, ((B47-1730)*2)+C47)+VLOOKUP(D47,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>10581</v>
+      </c>
+      <c r="F47">
+        <v>75</v>
+      </c>
+      <c r="G47">
+        <v>4</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" ref="H47" si="43">SQRT(F47*G47)/$B$1</f>
+        <v>57.735026918962582</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" ref="I47" si="44">H47*0.9</f>
+        <v>51.961524227066327</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48">
+        <v>1997</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>62</v>
+      </c>
+      <c r="E48">
+        <f>IF(B48 &gt; 1900, ((B48-1900)*10)+400+C48, ((B48-1730)*2)+C48)+VLOOKUP(D48,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>10971</v>
+      </c>
+      <c r="F48">
+        <v>81</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" ref="H48:H52" si="45">SQRT(F48*G48)/$B$1</f>
+        <v>67.082039324993701</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" ref="I48:I52" si="46">H48*0.9</f>
+        <v>60.373835392494335</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49">
+        <v>1976</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>62</v>
+      </c>
+      <c r="E49">
+        <f>IF(B49 &gt; 1900, ((B49-1900)*10)+400+C49, ((B49-1730)*2)+C49)+VLOOKUP(D49,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>10761</v>
+      </c>
+      <c r="F49">
+        <v>90</v>
+      </c>
+      <c r="G49">
+        <v>4</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="45"/>
+        <v>63.245553203367592</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="46"/>
+        <v>56.920997883030836</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50">
+        <v>1994</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>62</v>
+      </c>
+      <c r="E50">
+        <f>IF(B50 &gt; 1900, ((B50-1900)*10)+400+C50, ((B50-1730)*2)+C50)+VLOOKUP(D50,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>10941</v>
+      </c>
+      <c r="F50">
+        <v>120</v>
+      </c>
+      <c r="G50">
+        <v>4</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="45"/>
+        <v>73.029674334022147</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="46"/>
+        <v>65.726706900619931</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51">
+        <v>2009</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>62</v>
+      </c>
+      <c r="E51">
+        <f>IF(B51 &gt; 1900, ((B51-1900)*10)+400+C51, ((B51-1730)*2)+C51)+VLOOKUP(D51,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>11091</v>
+      </c>
+      <c r="F51">
+        <v>112</v>
+      </c>
+      <c r="G51">
+        <v>4</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="45"/>
+        <v>70.553368295055762</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="46"/>
+        <v>63.498031465550184</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52">
+        <v>2004</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>62</v>
+      </c>
+      <c r="E52">
+        <f>IF(B52 &gt; 1900, ((B52-1900)*10)+400+C52, ((B52-1730)*2)+C52)+VLOOKUP(D52,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>11041</v>
+      </c>
+      <c r="F52">
+        <v>145</v>
+      </c>
+      <c r="G52">
+        <v>4</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="45"/>
+        <v>80.277297191948648</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="46"/>
+        <v>72.249567472753782</v>
+      </c>
+      <c r="J52" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2151,7 +2394,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
-            <xm:f>'ID Scheme'!$A$2:$A$4</xm:f>
+            <xm:f>'ID Scheme'!$A$2:$A$5</xm:f>
           </x14:formula1>
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
@@ -2163,11 +2406,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2206,6 +2447,14 @@
         <v>6600</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5">
+        <v>9600</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Ford Model T
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308D7107-4A2B-441B-95D5-5600B6F91802}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AF8876-811C-4FE9-99EE-A2EF6320923C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="72">
   <si>
     <t>Vehicle</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>88hp</t>
+  </si>
+  <si>
+    <t>Ford Model T</t>
   </si>
 </sst>
 </file>
@@ -595,11 +598,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,6 +2383,41 @@
         <v>72.249567472753782</v>
       </c>
       <c r="J52" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53">
+        <v>1908</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53">
+        <f>IF(B53 &gt; 1900, ((B53-1900)*10)+400+C53, ((B53-1730)*2)+C53)+VLOOKUP(D53,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>7081</v>
+      </c>
+      <c r="F53">
+        <v>40</v>
+      </c>
+      <c r="G53">
+        <v>4</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" ref="H53" si="47">SQRT(F53*G53)/$B$1</f>
+        <v>42.163702135578397</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" ref="I53" si="48">H53*0.9</f>
+        <v>37.94733192202056</v>
+      </c>
+      <c r="J53" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Leyland Leopard and Mercedes Citaro
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AF8876-811C-4FE9-99EE-A2EF6320923C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED978EC5-E140-42E0-BA03-61D140E09E3B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="74">
   <si>
     <t>Vehicle</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>Ford Model T</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz Citaro</t>
+  </si>
+  <si>
+    <t>Leyland Leopard</t>
   </si>
 </sst>
 </file>
@@ -598,11 +604,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I53" sqref="I53"/>
+      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2391,7 +2397,7 @@
         <v>71</v>
       </c>
       <c r="B53">
-        <v>1908</v>
+        <v>1912</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -2401,7 +2407,7 @@
       </c>
       <c r="E53">
         <f>IF(B53 &gt; 1900, ((B53-1900)*10)+400+C53, ((B53-1730)*2)+C53)+VLOOKUP(D53,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7081</v>
+        <v>7121</v>
       </c>
       <c r="F53">
         <v>40</v>
@@ -2418,6 +2424,76 @@
         <v>37.94733192202056</v>
       </c>
       <c r="J53" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54">
+        <v>2001</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54">
+        <f>IF(B54 &gt; 1900, ((B54-1900)*10)+400+C54, ((B54-1730)*2)+C54)+VLOOKUP(D54,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>2012</v>
+      </c>
+      <c r="F54">
+        <v>55</v>
+      </c>
+      <c r="G54">
+        <v>140</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" ref="H54" si="49">SQRT(F54*G54)/$B$1</f>
+        <v>292.49881291307071</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" ref="I54" si="50">H54*0.9</f>
+        <v>263.24893162176363</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55">
+        <v>1958</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55" t="s">
+        <v>21</v>
+      </c>
+      <c r="E55">
+        <f>IF(B55 &gt; 1900, ((B55-1900)*10)+400+C55, ((B55-1730)*2)+C55)+VLOOKUP(D55,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>1582</v>
+      </c>
+      <c r="F55">
+        <v>55</v>
+      </c>
+      <c r="G55">
+        <v>57</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" ref="H55" si="51">SQRT(F55*G55)/$B$1</f>
+        <v>186.63690238892559</v>
+      </c>
+      <c r="I55" s="2">
+        <f t="shared" ref="I55" si="52">H55*0.9</f>
+        <v>167.97321215003305</v>
+      </c>
+      <c r="J55" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New vehicles and bug fixes
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED978EC5-E140-42E0-BA03-61D140E09E3B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7E701D-FD42-4B4F-9919-78BDEF293682}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="78">
   <si>
     <t>Vehicle</t>
   </si>
@@ -243,6 +243,18 @@
   </si>
   <si>
     <t>Leyland Leopard</t>
+  </si>
+  <si>
+    <t>Sentinel DG4</t>
+  </si>
+  <si>
+    <t>AEC Mammoth Major 8</t>
+  </si>
+  <si>
+    <t>Commer FC</t>
+  </si>
+  <si>
+    <t>Austin 10hp</t>
   </si>
 </sst>
 </file>
@@ -604,11 +616,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
+      <pane ySplit="3" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2494,6 +2506,146 @@
         <v>167.97321215003305</v>
       </c>
       <c r="J55" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56">
+        <v>1928</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56">
+        <f>IF(B56 &gt; 1900, ((B56-1900)*10)+400+C56, ((B56-1730)*2)+C56)+VLOOKUP(D56,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4281</v>
+      </c>
+      <c r="F56">
+        <v>37</v>
+      </c>
+      <c r="G56">
+        <v>15</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" ref="H56" si="53">SQRT(F56*G56)/$B$1</f>
+        <v>78.528126595931653</v>
+      </c>
+      <c r="I56" s="2">
+        <f t="shared" ref="I56" si="54">H56*0.9</f>
+        <v>70.675313936338483</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57">
+        <v>1935</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57">
+        <f>IF(B57 &gt; 1900, ((B57-1900)*10)+400+C57, ((B57-1730)*2)+C57)+VLOOKUP(D57,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4351</v>
+      </c>
+      <c r="F57">
+        <v>35</v>
+      </c>
+      <c r="G57">
+        <v>24</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" ref="H57" si="55">SQRT(F57*G57)/$B$1</f>
+        <v>96.609178307929596</v>
+      </c>
+      <c r="I57" s="2">
+        <f t="shared" ref="I57" si="56">H57*0.9</f>
+        <v>86.948260477136643</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58">
+        <v>1960</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58">
+        <f>IF(B58 &gt; 1900, ((B58-1900)*10)+400+C58, ((B58-1730)*2)+C58)+VLOOKUP(D58,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>7601</v>
+      </c>
+      <c r="F58">
+        <v>60</v>
+      </c>
+      <c r="G58">
+        <v>8</v>
+      </c>
+      <c r="H58" s="2">
+        <f t="shared" ref="H58" si="57">SQRT(F58*G58)/$B$1</f>
+        <v>73.029674334022147</v>
+      </c>
+      <c r="I58" s="2">
+        <f t="shared" ref="I58" si="58">H58*0.9</f>
+        <v>65.726706900619931</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59">
+        <v>1938</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>23</v>
+      </c>
+      <c r="E59">
+        <f>IF(B59 &gt; 1900, ((B59-1900)*10)+400+C59, ((B59-1730)*2)+C59)+VLOOKUP(D59,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>7381</v>
+      </c>
+      <c r="F59">
+        <v>45</v>
+      </c>
+      <c r="G59">
+        <v>5</v>
+      </c>
+      <c r="H59" s="2">
+        <f t="shared" ref="H59" si="59">SQRT(F59*G59)/$B$1</f>
+        <v>50</v>
+      </c>
+      <c r="I59" s="2">
+        <f t="shared" ref="I59" si="60">H59*0.9</f>
+        <v>45</v>
+      </c>
+      <c r="J59" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugfixes and new Scammell artic
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFC20A4-A002-4E8F-AF9C-8C4897B49DEB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A31EAEA-54A4-47CA-9CE1-EF5DF07A4A1F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="88">
   <si>
     <t>Vehicle</t>
   </si>
@@ -264,12 +264,36 @@
   </si>
   <si>
     <t>Wrightbus New Routemaster</t>
+  </si>
+  <si>
+    <t>Length (m)</t>
+  </si>
+  <si>
+    <t>Width (m)</t>
+  </si>
+  <si>
+    <t>Height (m)</t>
+  </si>
+  <si>
+    <t>Voxel Size</t>
+  </si>
+  <si>
+    <t>Length Scale</t>
+  </si>
+  <si>
+    <t>Height Scale</t>
+  </si>
+  <si>
+    <t>Width Scale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -307,10 +331,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,11 +650,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,10 +668,10 @@
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="10" max="14" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -654,7 +679,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,10 +711,22 @@
         <v>32</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -713,18 +750,22 @@
         <v>14</v>
       </c>
       <c r="H4" s="2">
-        <f>SQRT(F4*G4)/$B$1</f>
+        <f t="shared" ref="H4:H35" si="0">SQRT(F4*G4)/$B$1</f>
         <v>52.915026221291818</v>
       </c>
       <c r="I4" s="2">
-        <f>H4*0.9</f>
+        <f t="shared" ref="I4:I35" si="1">H4*0.9</f>
         <v>47.623523599162638</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -748,18 +789,22 @@
         <v>22</v>
       </c>
       <c r="H5" s="2">
-        <f>SQRT(F5*G5)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>66.332495807108003</v>
       </c>
       <c r="I5" s="2">
-        <f>H5*0.9</f>
+        <f t="shared" si="1"/>
         <v>59.699246226397207</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -783,18 +828,22 @@
         <v>36</v>
       </c>
       <c r="H6" s="2">
-        <f>SQRT(F6*G6)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>89.442719099991592</v>
       </c>
       <c r="I6" s="2">
-        <f>H6*0.9</f>
+        <f t="shared" si="1"/>
         <v>80.498447189992433</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -818,18 +867,22 @@
         <v>32</v>
       </c>
       <c r="H7" s="2">
-        <f>SQRT(F7*G7)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>113.13708498984759</v>
       </c>
       <c r="I7" s="2">
-        <f>H7*0.9</f>
+        <f t="shared" si="1"/>
         <v>101.82337649086284</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -853,18 +906,22 @@
         <v>35</v>
       </c>
       <c r="H8" s="2">
-        <f>SQRT(F8*G8)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>127.80193008453877</v>
       </c>
       <c r="I8" s="2">
-        <f>H8*0.9</f>
+        <f t="shared" si="1"/>
         <v>115.02173707608489</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -888,18 +945,22 @@
         <v>50</v>
       </c>
       <c r="H9" s="2">
-        <f>SQRT(F9*G9)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>126.92955176439848</v>
       </c>
       <c r="I9" s="2">
-        <f>H9*0.9</f>
+        <f t="shared" si="1"/>
         <v>114.23659658795863</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -923,18 +984,22 @@
         <v>44</v>
       </c>
       <c r="H10" s="2">
-        <f>SQRT(F10*G10)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>139.84117975602021</v>
       </c>
       <c r="I10" s="2">
-        <f>H10*0.9</f>
+        <f t="shared" si="1"/>
         <v>125.85706178041819</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -958,18 +1023,22 @@
         <v>57</v>
       </c>
       <c r="H11" s="2">
-        <f>SQRT(F11*G11)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>155.13435037626795</v>
       </c>
       <c r="I11" s="2">
-        <f>H11*0.9</f>
+        <f t="shared" si="1"/>
         <v>139.62091533864117</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -993,18 +1062,22 @@
         <v>72</v>
       </c>
       <c r="H12" s="2">
-        <f>SQRT(F12*G12)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>178.88543819998318</v>
       </c>
       <c r="I12" s="2">
-        <f>H12*0.9</f>
+        <f t="shared" si="1"/>
         <v>160.99689437998487</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1028,18 +1101,22 @@
         <v>34</v>
       </c>
       <c r="H13" s="2">
-        <f>SQRT(F13*G13)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>169.44353369518447</v>
       </c>
       <c r="I13" s="2">
-        <f>H13*0.9</f>
+        <f t="shared" si="1"/>
         <v>152.49918032566603</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -1063,18 +1140,22 @@
         <v>57</v>
       </c>
       <c r="H14" s="2">
-        <f>SQRT(F14*G14)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>186.63690238892559</v>
       </c>
       <c r="I14" s="2">
-        <f>H14*0.9</f>
+        <f t="shared" si="1"/>
         <v>167.97321215003305</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1098,18 +1179,22 @@
         <v>52</v>
       </c>
       <c r="H15" s="2">
-        <f>SQRT(F15*G15)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>178.26322609494585</v>
       </c>
       <c r="I15" s="2">
-        <f>H15*0.9</f>
+        <f t="shared" si="1"/>
         <v>160.43690348545127</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1133,18 +1218,22 @@
         <v>58</v>
       </c>
       <c r="H16" s="2">
-        <f>SQRT(F16*G16)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>183.06040290327977</v>
       </c>
       <c r="I16" s="2">
-        <f>H16*0.9</f>
+        <f t="shared" si="1"/>
         <v>164.75436261295178</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1168,18 +1257,34 @@
         <v>55</v>
       </c>
       <c r="H17" s="2">
-        <f>SQRT(F17*G17)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>194.65068427541911</v>
       </c>
       <c r="I17" s="2">
-        <f>H17*0.9</f>
+        <f t="shared" si="1"/>
         <v>175.18561584787722</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="3">
+        <v>12</v>
+      </c>
+      <c r="L17" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M17" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="N17" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K17*VLOOKUP(D17,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M17*VLOOKUP(D17,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L17*VLOOKUP(D17,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>56x16x18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1203,18 +1308,34 @@
         <v>73</v>
       </c>
       <c r="H18" s="2">
-        <f>SQRT(F18*G18)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>195.2491286080996</v>
       </c>
       <c r="I18" s="2">
-        <f>H18*0.9</f>
+        <f t="shared" si="1"/>
         <v>175.72421574728963</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="3">
+        <v>12</v>
+      </c>
+      <c r="L18" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M18" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="N18" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K18*VLOOKUP(D18,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M18*VLOOKUP(D18,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L18*VLOOKUP(D18,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>56x20x18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -1238,18 +1359,34 @@
         <v>50</v>
       </c>
       <c r="H19" s="2">
-        <f>SQRT(F19*G19)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>176.38342073763937</v>
       </c>
       <c r="I19" s="2">
-        <f>H19*0.9</f>
+        <f t="shared" si="1"/>
         <v>158.74507866387543</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="L19" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="M19" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="N19" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K19*VLOOKUP(D19,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M19*VLOOKUP(D19,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L19*VLOOKUP(D19,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>48x13x17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -1273,18 +1410,22 @@
         <v>33</v>
       </c>
       <c r="H20" s="2">
-        <f>SQRT(F20*G20)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>147.08274315273474</v>
       </c>
       <c r="I20" s="2">
-        <f>H20*0.9</f>
+        <f t="shared" si="1"/>
         <v>132.37446883746128</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1308,18 +1449,22 @@
         <v>35</v>
       </c>
       <c r="H21" s="2">
-        <f>SQRT(F21*G21)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>152.75252316519467</v>
       </c>
       <c r="I21" s="2">
-        <f>H21*0.9</f>
+        <f t="shared" si="1"/>
         <v>137.4772708486752</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1343,18 +1488,22 @@
         <v>58</v>
       </c>
       <c r="H22" s="2">
-        <f>SQRT(F22*G22)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>212.39376429431988</v>
       </c>
       <c r="I22" s="2">
-        <f>H22*0.9</f>
+        <f t="shared" si="1"/>
         <v>191.15438786488789</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -1378,18 +1527,22 @@
         <v>140</v>
       </c>
       <c r="H23" s="2">
-        <f>SQRT(F23*G23)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>292.49881291307071</v>
       </c>
       <c r="I23" s="2">
-        <f>H23*0.9</f>
+        <f t="shared" si="1"/>
         <v>263.24893162176363</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1413,18 +1566,22 @@
         <v>90</v>
       </c>
       <c r="H24" s="2">
-        <f>SQRT(F24*G24)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>244.94897427831785</v>
       </c>
       <c r="I24" s="2">
-        <f>H24*0.9</f>
+        <f t="shared" si="1"/>
         <v>220.45407685048608</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1448,18 +1605,22 @@
         <v>12</v>
       </c>
       <c r="H25" s="2">
-        <f>SQRT(F25*G25)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>46.188021535170058</v>
       </c>
       <c r="I25" s="2">
-        <f>H25*0.9</f>
+        <f t="shared" si="1"/>
         <v>41.569219381653056</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1483,18 +1644,22 @@
         <v>14</v>
       </c>
       <c r="H26" s="2">
-        <f>SQRT(F26*G26)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>52.915026221291818</v>
       </c>
       <c r="I26" s="2">
-        <f>H26*0.9</f>
+        <f t="shared" si="1"/>
         <v>47.623523599162638</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1518,18 +1683,22 @@
         <v>16</v>
       </c>
       <c r="H27" s="2">
-        <f>SQRT(F27*G27)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>56.568542494923797</v>
       </c>
       <c r="I27" s="2">
-        <f>H27*0.9</f>
+        <f t="shared" si="1"/>
         <v>50.911688245431421</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1553,18 +1722,22 @@
         <v>18</v>
       </c>
       <c r="H28" s="2">
-        <f>SQRT(F28*G28)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>63.245553203367592</v>
       </c>
       <c r="I28" s="2">
-        <f>H28*0.9</f>
+        <f t="shared" si="1"/>
         <v>56.920997883030836</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1588,18 +1761,22 @@
         <v>18</v>
       </c>
       <c r="H29" s="2">
-        <f>SQRT(F29*G29)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>66.332495807108003</v>
       </c>
       <c r="I29" s="2">
-        <f>H29*0.9</f>
+        <f t="shared" si="1"/>
         <v>59.699246226397207</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -1623,18 +1800,22 @@
         <v>15</v>
       </c>
       <c r="H30" s="2">
-        <f>SQRT(F30*G30)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>78.528126595931653</v>
       </c>
       <c r="I30" s="2">
-        <f>H30*0.9</f>
+        <f t="shared" si="1"/>
         <v>70.675313936338483</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -1658,18 +1839,22 @@
         <v>24</v>
       </c>
       <c r="H31" s="2">
-        <f>SQRT(F31*G31)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>96.609178307929596</v>
       </c>
       <c r="I31" s="2">
-        <f>H31*0.9</f>
+        <f t="shared" si="1"/>
         <v>86.948260477136643</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1693,18 +1878,22 @@
         <v>20</v>
       </c>
       <c r="H32" s="2">
-        <f>SQRT(F32*G32)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>81.649658092772611</v>
       </c>
       <c r="I32" s="2">
-        <f>H32*0.9</f>
+        <f t="shared" si="1"/>
         <v>73.484692283495349</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1728,18 +1917,22 @@
         <v>25</v>
       </c>
       <c r="H33" s="2">
-        <f>SQRT(F33*G33)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>102.74023338281629</v>
       </c>
       <c r="I33" s="2">
-        <f>H33*0.9</f>
+        <f t="shared" si="1"/>
         <v>92.466210044534662</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1763,18 +1956,22 @@
         <v>21</v>
       </c>
       <c r="H34" s="2">
-        <f>SQRT(F34*G34)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>97.809338340808068</v>
       </c>
       <c r="I34" s="2">
-        <f>H34*0.9</f>
+        <f t="shared" si="1"/>
         <v>88.02840450672727</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1798,18 +1995,22 @@
         <v>24</v>
       </c>
       <c r="H35" s="2">
-        <f>SQRT(F35*G35)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>108.32051206181282</v>
       </c>
       <c r="I35" s="2">
-        <f>H35*0.9</f>
+        <f t="shared" si="1"/>
         <v>97.488460855631544</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -1833,18 +2034,22 @@
         <v>36</v>
       </c>
       <c r="H36" s="2">
-        <f>SQRT(F36*G36)/$B$1</f>
+        <f t="shared" ref="H36:H67" si="2">SQRT(F36*G36)/$B$1</f>
         <v>146.9693845669907</v>
       </c>
       <c r="I36" s="2">
-        <f>H36*0.9</f>
+        <f t="shared" ref="I36:I67" si="3">H36*0.9</f>
         <v>132.27244611029164</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1868,21 +2073,25 @@
         <v>22</v>
       </c>
       <c r="H37" s="2">
-        <f>SQRT(F37*G37)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>114.89125293076057</v>
       </c>
       <c r="I37" s="2">
-        <f>H37*0.9</f>
+        <f t="shared" si="3"/>
         <v>103.40212763768452</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1906,18 +2115,22 @@
         <v>36</v>
       </c>
       <c r="H38" s="2">
-        <f>SQRT(F38*G38)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>150.99668870541501</v>
       </c>
       <c r="I38" s="2">
-        <f>H38*0.9</f>
+        <f t="shared" si="3"/>
         <v>135.8970198348735</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1941,18 +2154,22 @@
         <v>36</v>
       </c>
       <c r="H39" s="2">
-        <f>SQRT(F39*G39)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>164.92422502470643</v>
       </c>
       <c r="I39" s="2">
-        <f>H39*0.9</f>
+        <f t="shared" si="3"/>
         <v>148.43180252223578</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1976,18 +2193,22 @@
         <v>42</v>
       </c>
       <c r="H40" s="2">
-        <f>SQRT(F40*G40)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>170.09801096230765</v>
       </c>
       <c r="I40" s="2">
-        <f>H40*0.9</f>
+        <f t="shared" si="3"/>
         <v>153.08820986607688</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -2011,18 +2232,22 @@
         <v>28</v>
       </c>
       <c r="H41" s="2">
-        <f>SQRT(F41*G41)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>136.62601021279465</v>
       </c>
       <c r="I41" s="2">
-        <f>H41*0.9</f>
+        <f t="shared" si="3"/>
         <v>122.9634091915152</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -2046,18 +2271,22 @@
         <v>30</v>
       </c>
       <c r="H42" s="2">
-        <f>SQRT(F42*G42)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>143.75905768565215</v>
       </c>
       <c r="I42" s="2">
-        <f>H42*0.9</f>
+        <f t="shared" si="3"/>
         <v>129.38315191708693</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -2081,18 +2310,22 @@
         <v>44</v>
       </c>
       <c r="H43" s="2">
-        <f>SQRT(F43*G43)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>178.26322609494585</v>
       </c>
       <c r="I43" s="2">
-        <f>H43*0.9</f>
+        <f t="shared" si="3"/>
         <v>160.43690348545127</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -2116,18 +2349,22 @@
         <v>48</v>
       </c>
       <c r="H44" s="2">
-        <f>SQRT(F44*G44)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>190.43809142780935</v>
       </c>
       <c r="I44" s="2">
-        <f>H44*0.9</f>
+        <f t="shared" si="3"/>
         <v>171.39428228502842</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -2151,18 +2388,22 @@
         <v>32</v>
       </c>
       <c r="H45" s="2">
-        <f>SQRT(F45*G45)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>157.76212754932311</v>
       </c>
       <c r="I45" s="2">
-        <f>H45*0.9</f>
+        <f t="shared" si="3"/>
         <v>141.98591479439079</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>27</v>
       </c>
@@ -2186,18 +2427,22 @@
         <v>54</v>
       </c>
       <c r="H46" s="2">
-        <f>SQRT(F46*G46)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>207.84609690826528</v>
       </c>
       <c r="I46" s="2">
-        <f>H46*0.9</f>
+        <f t="shared" si="3"/>
         <v>187.06148721743875</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -2221,18 +2466,22 @@
         <v>4</v>
       </c>
       <c r="H47" s="2">
-        <f>SQRT(F47*G47)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>42.163702135578397</v>
       </c>
       <c r="I47" s="2">
-        <f>H47*0.9</f>
+        <f t="shared" si="3"/>
         <v>37.94733192202056</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -2256,18 +2505,22 @@
         <v>5</v>
       </c>
       <c r="H48" s="2">
-        <f>SQRT(F48*G48)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="I48" s="2">
-        <f>H48*0.9</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -2291,18 +2544,22 @@
         <v>6</v>
       </c>
       <c r="H49" s="2">
-        <f>SQRT(F49*G49)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>63.245553203367592</v>
       </c>
       <c r="I49" s="2">
-        <f>H49*0.9</f>
+        <f t="shared" si="3"/>
         <v>56.920997883030836</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>76</v>
       </c>
@@ -2326,18 +2583,22 @@
         <v>8</v>
       </c>
       <c r="H50" s="2">
-        <f>SQRT(F50*G50)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>73.029674334022147</v>
       </c>
       <c r="I50" s="2">
-        <f>H50*0.9</f>
+        <f t="shared" si="3"/>
         <v>65.726706900619931</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2361,18 +2622,22 @@
         <v>8</v>
       </c>
       <c r="H51" s="2">
-        <f>SQRT(F51*G51)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>76.011695006609202</v>
       </c>
       <c r="I51" s="2">
-        <f>H51*0.9</f>
+        <f t="shared" si="3"/>
         <v>68.410525505948286</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2396,18 +2661,22 @@
         <v>10</v>
       </c>
       <c r="H52" s="2">
-        <f>SQRT(F52*G52)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>94.28090415820634</v>
       </c>
       <c r="I52" s="2">
-        <f>H52*0.9</f>
+        <f t="shared" si="3"/>
         <v>84.852813742385706</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2431,18 +2700,22 @@
         <v>4</v>
       </c>
       <c r="H53" s="2">
-        <f>SQRT(F53*G53)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>53.748384988656994</v>
       </c>
       <c r="I53" s="2">
-        <f>H53*0.9</f>
+        <f t="shared" si="3"/>
         <v>48.373546489791295</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -2466,18 +2739,22 @@
         <v>12</v>
       </c>
       <c r="H54" s="2">
-        <f>SQRT(F54*G54)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>106.45812948447541</v>
       </c>
       <c r="I54" s="2">
-        <f>H54*0.9</f>
+        <f t="shared" si="3"/>
         <v>95.812316536027865</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2501,18 +2778,22 @@
         <v>10</v>
       </c>
       <c r="H55" s="2">
-        <f>SQRT(F55*G55)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>101.10500592068735</v>
       </c>
       <c r="I55" s="2">
-        <f>H55*0.9</f>
+        <f t="shared" si="3"/>
         <v>90.994505328618615</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -2536,21 +2817,25 @@
         <v>4</v>
       </c>
       <c r="H56" s="2">
-        <f>SQRT(F56*G56)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>57.735026918962582</v>
       </c>
       <c r="I56" s="2">
-        <f>H56*0.9</f>
+        <f t="shared" si="3"/>
         <v>51.961524227066327</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K56" t="s">
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -2574,18 +2859,22 @@
         <v>4</v>
       </c>
       <c r="H57" s="2">
-        <f>SQRT(F57*G57)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>63.245553203367592</v>
       </c>
       <c r="I57" s="2">
-        <f>H57*0.9</f>
+        <f t="shared" si="3"/>
         <v>56.920997883030836</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -2609,18 +2898,22 @@
         <v>4</v>
       </c>
       <c r="H58" s="2">
-        <f>SQRT(F58*G58)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>73.029674334022147</v>
       </c>
       <c r="I58" s="2">
-        <f>H58*0.9</f>
+        <f t="shared" si="3"/>
         <v>65.726706900619931</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -2644,21 +2937,25 @@
         <v>5</v>
       </c>
       <c r="H59" s="2">
-        <f>SQRT(F59*G59)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>67.082039324993701</v>
       </c>
       <c r="I59" s="2">
-        <f>H59*0.9</f>
+        <f t="shared" si="3"/>
         <v>60.373835392494335</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -2682,18 +2979,22 @@
         <v>4</v>
       </c>
       <c r="H60" s="2">
-        <f>SQRT(F60*G60)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>80.277297191948648</v>
       </c>
       <c r="I60" s="2">
-        <f>H60*0.9</f>
+        <f t="shared" si="3"/>
         <v>72.249567472753782</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -2717,18 +3018,22 @@
         <v>4</v>
       </c>
       <c r="H61" s="2">
-        <f>SQRT(F61*G61)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>70.553368295055762</v>
       </c>
       <c r="I61" s="2">
-        <f>H61*0.9</f>
+        <f t="shared" si="3"/>
         <v>63.498031465550184</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>80</v>
       </c>
@@ -2752,19 +3057,23 @@
         <v>87</v>
       </c>
       <c r="H62" s="2">
-        <f>SQRT(F62*G62)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>219.84843263788198</v>
       </c>
       <c r="I62" s="2">
-        <f>H62*0.9</f>
+        <f t="shared" si="3"/>
         <v>197.86358937409378</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A4:K61">
+  <sortState ref="A4:O61">
     <sortCondition ref="E33"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2786,53 +3095,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2">
         <v>600</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>4.67</v>
+      </c>
+      <c r="D2">
+        <v>4.84</v>
+      </c>
+      <c r="E2">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3">
         <v>3600</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>4.67</v>
+      </c>
+      <c r="D3">
+        <v>4.84</v>
+      </c>
+      <c r="E3">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
       <c r="B4">
         <v>6600</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>4.67</v>
+      </c>
+      <c r="D4">
+        <v>4.84</v>
+      </c>
+      <c r="E4">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>62</v>
       </c>
       <c r="B5">
         <v>9600</v>
+      </c>
+      <c r="C5">
+        <v>4.67</v>
+      </c>
+      <c r="D5">
+        <v>4.84</v>
+      </c>
+      <c r="E5">
+        <v>7.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modern trailer alignment fix
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A31EAEA-54A4-47CA-9CE1-EF5DF07A4A1F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20EF153-BD9F-40E2-984B-F89D92B0078D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="89">
   <si>
     <t>Vehicle</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>Width Scale</t>
+  </si>
+  <si>
+    <t>Scammell 7.5 Ton</t>
   </si>
 </sst>
 </file>
@@ -650,11 +653,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O62"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
+      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M58" sqref="M58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,9 +764,15 @@
         <v>33</v>
       </c>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="L4" s="3"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="N4" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K4*VLOOKUP(D4,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M4*VLOOKUP(D4,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L4*VLOOKUP(D4,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -800,9 +809,15 @@
         <v>33</v>
       </c>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="L5" s="3"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K5*VLOOKUP(D5,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M5*VLOOKUP(D5,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L5*VLOOKUP(D5,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -839,9 +854,15 @@
         <v>33</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="L6" s="3"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="N6" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K6*VLOOKUP(D6,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M6*VLOOKUP(D6,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L6*VLOOKUP(D6,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -878,9 +899,15 @@
         <v>33</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="L7" s="3"/>
       <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="N7" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K7*VLOOKUP(D7,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M7*VLOOKUP(D7,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L7*VLOOKUP(D7,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -917,9 +944,15 @@
         <v>33</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="L8" s="3"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="N8" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K8*VLOOKUP(D8,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M8*VLOOKUP(D8,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L8*VLOOKUP(D8,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -956,9 +989,15 @@
         <v>33</v>
       </c>
       <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="L9" s="3"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+      <c r="N9" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K9*VLOOKUP(D9,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M9*VLOOKUP(D9,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L9*VLOOKUP(D9,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -995,9 +1034,15 @@
         <v>33</v>
       </c>
       <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="L10" s="3"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="N10" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K10*VLOOKUP(D10,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M10*VLOOKUP(D10,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L10*VLOOKUP(D10,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1034,9 +1079,15 @@
         <v>33</v>
       </c>
       <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="L11" s="3"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="N11" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K11*VLOOKUP(D11,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M11*VLOOKUP(D11,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L11*VLOOKUP(D11,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1073,9 +1124,15 @@
         <v>33</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="L12" s="3"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+      <c r="N12" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K12*VLOOKUP(D12,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M12*VLOOKUP(D12,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L12*VLOOKUP(D12,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1112,9 +1169,15 @@
         <v>33</v>
       </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+      <c r="L13" s="3"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="N13" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K13*VLOOKUP(D13,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M13*VLOOKUP(D13,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L13*VLOOKUP(D13,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1151,9 +1214,15 @@
         <v>33</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="L14" s="3"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="N14" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K14*VLOOKUP(D14,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M14*VLOOKUP(D14,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L14*VLOOKUP(D14,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1190,9 +1259,15 @@
         <v>33</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+      <c r="L15" s="3"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="N15" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1229,9 +1304,15 @@
         <v>33</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+      <c r="L16" s="3"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+      <c r="N16" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1421,9 +1502,15 @@
         <v>33</v>
       </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1460,9 +1547,15 @@
         <v>33</v>
       </c>
       <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1499,9 +1592,15 @@
         <v>33</v>
       </c>
       <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1538,9 +1637,15 @@
         <v>33</v>
       </c>
       <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1577,9 +1682,15 @@
         <v>33</v>
       </c>
       <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K24*VLOOKUP(D24,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M24*VLOOKUP(D24,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L24*VLOOKUP(D24,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1616,9 +1727,15 @@
         <v>33</v>
       </c>
       <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1655,9 +1772,15 @@
         <v>33</v>
       </c>
       <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K26*VLOOKUP(D26,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M26*VLOOKUP(D26,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L26*VLOOKUP(D26,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1694,9 +1817,15 @@
         <v>33</v>
       </c>
       <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K27*VLOOKUP(D27,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M27*VLOOKUP(D27,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L27*VLOOKUP(D27,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1733,9 +1862,15 @@
         <v>33</v>
       </c>
       <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K28*VLOOKUP(D28,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M28*VLOOKUP(D28,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L28*VLOOKUP(D28,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1772,9 +1907,15 @@
         <v>33</v>
       </c>
       <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K29*VLOOKUP(D29,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M29*VLOOKUP(D29,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L29*VLOOKUP(D29,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1811,9 +1952,15 @@
         <v>33</v>
       </c>
       <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K30*VLOOKUP(D30,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M30*VLOOKUP(D30,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L30*VLOOKUP(D30,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1850,9 +1997,15 @@
         <v>33</v>
       </c>
       <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1889,9 +2042,15 @@
         <v>33</v>
       </c>
       <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K32*VLOOKUP(D32,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M32*VLOOKUP(D32,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L32*VLOOKUP(D32,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1928,9 +2087,15 @@
         <v>33</v>
       </c>
       <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K33*VLOOKUP(D33,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M33*VLOOKUP(D33,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L33*VLOOKUP(D33,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1967,9 +2132,15 @@
         <v>33</v>
       </c>
       <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K34*VLOOKUP(D34,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M34*VLOOKUP(D34,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L34*VLOOKUP(D34,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -2006,9 +2177,15 @@
         <v>33</v>
       </c>
       <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K35*VLOOKUP(D35,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M35*VLOOKUP(D35,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L35*VLOOKUP(D35,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -2034,20 +2211,26 @@
         <v>36</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" ref="H36:H67" si="2">SQRT(F36*G36)/$B$1</f>
+        <f t="shared" ref="H36:H62" si="2">SQRT(F36*G36)/$B$1</f>
         <v>146.9693845669907</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" ref="I36:I67" si="3">H36*0.9</f>
+        <f t="shared" ref="I36:I62" si="3">H36*0.9</f>
         <v>132.27244611029164</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K36*VLOOKUP(D36,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M36*VLOOKUP(D36,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L36*VLOOKUP(D36,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -2084,9 +2267,15 @@
         <v>33</v>
       </c>
       <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K37*VLOOKUP(D37,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M37*VLOOKUP(D37,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L37*VLOOKUP(D37,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
       <c r="O37" t="s">
         <v>31</v>
       </c>
@@ -2126,9 +2315,15 @@
         <v>33</v>
       </c>
       <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K38*VLOOKUP(D38,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M38*VLOOKUP(D38,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L38*VLOOKUP(D38,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -2165,9 +2360,15 @@
         <v>33</v>
       </c>
       <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K39*VLOOKUP(D39,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M39*VLOOKUP(D39,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L39*VLOOKUP(D39,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -2204,9 +2405,15 @@
         <v>33</v>
       </c>
       <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K40*VLOOKUP(D40,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M40*VLOOKUP(D40,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L40*VLOOKUP(D40,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -2243,9 +2450,15 @@
         <v>33</v>
       </c>
       <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K41*VLOOKUP(D41,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M41*VLOOKUP(D41,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L41*VLOOKUP(D41,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -2282,9 +2495,15 @@
         <v>33</v>
       </c>
       <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K42*VLOOKUP(D42,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M42*VLOOKUP(D42,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L42*VLOOKUP(D42,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -2321,9 +2540,15 @@
         <v>33</v>
       </c>
       <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K43*VLOOKUP(D43,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M43*VLOOKUP(D43,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L43*VLOOKUP(D43,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -2360,9 +2585,15 @@
         <v>33</v>
       </c>
       <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K44*VLOOKUP(D44,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M44*VLOOKUP(D44,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L44*VLOOKUP(D44,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -2399,9 +2630,15 @@
         <v>33</v>
       </c>
       <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K45*VLOOKUP(D45,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M45*VLOOKUP(D45,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L45*VLOOKUP(D45,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -2438,9 +2675,15 @@
         <v>33</v>
       </c>
       <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K46*VLOOKUP(D46,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M46*VLOOKUP(D46,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L46*VLOOKUP(D46,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -2477,9 +2720,15 @@
         <v>33</v>
       </c>
       <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K47*VLOOKUP(D47,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M47*VLOOKUP(D47,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L47*VLOOKUP(D47,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -2516,9 +2765,15 @@
         <v>33</v>
       </c>
       <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K48*VLOOKUP(D48,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M48*VLOOKUP(D48,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L48*VLOOKUP(D48,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -2534,7 +2789,7 @@
         <v>23</v>
       </c>
       <c r="E49">
-        <f>IF(B49 &gt; 1900, ((B49-1900)*10)+400+C49, ((B49-1730)*2)+C49)+VLOOKUP(D49,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B49 &gt; 1900, ((B49-1900)*10)+400+C49, ((B49-1730)*2)+C49)+VLOOKUP(D49,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>7571</v>
       </c>
       <c r="F49">
@@ -2555,9 +2810,15 @@
         <v>33</v>
       </c>
       <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K49*VLOOKUP(D49,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M49*VLOOKUP(D49,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L49*VLOOKUP(D49,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -2594,9 +2855,15 @@
         <v>33</v>
       </c>
       <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K50*VLOOKUP(D50,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M50*VLOOKUP(D50,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L50*VLOOKUP(D50,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -2633,9 +2900,15 @@
         <v>33</v>
       </c>
       <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K51*VLOOKUP(D51,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M51*VLOOKUP(D51,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L51*VLOOKUP(D51,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -2672,9 +2945,15 @@
         <v>33</v>
       </c>
       <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K52*VLOOKUP(D52,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M52*VLOOKUP(D52,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L52*VLOOKUP(D52,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -2711,9 +2990,15 @@
         <v>33</v>
       </c>
       <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K53*VLOOKUP(D53,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M53*VLOOKUP(D53,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L53*VLOOKUP(D53,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -2750,9 +3035,15 @@
         <v>33</v>
       </c>
       <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K54*VLOOKUP(D54,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M54*VLOOKUP(D54,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L54*VLOOKUP(D54,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -2789,9 +3080,15 @@
         <v>33</v>
       </c>
       <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K55*VLOOKUP(D55,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M55*VLOOKUP(D55,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L55*VLOOKUP(D55,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -2828,9 +3125,15 @@
         <v>33</v>
       </c>
       <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K56*VLOOKUP(D56,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M56*VLOOKUP(D56,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L56*VLOOKUP(D56,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
       <c r="O56" t="s">
         <v>69</v>
       </c>
@@ -2869,10 +3172,22 @@
       <c r="J57" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
+      <c r="K57" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L57" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="M57" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="N57" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>21x7x13</v>
+      </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -2908,10 +3223,22 @@
       <c r="J58" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2"/>
+      <c r="K58" s="2">
+        <v>5</v>
+      </c>
+      <c r="L58" s="3">
+        <v>2</v>
+      </c>
+      <c r="M58" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="N58" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>23x7x14</v>
+      </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -2948,9 +3275,15 @@
         <v>33</v>
       </c>
       <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K59*VLOOKUP(D59,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M59*VLOOKUP(D59,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L59*VLOOKUP(D59,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
       <c r="O59" t="s">
         <v>70</v>
       </c>
@@ -2990,9 +3323,15 @@
         <v>33</v>
       </c>
       <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K60*VLOOKUP(D60,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M60*VLOOKUP(D60,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L60*VLOOKUP(D60,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -3029,9 +3368,15 @@
         <v>33</v>
       </c>
       <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
-      <c r="M61" s="2"/>
-      <c r="N61" s="2"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K61*VLOOKUP(D61,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M61*VLOOKUP(D61,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L61*VLOOKUP(D61,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -3068,9 +3413,66 @@
         <v>33</v>
       </c>
       <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K62*VLOOKUP(D62,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M62*VLOOKUP(D62,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L62*VLOOKUP(D62,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63">
+        <v>1920</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63">
+        <f>IF(B63 &gt; 1900, ((B63-1900)*10)+400+C63, ((B63-1730)*2)+C63)+VLOOKUP(D63,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4201</v>
+      </c>
+      <c r="F63">
+        <v>18</v>
+      </c>
+      <c r="G63">
+        <v>28</v>
+      </c>
+      <c r="H63" s="2">
+        <f t="shared" ref="H63" si="4">SQRT(F63*G63)/$B$1</f>
+        <v>74.833147735478832</v>
+      </c>
+      <c r="I63" s="2">
+        <f t="shared" ref="I63" si="5">H63*0.9</f>
+        <v>67.349832961930957</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K63">
+        <v>3.4</v>
+      </c>
+      <c r="L63" s="3">
+        <v>2</v>
+      </c>
+      <c r="M63">
+        <v>2.5</v>
+      </c>
+      <c r="N63" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>16x12x14</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A4:O61">

</xml_diff>

<commit_message>
Rescaled early vehicles, added Sherpa and Scarab
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20EF153-BD9F-40E2-984B-F89D92B0078D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCA59F8-E0AE-4107-8D10-1804E2456EDC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="91">
   <si>
     <t>Vehicle</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>Scammell 7.5 Ton</t>
+  </si>
+  <si>
+    <t>Leyland Sherpa</t>
+  </si>
+  <si>
+    <t>Scammell Scarab</t>
   </si>
 </sst>
 </file>
@@ -653,11 +659,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M58" sqref="M58"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +749,7 @@
         <v>21</v>
       </c>
       <c r="E4">
-        <f>IF(B4 &gt; 1900, ((B4-1900)*10)+400+C4, ((B4-1730)*2)+C4)+VLOOKUP(D4,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B4 &gt; 1900, ((B4-1900)*10)+400+C4, ((B4-1730)*2)+C4)+VLOOKUP(D4,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>741</v>
       </c>
       <c r="F4">
@@ -753,17 +759,17 @@
         <v>14</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H35" si="0">SQRT(F4*G4)/$B$1</f>
+        <f>SQRT(F4*G4)/$B$1</f>
         <v>52.915026221291818</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I4:I35" si="1">H4*0.9</f>
+        <f>H4*0.9</f>
         <v>47.623523599162638</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="2"/>
+      <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="str">
@@ -788,7 +794,7 @@
         <v>21</v>
       </c>
       <c r="E5">
-        <f>IF(B5 &gt; 1900, ((B5-1900)*10)+400+C5, ((B5-1730)*2)+C5)+VLOOKUP(D5,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B5 &gt; 1900, ((B5-1900)*10)+400+C5, ((B5-1730)*2)+C5)+VLOOKUP(D5,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>807</v>
       </c>
       <c r="F5">
@@ -798,17 +804,17 @@
         <v>22</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F5*G5)/$B$1</f>
         <v>66.332495807108003</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="1"/>
+        <f>H5*0.9</f>
         <v>59.699246226397207</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2" t="str">
@@ -833,7 +839,7 @@
         <v>21</v>
       </c>
       <c r="E6">
-        <f>IF(B6 &gt; 1900, ((B6-1900)*10)+400+C6, ((B6-1730)*2)+C6)+VLOOKUP(D6,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B6 &gt; 1900, ((B6-1900)*10)+400+C6, ((B6-1730)*2)+C6)+VLOOKUP(D6,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1111</v>
       </c>
       <c r="F6">
@@ -843,17 +849,17 @@
         <v>36</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F6*G6)/$B$1</f>
         <v>89.442719099991592</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="1"/>
+        <f>H6*0.9</f>
         <v>80.498447189992433</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="2"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2" t="str">
@@ -878,7 +884,7 @@
         <v>21</v>
       </c>
       <c r="E7">
-        <f>IF(B7 &gt; 1900, ((B7-1900)*10)+400+C7, ((B7-1730)*2)+C7)+VLOOKUP(D7,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B7 &gt; 1900, ((B7-1900)*10)+400+C7, ((B7-1730)*2)+C7)+VLOOKUP(D7,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1241</v>
       </c>
       <c r="F7">
@@ -888,17 +894,17 @@
         <v>32</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F7*G7)/$B$1</f>
         <v>113.13708498984759</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="1"/>
+        <f>H7*0.9</f>
         <v>101.82337649086284</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="str">
@@ -923,7 +929,7 @@
         <v>21</v>
       </c>
       <c r="E8">
-        <f>IF(B8 &gt; 1900, ((B8-1900)*10)+400+C8, ((B8-1730)*2)+C8)+VLOOKUP(D8,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B8 &gt; 1900, ((B8-1900)*10)+400+C8, ((B8-1730)*2)+C8)+VLOOKUP(D8,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1271</v>
       </c>
       <c r="F8">
@@ -933,17 +939,17 @@
         <v>35</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F8*G8)/$B$1</f>
         <v>127.80193008453877</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="1"/>
+        <f>H8*0.9</f>
         <v>115.02173707608489</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2" t="str">
@@ -968,7 +974,7 @@
         <v>21</v>
       </c>
       <c r="E9">
-        <f>IF(B9 &gt; 1900, ((B9-1900)*10)+400+C9, ((B9-1730)*2)+C9)+VLOOKUP(D9,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B9 &gt; 1900, ((B9-1900)*10)+400+C9, ((B9-1730)*2)+C9)+VLOOKUP(D9,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1291</v>
       </c>
       <c r="F9">
@@ -978,17 +984,17 @@
         <v>50</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F9*G9)/$B$1</f>
         <v>126.92955176439848</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="1"/>
+        <f>H9*0.9</f>
         <v>114.23659658795863</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="2"/>
+      <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2" t="str">
@@ -1013,7 +1019,7 @@
         <v>21</v>
       </c>
       <c r="E10">
-        <f>IF(B10 &gt; 1900, ((B10-1900)*10)+400+C10, ((B10-1730)*2)+C10)+VLOOKUP(D10,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B10 &gt; 1900, ((B10-1900)*10)+400+C10, ((B10-1730)*2)+C10)+VLOOKUP(D10,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1331</v>
       </c>
       <c r="F10">
@@ -1023,17 +1029,17 @@
         <v>44</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F10*G10)/$B$1</f>
         <v>139.84117975602021</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="1"/>
+        <f>H10*0.9</f>
         <v>125.85706178041819</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="2"/>
+      <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2" t="str">
@@ -1058,7 +1064,7 @@
         <v>21</v>
       </c>
       <c r="E11">
-        <f>IF(B11 &gt; 1900, ((B11-1900)*10)+400+C11, ((B11-1730)*2)+C11)+VLOOKUP(D11,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B11 &gt; 1900, ((B11-1900)*10)+400+C11, ((B11-1730)*2)+C11)+VLOOKUP(D11,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1451</v>
       </c>
       <c r="F11">
@@ -1068,17 +1074,17 @@
         <v>57</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F11*G11)/$B$1</f>
         <v>155.13435037626795</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="1"/>
+        <f>H11*0.9</f>
         <v>139.62091533864117</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2" t="str">
@@ -1103,7 +1109,7 @@
         <v>21</v>
       </c>
       <c r="E12">
-        <f>IF(B12 &gt; 1900, ((B12-1900)*10)+400+C12, ((B12-1730)*2)+C12)+VLOOKUP(D12,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B12 &gt; 1900, ((B12-1900)*10)+400+C12, ((B12-1730)*2)+C12)+VLOOKUP(D12,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1541</v>
       </c>
       <c r="F12">
@@ -1113,17 +1119,17 @@
         <v>72</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F12*G12)/$B$1</f>
         <v>178.88543819998318</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" si="1"/>
+        <f>H12*0.9</f>
         <v>160.99689437998487</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="2"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2" t="str">
@@ -1148,7 +1154,7 @@
         <v>21</v>
       </c>
       <c r="E13">
-        <f>IF(B13 &gt; 1900, ((B13-1900)*10)+400+C13, ((B13-1730)*2)+C13)+VLOOKUP(D13,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B13 &gt; 1900, ((B13-1900)*10)+400+C13, ((B13-1730)*2)+C13)+VLOOKUP(D13,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1581</v>
       </c>
       <c r="F13">
@@ -1158,17 +1164,17 @@
         <v>34</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F13*G13)/$B$1</f>
         <v>169.44353369518447</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="1"/>
+        <f>H13*0.9</f>
         <v>152.49918032566603</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="2"/>
+      <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2" t="str">
@@ -1193,7 +1199,7 @@
         <v>21</v>
       </c>
       <c r="E14">
-        <f>IF(B14 &gt; 1900, ((B14-1900)*10)+400+C14, ((B14-1730)*2)+C14)+VLOOKUP(D14,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B14 &gt; 1900, ((B14-1900)*10)+400+C14, ((B14-1730)*2)+C14)+VLOOKUP(D14,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1582</v>
       </c>
       <c r="F14">
@@ -1203,17 +1209,17 @@
         <v>57</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F14*G14)/$B$1</f>
         <v>186.63690238892559</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="1"/>
+        <f>H14*0.9</f>
         <v>167.97321215003305</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2" t="str">
@@ -1238,7 +1244,7 @@
         <v>21</v>
       </c>
       <c r="E15">
-        <f>IF(B15 &gt; 1900, ((B15-1900)*10)+400+C15, ((B15-1730)*2)+C15)+VLOOKUP(D15,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B15 &gt; 1900, ((B15-1900)*10)+400+C15, ((B15-1730)*2)+C15)+VLOOKUP(D15,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1631</v>
       </c>
       <c r="F15">
@@ -1248,25 +1254,29 @@
         <v>52</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F15*G15)/$B$1</f>
         <v>178.26322609494585</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="1"/>
+        <f>H15*0.9</f>
         <v>160.43690348545127</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="3"/>
+      <c r="K15" s="3">
+        <v>11</v>
+      </c>
+      <c r="L15" s="3">
+        <v>2.5</v>
+      </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+        <v>51x0x18</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1283,7 +1293,7 @@
         <v>21</v>
       </c>
       <c r="E16">
-        <f>IF(B16 &gt; 1900, ((B16-1900)*10)+400+C16, ((B16-1730)*2)+C16)+VLOOKUP(D16,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B16 &gt; 1900, ((B16-1900)*10)+400+C16, ((B16-1730)*2)+C16)+VLOOKUP(D16,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1721</v>
       </c>
       <c r="F16">
@@ -1293,25 +1303,29 @@
         <v>58</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F16*G16)/$B$1</f>
         <v>183.06040290327977</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="1"/>
+        <f>H16*0.9</f>
         <v>164.75436261295178</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="3"/>
+      <c r="K16" s="3">
+        <v>11.3</v>
+      </c>
+      <c r="L16" s="3">
+        <v>2.5</v>
+      </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+        <v>53x0x18</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1328,7 +1342,7 @@
         <v>21</v>
       </c>
       <c r="E17">
-        <f>IF(B17 &gt; 1900, ((B17-1900)*10)+400+C17, ((B17-1730)*2)+C17)+VLOOKUP(D17,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B17 &gt; 1900, ((B17-1900)*10)+400+C17, ((B17-1730)*2)+C17)+VLOOKUP(D17,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1781</v>
       </c>
       <c r="F17">
@@ -1338,11 +1352,11 @@
         <v>55</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F17*G17)/$B$1</f>
         <v>194.65068427541911</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="1"/>
+        <f>H17*0.9</f>
         <v>175.18561584787722</v>
       </c>
       <c r="J17" s="2" t="s">
@@ -1379,7 +1393,7 @@
         <v>21</v>
       </c>
       <c r="E18">
-        <f>IF(B18 &gt; 1900, ((B18-1900)*10)+400+C18, ((B18-1730)*2)+C18)+VLOOKUP(D18,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B18 &gt; 1900, ((B18-1900)*10)+400+C18, ((B18-1730)*2)+C18)+VLOOKUP(D18,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1801</v>
       </c>
       <c r="F18">
@@ -1389,11 +1403,11 @@
         <v>73</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F18*G18)/$B$1</f>
         <v>195.2491286080996</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="1"/>
+        <f>H18*0.9</f>
         <v>175.72421574728963</v>
       </c>
       <c r="J18" s="2" t="s">
@@ -1430,7 +1444,7 @@
         <v>21</v>
       </c>
       <c r="E19">
-        <f>IF(B19 &gt; 1900, ((B19-1900)*10)+400+C19, ((B19-1730)*2)+C19)+VLOOKUP(D19,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B19 &gt; 1900, ((B19-1900)*10)+400+C19, ((B19-1730)*2)+C19)+VLOOKUP(D19,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1891</v>
       </c>
       <c r="F19">
@@ -1440,11 +1454,11 @@
         <v>50</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F19*G19)/$B$1</f>
         <v>176.38342073763937</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="1"/>
+        <f>H19*0.9</f>
         <v>158.74507866387543</v>
       </c>
       <c r="J19" s="2" t="s">
@@ -1481,7 +1495,7 @@
         <v>21</v>
       </c>
       <c r="E20">
-        <f>IF(B20 &gt; 1900, ((B20-1900)*10)+400+C20, ((B20-1730)*2)+C20)+VLOOKUP(D20,'ID Scheme'!$A$2:$B$5,2)</f>
+        <f>IF(B20 &gt; 1900, ((B20-1900)*10)+400+C20, ((B20-1730)*2)+C20)+VLOOKUP(D20,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
         <v>1981</v>
       </c>
       <c r="F20">
@@ -1491,168 +1505,192 @@
         <v>33</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F20*G20)/$B$1</f>
         <v>147.08274315273474</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="1"/>
+        <f>H20*0.9</f>
         <v>132.37446883746128</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="K20" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="L20" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M20" s="3">
+        <v>2.7</v>
+      </c>
       <c r="N20" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+        <v>48x13x17</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="B21">
-        <v>2012</v>
+        <v>2001</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
       <c r="E21">
-        <f>IF(B21 &gt; 1900, ((B21-1900)*10)+400+C21, ((B21-1730)*2)+C21)+VLOOKUP(D21,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>2122</v>
+        <f>IF(B21 &gt; 1900, ((B21-1900)*10)+400+C21, ((B21-1730)*2)+C21)+VLOOKUP(D21,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>2011</v>
       </c>
       <c r="F21">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G21">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="0"/>
-        <v>152.75252316519467</v>
+        <f>SQRT(F21*G21)/$B$1</f>
+        <v>212.39376429431988</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="1"/>
-        <v>137.4772708486752</v>
+        <f>H21*0.9</f>
+        <v>191.15438786488789</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="K21" s="3">
+        <v>12</v>
+      </c>
+      <c r="L21" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M21" s="3">
+        <v>3.3</v>
+      </c>
       <c r="N21" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+        <v>56x16x18</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B22">
         <v>2001</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
       </c>
       <c r="E22">
-        <f>IF(B22 &gt; 1900, ((B22-1900)*10)+400+C22, ((B22-1730)*2)+C22)+VLOOKUP(D22,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>2011</v>
+        <f>IF(B22 &gt; 1900, ((B22-1900)*10)+400+C22, ((B22-1730)*2)+C22)+VLOOKUP(D22,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>2012</v>
       </c>
       <c r="F22">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="G22">
-        <v>58</v>
+        <v>140</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" si="0"/>
-        <v>212.39376429431988</v>
+        <f>SQRT(F22*G22)/$B$1</f>
+        <v>292.49881291307071</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="1"/>
-        <v>191.15438786488789</v>
+        <f>H22*0.9</f>
+        <v>263.24893162176363</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="K22" s="3">
+        <v>18</v>
+      </c>
+      <c r="L22" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M22" s="3">
+        <v>3.2</v>
+      </c>
       <c r="N22" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+        <v>84x15x18</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="B23">
-        <v>2001</v>
+        <v>2005</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
       </c>
       <c r="E23">
-        <f>IF(B23 &gt; 1900, ((B23-1900)*10)+400+C23, ((B23-1730)*2)+C23)+VLOOKUP(D23,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>2012</v>
+        <f>IF(B23 &gt; 1900, ((B23-1900)*10)+400+C23, ((B23-1730)*2)+C23)+VLOOKUP(D23,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>2051</v>
       </c>
       <c r="F23">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G23">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="0"/>
-        <v>292.49881291307071</v>
+        <f>SQRT(F23*G23)/$B$1</f>
+        <v>244.94897427831785</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="1"/>
-        <v>263.24893162176363</v>
+        <f>H23*0.9</f>
+        <v>220.45407685048608</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K23" s="2"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+      <c r="K23" s="3">
+        <v>11.4</v>
+      </c>
+      <c r="L23" s="3">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="M23" s="3">
+        <v>4.2</v>
+      </c>
       <c r="N23" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+        <v>53x20x18</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B24">
-        <v>2005</v>
+        <v>2012</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1661,27 +1699,27 @@
         <v>21</v>
       </c>
       <c r="E24">
-        <f>IF(B24 &gt; 1900, ((B24-1900)*10)+400+C24, ((B24-1730)*2)+C24)+VLOOKUP(D24,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>2051</v>
+        <f>IF(B24 &gt; 1900, ((B24-1900)*10)+400+C24, ((B24-1730)*2)+C24)+VLOOKUP(D24,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>2121</v>
       </c>
       <c r="F24">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G24">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="0"/>
-        <v>244.94897427831785</v>
+        <f>SQRT(F24*G24)/$B$1</f>
+        <v>219.84843263788198</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="1"/>
-        <v>220.45407685048608</v>
+        <f>H24*0.9</f>
+        <v>197.86358937409378</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="2"/>
+      <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="2" t="str">
@@ -1694,55 +1732,61 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="B25">
-        <v>1800</v>
+        <v>2012</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E25">
-        <f>IF(B25 &gt; 1900, ((B25-1900)*10)+400+C25, ((B25-1730)*2)+C25)+VLOOKUP(D25,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>3741</v>
+        <f>IF(B25 &gt; 1900, ((B25-1900)*10)+400+C25, ((B25-1730)*2)+C25)+VLOOKUP(D25,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>2122</v>
       </c>
       <c r="F25">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G25">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" si="0"/>
-        <v>46.188021535170058</v>
+        <f>SQRT(F25*G25)/$B$1</f>
+        <v>152.75252316519467</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="1"/>
-        <v>41.569219381653056</v>
+        <f>H25*0.9</f>
+        <v>137.4772708486752</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="2"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="K25" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="L25" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M25" s="3">
+        <v>2.7</v>
+      </c>
       <c r="N25" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+        <v>48x13x17</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B26">
-        <v>1897</v>
+        <v>1800</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1751,27 +1795,27 @@
         <v>22</v>
       </c>
       <c r="E26">
-        <f>IF(B26 &gt; 1900, ((B26-1900)*10)+400+C26, ((B26-1730)*2)+C26)+VLOOKUP(D26,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>3935</v>
+        <f>IF(B26 &gt; 1900, ((B26-1900)*10)+400+C26, ((B26-1730)*2)+C26)+VLOOKUP(D26,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>3741</v>
       </c>
       <c r="F26">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G26">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="0"/>
-        <v>52.915026221291818</v>
+        <f>SQRT(F26*G26)/$B$1</f>
+        <v>46.188021535170058</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="1"/>
-        <v>47.623523599162638</v>
+        <f>H26*0.9</f>
+        <v>41.569219381653056</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K26" s="2"/>
+      <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="2" t="str">
@@ -1784,10 +1828,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B27">
-        <v>1902</v>
+        <v>1897</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1796,27 +1840,27 @@
         <v>22</v>
       </c>
       <c r="E27">
-        <f>IF(B27 &gt; 1900, ((B27-1900)*10)+400+C27, ((B27-1730)*2)+C27)+VLOOKUP(D27,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4021</v>
+        <f>IF(B27 &gt; 1900, ((B27-1900)*10)+400+C27, ((B27-1730)*2)+C27)+VLOOKUP(D27,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>3935</v>
       </c>
       <c r="F27">
         <v>18</v>
       </c>
       <c r="G27">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="0"/>
-        <v>56.568542494923797</v>
+        <f>SQRT(F27*G27)/$B$1</f>
+        <v>52.915026221291818</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="1"/>
-        <v>50.911688245431421</v>
+        <f>H27*0.9</f>
+        <v>47.623523599162638</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K27" s="2"/>
+      <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="2" t="str">
@@ -1829,10 +1873,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B28">
-        <v>1907</v>
+        <v>1902</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1841,27 +1885,27 @@
         <v>22</v>
       </c>
       <c r="E28">
-        <f>IF(B28 &gt; 1900, ((B28-1900)*10)+400+C28, ((B28-1730)*2)+C28)+VLOOKUP(D28,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4071</v>
+        <f>IF(B28 &gt; 1900, ((B28-1900)*10)+400+C28, ((B28-1730)*2)+C28)+VLOOKUP(D28,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4021</v>
       </c>
       <c r="F28">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G28">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="0"/>
-        <v>63.245553203367592</v>
+        <f>SQRT(F28*G28)/$B$1</f>
+        <v>56.568542494923797</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="1"/>
-        <v>56.920997883030836</v>
+        <f>H28*0.9</f>
+        <v>50.911688245431421</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K28" s="2"/>
+      <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="2" t="str">
@@ -1874,10 +1918,10 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B29">
-        <v>1913</v>
+        <v>1907</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1886,27 +1930,27 @@
         <v>22</v>
       </c>
       <c r="E29">
-        <f>IF(B29 &gt; 1900, ((B29-1900)*10)+400+C29, ((B29-1730)*2)+C29)+VLOOKUP(D29,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4131</v>
+        <f>IF(B29 &gt; 1900, ((B29-1900)*10)+400+C29, ((B29-1730)*2)+C29)+VLOOKUP(D29,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4071</v>
       </c>
       <c r="F29">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G29">
         <v>18</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" si="0"/>
-        <v>66.332495807108003</v>
+        <f>SQRT(F29*G29)/$B$1</f>
+        <v>63.245553203367592</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="1"/>
-        <v>59.699246226397207</v>
+        <f>H29*0.9</f>
+        <v>56.920997883030836</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K29" s="2"/>
+      <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="2" t="str">
@@ -1919,10 +1963,10 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="B30">
-        <v>1928</v>
+        <v>1913</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1932,26 +1976,26 @@
       </c>
       <c r="E30">
         <f>IF(B30 &gt; 1900, ((B30-1900)*10)+400+C30, ((B30-1730)*2)+C30)+VLOOKUP(D30,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4281</v>
+        <v>4131</v>
       </c>
       <c r="F30">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G30">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="0"/>
-        <v>78.528126595931653</v>
+        <f>SQRT(F30*G30)/$B$1</f>
+        <v>66.332495807108003</v>
       </c>
       <c r="I30" s="2">
-        <f t="shared" si="1"/>
-        <v>70.675313936338483</v>
+        <f>H30*0.9</f>
+        <v>59.699246226397207</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K30" s="2"/>
+      <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="2" t="str">
@@ -1964,10 +2008,10 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B31">
-        <v>1935</v>
+        <v>1920</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1977,42 +2021,48 @@
       </c>
       <c r="E31">
         <f>IF(B31 &gt; 1900, ((B31-1900)*10)+400+C31, ((B31-1730)*2)+C31)+VLOOKUP(D31,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4351</v>
+        <v>4201</v>
       </c>
       <c r="F31">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="G31">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="0"/>
-        <v>96.609178307929596</v>
+        <f>SQRT(F31*G31)/$B$1</f>
+        <v>74.833147735478832</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="1"/>
-        <v>86.948260477136643</v>
+        <f>H31*0.9</f>
+        <v>67.349832961930957</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K31" s="2"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
+      <c r="K31" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="L31" s="3">
+        <v>2</v>
+      </c>
+      <c r="M31">
+        <v>2.5</v>
+      </c>
       <c r="N31" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+        <v>16x12x14</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="B32">
-        <v>1936</v>
+        <v>1928</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2021,27 +2071,27 @@
         <v>22</v>
       </c>
       <c r="E32">
-        <f>IF(B32 &gt; 1900, ((B32-1900)*10)+400+C32, ((B32-1730)*2)+C32)+VLOOKUP(D32,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4361</v>
+        <f>IF(B32 &gt; 1900, ((B32-1900)*10)+400+C32, ((B32-1730)*2)+C32)+VLOOKUP(D32,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4281</v>
       </c>
       <c r="F32">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G32">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="0"/>
-        <v>81.649658092772611</v>
+        <f>SQRT(F32*G32)/$B$1</f>
+        <v>78.528126595931653</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="1"/>
-        <v>73.484692283495349</v>
+        <f>H32*0.9</f>
+        <v>70.675313936338483</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K32" s="2"/>
+      <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="2" t="str">
@@ -2054,10 +2104,10 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="B33">
-        <v>1952</v>
+        <v>1935</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2066,27 +2116,27 @@
         <v>22</v>
       </c>
       <c r="E33">
-        <f>IF(B33 &gt; 1900, ((B33-1900)*10)+400+C33, ((B33-1730)*2)+C33)+VLOOKUP(D33,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4521</v>
+        <f>IF(B33 &gt; 1900, ((B33-1900)*10)+400+C33, ((B33-1730)*2)+C33)+VLOOKUP(D33,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4351</v>
       </c>
       <c r="F33">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G33">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="0"/>
-        <v>102.74023338281629</v>
+        <f>SQRT(F33*G33)/$B$1</f>
+        <v>96.609178307929596</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="1"/>
-        <v>92.466210044534662</v>
+        <f>H33*0.9</f>
+        <v>86.948260477136643</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K33" s="2"/>
+      <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="2" t="str">
@@ -2099,10 +2149,10 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B34">
-        <v>1957</v>
+        <v>1936</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2111,27 +2161,27 @@
         <v>22</v>
       </c>
       <c r="E34">
-        <f>IF(B34 &gt; 1900, ((B34-1900)*10)+400+C34, ((B34-1730)*2)+C34)+VLOOKUP(D34,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4571</v>
+        <f>IF(B34 &gt; 1900, ((B34-1900)*10)+400+C34, ((B34-1730)*2)+C34)+VLOOKUP(D34,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4361</v>
       </c>
       <c r="F34">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G34">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="0"/>
-        <v>97.809338340808068</v>
+        <f>SQRT(F34*G34)/$B$1</f>
+        <v>81.649658092772611</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" si="1"/>
-        <v>88.02840450672727</v>
+        <f>H34*0.9</f>
+        <v>73.484692283495349</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K34" s="2"/>
+      <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="2" t="str">
@@ -2144,10 +2194,10 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="B35">
-        <v>1963</v>
+        <v>1948</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2156,43 +2206,33 @@
         <v>22</v>
       </c>
       <c r="E35">
-        <f>IF(B35 &gt; 1900, ((B35-1900)*10)+400+C35, ((B35-1730)*2)+C35)+VLOOKUP(D35,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4631</v>
+        <f>IF(B35 &gt; 1900, ((B35-1900)*10)+400+C35, ((B35-1730)*2)+C35)+VLOOKUP(D35,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4481</v>
       </c>
       <c r="F35">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G35">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" si="0"/>
-        <v>108.32051206181282</v>
+        <f>SQRT(F35*G35)/$B$1</f>
+        <v>53.541261347363367</v>
       </c>
       <c r="I35" s="2">
-        <f t="shared" si="1"/>
-        <v>97.488460855631544</v>
+        <f>H35*0.9</f>
+        <v>48.187135212627034</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="K35" s="2"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="2" t="str">
-        <f>CONCATENATE(
-ROUND(K35*VLOOKUP(D35,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M35*VLOOKUP(D35,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L35*VLOOKUP(D35,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B36">
-        <v>1964</v>
+        <v>1952</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2201,27 +2241,27 @@
         <v>22</v>
       </c>
       <c r="E36">
-        <f>IF(B36 &gt; 1900, ((B36-1900)*10)+400+C36, ((B36-1730)*2)+C36)+VLOOKUP(D36,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4641</v>
+        <f>IF(B36 &gt; 1900, ((B36-1900)*10)+400+C36, ((B36-1730)*2)+C36)+VLOOKUP(D36,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4521</v>
       </c>
       <c r="F36">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="G36">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" ref="H36:H62" si="2">SQRT(F36*G36)/$B$1</f>
-        <v>146.9693845669907</v>
+        <f>SQRT(F36*G36)/$B$1</f>
+        <v>102.74023338281629</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" ref="I36:I62" si="3">H36*0.9</f>
-        <v>132.27244611029164</v>
+        <f>H36*0.9</f>
+        <v>92.466210044534662</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K36" s="2"/>
+      <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="2" t="str">
@@ -2234,39 +2274,39 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B37">
-        <v>1964</v>
+        <v>1957</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" t="s">
         <v>22</v>
       </c>
       <c r="E37">
-        <f>IF(B37 &gt; 1900, ((B37-1900)*10)+400+C37, ((B37-1730)*2)+C37)+VLOOKUP(D37,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4642</v>
+        <f>IF(B37 &gt; 1900, ((B37-1900)*10)+400+C37, ((B37-1730)*2)+C37)+VLOOKUP(D37,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4571</v>
       </c>
       <c r="F37">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="G37">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="2"/>
-        <v>114.89125293076057</v>
+        <f>SQRT(F37*G37)/$B$1</f>
+        <v>97.809338340808068</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="3"/>
-        <v>103.40212763768452</v>
+        <f>H37*0.9</f>
+        <v>88.02840450672727</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K37" s="2"/>
+      <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="2" t="str">
@@ -2276,16 +2316,13 @@
 ROUND(L37*VLOOKUP(D37,'ID Scheme'!$A$2:$E$5,5),0))</f>
         <v>0x0x0</v>
       </c>
-      <c r="O37" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B38">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2294,27 +2331,27 @@
         <v>22</v>
       </c>
       <c r="E38">
-        <f>IF(B38 &gt; 1900, ((B38-1900)*10)+400+C38, ((B38-1730)*2)+C38)+VLOOKUP(D38,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4651</v>
+        <f>IF(B38 &gt; 1900, ((B38-1900)*10)+400+C38, ((B38-1730)*2)+C38)+VLOOKUP(D38,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4631</v>
       </c>
       <c r="F38">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="G38">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="2"/>
-        <v>150.99668870541501</v>
+        <f>SQRT(F38*G38)/$B$1</f>
+        <v>108.32051206181282</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="3"/>
-        <v>135.8970198348735</v>
+        <f>H38*0.9</f>
+        <v>97.488460855631544</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K38" s="2"/>
+      <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="2" t="str">
@@ -2327,10 +2364,10 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B39">
-        <v>1968</v>
+        <v>1964</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2339,27 +2376,27 @@
         <v>22</v>
       </c>
       <c r="E39">
-        <f>IF(B39 &gt; 1900, ((B39-1900)*10)+400+C39, ((B39-1730)*2)+C39)+VLOOKUP(D39,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4681</v>
+        <f>IF(B39 &gt; 1900, ((B39-1900)*10)+400+C39, ((B39-1730)*2)+C39)+VLOOKUP(D39,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4641</v>
       </c>
       <c r="F39">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="G39">
         <v>36</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="2"/>
-        <v>164.92422502470643</v>
+        <f>SQRT(F39*G39)/$B$1</f>
+        <v>146.9693845669907</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" si="3"/>
-        <v>148.43180252223578</v>
+        <f>H39*0.9</f>
+        <v>132.27244611029164</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K39" s="2"/>
+      <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="2" t="str">
@@ -2372,39 +2409,39 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B40">
-        <v>1980</v>
+        <v>1964</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40" t="s">
         <v>22</v>
       </c>
       <c r="E40">
-        <f>IF(B40 &gt; 1900, ((B40-1900)*10)+400+C40, ((B40-1730)*2)+C40)+VLOOKUP(D40,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4801</v>
+        <f>IF(B40 &gt; 1900, ((B40-1900)*10)+400+C40, ((B40-1730)*2)+C40)+VLOOKUP(D40,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4642</v>
       </c>
       <c r="F40">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G40">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="H40" s="2">
-        <f t="shared" si="2"/>
-        <v>170.09801096230765</v>
+        <f>SQRT(F40*G40)/$B$1</f>
+        <v>114.89125293076057</v>
       </c>
       <c r="I40" s="2">
-        <f t="shared" si="3"/>
-        <v>153.08820986607688</v>
+        <f>H40*0.9</f>
+        <v>103.40212763768452</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K40" s="2"/>
+      <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="2" t="str">
@@ -2414,13 +2451,16 @@
 ROUND(L40*VLOOKUP(D40,'ID Scheme'!$A$2:$E$5,5),0))</f>
         <v>0x0x0</v>
       </c>
+      <c r="O40" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B41">
-        <v>1982</v>
+        <v>1965</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2429,27 +2469,27 @@
         <v>22</v>
       </c>
       <c r="E41">
-        <f>IF(B41 &gt; 1900, ((B41-1900)*10)+400+C41, ((B41-1730)*2)+C41)+VLOOKUP(D41,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4821</v>
+        <f>IF(B41 &gt; 1900, ((B41-1900)*10)+400+C41, ((B41-1730)*2)+C41)+VLOOKUP(D41,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4651</v>
       </c>
       <c r="F41">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G41">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H41" s="2">
-        <f t="shared" si="2"/>
-        <v>136.62601021279465</v>
+        <f>SQRT(F41*G41)/$B$1</f>
+        <v>150.99668870541501</v>
       </c>
       <c r="I41" s="2">
-        <f t="shared" si="3"/>
-        <v>122.9634091915152</v>
+        <f>H41*0.9</f>
+        <v>135.8970198348735</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K41" s="2"/>
+      <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="2" t="str">
@@ -2462,10 +2502,10 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="B42">
-        <v>1986</v>
+        <v>1968</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2474,27 +2514,27 @@
         <v>22</v>
       </c>
       <c r="E42">
-        <f>IF(B42 &gt; 1900, ((B42-1900)*10)+400+C42, ((B42-1730)*2)+C42)+VLOOKUP(D42,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4861</v>
+        <f>IF(B42 &gt; 1900, ((B42-1900)*10)+400+C42, ((B42-1730)*2)+C42)+VLOOKUP(D42,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4681</v>
       </c>
       <c r="F42">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="G42">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" si="2"/>
-        <v>143.75905768565215</v>
+        <f>SQRT(F42*G42)/$B$1</f>
+        <v>164.92422502470643</v>
       </c>
       <c r="I42" s="2">
-        <f t="shared" si="3"/>
-        <v>129.38315191708693</v>
+        <f>H42*0.9</f>
+        <v>148.43180252223578</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K42" s="2"/>
+      <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="2" t="str">
@@ -2507,10 +2547,10 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B43">
-        <v>1987</v>
+        <v>1980</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2519,27 +2559,27 @@
         <v>22</v>
       </c>
       <c r="E43">
-        <f>IF(B43 &gt; 1900, ((B43-1900)*10)+400+C43, ((B43-1730)*2)+C43)+VLOOKUP(D43,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4871</v>
+        <f>IF(B43 &gt; 1900, ((B43-1900)*10)+400+C43, ((B43-1730)*2)+C43)+VLOOKUP(D43,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4801</v>
       </c>
       <c r="F43">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G43">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" si="2"/>
-        <v>178.26322609494585</v>
+        <f>SQRT(F43*G43)/$B$1</f>
+        <v>170.09801096230765</v>
       </c>
       <c r="I43" s="2">
-        <f t="shared" si="3"/>
-        <v>160.43690348545127</v>
+        <f>H43*0.9</f>
+        <v>153.08820986607688</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K43" s="2"/>
+      <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="2" t="str">
@@ -2552,10 +2592,10 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B44">
-        <v>1995</v>
+        <v>1982</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -2564,27 +2604,27 @@
         <v>22</v>
       </c>
       <c r="E44">
-        <f>IF(B44 &gt; 1900, ((B44-1900)*10)+400+C44, ((B44-1730)*2)+C44)+VLOOKUP(D44,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4951</v>
+        <f>IF(B44 &gt; 1900, ((B44-1900)*10)+400+C44, ((B44-1730)*2)+C44)+VLOOKUP(D44,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4821</v>
       </c>
       <c r="F44">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G44">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="H44" s="2">
-        <f t="shared" si="2"/>
-        <v>190.43809142780935</v>
+        <f>SQRT(F44*G44)/$B$1</f>
+        <v>136.62601021279465</v>
       </c>
       <c r="I44" s="2">
-        <f t="shared" si="3"/>
-        <v>171.39428228502842</v>
+        <f>H44*0.9</f>
+        <v>122.9634091915152</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K44" s="2"/>
+      <c r="K44" s="3"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="2" t="str">
@@ -2597,10 +2637,10 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B45">
-        <v>1997</v>
+        <v>1986</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2609,27 +2649,27 @@
         <v>22</v>
       </c>
       <c r="E45">
-        <f>IF(B45 &gt; 1900, ((B45-1900)*10)+400+C45, ((B45-1730)*2)+C45)+VLOOKUP(D45,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>4971</v>
+        <f>IF(B45 &gt; 1900, ((B45-1900)*10)+400+C45, ((B45-1730)*2)+C45)+VLOOKUP(D45,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4861</v>
       </c>
       <c r="F45">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G45">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H45" s="2">
-        <f t="shared" si="2"/>
-        <v>157.76212754932311</v>
+        <f>SQRT(F45*G45)/$B$1</f>
+        <v>143.75905768565215</v>
       </c>
       <c r="I45" s="2">
-        <f t="shared" si="3"/>
-        <v>141.98591479439079</v>
+        <f>H45*0.9</f>
+        <v>129.38315191708693</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K45" s="2"/>
+      <c r="K45" s="3"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="2" t="str">
@@ -2642,10 +2682,10 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B46">
-        <v>2004</v>
+        <v>1987</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -2654,27 +2694,27 @@
         <v>22</v>
       </c>
       <c r="E46">
-        <f>IF(B46 &gt; 1900, ((B46-1900)*10)+400+C46, ((B46-1730)*2)+C46)+VLOOKUP(D46,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>5041</v>
+        <f>IF(B46 &gt; 1900, ((B46-1900)*10)+400+C46, ((B46-1730)*2)+C46)+VLOOKUP(D46,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4871</v>
       </c>
       <c r="F46">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G46">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" si="2"/>
-        <v>207.84609690826528</v>
+        <f>SQRT(F46*G46)/$B$1</f>
+        <v>178.26322609494585</v>
       </c>
       <c r="I46" s="2">
-        <f t="shared" si="3"/>
-        <v>187.06148721743875</v>
+        <f>H46*0.9</f>
+        <v>160.43690348545127</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K46" s="2"/>
+      <c r="K46" s="3"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="2" t="str">
@@ -2687,39 +2727,39 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="B47">
-        <v>1912</v>
+        <v>1995</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E47">
         <f>IF(B47 &gt; 1900, ((B47-1900)*10)+400+C47, ((B47-1730)*2)+C47)+VLOOKUP(D47,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7121</v>
+        <v>4951</v>
       </c>
       <c r="F47">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="G47">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" si="2"/>
-        <v>42.163702135578397</v>
+        <f>SQRT(F47*G47)/$B$1</f>
+        <v>190.43809142780935</v>
       </c>
       <c r="I47" s="2">
-        <f t="shared" si="3"/>
-        <v>37.94733192202056</v>
+        <f>H47*0.9</f>
+        <v>171.39428228502842</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K47" s="2"/>
+      <c r="K47" s="3"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="2" t="str">
@@ -2732,39 +2772,39 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="B48">
-        <v>1938</v>
+        <v>1997</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E48">
         <f>IF(B48 &gt; 1900, ((B48-1900)*10)+400+C48, ((B48-1730)*2)+C48)+VLOOKUP(D48,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7381</v>
+        <v>4971</v>
       </c>
       <c r="F48">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="G48">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" si="2"/>
-        <v>50</v>
+        <f>SQRT(F48*G48)/$B$1</f>
+        <v>157.76212754932311</v>
       </c>
       <c r="I48" s="2">
-        <f t="shared" si="3"/>
-        <v>45</v>
+        <f>H48*0.9</f>
+        <v>141.98591479439079</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K48" s="2"/>
+      <c r="K48" s="3"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="2" t="str">
@@ -2777,39 +2817,39 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="B49">
-        <v>1957</v>
+        <v>2004</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E49">
         <f>IF(B49 &gt; 1900, ((B49-1900)*10)+400+C49, ((B49-1730)*2)+C49)+VLOOKUP(D49,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7571</v>
+        <v>5041</v>
       </c>
       <c r="F49">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="G49">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="H49" s="2">
-        <f t="shared" si="2"/>
-        <v>63.245553203367592</v>
+        <f>SQRT(F49*G49)/$B$1</f>
+        <v>207.84609690826528</v>
       </c>
       <c r="I49" s="2">
-        <f t="shared" si="3"/>
-        <v>56.920997883030836</v>
+        <f>H49*0.9</f>
+        <v>187.06148721743875</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K49" s="2"/>
+      <c r="K49" s="3"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="2" t="str">
@@ -2822,10 +2862,10 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B50">
-        <v>1960</v>
+        <v>1912</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2835,26 +2875,26 @@
       </c>
       <c r="E50">
         <f>IF(B50 &gt; 1900, ((B50-1900)*10)+400+C50, ((B50-1730)*2)+C50)+VLOOKUP(D50,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7601</v>
+        <v>7121</v>
       </c>
       <c r="F50">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="G50">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" si="2"/>
-        <v>73.029674334022147</v>
+        <f>SQRT(F50*G50)/$B$1</f>
+        <v>42.163702135578397</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" si="3"/>
-        <v>65.726706900619931</v>
+        <f>H50*0.9</f>
+        <v>37.94733192202056</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K50" s="2"/>
+      <c r="K50" s="3"/>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="2" t="str">
@@ -2867,10 +2907,10 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="B51">
-        <v>1965</v>
+        <v>1938</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -2879,27 +2919,27 @@
         <v>23</v>
       </c>
       <c r="E51">
-        <f>IF(B51 &gt; 1900, ((B51-1900)*10)+400+C51, ((B51-1730)*2)+C51)+VLOOKUP(D51,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>7651</v>
+        <f>IF(B51 &gt; 1900, ((B51-1900)*10)+400+C51, ((B51-1730)*2)+C51)+VLOOKUP(D51,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>7381</v>
       </c>
       <c r="F51">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="G51">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" si="2"/>
-        <v>76.011695006609202</v>
+        <f>SQRT(F51*G51)/$B$1</f>
+        <v>50</v>
       </c>
       <c r="I51" s="2">
-        <f t="shared" si="3"/>
-        <v>68.410525505948286</v>
+        <f>H51*0.9</f>
+        <v>45</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K51" s="2"/>
+      <c r="K51" s="3"/>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="2" t="str">
@@ -2912,10 +2952,10 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B52">
-        <v>1986</v>
+        <v>1957</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -2924,27 +2964,27 @@
         <v>23</v>
       </c>
       <c r="E52">
-        <f>IF(B52 &gt; 1900, ((B52-1900)*10)+400+C52, ((B52-1730)*2)+C52)+VLOOKUP(D52,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>7861</v>
+        <f>IF(B52 &gt; 1900, ((B52-1900)*10)+400+C52, ((B52-1730)*2)+C52)+VLOOKUP(D52,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>7571</v>
       </c>
       <c r="F52">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="G52">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" si="2"/>
-        <v>94.28090415820634</v>
+        <f>SQRT(F52*G52)/$B$1</f>
+        <v>63.245553203367592</v>
       </c>
       <c r="I52" s="2">
-        <f t="shared" si="3"/>
-        <v>84.852813742385706</v>
+        <f>H52*0.9</f>
+        <v>56.920997883030836</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K52" s="2"/>
+      <c r="K52" s="3"/>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="2" t="str">
@@ -2957,39 +2997,39 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B53">
-        <v>1986</v>
+        <v>1960</v>
       </c>
       <c r="C53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53" t="s">
         <v>23</v>
       </c>
       <c r="E53">
-        <f>IF(B53 &gt; 1900, ((B53-1900)*10)+400+C53, ((B53-1730)*2)+C53)+VLOOKUP(D53,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>7862</v>
+        <f>IF(B53 &gt; 1900, ((B53-1900)*10)+400+C53, ((B53-1730)*2)+C53)+VLOOKUP(D53,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>7601</v>
       </c>
       <c r="F53">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G53">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H53" s="2">
-        <f t="shared" si="2"/>
-        <v>53.748384988656994</v>
+        <f>SQRT(F53*G53)/$B$1</f>
+        <v>73.029674334022147</v>
       </c>
       <c r="I53" s="2">
-        <f t="shared" si="3"/>
-        <v>48.373546489791295</v>
+        <f>H53*0.9</f>
+        <v>65.726706900619931</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K53" s="2"/>
+      <c r="K53" s="3"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="2" t="str">
@@ -3002,10 +3042,10 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B54">
-        <v>2006</v>
+        <v>1965</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -3014,27 +3054,27 @@
         <v>23</v>
       </c>
       <c r="E54">
-        <f>IF(B54 &gt; 1900, ((B54-1900)*10)+400+C54, ((B54-1730)*2)+C54)+VLOOKUP(D54,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>8061</v>
+        <f>IF(B54 &gt; 1900, ((B54-1900)*10)+400+C54, ((B54-1730)*2)+C54)+VLOOKUP(D54,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>7651</v>
       </c>
       <c r="F54">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G54">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H54" s="2">
-        <f t="shared" si="2"/>
-        <v>106.45812948447541</v>
+        <f>SQRT(F54*G54)/$B$1</f>
+        <v>76.011695006609202</v>
       </c>
       <c r="I54" s="2">
-        <f t="shared" si="3"/>
-        <v>95.812316536027865</v>
+        <f>H54*0.9</f>
+        <v>68.410525505948286</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K54" s="2"/>
+      <c r="K54" s="3"/>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="2" t="str">
@@ -3047,10 +3087,10 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B55">
-        <v>2012</v>
+        <v>1986</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -3059,27 +3099,27 @@
         <v>23</v>
       </c>
       <c r="E55">
-        <f>IF(B55 &gt; 1900, ((B55-1900)*10)+400+C55, ((B55-1730)*2)+C55)+VLOOKUP(D55,'ID Scheme'!$A$2:$B$5,2)</f>
-        <v>8121</v>
+        <f>IF(B55 &gt; 1900, ((B55-1900)*10)+400+C55, ((B55-1730)*2)+C55)+VLOOKUP(D55,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>7861</v>
       </c>
       <c r="F55">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G55">
         <v>10</v>
       </c>
       <c r="H55" s="2">
-        <f t="shared" si="2"/>
-        <v>101.10500592068735</v>
+        <f>SQRT(F55*G55)/$B$1</f>
+        <v>94.28090415820634</v>
       </c>
       <c r="I55" s="2">
-        <f t="shared" si="3"/>
-        <v>90.994505328618615</v>
+        <f>H55*0.9</f>
+        <v>84.852813742385706</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K55" s="2"/>
+      <c r="K55" s="3"/>
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
       <c r="N55" s="2" t="str">
@@ -3092,39 +3132,39 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B56">
-        <v>1958</v>
+        <v>1986</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E56">
         <f>IF(B56 &gt; 1900, ((B56-1900)*10)+400+C56, ((B56-1730)*2)+C56)+VLOOKUP(D56,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10581</v>
+        <v>7862</v>
       </c>
       <c r="F56">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="G56">
         <v>4</v>
       </c>
       <c r="H56" s="2">
-        <f t="shared" si="2"/>
-        <v>57.735026918962582</v>
+        <f>SQRT(F56*G56)/$B$1</f>
+        <v>53.748384988656994</v>
       </c>
       <c r="I56" s="2">
-        <f t="shared" si="3"/>
-        <v>51.961524227066327</v>
+        <f>H56*0.9</f>
+        <v>48.373546489791295</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K56" s="2"/>
+      <c r="K56" s="3"/>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
       <c r="N56" s="2" t="str">
@@ -3134,118 +3174,103 @@
 ROUND(L56*VLOOKUP(D56,'ID Scheme'!$A$2:$E$5,5),0))</f>
         <v>0x0x0</v>
       </c>
-      <c r="O56" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B57">
-        <v>1976</v>
+        <v>2006</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E57">
         <f>IF(B57 &gt; 1900, ((B57-1900)*10)+400+C57, ((B57-1730)*2)+C57)+VLOOKUP(D57,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10761</v>
+        <v>8061</v>
       </c>
       <c r="F57">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G57">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H57" s="2">
-        <f t="shared" si="2"/>
-        <v>63.245553203367592</v>
+        <f>SQRT(F57*G57)/$B$1</f>
+        <v>106.45812948447541</v>
       </c>
       <c r="I57" s="2">
-        <f t="shared" si="3"/>
-        <v>56.920997883030836</v>
+        <f>H57*0.9</f>
+        <v>95.812316536027865</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K57" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="L57" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="M57" s="3">
-        <v>1.5</v>
-      </c>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
       <c r="N57" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>21x7x13</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B58">
-        <v>1994</v>
+        <v>2012</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E58">
         <f>IF(B58 &gt; 1900, ((B58-1900)*10)+400+C58, ((B58-1730)*2)+C58)+VLOOKUP(D58,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10941</v>
+        <v>8121</v>
       </c>
       <c r="F58">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="G58">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H58" s="2">
-        <f t="shared" si="2"/>
-        <v>73.029674334022147</v>
+        <f>SQRT(F58*G58)/$B$1</f>
+        <v>101.10500592068735</v>
       </c>
       <c r="I58" s="2">
-        <f t="shared" si="3"/>
-        <v>65.726706900619931</v>
+        <f>H58*0.9</f>
+        <v>90.994505328618615</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K58" s="2">
-        <v>5</v>
-      </c>
-      <c r="L58" s="3">
-        <v>2</v>
-      </c>
-      <c r="M58" s="3">
-        <v>1.5</v>
-      </c>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
       <c r="N58" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>23x7x14</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59">
-        <v>1997</v>
+        <v>1958</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -3255,26 +3280,26 @@
       </c>
       <c r="E59">
         <f>IF(B59 &gt; 1900, ((B59-1900)*10)+400+C59, ((B59-1730)*2)+C59)+VLOOKUP(D59,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10971</v>
+        <v>10581</v>
       </c>
       <c r="F59">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H59" s="2">
-        <f t="shared" si="2"/>
-        <v>67.082039324993701</v>
+        <f>SQRT(F59*G59)/$B$1</f>
+        <v>57.735026918962582</v>
       </c>
       <c r="I59" s="2">
-        <f t="shared" si="3"/>
-        <v>60.373835392494335</v>
+        <f>H59*0.9</f>
+        <v>51.961524227066327</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K59" s="2"/>
+      <c r="K59" s="3"/>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
       <c r="N59" s="2" t="str">
@@ -3285,15 +3310,15 @@
         <v>0x0x0</v>
       </c>
       <c r="O59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="B60">
-        <v>2004</v>
+        <v>1974</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -3303,42 +3328,32 @@
       </c>
       <c r="E60">
         <f>IF(B60 &gt; 1900, ((B60-1900)*10)+400+C60, ((B60-1730)*2)+C60)+VLOOKUP(D60,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>11041</v>
+        <v>10741</v>
       </c>
       <c r="F60">
-        <v>145</v>
+        <v>63</v>
       </c>
       <c r="G60">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H60" s="2">
-        <f t="shared" si="2"/>
-        <v>80.277297191948648</v>
+        <f>SQRT(F60*G60)/$B$1</f>
+        <v>74.833147735478832</v>
       </c>
       <c r="I60" s="2">
-        <f t="shared" si="3"/>
-        <v>72.249567472753782</v>
+        <f>H60*0.9</f>
+        <v>67.349832961930957</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="K60" s="2"/>
-      <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="2" t="str">
-        <f>CONCATENATE(
-ROUND(K60*VLOOKUP(D60,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M60*VLOOKUP(D60,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L60*VLOOKUP(D60,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B61">
-        <v>2009</v>
+        <v>1976</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -3348,135 +3363,234 @@
       </c>
       <c r="E61">
         <f>IF(B61 &gt; 1900, ((B61-1900)*10)+400+C61, ((B61-1730)*2)+C61)+VLOOKUP(D61,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>11091</v>
+        <v>10761</v>
       </c>
       <c r="F61">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="G61">
         <v>4</v>
       </c>
       <c r="H61" s="2">
-        <f t="shared" si="2"/>
-        <v>70.553368295055762</v>
+        <f>SQRT(F61*G61)/$B$1</f>
+        <v>63.245553203367592</v>
       </c>
       <c r="I61" s="2">
-        <f t="shared" si="3"/>
-        <v>63.498031465550184</v>
+        <f>H61*0.9</f>
+        <v>56.920997883030836</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K61" s="2"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
+      <c r="K61" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L61" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="M61" s="3">
+        <v>1.5</v>
+      </c>
       <c r="N61" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K61*VLOOKUP(D61,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M61*VLOOKUP(D61,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L61*VLOOKUP(D61,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+        <v>21x7x13</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B62">
-        <v>2012</v>
+        <v>1994</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="E62">
         <f>IF(B62 &gt; 1900, ((B62-1900)*10)+400+C62, ((B62-1730)*2)+C62)+VLOOKUP(D62,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>2121</v>
+        <v>10941</v>
       </c>
       <c r="F62">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="G62">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="H62" s="2">
-        <f t="shared" si="2"/>
-        <v>219.84843263788198</v>
+        <f>SQRT(F62*G62)/$B$1</f>
+        <v>73.029674334022147</v>
       </c>
       <c r="I62" s="2">
-        <f t="shared" si="3"/>
-        <v>197.86358937409378</v>
+        <f>H62*0.9</f>
+        <v>65.726706900619931</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K62" s="2"/>
-      <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
+      <c r="K62" s="3">
+        <v>5</v>
+      </c>
+      <c r="L62" s="3">
+        <v>2</v>
+      </c>
+      <c r="M62" s="3">
+        <v>1.5</v>
+      </c>
       <c r="N62" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K62*VLOOKUP(D62,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M62*VLOOKUP(D62,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L62*VLOOKUP(D62,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+        <v>23x7x14</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B63">
-        <v>1920</v>
+        <v>1997</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E63">
         <f>IF(B63 &gt; 1900, ((B63-1900)*10)+400+C63, ((B63-1730)*2)+C63)+VLOOKUP(D63,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4201</v>
+        <v>10971</v>
       </c>
       <c r="F63">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="G63">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="H63" s="2">
-        <f t="shared" ref="H63" si="4">SQRT(F63*G63)/$B$1</f>
-        <v>74.833147735478832</v>
+        <f>SQRT(F63*G63)/$B$1</f>
+        <v>67.082039324993701</v>
       </c>
       <c r="I63" s="2">
-        <f t="shared" ref="I63" si="5">H63*0.9</f>
-        <v>67.349832961930957</v>
+        <f>H63*0.9</f>
+        <v>60.373835392494335</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K63">
-        <v>3.4</v>
-      </c>
-      <c r="L63" s="3">
-        <v>2</v>
-      </c>
-      <c r="M63">
-        <v>2.5</v>
-      </c>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
       <c r="N63" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>16x12x14</v>
+        <v>0x0x0</v>
+      </c>
+      <c r="O63" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64">
+        <v>2004</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>62</v>
+      </c>
+      <c r="E64">
+        <f>IF(B64 &gt; 1900, ((B64-1900)*10)+400+C64, ((B64-1730)*2)+C64)+VLOOKUP(D64,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>11041</v>
+      </c>
+      <c r="F64">
+        <v>145</v>
+      </c>
+      <c r="G64">
+        <v>4</v>
+      </c>
+      <c r="H64" s="2">
+        <f>SQRT(F64*G64)/$B$1</f>
+        <v>80.277297191948648</v>
+      </c>
+      <c r="I64" s="2">
+        <f>H64*0.9</f>
+        <v>72.249567472753782</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K64*VLOOKUP(D64,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M64*VLOOKUP(D64,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L64*VLOOKUP(D64,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65">
+        <v>2009</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>62</v>
+      </c>
+      <c r="E65">
+        <f>IF(B65 &gt; 1900, ((B65-1900)*10)+400+C65, ((B65-1730)*2)+C65)+VLOOKUP(D65,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>11091</v>
+      </c>
+      <c r="F65">
+        <v>112</v>
+      </c>
+      <c r="G65">
+        <v>4</v>
+      </c>
+      <c r="H65" s="2">
+        <f>SQRT(F65*G65)/$B$1</f>
+        <v>70.553368295055762</v>
+      </c>
+      <c r="I65" s="2">
+        <f>H65*0.9</f>
+        <v>63.498031465550184</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>0x0x0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:O61">
-    <sortCondition ref="E33"/>
+  <sortState ref="A4:O65">
+    <sortCondition ref="E65"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added mid-size trucks (Ford Cargo etc)
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCA59F8-E0AE-4107-8D10-1804E2456EDC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C41D3CC-A7C2-4519-AD85-76753EFE04B6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="101">
   <si>
     <t>Vehicle</t>
   </si>
@@ -294,6 +294,36 @@
   </si>
   <si>
     <t>Scammell Scarab</t>
+  </si>
+  <si>
+    <t>Ford Cargo</t>
+  </si>
+  <si>
+    <t>Bedford TK</t>
+  </si>
+  <si>
+    <t>Ford D Series</t>
+  </si>
+  <si>
+    <t>Iveco Eurocargo</t>
+  </si>
+  <si>
+    <t>Mitsubishi Fuso Canter</t>
+  </si>
+  <si>
+    <t>175hp</t>
+  </si>
+  <si>
+    <t>90hp</t>
+  </si>
+  <si>
+    <t>82hp</t>
+  </si>
+  <si>
+    <t>72hp</t>
+  </si>
+  <si>
+    <t>105hp</t>
   </si>
 </sst>
 </file>
@@ -659,11 +689,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+      <pane ySplit="3" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,11 +789,11 @@
         <v>14</v>
       </c>
       <c r="H4" s="2">
-        <f>SQRT(F4*G4)/$B$1</f>
+        <f t="shared" ref="H4:H35" si="0">SQRT(F4*G4)/$B$1</f>
         <v>52.915026221291818</v>
       </c>
       <c r="I4" s="2">
-        <f>H4*0.9</f>
+        <f t="shared" ref="I4:I35" si="1">H4*0.9</f>
         <v>47.623523599162638</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -804,11 +834,11 @@
         <v>22</v>
       </c>
       <c r="H5" s="2">
-        <f>SQRT(F5*G5)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>66.332495807108003</v>
       </c>
       <c r="I5" s="2">
-        <f>H5*0.9</f>
+        <f t="shared" si="1"/>
         <v>59.699246226397207</v>
       </c>
       <c r="J5" s="2" t="s">
@@ -849,11 +879,11 @@
         <v>36</v>
       </c>
       <c r="H6" s="2">
-        <f>SQRT(F6*G6)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>89.442719099991592</v>
       </c>
       <c r="I6" s="2">
-        <f>H6*0.9</f>
+        <f t="shared" si="1"/>
         <v>80.498447189992433</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -894,11 +924,11 @@
         <v>32</v>
       </c>
       <c r="H7" s="2">
-        <f>SQRT(F7*G7)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>113.13708498984759</v>
       </c>
       <c r="I7" s="2">
-        <f>H7*0.9</f>
+        <f t="shared" si="1"/>
         <v>101.82337649086284</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -939,11 +969,11 @@
         <v>35</v>
       </c>
       <c r="H8" s="2">
-        <f>SQRT(F8*G8)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>127.80193008453877</v>
       </c>
       <c r="I8" s="2">
-        <f>H8*0.9</f>
+        <f t="shared" si="1"/>
         <v>115.02173707608489</v>
       </c>
       <c r="J8" s="2" t="s">
@@ -984,11 +1014,11 @@
         <v>50</v>
       </c>
       <c r="H9" s="2">
-        <f>SQRT(F9*G9)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>126.92955176439848</v>
       </c>
       <c r="I9" s="2">
-        <f>H9*0.9</f>
+        <f t="shared" si="1"/>
         <v>114.23659658795863</v>
       </c>
       <c r="J9" s="2" t="s">
@@ -1029,11 +1059,11 @@
         <v>44</v>
       </c>
       <c r="H10" s="2">
-        <f>SQRT(F10*G10)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>139.84117975602021</v>
       </c>
       <c r="I10" s="2">
-        <f>H10*0.9</f>
+        <f t="shared" si="1"/>
         <v>125.85706178041819</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -1074,11 +1104,11 @@
         <v>57</v>
       </c>
       <c r="H11" s="2">
-        <f>SQRT(F11*G11)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>155.13435037626795</v>
       </c>
       <c r="I11" s="2">
-        <f>H11*0.9</f>
+        <f t="shared" si="1"/>
         <v>139.62091533864117</v>
       </c>
       <c r="J11" s="2" t="s">
@@ -1119,11 +1149,11 @@
         <v>72</v>
       </c>
       <c r="H12" s="2">
-        <f>SQRT(F12*G12)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>178.88543819998318</v>
       </c>
       <c r="I12" s="2">
-        <f>H12*0.9</f>
+        <f t="shared" si="1"/>
         <v>160.99689437998487</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -1164,11 +1194,11 @@
         <v>34</v>
       </c>
       <c r="H13" s="2">
-        <f>SQRT(F13*G13)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>169.44353369518447</v>
       </c>
       <c r="I13" s="2">
-        <f>H13*0.9</f>
+        <f t="shared" si="1"/>
         <v>152.49918032566603</v>
       </c>
       <c r="J13" s="2" t="s">
@@ -1209,11 +1239,11 @@
         <v>57</v>
       </c>
       <c r="H14" s="2">
-        <f>SQRT(F14*G14)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>186.63690238892559</v>
       </c>
       <c r="I14" s="2">
-        <f>H14*0.9</f>
+        <f t="shared" si="1"/>
         <v>167.97321215003305</v>
       </c>
       <c r="J14" s="2" t="s">
@@ -1254,11 +1284,11 @@
         <v>52</v>
       </c>
       <c r="H15" s="2">
-        <f>SQRT(F15*G15)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>178.26322609494585</v>
       </c>
       <c r="I15" s="2">
-        <f>H15*0.9</f>
+        <f t="shared" si="1"/>
         <v>160.43690348545127</v>
       </c>
       <c r="J15" s="2" t="s">
@@ -1303,11 +1333,11 @@
         <v>58</v>
       </c>
       <c r="H16" s="2">
-        <f>SQRT(F16*G16)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>183.06040290327977</v>
       </c>
       <c r="I16" s="2">
-        <f>H16*0.9</f>
+        <f t="shared" si="1"/>
         <v>164.75436261295178</v>
       </c>
       <c r="J16" s="2" t="s">
@@ -1352,11 +1382,11 @@
         <v>55</v>
       </c>
       <c r="H17" s="2">
-        <f>SQRT(F17*G17)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>194.65068427541911</v>
       </c>
       <c r="I17" s="2">
-        <f>H17*0.9</f>
+        <f t="shared" si="1"/>
         <v>175.18561584787722</v>
       </c>
       <c r="J17" s="2" t="s">
@@ -1403,11 +1433,11 @@
         <v>73</v>
       </c>
       <c r="H18" s="2">
-        <f>SQRT(F18*G18)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>195.2491286080996</v>
       </c>
       <c r="I18" s="2">
-        <f>H18*0.9</f>
+        <f t="shared" si="1"/>
         <v>175.72421574728963</v>
       </c>
       <c r="J18" s="2" t="s">
@@ -1454,11 +1484,11 @@
         <v>50</v>
       </c>
       <c r="H19" s="2">
-        <f>SQRT(F19*G19)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>176.38342073763937</v>
       </c>
       <c r="I19" s="2">
-        <f>H19*0.9</f>
+        <f t="shared" si="1"/>
         <v>158.74507866387543</v>
       </c>
       <c r="J19" s="2" t="s">
@@ -1505,11 +1535,11 @@
         <v>33</v>
       </c>
       <c r="H20" s="2">
-        <f>SQRT(F20*G20)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>147.08274315273474</v>
       </c>
       <c r="I20" s="2">
-        <f>H20*0.9</f>
+        <f t="shared" si="1"/>
         <v>132.37446883746128</v>
       </c>
       <c r="J20" s="2" t="s">
@@ -1556,11 +1586,11 @@
         <v>58</v>
       </c>
       <c r="H21" s="2">
-        <f>SQRT(F21*G21)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>212.39376429431988</v>
       </c>
       <c r="I21" s="2">
-        <f>H21*0.9</f>
+        <f t="shared" si="1"/>
         <v>191.15438786488789</v>
       </c>
       <c r="J21" s="2" t="s">
@@ -1607,11 +1637,11 @@
         <v>140</v>
       </c>
       <c r="H22" s="2">
-        <f>SQRT(F22*G22)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>292.49881291307071</v>
       </c>
       <c r="I22" s="2">
-        <f>H22*0.9</f>
+        <f t="shared" si="1"/>
         <v>263.24893162176363</v>
       </c>
       <c r="J22" s="2" t="s">
@@ -1658,11 +1688,11 @@
         <v>90</v>
       </c>
       <c r="H23" s="2">
-        <f>SQRT(F23*G23)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>244.94897427831785</v>
       </c>
       <c r="I23" s="2">
-        <f>H23*0.9</f>
+        <f t="shared" si="1"/>
         <v>220.45407685048608</v>
       </c>
       <c r="J23" s="2" t="s">
@@ -1709,11 +1739,11 @@
         <v>87</v>
       </c>
       <c r="H24" s="2">
-        <f>SQRT(F24*G24)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>219.84843263788198</v>
       </c>
       <c r="I24" s="2">
-        <f>H24*0.9</f>
+        <f t="shared" si="1"/>
         <v>197.86358937409378</v>
       </c>
       <c r="J24" s="2" t="s">
@@ -1754,11 +1784,11 @@
         <v>35</v>
       </c>
       <c r="H25" s="2">
-        <f>SQRT(F25*G25)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>152.75252316519467</v>
       </c>
       <c r="I25" s="2">
-        <f>H25*0.9</f>
+        <f t="shared" si="1"/>
         <v>137.4772708486752</v>
       </c>
       <c r="J25" s="2" t="s">
@@ -1805,11 +1835,11 @@
         <v>12</v>
       </c>
       <c r="H26" s="2">
-        <f>SQRT(F26*G26)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>46.188021535170058</v>
       </c>
       <c r="I26" s="2">
-        <f>H26*0.9</f>
+        <f t="shared" si="1"/>
         <v>41.569219381653056</v>
       </c>
       <c r="J26" s="2" t="s">
@@ -1850,11 +1880,11 @@
         <v>14</v>
       </c>
       <c r="H27" s="2">
-        <f>SQRT(F27*G27)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>52.915026221291818</v>
       </c>
       <c r="I27" s="2">
-        <f>H27*0.9</f>
+        <f t="shared" si="1"/>
         <v>47.623523599162638</v>
       </c>
       <c r="J27" s="2" t="s">
@@ -1895,11 +1925,11 @@
         <v>16</v>
       </c>
       <c r="H28" s="2">
-        <f>SQRT(F28*G28)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>56.568542494923797</v>
       </c>
       <c r="I28" s="2">
-        <f>H28*0.9</f>
+        <f t="shared" si="1"/>
         <v>50.911688245431421</v>
       </c>
       <c r="J28" s="2" t="s">
@@ -1940,11 +1970,11 @@
         <v>18</v>
       </c>
       <c r="H29" s="2">
-        <f>SQRT(F29*G29)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>63.245553203367592</v>
       </c>
       <c r="I29" s="2">
-        <f>H29*0.9</f>
+        <f t="shared" si="1"/>
         <v>56.920997883030836</v>
       </c>
       <c r="J29" s="2" t="s">
@@ -1985,11 +2015,11 @@
         <v>18</v>
       </c>
       <c r="H30" s="2">
-        <f>SQRT(F30*G30)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>66.332495807108003</v>
       </c>
       <c r="I30" s="2">
-        <f>H30*0.9</f>
+        <f t="shared" si="1"/>
         <v>59.699246226397207</v>
       </c>
       <c r="J30" s="2" t="s">
@@ -2030,11 +2060,11 @@
         <v>28</v>
       </c>
       <c r="H31" s="2">
-        <f>SQRT(F31*G31)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>74.833147735478832</v>
       </c>
       <c r="I31" s="2">
-        <f>H31*0.9</f>
+        <f t="shared" si="1"/>
         <v>67.349832961930957</v>
       </c>
       <c r="J31" s="2" t="s">
@@ -2081,11 +2111,11 @@
         <v>15</v>
       </c>
       <c r="H32" s="2">
-        <f>SQRT(F32*G32)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>78.528126595931653</v>
       </c>
       <c r="I32" s="2">
-        <f>H32*0.9</f>
+        <f t="shared" si="1"/>
         <v>70.675313936338483</v>
       </c>
       <c r="J32" s="2" t="s">
@@ -2126,11 +2156,11 @@
         <v>24</v>
       </c>
       <c r="H33" s="2">
-        <f>SQRT(F33*G33)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>96.609178307929596</v>
       </c>
       <c r="I33" s="2">
-        <f>H33*0.9</f>
+        <f t="shared" si="1"/>
         <v>86.948260477136643</v>
       </c>
       <c r="J33" s="2" t="s">
@@ -2171,11 +2201,11 @@
         <v>20</v>
       </c>
       <c r="H34" s="2">
-        <f>SQRT(F34*G34)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>81.649658092772611</v>
       </c>
       <c r="I34" s="2">
-        <f>H34*0.9</f>
+        <f t="shared" si="1"/>
         <v>73.484692283495349</v>
       </c>
       <c r="J34" s="2" t="s">
@@ -2216,11 +2246,11 @@
         <v>6</v>
       </c>
       <c r="H35" s="2">
-        <f>SQRT(F35*G35)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>53.541261347363367</v>
       </c>
       <c r="I35" s="2">
-        <f>H35*0.9</f>
+        <f t="shared" si="1"/>
         <v>48.187135212627034</v>
       </c>
       <c r="J35" s="2" t="s">
@@ -2251,11 +2281,11 @@
         <v>25</v>
       </c>
       <c r="H36" s="2">
-        <f>SQRT(F36*G36)/$B$1</f>
+        <f t="shared" ref="H36:H67" si="2">SQRT(F36*G36)/$B$1</f>
         <v>102.74023338281629</v>
       </c>
       <c r="I36" s="2">
-        <f>H36*0.9</f>
+        <f t="shared" ref="I36:I70" si="3">H36*0.9</f>
         <v>92.466210044534662</v>
       </c>
       <c r="J36" s="2" t="s">
@@ -2296,11 +2326,11 @@
         <v>21</v>
       </c>
       <c r="H37" s="2">
-        <f>SQRT(F37*G37)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>97.809338340808068</v>
       </c>
       <c r="I37" s="2">
-        <f>H37*0.9</f>
+        <f t="shared" si="3"/>
         <v>88.02840450672727</v>
       </c>
       <c r="J37" s="2" t="s">
@@ -2341,11 +2371,11 @@
         <v>24</v>
       </c>
       <c r="H38" s="2">
-        <f>SQRT(F38*G38)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>108.32051206181282</v>
       </c>
       <c r="I38" s="2">
-        <f>H38*0.9</f>
+        <f t="shared" si="3"/>
         <v>97.488460855631544</v>
       </c>
       <c r="J38" s="2" t="s">
@@ -2386,11 +2416,11 @@
         <v>36</v>
       </c>
       <c r="H39" s="2">
-        <f>SQRT(F39*G39)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>146.9693845669907</v>
       </c>
       <c r="I39" s="2">
-        <f>H39*0.9</f>
+        <f t="shared" si="3"/>
         <v>132.27244611029164</v>
       </c>
       <c r="J39" s="2" t="s">
@@ -2431,11 +2461,11 @@
         <v>22</v>
       </c>
       <c r="H40" s="2">
-        <f>SQRT(F40*G40)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>114.89125293076057</v>
       </c>
       <c r="I40" s="2">
-        <f>H40*0.9</f>
+        <f t="shared" si="3"/>
         <v>103.40212763768452</v>
       </c>
       <c r="J40" s="2" t="s">
@@ -2479,11 +2509,11 @@
         <v>36</v>
       </c>
       <c r="H41" s="2">
-        <f>SQRT(F41*G41)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>150.99668870541501</v>
       </c>
       <c r="I41" s="2">
-        <f>H41*0.9</f>
+        <f t="shared" si="3"/>
         <v>135.8970198348735</v>
       </c>
       <c r="J41" s="2" t="s">
@@ -2524,11 +2554,11 @@
         <v>36</v>
       </c>
       <c r="H42" s="2">
-        <f>SQRT(F42*G42)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>164.92422502470643</v>
       </c>
       <c r="I42" s="2">
-        <f>H42*0.9</f>
+        <f t="shared" si="3"/>
         <v>148.43180252223578</v>
       </c>
       <c r="J42" s="2" t="s">
@@ -2569,11 +2599,11 @@
         <v>42</v>
       </c>
       <c r="H43" s="2">
-        <f>SQRT(F43*G43)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>170.09801096230765</v>
       </c>
       <c r="I43" s="2">
-        <f>H43*0.9</f>
+        <f t="shared" si="3"/>
         <v>153.08820986607688</v>
       </c>
       <c r="J43" s="2" t="s">
@@ -2614,11 +2644,11 @@
         <v>28</v>
       </c>
       <c r="H44" s="2">
-        <f>SQRT(F44*G44)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>136.62601021279465</v>
       </c>
       <c r="I44" s="2">
-        <f>H44*0.9</f>
+        <f t="shared" si="3"/>
         <v>122.9634091915152</v>
       </c>
       <c r="J44" s="2" t="s">
@@ -2659,11 +2689,11 @@
         <v>30</v>
       </c>
       <c r="H45" s="2">
-        <f>SQRT(F45*G45)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>143.75905768565215</v>
       </c>
       <c r="I45" s="2">
-        <f>H45*0.9</f>
+        <f t="shared" si="3"/>
         <v>129.38315191708693</v>
       </c>
       <c r="J45" s="2" t="s">
@@ -2704,11 +2734,11 @@
         <v>44</v>
       </c>
       <c r="H46" s="2">
-        <f>SQRT(F46*G46)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>178.26322609494585</v>
       </c>
       <c r="I46" s="2">
-        <f>H46*0.9</f>
+        <f t="shared" si="3"/>
         <v>160.43690348545127</v>
       </c>
       <c r="J46" s="2" t="s">
@@ -2749,11 +2779,11 @@
         <v>48</v>
       </c>
       <c r="H47" s="2">
-        <f>SQRT(F47*G47)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>190.43809142780935</v>
       </c>
       <c r="I47" s="2">
-        <f>H47*0.9</f>
+        <f t="shared" si="3"/>
         <v>171.39428228502842</v>
       </c>
       <c r="J47" s="2" t="s">
@@ -2794,11 +2824,11 @@
         <v>32</v>
       </c>
       <c r="H48" s="2">
-        <f>SQRT(F48*G48)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>157.76212754932311</v>
       </c>
       <c r="I48" s="2">
-        <f>H48*0.9</f>
+        <f t="shared" si="3"/>
         <v>141.98591479439079</v>
       </c>
       <c r="J48" s="2" t="s">
@@ -2839,11 +2869,11 @@
         <v>54</v>
       </c>
       <c r="H49" s="2">
-        <f>SQRT(F49*G49)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>207.84609690826528</v>
       </c>
       <c r="I49" s="2">
-        <f>H49*0.9</f>
+        <f t="shared" si="3"/>
         <v>187.06148721743875</v>
       </c>
       <c r="J49" s="2" t="s">
@@ -2884,11 +2914,11 @@
         <v>4</v>
       </c>
       <c r="H50" s="2">
-        <f>SQRT(F50*G50)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>42.163702135578397</v>
       </c>
       <c r="I50" s="2">
-        <f>H50*0.9</f>
+        <f t="shared" si="3"/>
         <v>37.94733192202056</v>
       </c>
       <c r="J50" s="2" t="s">
@@ -2929,11 +2959,11 @@
         <v>5</v>
       </c>
       <c r="H51" s="2">
-        <f>SQRT(F51*G51)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="I51" s="2">
-        <f>H51*0.9</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="J51" s="2" t="s">
@@ -2974,11 +3004,11 @@
         <v>6</v>
       </c>
       <c r="H52" s="2">
-        <f>SQRT(F52*G52)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>63.245553203367592</v>
       </c>
       <c r="I52" s="2">
-        <f>H52*0.9</f>
+        <f t="shared" si="3"/>
         <v>56.920997883030836</v>
       </c>
       <c r="J52" s="2" t="s">
@@ -3019,11 +3049,11 @@
         <v>8</v>
       </c>
       <c r="H53" s="2">
-        <f>SQRT(F53*G53)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>73.029674334022147</v>
       </c>
       <c r="I53" s="2">
-        <f>H53*0.9</f>
+        <f t="shared" si="3"/>
         <v>65.726706900619931</v>
       </c>
       <c r="J53" s="2" t="s">
@@ -3064,11 +3094,11 @@
         <v>8</v>
       </c>
       <c r="H54" s="2">
-        <f>SQRT(F54*G54)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>76.011695006609202</v>
       </c>
       <c r="I54" s="2">
-        <f>H54*0.9</f>
+        <f t="shared" si="3"/>
         <v>68.410525505948286</v>
       </c>
       <c r="J54" s="2" t="s">
@@ -3109,11 +3139,11 @@
         <v>10</v>
       </c>
       <c r="H55" s="2">
-        <f>SQRT(F55*G55)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>94.28090415820634</v>
       </c>
       <c r="I55" s="2">
-        <f>H55*0.9</f>
+        <f t="shared" si="3"/>
         <v>84.852813742385706</v>
       </c>
       <c r="J55" s="2" t="s">
@@ -3154,11 +3184,11 @@
         <v>4</v>
       </c>
       <c r="H56" s="2">
-        <f>SQRT(F56*G56)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>53.748384988656994</v>
       </c>
       <c r="I56" s="2">
-        <f>H56*0.9</f>
+        <f t="shared" si="3"/>
         <v>48.373546489791295</v>
       </c>
       <c r="J56" s="2" t="s">
@@ -3199,11 +3229,11 @@
         <v>12</v>
       </c>
       <c r="H57" s="2">
-        <f>SQRT(F57*G57)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>106.45812948447541</v>
       </c>
       <c r="I57" s="2">
-        <f>H57*0.9</f>
+        <f t="shared" si="3"/>
         <v>95.812316536027865</v>
       </c>
       <c r="J57" s="2" t="s">
@@ -3244,11 +3274,11 @@
         <v>10</v>
       </c>
       <c r="H58" s="2">
-        <f>SQRT(F58*G58)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>101.10500592068735</v>
       </c>
       <c r="I58" s="2">
-        <f>H58*0.9</f>
+        <f t="shared" si="3"/>
         <v>90.994505328618615</v>
       </c>
       <c r="J58" s="2" t="s">
@@ -3289,11 +3319,11 @@
         <v>4</v>
       </c>
       <c r="H59" s="2">
-        <f>SQRT(F59*G59)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>57.735026918962582</v>
       </c>
       <c r="I59" s="2">
-        <f>H59*0.9</f>
+        <f t="shared" si="3"/>
         <v>51.961524227066327</v>
       </c>
       <c r="J59" s="2" t="s">
@@ -3337,11 +3367,11 @@
         <v>8</v>
       </c>
       <c r="H60" s="2">
-        <f>SQRT(F60*G60)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>74.833147735478832</v>
       </c>
       <c r="I60" s="2">
-        <f>H60*0.9</f>
+        <f t="shared" si="3"/>
         <v>67.349832961930957</v>
       </c>
       <c r="J60" s="2" t="s">
@@ -3372,11 +3402,11 @@
         <v>4</v>
       </c>
       <c r="H61" s="2">
-        <f>SQRT(F61*G61)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>63.245553203367592</v>
       </c>
       <c r="I61" s="2">
-        <f>H61*0.9</f>
+        <f t="shared" si="3"/>
         <v>56.920997883030836</v>
       </c>
       <c r="J61" s="2" t="s">
@@ -3423,11 +3453,11 @@
         <v>4</v>
       </c>
       <c r="H62" s="2">
-        <f>SQRT(F62*G62)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>73.029674334022147</v>
       </c>
       <c r="I62" s="2">
-        <f>H62*0.9</f>
+        <f t="shared" si="3"/>
         <v>65.726706900619931</v>
       </c>
       <c r="J62" s="2" t="s">
@@ -3474,11 +3504,11 @@
         <v>5</v>
       </c>
       <c r="H63" s="2">
-        <f>SQRT(F63*G63)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>67.082039324993701</v>
       </c>
       <c r="I63" s="2">
-        <f>H63*0.9</f>
+        <f t="shared" si="3"/>
         <v>60.373835392494335</v>
       </c>
       <c r="J63" s="2" t="s">
@@ -3522,11 +3552,11 @@
         <v>4</v>
       </c>
       <c r="H64" s="2">
-        <f>SQRT(F64*G64)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>80.277297191948648</v>
       </c>
       <c r="I64" s="2">
-        <f>H64*0.9</f>
+        <f t="shared" si="3"/>
         <v>72.249567472753782</v>
       </c>
       <c r="J64" s="2" t="s">
@@ -3543,7 +3573,7 @@
         <v>0x0x0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -3567,11 +3597,11 @@
         <v>4</v>
       </c>
       <c r="H65" s="2">
-        <f>SQRT(F65*G65)/$B$1</f>
+        <f t="shared" si="2"/>
         <v>70.553368295055762</v>
       </c>
       <c r="I65" s="2">
-        <f>H65*0.9</f>
+        <f t="shared" si="3"/>
         <v>63.498031465550184</v>
       </c>
       <c r="J65" s="2" t="s">
@@ -3586,6 +3616,276 @@
 ROUND(M65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,4),0), "x",
 ROUND(L65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,5),0))</f>
         <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>91</v>
+      </c>
+      <c r="B66">
+        <v>1981</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66">
+        <f>IF(B66 &gt; 1900, ((B66-1900)*10)+400+C66, ((B66-1730)*2)+C66)+VLOOKUP(D66,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4811</v>
+      </c>
+      <c r="F66">
+        <v>112</v>
+      </c>
+      <c r="G66">
+        <v>18</v>
+      </c>
+      <c r="H66" s="2">
+        <f t="shared" ref="H66" si="4">SQRT(F66*G66)/$B$1</f>
+        <v>149.66629547095766</v>
+      </c>
+      <c r="I66" s="2">
+        <f t="shared" si="3"/>
+        <v>134.69966592386191</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K66" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L66" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M66" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="N66" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K66*VLOOKUP(D66,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M66*VLOOKUP(D66,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L66*VLOOKUP(D66,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>29x13x16</v>
+      </c>
+      <c r="O66" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>92</v>
+      </c>
+      <c r="B67">
+        <v>1959</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67">
+        <f>IF(B67 &gt; 1900, ((B67-1900)*10)+400+C67, ((B67-1730)*2)+C67)+VLOOKUP(D67,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4591</v>
+      </c>
+      <c r="F67">
+        <v>58</v>
+      </c>
+      <c r="G67">
+        <v>16</v>
+      </c>
+      <c r="H67" s="2">
+        <f t="shared" ref="H67:H69" si="5">SQRT(F67*G67)/$B$1</f>
+        <v>101.54364141151879</v>
+      </c>
+      <c r="I67" s="2">
+        <f t="shared" si="3"/>
+        <v>91.389277270366918</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K67" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L67" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M67" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="N67" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K67*VLOOKUP(D67,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M67*VLOOKUP(D67,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L67*VLOOKUP(D67,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>29x13x16</v>
+      </c>
+      <c r="O67" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>93</v>
+      </c>
+      <c r="B68">
+        <v>1965</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68">
+        <f>IF(B68 &gt; 1900, ((B68-1900)*10)+400+C68, ((B68-1730)*2)+C68)+VLOOKUP(D68,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4651</v>
+      </c>
+      <c r="F68">
+        <v>60</v>
+      </c>
+      <c r="G68">
+        <v>16</v>
+      </c>
+      <c r="H68" s="2">
+        <f t="shared" si="5"/>
+        <v>103.27955589886446</v>
+      </c>
+      <c r="I68" s="2">
+        <f t="shared" si="3"/>
+        <v>92.951600308978016</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K68" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L68" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M68" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="N68" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K68*VLOOKUP(D68,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M68*VLOOKUP(D68,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L68*VLOOKUP(D68,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>29x13x16</v>
+      </c>
+      <c r="O68" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>94</v>
+      </c>
+      <c r="B69">
+        <v>1993</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>22</v>
+      </c>
+      <c r="E69">
+        <f>IF(B69 &gt; 1900, ((B69-1900)*10)+400+C69, ((B69-1730)*2)+C69)+VLOOKUP(D69,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>4931</v>
+      </c>
+      <c r="F69">
+        <v>72</v>
+      </c>
+      <c r="G69">
+        <v>18</v>
+      </c>
+      <c r="H69" s="2">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="I69" s="2">
+        <f t="shared" si="3"/>
+        <v>108</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K69" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L69" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M69" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="N69" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K69*VLOOKUP(D69,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M69*VLOOKUP(D69,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L69*VLOOKUP(D69,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>29x13x16</v>
+      </c>
+      <c r="O69" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70">
+        <v>2005</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
+        <v>22</v>
+      </c>
+      <c r="E70">
+        <f>IF(B70 &gt; 1900, ((B70-1900)*10)+400+C70, ((B70-1730)*2)+C70)+VLOOKUP(D70,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>5051</v>
+      </c>
+      <c r="F70">
+        <v>80</v>
+      </c>
+      <c r="G70">
+        <v>18</v>
+      </c>
+      <c r="H70" s="2">
+        <f t="shared" ref="H70" si="6">SQRT(F70*G70)/$B$1</f>
+        <v>126.49110640673518</v>
+      </c>
+      <c r="I70" s="2">
+        <f t="shared" si="3"/>
+        <v>113.84199576606167</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K70" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L70" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M70" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="N70" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K70*VLOOKUP(D70,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M70*VLOOKUP(D70,'ID Scheme'!$A$2:$E$5,4),0), "x",
+ROUND(L70*VLOOKUP(D70,'ID Scheme'!$A$2:$E$5,5),0))</f>
+        <v>29x13x16</v>
+      </c>
+      <c r="O70" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Saviem SG and Renault Magnum. Boosted mail capacity of vans in realistic mode.
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C41D3CC-A7C2-4519-AD85-76753EFE04B6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215108A2-12D7-47EB-B1ED-E296F66A7264}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="102">
   <si>
     <t>Vehicle</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>105hp</t>
+  </si>
+  <si>
+    <t>Saviem SM</t>
   </si>
 </sst>
 </file>
@@ -689,11 +692,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:O71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G69" sqref="G69"/>
+      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,11 +792,11 @@
         <v>14</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H35" si="0">SQRT(F4*G4)/$B$1</f>
+        <f>SQRT(F4*G4)/$B$1</f>
         <v>52.915026221291818</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I4:I35" si="1">H4*0.9</f>
+        <f>H4*0.9</f>
         <v>47.623523599162638</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -805,8 +808,8 @@
       <c r="N4" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K4*VLOOKUP(D4,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M4*VLOOKUP(D4,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L4*VLOOKUP(D4,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L4*VLOOKUP(D4,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M4*VLOOKUP(D4,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -834,11 +837,11 @@
         <v>22</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F5*G5)/$B$1</f>
         <v>66.332495807108003</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="1"/>
+        <f>H5*0.9</f>
         <v>59.699246226397207</v>
       </c>
       <c r="J5" s="2" t="s">
@@ -850,8 +853,8 @@
       <c r="N5" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K5*VLOOKUP(D5,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M5*VLOOKUP(D5,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L5*VLOOKUP(D5,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L5*VLOOKUP(D5,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M5*VLOOKUP(D5,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -879,11 +882,11 @@
         <v>36</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F6*G6)/$B$1</f>
         <v>89.442719099991592</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="1"/>
+        <f>H6*0.9</f>
         <v>80.498447189992433</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -895,8 +898,8 @@
       <c r="N6" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K6*VLOOKUP(D6,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M6*VLOOKUP(D6,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L6*VLOOKUP(D6,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L6*VLOOKUP(D6,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M6*VLOOKUP(D6,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -924,11 +927,11 @@
         <v>32</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F7*G7)/$B$1</f>
         <v>113.13708498984759</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="1"/>
+        <f>H7*0.9</f>
         <v>101.82337649086284</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -940,8 +943,8 @@
       <c r="N7" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K7*VLOOKUP(D7,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M7*VLOOKUP(D7,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L7*VLOOKUP(D7,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L7*VLOOKUP(D7,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M7*VLOOKUP(D7,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -969,11 +972,11 @@
         <v>35</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F8*G8)/$B$1</f>
         <v>127.80193008453877</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="1"/>
+        <f>H8*0.9</f>
         <v>115.02173707608489</v>
       </c>
       <c r="J8" s="2" t="s">
@@ -985,8 +988,8 @@
       <c r="N8" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K8*VLOOKUP(D8,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M8*VLOOKUP(D8,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L8*VLOOKUP(D8,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L8*VLOOKUP(D8,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M8*VLOOKUP(D8,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -1014,11 +1017,11 @@
         <v>50</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F9*G9)/$B$1</f>
         <v>126.92955176439848</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="1"/>
+        <f>H9*0.9</f>
         <v>114.23659658795863</v>
       </c>
       <c r="J9" s="2" t="s">
@@ -1030,8 +1033,8 @@
       <c r="N9" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K9*VLOOKUP(D9,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M9*VLOOKUP(D9,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L9*VLOOKUP(D9,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L9*VLOOKUP(D9,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M9*VLOOKUP(D9,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -1059,11 +1062,11 @@
         <v>44</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F10*G10)/$B$1</f>
         <v>139.84117975602021</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="1"/>
+        <f>H10*0.9</f>
         <v>125.85706178041819</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -1075,8 +1078,8 @@
       <c r="N10" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K10*VLOOKUP(D10,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M10*VLOOKUP(D10,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L10*VLOOKUP(D10,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L10*VLOOKUP(D10,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M10*VLOOKUP(D10,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -1104,11 +1107,11 @@
         <v>57</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F11*G11)/$B$1</f>
         <v>155.13435037626795</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="1"/>
+        <f>H11*0.9</f>
         <v>139.62091533864117</v>
       </c>
       <c r="J11" s="2" t="s">
@@ -1120,8 +1123,8 @@
       <c r="N11" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K11*VLOOKUP(D11,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M11*VLOOKUP(D11,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L11*VLOOKUP(D11,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L11*VLOOKUP(D11,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M11*VLOOKUP(D11,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -1149,11 +1152,11 @@
         <v>72</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F12*G12)/$B$1</f>
         <v>178.88543819998318</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" si="1"/>
+        <f>H12*0.9</f>
         <v>160.99689437998487</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -1165,8 +1168,8 @@
       <c r="N12" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K12*VLOOKUP(D12,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M12*VLOOKUP(D12,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L12*VLOOKUP(D12,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L12*VLOOKUP(D12,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M12*VLOOKUP(D12,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -1194,11 +1197,11 @@
         <v>34</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F13*G13)/$B$1</f>
         <v>169.44353369518447</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="1"/>
+        <f>H13*0.9</f>
         <v>152.49918032566603</v>
       </c>
       <c r="J13" s="2" t="s">
@@ -1210,8 +1213,8 @@
       <c r="N13" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K13*VLOOKUP(D13,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M13*VLOOKUP(D13,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L13*VLOOKUP(D13,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L13*VLOOKUP(D13,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M13*VLOOKUP(D13,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -1239,11 +1242,11 @@
         <v>57</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F14*G14)/$B$1</f>
         <v>186.63690238892559</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="1"/>
+        <f>H14*0.9</f>
         <v>167.97321215003305</v>
       </c>
       <c r="J14" s="2" t="s">
@@ -1255,8 +1258,8 @@
       <c r="N14" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K14*VLOOKUP(D14,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M14*VLOOKUP(D14,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L14*VLOOKUP(D14,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L14*VLOOKUP(D14,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M14*VLOOKUP(D14,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -1284,11 +1287,11 @@
         <v>52</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F15*G15)/$B$1</f>
         <v>178.26322609494585</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="1"/>
+        <f>H15*0.9</f>
         <v>160.43690348545127</v>
       </c>
       <c r="J15" s="2" t="s">
@@ -1304,9 +1307,9 @@
       <c r="N15" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>51x0x18</v>
+ROUND(L15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>51x18x0</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1333,11 +1336,11 @@
         <v>58</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F16*G16)/$B$1</f>
         <v>183.06040290327977</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="1"/>
+        <f>H16*0.9</f>
         <v>164.75436261295178</v>
       </c>
       <c r="J16" s="2" t="s">
@@ -1353,9 +1356,9 @@
       <c r="N16" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>53x0x18</v>
+ROUND(L16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>53x18x0</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1382,11 +1385,11 @@
         <v>55</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F17*G17)/$B$1</f>
         <v>194.65068427541911</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="1"/>
+        <f>H17*0.9</f>
         <v>175.18561584787722</v>
       </c>
       <c r="J17" s="2" t="s">
@@ -1404,9 +1407,9 @@
       <c r="N17" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K17*VLOOKUP(D17,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M17*VLOOKUP(D17,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L17*VLOOKUP(D17,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>56x16x18</v>
+ROUND(L17*VLOOKUP(D17,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M17*VLOOKUP(D17,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>56x18x16</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1433,11 +1436,11 @@
         <v>73</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F18*G18)/$B$1</f>
         <v>195.2491286080996</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="1"/>
+        <f>H18*0.9</f>
         <v>175.72421574728963</v>
       </c>
       <c r="J18" s="2" t="s">
@@ -1455,9 +1458,9 @@
       <c r="N18" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K18*VLOOKUP(D18,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M18*VLOOKUP(D18,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L18*VLOOKUP(D18,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>56x20x18</v>
+ROUND(L18*VLOOKUP(D18,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M18*VLOOKUP(D18,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>56x18x20</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1484,11 +1487,11 @@
         <v>50</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F19*G19)/$B$1</f>
         <v>176.38342073763937</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="1"/>
+        <f>H19*0.9</f>
         <v>158.74507866387543</v>
       </c>
       <c r="J19" s="2" t="s">
@@ -1506,9 +1509,9 @@
       <c r="N19" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K19*VLOOKUP(D19,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M19*VLOOKUP(D19,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L19*VLOOKUP(D19,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>48x13x17</v>
+ROUND(L19*VLOOKUP(D19,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M19*VLOOKUP(D19,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>48x17x13</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1535,11 +1538,11 @@
         <v>33</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F20*G20)/$B$1</f>
         <v>147.08274315273474</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="1"/>
+        <f>H20*0.9</f>
         <v>132.37446883746128</v>
       </c>
       <c r="J20" s="2" t="s">
@@ -1557,9 +1560,9 @@
       <c r="N20" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>48x13x17</v>
+ROUND(L20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>48x17x13</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1586,11 +1589,11 @@
         <v>58</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F21*G21)/$B$1</f>
         <v>212.39376429431988</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="1"/>
+        <f>H21*0.9</f>
         <v>191.15438786488789</v>
       </c>
       <c r="J21" s="2" t="s">
@@ -1608,9 +1611,9 @@
       <c r="N21" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>56x16x18</v>
+ROUND(L21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>56x18x16</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1637,11 +1640,11 @@
         <v>140</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F22*G22)/$B$1</f>
         <v>292.49881291307071</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="1"/>
+        <f>H22*0.9</f>
         <v>263.24893162176363</v>
       </c>
       <c r="J22" s="2" t="s">
@@ -1659,9 +1662,9 @@
       <c r="N22" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>84x15x18</v>
+ROUND(L22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>84x18x15</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1688,11 +1691,11 @@
         <v>90</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F23*G23)/$B$1</f>
         <v>244.94897427831785</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="1"/>
+        <f>H23*0.9</f>
         <v>220.45407685048608</v>
       </c>
       <c r="J23" s="2" t="s">
@@ -1710,9 +1713,9 @@
       <c r="N23" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>53x20x18</v>
+ROUND(L23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>53x18x20</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1739,11 +1742,11 @@
         <v>87</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F24*G24)/$B$1</f>
         <v>219.84843263788198</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="1"/>
+        <f>H24*0.9</f>
         <v>197.86358937409378</v>
       </c>
       <c r="J24" s="2" t="s">
@@ -1755,8 +1758,8 @@
       <c r="N24" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K24*VLOOKUP(D24,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M24*VLOOKUP(D24,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L24*VLOOKUP(D24,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L24*VLOOKUP(D24,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M24*VLOOKUP(D24,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -1784,11 +1787,11 @@
         <v>35</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F25*G25)/$B$1</f>
         <v>152.75252316519467</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="1"/>
+        <f>H25*0.9</f>
         <v>137.4772708486752</v>
       </c>
       <c r="J25" s="2" t="s">
@@ -1806,9 +1809,9 @@
       <c r="N25" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>48x13x17</v>
+ROUND(L25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>48x17x13</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -1835,11 +1838,11 @@
         <v>12</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F26*G26)/$B$1</f>
         <v>46.188021535170058</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="1"/>
+        <f>H26*0.9</f>
         <v>41.569219381653056</v>
       </c>
       <c r="J26" s="2" t="s">
@@ -1851,8 +1854,8 @@
       <c r="N26" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K26*VLOOKUP(D26,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M26*VLOOKUP(D26,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L26*VLOOKUP(D26,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L26*VLOOKUP(D26,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M26*VLOOKUP(D26,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -1880,11 +1883,11 @@
         <v>14</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F27*G27)/$B$1</f>
         <v>52.915026221291818</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="1"/>
+        <f>H27*0.9</f>
         <v>47.623523599162638</v>
       </c>
       <c r="J27" s="2" t="s">
@@ -1896,8 +1899,8 @@
       <c r="N27" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K27*VLOOKUP(D27,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M27*VLOOKUP(D27,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L27*VLOOKUP(D27,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L27*VLOOKUP(D27,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M27*VLOOKUP(D27,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -1925,11 +1928,11 @@
         <v>16</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F28*G28)/$B$1</f>
         <v>56.568542494923797</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="1"/>
+        <f>H28*0.9</f>
         <v>50.911688245431421</v>
       </c>
       <c r="J28" s="2" t="s">
@@ -1941,8 +1944,8 @@
       <c r="N28" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K28*VLOOKUP(D28,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M28*VLOOKUP(D28,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L28*VLOOKUP(D28,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L28*VLOOKUP(D28,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M28*VLOOKUP(D28,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -1970,11 +1973,11 @@
         <v>18</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F29*G29)/$B$1</f>
         <v>63.245553203367592</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="1"/>
+        <f>H29*0.9</f>
         <v>56.920997883030836</v>
       </c>
       <c r="J29" s="2" t="s">
@@ -1986,8 +1989,8 @@
       <c r="N29" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K29*VLOOKUP(D29,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M29*VLOOKUP(D29,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L29*VLOOKUP(D29,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L29*VLOOKUP(D29,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M29*VLOOKUP(D29,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -2015,11 +2018,11 @@
         <v>18</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F30*G30)/$B$1</f>
         <v>66.332495807108003</v>
       </c>
       <c r="I30" s="2">
-        <f t="shared" si="1"/>
+        <f>H30*0.9</f>
         <v>59.699246226397207</v>
       </c>
       <c r="J30" s="2" t="s">
@@ -2031,8 +2034,8 @@
       <c r="N30" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K30*VLOOKUP(D30,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M30*VLOOKUP(D30,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L30*VLOOKUP(D30,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L30*VLOOKUP(D30,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M30*VLOOKUP(D30,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -2060,11 +2063,11 @@
         <v>28</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F31*G31)/$B$1</f>
         <v>74.833147735478832</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="1"/>
+        <f>H31*0.9</f>
         <v>67.349832961930957</v>
       </c>
       <c r="J31" s="2" t="s">
@@ -2082,9 +2085,9 @@
       <c r="N31" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>16x12x14</v>
+ROUND(L31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>16x14x12</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -2111,11 +2114,11 @@
         <v>15</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F32*G32)/$B$1</f>
         <v>78.528126595931653</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="1"/>
+        <f>H32*0.9</f>
         <v>70.675313936338483</v>
       </c>
       <c r="J32" s="2" t="s">
@@ -2127,8 +2130,8 @@
       <c r="N32" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K32*VLOOKUP(D32,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M32*VLOOKUP(D32,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L32*VLOOKUP(D32,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L32*VLOOKUP(D32,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M32*VLOOKUP(D32,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -2156,11 +2159,11 @@
         <v>24</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F33*G33)/$B$1</f>
         <v>96.609178307929596</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="1"/>
+        <f>H33*0.9</f>
         <v>86.948260477136643</v>
       </c>
       <c r="J33" s="2" t="s">
@@ -2172,8 +2175,8 @@
       <c r="N33" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K33*VLOOKUP(D33,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M33*VLOOKUP(D33,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L33*VLOOKUP(D33,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L33*VLOOKUP(D33,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M33*VLOOKUP(D33,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -2201,11 +2204,11 @@
         <v>20</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F34*G34)/$B$1</f>
         <v>81.649658092772611</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" si="1"/>
+        <f>H34*0.9</f>
         <v>73.484692283495349</v>
       </c>
       <c r="J34" s="2" t="s">
@@ -2217,8 +2220,8 @@
       <c r="N34" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K34*VLOOKUP(D34,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M34*VLOOKUP(D34,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L34*VLOOKUP(D34,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L34*VLOOKUP(D34,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M34*VLOOKUP(D34,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -2246,15 +2249,22 @@
         <v>6</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" si="0"/>
+        <f>SQRT(F35*G35)/$B$1</f>
         <v>53.541261347363367</v>
       </c>
       <c r="I35" s="2">
-        <f t="shared" si="1"/>
+        <f>H35*0.9</f>
         <v>48.187135212627034</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="N35" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K35*VLOOKUP(D35,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(L35*VLOOKUP(D35,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M35*VLOOKUP(D35,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -2281,11 +2291,11 @@
         <v>25</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" ref="H36:H67" si="2">SQRT(F36*G36)/$B$1</f>
+        <f>SQRT(F36*G36)/$B$1</f>
         <v>102.74023338281629</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" ref="I36:I70" si="3">H36*0.9</f>
+        <f>H36*0.9</f>
         <v>92.466210044534662</v>
       </c>
       <c r="J36" s="2" t="s">
@@ -2297,8 +2307,8 @@
       <c r="N36" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K36*VLOOKUP(D36,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M36*VLOOKUP(D36,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L36*VLOOKUP(D36,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L36*VLOOKUP(D36,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M36*VLOOKUP(D36,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
@@ -2326,11 +2336,11 @@
         <v>21</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="2"/>
+        <f>SQRT(F37*G37)/$B$1</f>
         <v>97.809338340808068</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="3"/>
+        <f>H37*0.9</f>
         <v>88.02840450672727</v>
       </c>
       <c r="J37" s="2" t="s">
@@ -2342,17 +2352,17 @@
       <c r="N37" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K37*VLOOKUP(D37,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M37*VLOOKUP(D37,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L37*VLOOKUP(D37,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L37*VLOOKUP(D37,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M37*VLOOKUP(D37,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="B38">
-        <v>1963</v>
+        <v>1959</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2362,42 +2372,51 @@
       </c>
       <c r="E38">
         <f>IF(B38 &gt; 1900, ((B38-1900)*10)+400+C38, ((B38-1730)*2)+C38)+VLOOKUP(D38,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4631</v>
+        <v>4591</v>
       </c>
       <c r="F38">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G38">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="2"/>
-        <v>108.32051206181282</v>
+        <f>SQRT(F38*G38)/$B$1</f>
+        <v>101.54364141151879</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="3"/>
-        <v>97.488460855631544</v>
+        <f>H38*0.9</f>
+        <v>91.389277270366918</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
+      <c r="K38" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L38" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M38" s="3">
+        <v>2.6</v>
+      </c>
       <c r="N38" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K38*VLOOKUP(D38,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M38*VLOOKUP(D38,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L38*VLOOKUP(D38,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+ROUND(L38*VLOOKUP(D38,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M38*VLOOKUP(D38,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>29x16x13</v>
+      </c>
+      <c r="O38" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B39">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2407,21 +2426,21 @@
       </c>
       <c r="E39">
         <f>IF(B39 &gt; 1900, ((B39-1900)*10)+400+C39, ((B39-1730)*2)+C39)+VLOOKUP(D39,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4641</v>
+        <v>4631</v>
       </c>
       <c r="F39">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G39">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="2"/>
-        <v>146.9693845669907</v>
+        <f>SQRT(F39*G39)/$B$1</f>
+        <v>108.32051206181282</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" si="3"/>
-        <v>132.27244611029164</v>
+        <f>H39*0.9</f>
+        <v>97.488460855631544</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>33</v>
@@ -2432,41 +2451,41 @@
       <c r="N39" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K39*VLOOKUP(D39,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M39*VLOOKUP(D39,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L39*VLOOKUP(D39,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L39*VLOOKUP(D39,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M39*VLOOKUP(D39,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40">
         <v>1964</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" t="s">
         <v>22</v>
       </c>
       <c r="E40">
         <f>IF(B40 &gt; 1900, ((B40-1900)*10)+400+C40, ((B40-1730)*2)+C40)+VLOOKUP(D40,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4642</v>
+        <v>4641</v>
       </c>
       <c r="F40">
         <v>54</v>
       </c>
       <c r="G40">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="H40" s="2">
-        <f t="shared" si="2"/>
-        <v>114.89125293076057</v>
+        <f>SQRT(F40*G40)/$B$1</f>
+        <v>146.9693845669907</v>
       </c>
       <c r="I40" s="2">
-        <f t="shared" si="3"/>
-        <v>103.40212763768452</v>
+        <f>H40*0.9</f>
+        <v>132.27244611029164</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>33</v>
@@ -2477,44 +2496,41 @@
       <c r="N40" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K40*VLOOKUP(D40,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M40*VLOOKUP(D40,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L40*VLOOKUP(D40,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
-      </c>
-      <c r="O40" t="s">
-        <v>31</v>
+ROUND(L40*VLOOKUP(D40,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M40*VLOOKUP(D40,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B41">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D41" t="s">
         <v>22</v>
       </c>
       <c r="E41">
         <f>IF(B41 &gt; 1900, ((B41-1900)*10)+400+C41, ((B41-1730)*2)+C41)+VLOOKUP(D41,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4651</v>
+        <v>4642</v>
       </c>
       <c r="F41">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G41">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="H41" s="2">
-        <f t="shared" si="2"/>
-        <v>150.99668870541501</v>
+        <f>SQRT(F41*G41)/$B$1</f>
+        <v>114.89125293076057</v>
       </c>
       <c r="I41" s="2">
-        <f t="shared" si="3"/>
-        <v>135.8970198348735</v>
+        <f>H41*0.9</f>
+        <v>103.40212763768452</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>33</v>
@@ -2525,17 +2541,20 @@
       <c r="N41" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K41*VLOOKUP(D41,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M41*VLOOKUP(D41,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L41*VLOOKUP(D41,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+ROUND(L41*VLOOKUP(D41,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M41*VLOOKUP(D41,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+      <c r="O41" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B42">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2545,21 +2564,21 @@
       </c>
       <c r="E42">
         <f>IF(B42 &gt; 1900, ((B42-1900)*10)+400+C42, ((B42-1730)*2)+C42)+VLOOKUP(D42,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4681</v>
+        <v>4651</v>
       </c>
       <c r="F42">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="G42">
         <v>36</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" si="2"/>
-        <v>164.92422502470643</v>
+        <f>SQRT(F42*G42)/$B$1</f>
+        <v>150.99668870541501</v>
       </c>
       <c r="I42" s="2">
-        <f t="shared" si="3"/>
-        <v>148.43180252223578</v>
+        <f>H42*0.9</f>
+        <v>135.8970198348735</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>33</v>
@@ -2570,62 +2589,71 @@
       <c r="N42" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K42*VLOOKUP(D42,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M42*VLOOKUP(D42,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L42*VLOOKUP(D42,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L42*VLOOKUP(D42,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M42*VLOOKUP(D42,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="B43">
-        <v>1980</v>
+        <v>1965</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43" t="s">
         <v>22</v>
       </c>
       <c r="E43">
         <f>IF(B43 &gt; 1900, ((B43-1900)*10)+400+C43, ((B43-1730)*2)+C43)+VLOOKUP(D43,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4801</v>
+        <v>4652</v>
       </c>
       <c r="F43">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G43">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" si="2"/>
-        <v>170.09801096230765</v>
+        <f>SQRT(F43*G43)/$B$1</f>
+        <v>103.27955589886446</v>
       </c>
       <c r="I43" s="2">
-        <f t="shared" si="3"/>
-        <v>153.08820986607688</v>
+        <f>H43*0.9</f>
+        <v>92.951600308978016</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
+      <c r="K43" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L43" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M43" s="3">
+        <v>2.6</v>
+      </c>
       <c r="N43" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K43*VLOOKUP(D43,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M43*VLOOKUP(D43,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L43*VLOOKUP(D43,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+ROUND(L43*VLOOKUP(D43,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M43*VLOOKUP(D43,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>29x16x13</v>
+      </c>
+      <c r="O43" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="B44">
-        <v>1982</v>
+        <v>1967</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -2635,42 +2663,51 @@
       </c>
       <c r="E44">
         <f>IF(B44 &gt; 1900, ((B44-1900)*10)+400+C44, ((B44-1730)*2)+C44)+VLOOKUP(D44,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4821</v>
+        <v>4671</v>
       </c>
       <c r="F44">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G44">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H44" s="2">
-        <f t="shared" si="2"/>
-        <v>136.62601021279465</v>
+        <f>SQRT(F44*G44)/$B$1</f>
+        <v>116.99952516522831</v>
       </c>
       <c r="I44" s="2">
-        <f t="shared" si="3"/>
-        <v>122.9634091915152</v>
+        <f>H44*0.9</f>
+        <v>105.29957264870548</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
+      <c r="K44" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="L44" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M44" s="3">
+        <v>2.8</v>
+      </c>
       <c r="N44" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K44*VLOOKUP(D44,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M44*VLOOKUP(D44,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L44*VLOOKUP(D44,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+ROUND(L44*VLOOKUP(D44,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M44*VLOOKUP(D44,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>40x18x14</v>
+      </c>
+      <c r="O44" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="B45">
-        <v>1986</v>
+        <v>1968</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2680,21 +2717,21 @@
       </c>
       <c r="E45">
         <f>IF(B45 &gt; 1900, ((B45-1900)*10)+400+C45, ((B45-1730)*2)+C45)+VLOOKUP(D45,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4861</v>
+        <v>4681</v>
       </c>
       <c r="F45">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="G45">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H45" s="2">
-        <f t="shared" si="2"/>
-        <v>143.75905768565215</v>
+        <f>SQRT(F45*G45)/$B$1</f>
+        <v>164.92422502470643</v>
       </c>
       <c r="I45" s="2">
-        <f t="shared" si="3"/>
-        <v>129.38315191708693</v>
+        <f>H45*0.9</f>
+        <v>148.43180252223578</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>33</v>
@@ -2705,17 +2742,17 @@
       <c r="N45" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K45*VLOOKUP(D45,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M45*VLOOKUP(D45,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L45*VLOOKUP(D45,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L45*VLOOKUP(D45,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M45*VLOOKUP(D45,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B46">
-        <v>1987</v>
+        <v>1980</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -2725,21 +2762,21 @@
       </c>
       <c r="E46">
         <f>IF(B46 &gt; 1900, ((B46-1900)*10)+400+C46, ((B46-1730)*2)+C46)+VLOOKUP(D46,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4871</v>
+        <v>4801</v>
       </c>
       <c r="F46">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G46">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" si="2"/>
-        <v>178.26322609494585</v>
+        <f>SQRT(F46*G46)/$B$1</f>
+        <v>170.09801096230765</v>
       </c>
       <c r="I46" s="2">
-        <f t="shared" si="3"/>
-        <v>160.43690348545127</v>
+        <f>H46*0.9</f>
+        <v>153.08820986607688</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>33</v>
@@ -2750,17 +2787,17 @@
       <c r="N46" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K46*VLOOKUP(D46,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M46*VLOOKUP(D46,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L46*VLOOKUP(D46,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L46*VLOOKUP(D46,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M46*VLOOKUP(D46,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="B47">
-        <v>1995</v>
+        <v>1981</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -2770,42 +2807,51 @@
       </c>
       <c r="E47">
         <f>IF(B47 &gt; 1900, ((B47-1900)*10)+400+C47, ((B47-1730)*2)+C47)+VLOOKUP(D47,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4951</v>
+        <v>4811</v>
       </c>
       <c r="F47">
         <v>68</v>
       </c>
       <c r="G47">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" si="2"/>
-        <v>190.43809142780935</v>
+        <f>SQRT(F47*G47)/$B$1</f>
+        <v>116.61903789690601</v>
       </c>
       <c r="I47" s="2">
-        <f t="shared" si="3"/>
-        <v>171.39428228502842</v>
+        <f>H47*0.9</f>
+        <v>104.95713410721541</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
+      <c r="K47" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L47" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M47" s="3">
+        <v>2.6</v>
+      </c>
       <c r="N47" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K47*VLOOKUP(D47,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M47*VLOOKUP(D47,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L47*VLOOKUP(D47,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+ROUND(L47*VLOOKUP(D47,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M47*VLOOKUP(D47,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>29x16x13</v>
+      </c>
+      <c r="O47" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B48">
-        <v>1997</v>
+        <v>1982</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -2815,21 +2861,21 @@
       </c>
       <c r="E48">
         <f>IF(B48 &gt; 1900, ((B48-1900)*10)+400+C48, ((B48-1730)*2)+C48)+VLOOKUP(D48,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4971</v>
+        <v>4821</v>
       </c>
       <c r="F48">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G48">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" si="2"/>
-        <v>157.76212754932311</v>
+        <f>SQRT(F48*G48)/$B$1</f>
+        <v>136.62601021279465</v>
       </c>
       <c r="I48" s="2">
-        <f t="shared" si="3"/>
-        <v>141.98591479439079</v>
+        <f>H48*0.9</f>
+        <v>122.9634091915152</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>33</v>
@@ -2840,17 +2886,17 @@
       <c r="N48" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K48*VLOOKUP(D48,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M48*VLOOKUP(D48,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L48*VLOOKUP(D48,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L48*VLOOKUP(D48,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M48*VLOOKUP(D48,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B49">
-        <v>2004</v>
+        <v>1986</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2860,21 +2906,21 @@
       </c>
       <c r="E49">
         <f>IF(B49 &gt; 1900, ((B49-1900)*10)+400+C49, ((B49-1730)*2)+C49)+VLOOKUP(D49,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>5041</v>
+        <v>4861</v>
       </c>
       <c r="F49">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G49">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="H49" s="2">
-        <f t="shared" si="2"/>
-        <v>207.84609690826528</v>
+        <f>SQRT(F49*G49)/$B$1</f>
+        <v>143.75905768565215</v>
       </c>
       <c r="I49" s="2">
-        <f t="shared" si="3"/>
-        <v>187.06148721743875</v>
+        <f>H49*0.9</f>
+        <v>129.38315191708693</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>33</v>
@@ -2885,41 +2931,41 @@
       <c r="N49" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K49*VLOOKUP(D49,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M49*VLOOKUP(D49,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L49*VLOOKUP(D49,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L49*VLOOKUP(D49,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M49*VLOOKUP(D49,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="B50">
-        <v>1912</v>
+        <v>1987</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E50">
         <f>IF(B50 &gt; 1900, ((B50-1900)*10)+400+C50, ((B50-1730)*2)+C50)+VLOOKUP(D50,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7121</v>
+        <v>4871</v>
       </c>
       <c r="F50">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="G50">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" si="2"/>
-        <v>42.163702135578397</v>
+        <f>SQRT(F50*G50)/$B$1</f>
+        <v>178.26322609494585</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" si="3"/>
-        <v>37.94733192202056</v>
+        <f>H50*0.9</f>
+        <v>160.43690348545127</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>33</v>
@@ -2930,86 +2976,95 @@
       <c r="N50" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K50*VLOOKUP(D50,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M50*VLOOKUP(D50,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L50*VLOOKUP(D50,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L50*VLOOKUP(D50,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M50*VLOOKUP(D50,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B51">
-        <v>1938</v>
+        <v>1993</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E51">
         <f>IF(B51 &gt; 1900, ((B51-1900)*10)+400+C51, ((B51-1730)*2)+C51)+VLOOKUP(D51,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7381</v>
+        <v>4931</v>
       </c>
       <c r="F51">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="G51">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" si="2"/>
-        <v>50</v>
+        <f>SQRT(F51*G51)/$B$1</f>
+        <v>120</v>
       </c>
       <c r="I51" s="2">
-        <f t="shared" si="3"/>
-        <v>45</v>
+        <f>H51*0.9</f>
+        <v>108</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
+      <c r="K51" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L51" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M51" s="3">
+        <v>2.6</v>
+      </c>
       <c r="N51" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K51*VLOOKUP(D51,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M51*VLOOKUP(D51,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L51*VLOOKUP(D51,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+ROUND(L51*VLOOKUP(D51,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M51*VLOOKUP(D51,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>29x16x13</v>
+      </c>
+      <c r="O51" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B52">
-        <v>1957</v>
+        <v>1995</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E52">
         <f>IF(B52 &gt; 1900, ((B52-1900)*10)+400+C52, ((B52-1730)*2)+C52)+VLOOKUP(D52,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7571</v>
+        <v>4951</v>
       </c>
       <c r="F52">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="G52">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" si="2"/>
-        <v>63.245553203367592</v>
+        <f>SQRT(F52*G52)/$B$1</f>
+        <v>190.43809142780935</v>
       </c>
       <c r="I52" s="2">
-        <f t="shared" si="3"/>
-        <v>56.920997883030836</v>
+        <f>H52*0.9</f>
+        <v>171.39428228502842</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>33</v>
@@ -3020,41 +3075,41 @@
       <c r="N52" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K52*VLOOKUP(D52,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M52*VLOOKUP(D52,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L52*VLOOKUP(D52,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L52*VLOOKUP(D52,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M52*VLOOKUP(D52,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="B53">
-        <v>1960</v>
+        <v>1997</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E53">
         <f>IF(B53 &gt; 1900, ((B53-1900)*10)+400+C53, ((B53-1730)*2)+C53)+VLOOKUP(D53,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7601</v>
+        <v>4971</v>
       </c>
       <c r="F53">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G53">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="H53" s="2">
-        <f t="shared" si="2"/>
-        <v>73.029674334022147</v>
+        <f>SQRT(F53*G53)/$B$1</f>
+        <v>157.76212754932311</v>
       </c>
       <c r="I53" s="2">
-        <f t="shared" si="3"/>
-        <v>65.726706900619931</v>
+        <f>H53*0.9</f>
+        <v>141.98591479439079</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>33</v>
@@ -3065,41 +3120,41 @@
       <c r="N53" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K53*VLOOKUP(D53,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M53*VLOOKUP(D53,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L53*VLOOKUP(D53,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L53*VLOOKUP(D53,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M53*VLOOKUP(D53,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B54">
-        <v>1965</v>
+        <v>2004</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E54">
         <f>IF(B54 &gt; 1900, ((B54-1900)*10)+400+C54, ((B54-1730)*2)+C54)+VLOOKUP(D54,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7651</v>
+        <v>5041</v>
       </c>
       <c r="F54">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="G54">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="H54" s="2">
-        <f t="shared" si="2"/>
-        <v>76.011695006609202</v>
+        <f>SQRT(F54*G54)/$B$1</f>
+        <v>207.84609690826528</v>
       </c>
       <c r="I54" s="2">
-        <f t="shared" si="3"/>
-        <v>68.410525505948286</v>
+        <f>H54*0.9</f>
+        <v>187.06148721743875</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>33</v>
@@ -3110,86 +3165,95 @@
       <c r="N54" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K54*VLOOKUP(D54,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M54*VLOOKUP(D54,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L54*VLOOKUP(D54,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L54*VLOOKUP(D54,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M54*VLOOKUP(D54,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="B55">
-        <v>1986</v>
+        <v>2005</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E55">
         <f>IF(B55 &gt; 1900, ((B55-1900)*10)+400+C55, ((B55-1730)*2)+C55)+VLOOKUP(D55,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7861</v>
+        <v>5051</v>
       </c>
       <c r="F55">
         <v>80</v>
       </c>
       <c r="G55">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H55" s="2">
-        <f t="shared" si="2"/>
-        <v>94.28090415820634</v>
+        <f>SQRT(F55*G55)/$B$1</f>
+        <v>126.49110640673518</v>
       </c>
       <c r="I55" s="2">
-        <f t="shared" si="3"/>
-        <v>84.852813742385706</v>
+        <f>H55*0.9</f>
+        <v>113.84199576606167</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
+      <c r="K55" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L55" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M55" s="3">
+        <v>2.6</v>
+      </c>
       <c r="N55" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K55*VLOOKUP(D55,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M55*VLOOKUP(D55,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L55*VLOOKUP(D55,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+ROUND(L55*VLOOKUP(D55,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M55*VLOOKUP(D55,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>29x16x13</v>
+      </c>
+      <c r="O55" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="B56">
-        <v>1986</v>
+        <v>1912</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56" t="s">
         <v>23</v>
       </c>
       <c r="E56">
         <f>IF(B56 &gt; 1900, ((B56-1900)*10)+400+C56, ((B56-1730)*2)+C56)+VLOOKUP(D56,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7862</v>
+        <v>7121</v>
       </c>
       <c r="F56">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="G56">
         <v>4</v>
       </c>
       <c r="H56" s="2">
-        <f t="shared" si="2"/>
-        <v>53.748384988656994</v>
+        <f>SQRT(F56*G56)/$B$1</f>
+        <v>42.163702135578397</v>
       </c>
       <c r="I56" s="2">
-        <f t="shared" si="3"/>
-        <v>48.373546489791295</v>
+        <f>H56*0.9</f>
+        <v>37.94733192202056</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>33</v>
@@ -3200,17 +3264,17 @@
       <c r="N56" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K56*VLOOKUP(D56,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M56*VLOOKUP(D56,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L56*VLOOKUP(D56,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L56*VLOOKUP(D56,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M56*VLOOKUP(D56,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B57">
-        <v>2006</v>
+        <v>1938</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -3220,21 +3284,21 @@
       </c>
       <c r="E57">
         <f>IF(B57 &gt; 1900, ((B57-1900)*10)+400+C57, ((B57-1730)*2)+C57)+VLOOKUP(D57,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>8061</v>
+        <v>7381</v>
       </c>
       <c r="F57">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="G57">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H57" s="2">
-        <f t="shared" si="2"/>
-        <v>106.45812948447541</v>
+        <f>SQRT(F57*G57)/$B$1</f>
+        <v>50</v>
       </c>
       <c r="I57" s="2">
-        <f t="shared" si="3"/>
-        <v>95.812316536027865</v>
+        <f>H57*0.9</f>
+        <v>45</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>33</v>
@@ -3245,17 +3309,17 @@
       <c r="N57" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B58">
-        <v>2012</v>
+        <v>1957</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -3265,21 +3329,21 @@
       </c>
       <c r="E58">
         <f>IF(B58 &gt; 1900, ((B58-1900)*10)+400+C58, ((B58-1730)*2)+C58)+VLOOKUP(D58,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>8121</v>
+        <v>7571</v>
       </c>
       <c r="F58">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="G58">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H58" s="2">
-        <f t="shared" si="2"/>
-        <v>101.10500592068735</v>
+        <f>SQRT(F58*G58)/$B$1</f>
+        <v>63.245553203367592</v>
       </c>
       <c r="I58" s="2">
-        <f t="shared" si="3"/>
-        <v>90.994505328618615</v>
+        <f>H58*0.9</f>
+        <v>56.920997883030836</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>33</v>
@@ -3290,41 +3354,41 @@
       <c r="N58" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="B59">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E59">
         <f>IF(B59 &gt; 1900, ((B59-1900)*10)+400+C59, ((B59-1730)*2)+C59)+VLOOKUP(D59,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10581</v>
+        <v>7601</v>
       </c>
       <c r="F59">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G59">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H59" s="2">
-        <f t="shared" si="2"/>
-        <v>57.735026918962582</v>
+        <f>SQRT(F59*G59)/$B$1</f>
+        <v>73.029674334022147</v>
       </c>
       <c r="I59" s="2">
-        <f t="shared" si="3"/>
-        <v>51.961524227066327</v>
+        <f>H59*0.9</f>
+        <v>65.726706900619931</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>33</v>
@@ -3335,181 +3399,176 @@
       <c r="N59" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K59*VLOOKUP(D59,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M59*VLOOKUP(D59,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L59*VLOOKUP(D59,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
-      </c>
-      <c r="O59" t="s">
-        <v>69</v>
+ROUND(L59*VLOOKUP(D59,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M59*VLOOKUP(D59,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B60">
-        <v>1974</v>
+        <v>1965</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E60">
         <f>IF(B60 &gt; 1900, ((B60-1900)*10)+400+C60, ((B60-1730)*2)+C60)+VLOOKUP(D60,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10741</v>
+        <v>7651</v>
       </c>
       <c r="F60">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G60">
         <v>8</v>
       </c>
       <c r="H60" s="2">
-        <f t="shared" si="2"/>
-        <v>74.833147735478832</v>
+        <f>SQRT(F60*G60)/$B$1</f>
+        <v>76.011695006609202</v>
       </c>
       <c r="I60" s="2">
-        <f t="shared" si="3"/>
-        <v>67.349832961930957</v>
+        <f>H60*0.9</f>
+        <v>68.410525505948286</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K60*VLOOKUP(D60,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(L60*VLOOKUP(D60,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M60*VLOOKUP(D60,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B61">
-        <v>1976</v>
+        <v>1986</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E61">
         <f>IF(B61 &gt; 1900, ((B61-1900)*10)+400+C61, ((B61-1730)*2)+C61)+VLOOKUP(D61,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10761</v>
+        <v>7861</v>
       </c>
       <c r="F61">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G61">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H61" s="2">
-        <f t="shared" si="2"/>
-        <v>63.245553203367592</v>
+        <f>SQRT(F61*G61)/$B$1</f>
+        <v>94.28090415820634</v>
       </c>
       <c r="I61" s="2">
-        <f t="shared" si="3"/>
-        <v>56.920997883030836</v>
+        <f>H61*0.9</f>
+        <v>84.852813742385706</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K61" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="L61" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="M61" s="3">
-        <v>1.5</v>
-      </c>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
       <c r="N61" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K61*VLOOKUP(D61,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M61*VLOOKUP(D61,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L61*VLOOKUP(D61,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>21x7x13</v>
+ROUND(L61*VLOOKUP(D61,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M61*VLOOKUP(D61,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B62">
-        <v>1994</v>
+        <v>1986</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E62">
         <f>IF(B62 &gt; 1900, ((B62-1900)*10)+400+C62, ((B62-1730)*2)+C62)+VLOOKUP(D62,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10941</v>
+        <v>7862</v>
       </c>
       <c r="F62">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="G62">
         <v>4</v>
       </c>
       <c r="H62" s="2">
-        <f t="shared" si="2"/>
-        <v>73.029674334022147</v>
+        <f>SQRT(F62*G62)/$B$1</f>
+        <v>53.748384988656994</v>
       </c>
       <c r="I62" s="2">
-        <f t="shared" si="3"/>
-        <v>65.726706900619931</v>
+        <f>H62*0.9</f>
+        <v>48.373546489791295</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K62" s="3">
-        <v>5</v>
-      </c>
-      <c r="L62" s="3">
-        <v>2</v>
-      </c>
-      <c r="M62" s="3">
-        <v>1.5</v>
-      </c>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
       <c r="N62" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K62*VLOOKUP(D62,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M62*VLOOKUP(D62,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L62*VLOOKUP(D62,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>23x7x14</v>
+ROUND(L62*VLOOKUP(D62,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M62*VLOOKUP(D62,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B63">
-        <v>1997</v>
+        <v>2006</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E63">
         <f>IF(B63 &gt; 1900, ((B63-1900)*10)+400+C63, ((B63-1730)*2)+C63)+VLOOKUP(D63,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10971</v>
+        <v>8061</v>
       </c>
       <c r="F63">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G63">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H63" s="2">
-        <f t="shared" si="2"/>
-        <v>67.082039324993701</v>
+        <f>SQRT(F63*G63)/$B$1</f>
+        <v>106.45812948447541</v>
       </c>
       <c r="I63" s="2">
-        <f t="shared" si="3"/>
-        <v>60.373835392494335</v>
+        <f>H63*0.9</f>
+        <v>95.812316536027865</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>33</v>
@@ -3520,44 +3579,41 @@
       <c r="N63" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
-      </c>
-      <c r="O63" t="s">
-        <v>70</v>
+ROUND(L63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B64">
-        <v>2004</v>
+        <v>2012</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E64">
         <f>IF(B64 &gt; 1900, ((B64-1900)*10)+400+C64, ((B64-1730)*2)+C64)+VLOOKUP(D64,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>11041</v>
+        <v>8121</v>
       </c>
       <c r="F64">
-        <v>145</v>
+        <v>92</v>
       </c>
       <c r="G64">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H64" s="2">
-        <f t="shared" si="2"/>
-        <v>80.277297191948648</v>
+        <f>SQRT(F64*G64)/$B$1</f>
+        <v>101.10500592068735</v>
       </c>
       <c r="I64" s="2">
-        <f t="shared" si="3"/>
-        <v>72.249567472753782</v>
+        <f>H64*0.9</f>
+        <v>90.994505328618615</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>33</v>
@@ -3568,17 +3624,17 @@
       <c r="N64" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K64*VLOOKUP(D64,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M64*VLOOKUP(D64,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L64*VLOOKUP(D64,'ID Scheme'!$A$2:$E$5,5),0))</f>
+ROUND(L64*VLOOKUP(D64,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M64*VLOOKUP(D64,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B65">
-        <v>2009</v>
+        <v>1958</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -3588,21 +3644,21 @@
       </c>
       <c r="E65">
         <f>IF(B65 &gt; 1900, ((B65-1900)*10)+400+C65, ((B65-1730)*2)+C65)+VLOOKUP(D65,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>11091</v>
+        <v>10581</v>
       </c>
       <c r="F65">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="G65">
         <v>4</v>
       </c>
       <c r="H65" s="2">
-        <f t="shared" si="2"/>
-        <v>70.553368295055762</v>
+        <f>SQRT(F65*G65)/$B$1</f>
+        <v>57.735026918962582</v>
       </c>
       <c r="I65" s="2">
-        <f t="shared" si="3"/>
-        <v>63.498031465550184</v>
+        <f>H65*0.9</f>
+        <v>51.961524227066327</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>33</v>
@@ -3613,284 +3669,299 @@
       <c r="N65" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>0x0x0</v>
+ROUND(L65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+      <c r="O65" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B66">
-        <v>1981</v>
+        <v>1974</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E66">
         <f>IF(B66 &gt; 1900, ((B66-1900)*10)+400+C66, ((B66-1730)*2)+C66)+VLOOKUP(D66,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4811</v>
+        <v>10741</v>
       </c>
       <c r="F66">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="G66">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H66" s="2">
-        <f t="shared" ref="H66" si="4">SQRT(F66*G66)/$B$1</f>
-        <v>149.66629547095766</v>
+        <f>SQRT(F66*G66)/$B$1</f>
+        <v>74.833147735478832</v>
       </c>
       <c r="I66" s="2">
-        <f t="shared" si="3"/>
-        <v>134.69966592386191</v>
+        <f>H66*0.9</f>
+        <v>67.349832961930957</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K66" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="L66" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M66" s="3">
-        <v>2.6</v>
-      </c>
       <c r="N66" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K66*VLOOKUP(D66,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M66*VLOOKUP(D66,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L66*VLOOKUP(D66,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>29x13x16</v>
-      </c>
-      <c r="O66" t="s">
-        <v>97</v>
+ROUND(L66*VLOOKUP(D66,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M66*VLOOKUP(D66,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="B67">
-        <v>1959</v>
+        <v>1976</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E67">
         <f>IF(B67 &gt; 1900, ((B67-1900)*10)+400+C67, ((B67-1730)*2)+C67)+VLOOKUP(D67,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4591</v>
+        <v>10761</v>
       </c>
       <c r="F67">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="G67">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="H67" s="2">
-        <f t="shared" ref="H67:H69" si="5">SQRT(F67*G67)/$B$1</f>
-        <v>101.54364141151879</v>
+        <f>SQRT(F67*G67)/$B$1</f>
+        <v>63.245553203367592</v>
       </c>
       <c r="I67" s="2">
-        <f t="shared" si="3"/>
-        <v>91.389277270366918</v>
+        <f>H67*0.9</f>
+        <v>56.920997883030836</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K67" s="3">
-        <v>6.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="L67" s="3">
-        <v>2.2000000000000002</v>
+        <v>1.8</v>
       </c>
       <c r="M67" s="3">
-        <v>2.6</v>
+        <v>1.5</v>
       </c>
       <c r="N67" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K67*VLOOKUP(D67,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M67*VLOOKUP(D67,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L67*VLOOKUP(D67,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>29x13x16</v>
-      </c>
-      <c r="O67" t="s">
-        <v>99</v>
+ROUND(L67*VLOOKUP(D67,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M67*VLOOKUP(D67,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>21x13x7</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="B68">
-        <v>1965</v>
+        <v>1994</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E68">
         <f>IF(B68 &gt; 1900, ((B68-1900)*10)+400+C68, ((B68-1730)*2)+C68)+VLOOKUP(D68,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4651</v>
+        <v>10941</v>
       </c>
       <c r="F68">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="G68">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="H68" s="2">
-        <f t="shared" si="5"/>
-        <v>103.27955589886446</v>
+        <f>SQRT(F68*G68)/$B$1</f>
+        <v>73.029674334022147</v>
       </c>
       <c r="I68" s="2">
-        <f t="shared" si="3"/>
-        <v>92.951600308978016</v>
+        <f>H68*0.9</f>
+        <v>65.726706900619931</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K68" s="3">
-        <v>6.2</v>
+        <v>5</v>
       </c>
       <c r="L68" s="3">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="M68" s="3">
-        <v>2.6</v>
+        <v>1.5</v>
       </c>
       <c r="N68" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K68*VLOOKUP(D68,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M68*VLOOKUP(D68,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L68*VLOOKUP(D68,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>29x13x16</v>
-      </c>
-      <c r="O68" t="s">
-        <v>98</v>
+ROUND(L68*VLOOKUP(D68,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M68*VLOOKUP(D68,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>23x14x7</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="B69">
-        <v>1993</v>
+        <v>1997</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E69">
         <f>IF(B69 &gt; 1900, ((B69-1900)*10)+400+C69, ((B69-1730)*2)+C69)+VLOOKUP(D69,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4931</v>
+        <v>10971</v>
       </c>
       <c r="F69">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G69">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="H69" s="2">
-        <f t="shared" si="5"/>
-        <v>120</v>
+        <f>SQRT(F69*G69)/$B$1</f>
+        <v>67.082039324993701</v>
       </c>
       <c r="I69" s="2">
-        <f t="shared" si="3"/>
-        <v>108</v>
+        <f>H69*0.9</f>
+        <v>60.373835392494335</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K69" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="L69" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M69" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
       <c r="N69" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K69*VLOOKUP(D69,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M69*VLOOKUP(D69,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L69*VLOOKUP(D69,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>29x13x16</v>
+ROUND(L69*VLOOKUP(D69,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M69*VLOOKUP(D69,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
       </c>
       <c r="O69" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="B70">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E70">
         <f>IF(B70 &gt; 1900, ((B70-1900)*10)+400+C70, ((B70-1730)*2)+C70)+VLOOKUP(D70,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>5051</v>
+        <v>11041</v>
       </c>
       <c r="F70">
-        <v>80</v>
+        <v>145</v>
       </c>
       <c r="G70">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="H70" s="2">
-        <f t="shared" ref="H70" si="6">SQRT(F70*G70)/$B$1</f>
-        <v>126.49110640673518</v>
+        <f>SQRT(F70*G70)/$B$1</f>
+        <v>80.277297191948648</v>
       </c>
       <c r="I70" s="2">
-        <f t="shared" si="3"/>
-        <v>113.84199576606167</v>
+        <f>H70*0.9</f>
+        <v>72.249567472753782</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K70" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="L70" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M70" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
       <c r="N70" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K70*VLOOKUP(D70,'ID Scheme'!$A$2:$E$5,3),0), "x",
-ROUND(M70*VLOOKUP(D70,'ID Scheme'!$A$2:$E$5,4),0), "x",
-ROUND(L70*VLOOKUP(D70,'ID Scheme'!$A$2:$E$5,5),0))</f>
-        <v>29x13x16</v>
-      </c>
-      <c r="O70" t="s">
-        <v>96</v>
+ROUND(L70*VLOOKUP(D70,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M70*VLOOKUP(D70,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>67</v>
+      </c>
+      <c r="B71">
+        <v>2009</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>62</v>
+      </c>
+      <c r="E71">
+        <f>IF(B71 &gt; 1900, ((B71-1900)*10)+400+C71, ((B71-1730)*2)+C71)+VLOOKUP(D71,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>11091</v>
+      </c>
+      <c r="F71">
+        <v>112</v>
+      </c>
+      <c r="G71">
+        <v>4</v>
+      </c>
+      <c r="H71" s="2">
+        <f>SQRT(F71*G71)/$B$1</f>
+        <v>70.553368295055762</v>
+      </c>
+      <c r="I71" s="2">
+        <f>H71*0.9</f>
+        <v>63.498031465550184</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K71*VLOOKUP(D71,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(L71*VLOOKUP(D71,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M71*VLOOKUP(D71,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:O65">
-    <sortCondition ref="E65"/>
+  <sortState ref="A4:O71">
+    <sortCondition ref="E71"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Bristol buses and Mercedes LK
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215108A2-12D7-47EB-B1ED-E296F66A7264}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A94BA2-5F6E-474C-B68C-1FA4AD606534}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="108">
   <si>
     <t>Vehicle</t>
   </si>
@@ -327,6 +327,24 @@
   </si>
   <si>
     <t>Saviem SM</t>
+  </si>
+  <si>
+    <t>Renault Magnum</t>
+  </si>
+  <si>
+    <t>Bristol LS</t>
+  </si>
+  <si>
+    <t>Bristol Lodekka</t>
+  </si>
+  <si>
+    <t>120hp</t>
+  </si>
+  <si>
+    <t>Mercedes LK</t>
+  </si>
+  <si>
+    <t>136hp</t>
   </si>
 </sst>
 </file>
@@ -692,11 +710,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O71"/>
+  <dimension ref="A1:O75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
+      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,41 +833,41 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B5">
-        <v>1833</v>
+        <v>1800</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5">
         <f>IF(B5 &gt; 1900, ((B5-1900)*10)+400+C5, ((B5-1730)*2)+C5)+VLOOKUP(D5,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>807</v>
+        <v>3741</v>
       </c>
       <c r="F5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G5">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2">
         <f>SQRT(F5*G5)/$B$1</f>
-        <v>66.332495807108003</v>
+        <v>46.188021535170058</v>
       </c>
       <c r="I5" s="2">
         <f>H5*0.9</f>
-        <v>59.699246226397207</v>
+        <v>41.569219381653056</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="2"/>
+      <c r="M5" s="3"/>
       <c r="N5" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K5*VLOOKUP(D5,'ID Scheme'!$A$2:$E$5,3),0), "x",
@@ -860,10 +878,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B6">
-        <v>1911</v>
+        <v>1833</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -873,21 +891,21 @@
       </c>
       <c r="E6">
         <f>IF(B6 &gt; 1900, ((B6-1900)*10)+400+C6, ((B6-1730)*2)+C6)+VLOOKUP(D6,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1111</v>
+        <v>807</v>
       </c>
       <c r="F6">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="H6" s="2">
         <f>SQRT(F6*G6)/$B$1</f>
-        <v>89.442719099991592</v>
+        <v>66.332495807108003</v>
       </c>
       <c r="I6" s="2">
         <f>H6*0.9</f>
-        <v>80.498447189992433</v>
+        <v>59.699246226397207</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>33</v>
@@ -905,41 +923,41 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B7">
-        <v>1924</v>
+        <v>1897</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <f>IF(B7 &gt; 1900, ((B7-1900)*10)+400+C7, ((B7-1730)*2)+C7)+VLOOKUP(D7,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1241</v>
+        <v>3935</v>
       </c>
       <c r="F7">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="G7">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="H7" s="2">
         <f>SQRT(F7*G7)/$B$1</f>
-        <v>113.13708498984759</v>
+        <v>52.915026221291818</v>
       </c>
       <c r="I7" s="2">
         <f>H7*0.9</f>
-        <v>101.82337649086284</v>
+        <v>47.623523599162638</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="2"/>
+      <c r="M7" s="3"/>
       <c r="N7" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K7*VLOOKUP(D7,'ID Scheme'!$A$2:$E$5,3),0), "x",
@@ -950,41 +968,41 @@
     </row>
     <row r="8" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <v>1927</v>
+        <v>1902</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <f>IF(B8 &gt; 1900, ((B8-1900)*10)+400+C8, ((B8-1730)*2)+C8)+VLOOKUP(D8,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1271</v>
+        <v>4021</v>
       </c>
       <c r="F8">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="G8">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="H8" s="2">
         <f>SQRT(F8*G8)/$B$1</f>
-        <v>127.80193008453877</v>
+        <v>56.568542494923797</v>
       </c>
       <c r="I8" s="2">
         <f>H8*0.9</f>
-        <v>115.02173707608489</v>
+        <v>50.911688245431421</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="2"/>
+      <c r="M8" s="3"/>
       <c r="N8" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K8*VLOOKUP(D8,'ID Scheme'!$A$2:$E$5,3),0), "x",
@@ -995,41 +1013,41 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B9">
-        <v>1929</v>
+        <v>1907</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9">
         <f>IF(B9 &gt; 1900, ((B9-1900)*10)+400+C9, ((B9-1730)*2)+C9)+VLOOKUP(D9,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1291</v>
+        <v>4071</v>
       </c>
       <c r="F9">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G9">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="H9" s="2">
         <f>SQRT(F9*G9)/$B$1</f>
-        <v>126.92955176439848</v>
+        <v>63.245553203367592</v>
       </c>
       <c r="I9" s="2">
         <f>H9*0.9</f>
-        <v>114.23659658795863</v>
+        <v>56.920997883030836</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="2"/>
+      <c r="M9" s="3"/>
       <c r="N9" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K9*VLOOKUP(D9,'ID Scheme'!$A$2:$E$5,3),0), "x",
@@ -1040,10 +1058,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B10">
-        <v>1933</v>
+        <v>1911</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1053,21 +1071,21 @@
       </c>
       <c r="E10">
         <f>IF(B10 &gt; 1900, ((B10-1900)*10)+400+C10, ((B10-1730)*2)+C10)+VLOOKUP(D10,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1331</v>
+        <v>1111</v>
       </c>
       <c r="F10">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G10">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H10" s="2">
         <f>SQRT(F10*G10)/$B$1</f>
-        <v>139.84117975602021</v>
+        <v>89.442719099991592</v>
       </c>
       <c r="I10" s="2">
         <f>H10*0.9</f>
-        <v>125.85706178041819</v>
+        <v>80.498447189992433</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>33</v>
@@ -1085,41 +1103,41 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="B11">
-        <v>1945</v>
+        <v>1912</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <f>IF(B11 &gt; 1900, ((B11-1900)*10)+400+C11, ((B11-1730)*2)+C11)+VLOOKUP(D11,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1451</v>
+        <v>7121</v>
       </c>
       <c r="F11">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G11">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="H11" s="2">
         <f>SQRT(F11*G11)/$B$1</f>
-        <v>155.13435037626795</v>
+        <v>42.163702135578397</v>
       </c>
       <c r="I11" s="2">
         <f>H11*0.9</f>
-        <v>139.62091533864117</v>
+        <v>37.94733192202056</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="2"/>
+      <c r="M11" s="3"/>
       <c r="N11" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K11*VLOOKUP(D11,'ID Scheme'!$A$2:$E$5,3),0), "x",
@@ -1130,41 +1148,41 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>1954</v>
+        <v>1913</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12">
         <f>IF(B12 &gt; 1900, ((B12-1900)*10)+400+C12, ((B12-1730)*2)+C12)+VLOOKUP(D12,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1541</v>
+        <v>4131</v>
       </c>
       <c r="F12">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G12">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="H12" s="2">
         <f>SQRT(F12*G12)/$B$1</f>
-        <v>178.88543819998318</v>
+        <v>66.332495807108003</v>
       </c>
       <c r="I12" s="2">
         <f>H12*0.9</f>
-        <v>160.99689437998487</v>
+        <v>59.699246226397207</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="2"/>
+      <c r="M12" s="3"/>
       <c r="N12" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K12*VLOOKUP(D12,'ID Scheme'!$A$2:$E$5,3),0), "x",
@@ -1175,79 +1193,85 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="B13">
-        <v>1958</v>
+        <v>1920</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13">
         <f>IF(B13 &gt; 1900, ((B13-1900)*10)+400+C13, ((B13-1730)*2)+C13)+VLOOKUP(D13,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1581</v>
+        <v>4201</v>
       </c>
       <c r="F13">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="G13">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H13" s="2">
         <f>SQRT(F13*G13)/$B$1</f>
-        <v>169.44353369518447</v>
+        <v>74.833147735478832</v>
       </c>
       <c r="I13" s="2">
         <f>H13*0.9</f>
-        <v>152.49918032566603</v>
+        <v>67.349832961930957</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="2"/>
+      <c r="K13" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="L13" s="3">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>2.5</v>
+      </c>
       <c r="N13" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K13*VLOOKUP(D13,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L13*VLOOKUP(D13,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M13*VLOOKUP(D13,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>16x14x12</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B14">
-        <v>1958</v>
+        <v>1924</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
       <c r="E14">
         <f>IF(B14 &gt; 1900, ((B14-1900)*10)+400+C14, ((B14-1730)*2)+C14)+VLOOKUP(D14,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1582</v>
+        <v>1241</v>
       </c>
       <c r="F14">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="G14">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="H14" s="2">
         <f>SQRT(F14*G14)/$B$1</f>
-        <v>186.63690238892559</v>
+        <v>113.13708498984759</v>
       </c>
       <c r="I14" s="2">
         <f>H14*0.9</f>
-        <v>167.97321215003305</v>
+        <v>101.82337649086284</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>33</v>
@@ -1265,10 +1289,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B15">
-        <v>1963</v>
+        <v>1927</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1278,95 +1302,87 @@
       </c>
       <c r="E15">
         <f>IF(B15 &gt; 1900, ((B15-1900)*10)+400+C15, ((B15-1730)*2)+C15)+VLOOKUP(D15,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1631</v>
+        <v>1271</v>
       </c>
       <c r="F15">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G15">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="H15" s="2">
         <f>SQRT(F15*G15)/$B$1</f>
-        <v>178.26322609494585</v>
+        <v>127.80193008453877</v>
       </c>
       <c r="I15" s="2">
         <f>H15*0.9</f>
-        <v>160.43690348545127</v>
+        <v>115.02173707608489</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="3">
-        <v>11</v>
-      </c>
-      <c r="L15" s="3">
-        <v>2.5</v>
-      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M15*VLOOKUP(D15,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>51x18x0</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B16">
-        <v>1972</v>
+        <v>1928</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E16">
         <f>IF(B16 &gt; 1900, ((B16-1900)*10)+400+C16, ((B16-1730)*2)+C16)+VLOOKUP(D16,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1721</v>
+        <v>4281</v>
       </c>
       <c r="F16">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="G16">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="H16" s="2">
         <f>SQRT(F16*G16)/$B$1</f>
-        <v>183.06040290327977</v>
+        <v>78.528126595931653</v>
       </c>
       <c r="I16" s="2">
         <f>H16*0.9</f>
-        <v>164.75436261295178</v>
+        <v>70.675313936338483</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="3">
-        <v>11.3</v>
-      </c>
-      <c r="L16" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="M16" s="2"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
       <c r="N16" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M16*VLOOKUP(D16,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>53x18x0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B17">
-        <v>1978</v>
+        <v>1929</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1376,48 +1392,42 @@
       </c>
       <c r="E17">
         <f>IF(B17 &gt; 1900, ((B17-1900)*10)+400+C17, ((B17-1730)*2)+C17)+VLOOKUP(D17,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1781</v>
+        <v>1291</v>
       </c>
       <c r="F17">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="G17">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H17" s="2">
         <f>SQRT(F17*G17)/$B$1</f>
-        <v>194.65068427541911</v>
+        <v>126.92955176439848</v>
       </c>
       <c r="I17" s="2">
         <f>H17*0.9</f>
-        <v>175.18561584787722</v>
+        <v>114.23659658795863</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="3">
-        <v>12</v>
-      </c>
-      <c r="L17" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="M17" s="3">
-        <v>3.3</v>
-      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="2"/>
       <c r="N17" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K17*VLOOKUP(D17,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L17*VLOOKUP(D17,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M17*VLOOKUP(D17,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>56x18x16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B18">
-        <v>1980</v>
+        <v>1933</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1427,303 +1437,264 @@
       </c>
       <c r="E18">
         <f>IF(B18 &gt; 1900, ((B18-1900)*10)+400+C18, ((B18-1730)*2)+C18)+VLOOKUP(D18,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1801</v>
+        <v>1331</v>
       </c>
       <c r="F18">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G18">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="H18" s="2">
         <f>SQRT(F18*G18)/$B$1</f>
-        <v>195.2491286080996</v>
+        <v>139.84117975602021</v>
       </c>
       <c r="I18" s="2">
         <f>H18*0.9</f>
-        <v>175.72421574728963</v>
+        <v>125.85706178041819</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K18" s="3">
-        <v>12</v>
-      </c>
-      <c r="L18" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="M18" s="3">
-        <v>4.2</v>
-      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="2"/>
       <c r="N18" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K18*VLOOKUP(D18,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L18*VLOOKUP(D18,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M18*VLOOKUP(D18,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>56x18x20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B19">
-        <v>1989</v>
+        <v>1935</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E19">
         <f>IF(B19 &gt; 1900, ((B19-1900)*10)+400+C19, ((B19-1730)*2)+C19)+VLOOKUP(D19,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1891</v>
+        <v>4351</v>
       </c>
       <c r="F19">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="G19">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="H19" s="2">
         <f>SQRT(F19*G19)/$B$1</f>
-        <v>176.38342073763937</v>
+        <v>96.609178307929596</v>
       </c>
       <c r="I19" s="2">
         <f>H19*0.9</f>
-        <v>158.74507866387543</v>
+        <v>86.948260477136643</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K19" s="3">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="L19" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="M19" s="3">
-        <v>2.7</v>
-      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
       <c r="N19" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K19*VLOOKUP(D19,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L19*VLOOKUP(D19,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M19*VLOOKUP(D19,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>48x17x13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>1998</v>
+        <v>1936</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E20">
         <f>IF(B20 &gt; 1900, ((B20-1900)*10)+400+C20, ((B20-1730)*2)+C20)+VLOOKUP(D20,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1981</v>
+        <v>4361</v>
       </c>
       <c r="F20">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="G20">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H20" s="2">
         <f>SQRT(F20*G20)/$B$1</f>
-        <v>147.08274315273474</v>
+        <v>81.649658092772611</v>
       </c>
       <c r="I20" s="2">
         <f>H20*0.9</f>
-        <v>132.37446883746128</v>
+        <v>73.484692283495349</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K20" s="3">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="L20" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="M20" s="3">
-        <v>2.7</v>
-      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
       <c r="N20" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M20*VLOOKUP(D20,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>48x17x13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="B21">
-        <v>2001</v>
+        <v>1938</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E21">
         <f>IF(B21 &gt; 1900, ((B21-1900)*10)+400+C21, ((B21-1730)*2)+C21)+VLOOKUP(D21,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>2011</v>
+        <v>7381</v>
       </c>
       <c r="F21">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="G21">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="H21" s="2">
         <f>SQRT(F21*G21)/$B$1</f>
-        <v>212.39376429431988</v>
+        <v>50</v>
       </c>
       <c r="I21" s="2">
         <f>H21*0.9</f>
-        <v>191.15438786488789</v>
+        <v>45</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K21" s="3">
-        <v>12</v>
-      </c>
-      <c r="L21" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="M21" s="3">
-        <v>3.3</v>
-      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
       <c r="N21" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M21*VLOOKUP(D21,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>56x18x16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="B22">
-        <v>2001</v>
+        <v>1945</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
       </c>
       <c r="E22">
         <f>IF(B22 &gt; 1900, ((B22-1900)*10)+400+C22, ((B22-1730)*2)+C22)+VLOOKUP(D22,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>2012</v>
+        <v>1451</v>
       </c>
       <c r="F22">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G22">
-        <v>140</v>
+        <v>57</v>
       </c>
       <c r="H22" s="2">
         <f>SQRT(F22*G22)/$B$1</f>
-        <v>292.49881291307071</v>
+        <v>155.13435037626795</v>
       </c>
       <c r="I22" s="2">
         <f>H22*0.9</f>
-        <v>263.24893162176363</v>
+        <v>139.62091533864117</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="3">
-        <v>18</v>
-      </c>
-      <c r="L22" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="M22" s="3">
-        <v>3.2</v>
-      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="2"/>
       <c r="N22" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M22*VLOOKUP(D22,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>84x18x15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="B23">
-        <v>2005</v>
+        <v>1948</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E23">
         <f>IF(B23 &gt; 1900, ((B23-1900)*10)+400+C23, ((B23-1730)*2)+C23)+VLOOKUP(D23,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>2051</v>
+        <v>4481</v>
       </c>
       <c r="F23">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="G23">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="H23" s="2">
         <f>SQRT(F23*G23)/$B$1</f>
-        <v>244.94897427831785</v>
+        <v>53.541261347363367</v>
       </c>
       <c r="I23" s="2">
         <f>H23*0.9</f>
-        <v>220.45407685048608</v>
+        <v>48.187135212627034</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="K23" s="3">
-        <v>11.4</v>
-      </c>
-      <c r="L23" s="3">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="M23" s="3">
-        <v>4.2</v>
       </c>
       <c r="N23" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M23*VLOOKUP(D23,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>53x18x20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="B24">
-        <v>2012</v>
+        <v>1949</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1733,93 +1704,105 @@
       </c>
       <c r="E24">
         <f>IF(B24 &gt; 1900, ((B24-1900)*10)+400+C24, ((B24-1730)*2)+C24)+VLOOKUP(D24,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>2121</v>
+        <v>1491</v>
       </c>
       <c r="F24">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G24">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="H24" s="2">
         <f>SQRT(F24*G24)/$B$1</f>
-        <v>219.84843263788198</v>
+        <v>164.51950239004088</v>
       </c>
       <c r="I24" s="2">
         <f>H24*0.9</f>
-        <v>197.86358937409378</v>
+        <v>148.06755215103681</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="K24" s="3">
+        <v>9.1</v>
+      </c>
+      <c r="L24" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="M24" s="2">
+        <v>3.9</v>
+      </c>
       <c r="N24" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K24*VLOOKUP(D24,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L24*VLOOKUP(D24,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M24*VLOOKUP(D24,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>42x17x19</v>
+      </c>
+      <c r="O24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="B25">
-        <v>2012</v>
+        <v>1950</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
         <v>21</v>
       </c>
       <c r="E25">
         <f>IF(B25 &gt; 1900, ((B25-1900)*10)+400+C25, ((B25-1730)*2)+C25)+VLOOKUP(D25,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>2122</v>
+        <v>1501</v>
       </c>
       <c r="F25">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="G25">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="H25" s="2">
         <f>SQRT(F25*G25)/$B$1</f>
-        <v>152.75252316519467</v>
+        <v>144.91376746189439</v>
       </c>
       <c r="I25" s="2">
         <f>H25*0.9</f>
-        <v>137.4772708486752</v>
+        <v>130.42239071570495</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K25" s="3">
-        <v>10.199999999999999</v>
+        <v>9.1</v>
       </c>
       <c r="L25" s="3">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="M25" s="3">
-        <v>2.7</v>
+        <v>2.6</v>
       </c>
       <c r="N25" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M25*VLOOKUP(D25,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>48x17x13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>42x17x13</v>
+      </c>
+      <c r="O25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>1800</v>
+        <v>1952</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1829,21 +1812,21 @@
       </c>
       <c r="E26">
         <f>IF(B26 &gt; 1900, ((B26-1900)*10)+400+C26, ((B26-1730)*2)+C26)+VLOOKUP(D26,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>3741</v>
+        <v>4521</v>
       </c>
       <c r="F26">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G26">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H26" s="2">
         <f>SQRT(F26*G26)/$B$1</f>
-        <v>46.188021535170058</v>
+        <v>102.74023338281629</v>
       </c>
       <c r="I26" s="2">
         <f>H26*0.9</f>
-        <v>41.569219381653056</v>
+        <v>92.466210044534662</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>33</v>
@@ -1859,43 +1842,43 @@
         <v>0x0x0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B27">
-        <v>1897</v>
+        <v>1954</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E27">
         <f>IF(B27 &gt; 1900, ((B27-1900)*10)+400+C27, ((B27-1730)*2)+C27)+VLOOKUP(D27,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>3935</v>
+        <v>1541</v>
       </c>
       <c r="F27">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="G27">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="H27" s="2">
         <f>SQRT(F27*G27)/$B$1</f>
-        <v>52.915026221291818</v>
+        <v>178.88543819998318</v>
       </c>
       <c r="I27" s="2">
         <f>H27*0.9</f>
-        <v>47.623523599162638</v>
+        <v>160.99689437998487</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
+      <c r="M27" s="2"/>
       <c r="N27" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K27*VLOOKUP(D27,'ID Scheme'!$A$2:$E$5,3),0), "x",
@@ -1904,12 +1887,12 @@
         <v>0x0x0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B28">
-        <v>1902</v>
+        <v>1957</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1919,21 +1902,21 @@
       </c>
       <c r="E28">
         <f>IF(B28 &gt; 1900, ((B28-1900)*10)+400+C28, ((B28-1730)*2)+C28)+VLOOKUP(D28,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4021</v>
+        <v>4571</v>
       </c>
       <c r="F28">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="G28">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H28" s="2">
         <f>SQRT(F28*G28)/$B$1</f>
-        <v>56.568542494923797</v>
+        <v>97.809338340808068</v>
       </c>
       <c r="I28" s="2">
         <f>H28*0.9</f>
-        <v>50.911688245431421</v>
+        <v>88.02840450672727</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>33</v>
@@ -1949,28 +1932,28 @@
         <v>0x0x0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B29">
-        <v>1907</v>
+        <v>1957</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E29">
         <f>IF(B29 &gt; 1900, ((B29-1900)*10)+400+C29, ((B29-1730)*2)+C29)+VLOOKUP(D29,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4071</v>
+        <v>7571</v>
       </c>
       <c r="F29">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G29">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H29" s="2">
         <f>SQRT(F29*G29)/$B$1</f>
@@ -1994,43 +1977,43 @@
         <v>0x0x0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B30">
-        <v>1913</v>
+        <v>1958</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E30">
         <f>IF(B30 &gt; 1900, ((B30-1900)*10)+400+C30, ((B30-1730)*2)+C30)+VLOOKUP(D30,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4131</v>
+        <v>1581</v>
       </c>
       <c r="F30">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="G30">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="H30" s="2">
         <f>SQRT(F30*G30)/$B$1</f>
-        <v>66.332495807108003</v>
+        <v>169.44353369518447</v>
       </c>
       <c r="I30" s="2">
         <f>H30*0.9</f>
-        <v>59.699246226397207</v>
+        <v>152.49918032566603</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
+      <c r="M30" s="2"/>
       <c r="N30" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K30*VLOOKUP(D30,'ID Scheme'!$A$2:$E$5,3),0), "x",
@@ -2039,87 +2022,81 @@
         <v>0x0x0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B31">
-        <v>1920</v>
+        <v>1958</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E31">
         <f>IF(B31 &gt; 1900, ((B31-1900)*10)+400+C31, ((B31-1730)*2)+C31)+VLOOKUP(D31,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4201</v>
+        <v>1582</v>
       </c>
       <c r="F31">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="G31">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="H31" s="2">
         <f>SQRT(F31*G31)/$B$1</f>
-        <v>74.833147735478832</v>
+        <v>186.63690238892559</v>
       </c>
       <c r="I31" s="2">
         <f>H31*0.9</f>
-        <v>67.349832961930957</v>
+        <v>167.97321215003305</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K31" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="L31" s="3">
-        <v>2</v>
-      </c>
-      <c r="M31">
-        <v>2.5</v>
-      </c>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="2"/>
       <c r="N31" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M31*VLOOKUP(D31,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>16x14x12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B32">
-        <v>1928</v>
+        <v>1958</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E32">
         <f>IF(B32 &gt; 1900, ((B32-1900)*10)+400+C32, ((B32-1730)*2)+C32)+VLOOKUP(D32,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4281</v>
+        <v>10581</v>
       </c>
       <c r="F32">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="G32">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H32" s="2">
         <f>SQRT(F32*G32)/$B$1</f>
-        <v>78.528126595931653</v>
+        <v>57.735026918962582</v>
       </c>
       <c r="I32" s="2">
         <f>H32*0.9</f>
-        <v>70.675313936338483</v>
+        <v>51.961524227066327</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>33</v>
@@ -2134,13 +2111,16 @@
 ROUND(M32*VLOOKUP(D32,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
+      <c r="O32" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B33">
-        <v>1935</v>
+        <v>1959</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2150,66 +2130,75 @@
       </c>
       <c r="E33">
         <f>IF(B33 &gt; 1900, ((B33-1900)*10)+400+C33, ((B33-1730)*2)+C33)+VLOOKUP(D33,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4351</v>
+        <v>4591</v>
       </c>
       <c r="F33">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="G33">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H33" s="2">
         <f>SQRT(F33*G33)/$B$1</f>
-        <v>96.609178307929596</v>
+        <v>101.54364141151879</v>
       </c>
       <c r="I33" s="2">
         <f>H33*0.9</f>
-        <v>86.948260477136643</v>
+        <v>91.389277270366918</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
+      <c r="K33" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L33" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M33" s="3">
+        <v>2.6</v>
+      </c>
       <c r="N33" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K33*VLOOKUP(D33,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L33*VLOOKUP(D33,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M33*VLOOKUP(D33,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>29x16x13</v>
+      </c>
+      <c r="O33" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="B34">
-        <v>1936</v>
+        <v>1960</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E34">
         <f>IF(B34 &gt; 1900, ((B34-1900)*10)+400+C34, ((B34-1730)*2)+C34)+VLOOKUP(D34,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4361</v>
+        <v>7601</v>
       </c>
       <c r="F34">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G34">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="H34" s="2">
         <f>SQRT(F34*G34)/$B$1</f>
-        <v>81.649658092772611</v>
+        <v>73.029674334022147</v>
       </c>
       <c r="I34" s="2">
         <f>H34*0.9</f>
-        <v>73.484692283495349</v>
+        <v>65.726706900619931</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>33</v>
@@ -2227,52 +2216,59 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="B35">
-        <v>1948</v>
+        <v>1963</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35">
         <f>IF(B35 &gt; 1900, ((B35-1900)*10)+400+C35, ((B35-1730)*2)+C35)+VLOOKUP(D35,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4481</v>
+        <v>1631</v>
       </c>
       <c r="F35">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G35">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="H35" s="2">
         <f>SQRT(F35*G35)/$B$1</f>
-        <v>53.541261347363367</v>
+        <v>178.26322609494585</v>
       </c>
       <c r="I35" s="2">
         <f>H35*0.9</f>
-        <v>48.187135212627034</v>
+        <v>160.43690348545127</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="K35" s="3">
+        <v>11</v>
+      </c>
+      <c r="L35" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M35" s="2"/>
       <c r="N35" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K35*VLOOKUP(D35,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L35*VLOOKUP(D35,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M35*VLOOKUP(D35,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>51x18x0</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B36">
-        <v>1952</v>
+        <v>1963</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2282,21 +2278,21 @@
       </c>
       <c r="E36">
         <f>IF(B36 &gt; 1900, ((B36-1900)*10)+400+C36, ((B36-1730)*2)+C36)+VLOOKUP(D36,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4521</v>
+        <v>4631</v>
       </c>
       <c r="F36">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G36">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H36" s="2">
         <f>SQRT(F36*G36)/$B$1</f>
-        <v>102.74023338281629</v>
+        <v>108.32051206181282</v>
       </c>
       <c r="I36" s="2">
         <f>H36*0.9</f>
-        <v>92.466210044534662</v>
+        <v>97.488460855631544</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>33</v>
@@ -2314,10 +2310,10 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B37">
-        <v>1957</v>
+        <v>1964</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2327,21 +2323,21 @@
       </c>
       <c r="E37">
         <f>IF(B37 &gt; 1900, ((B37-1900)*10)+400+C37, ((B37-1730)*2)+C37)+VLOOKUP(D37,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4571</v>
+        <v>4641</v>
       </c>
       <c r="F37">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="G37">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H37" s="2">
         <f>SQRT(F37*G37)/$B$1</f>
-        <v>97.809338340808068</v>
+        <v>146.9693845669907</v>
       </c>
       <c r="I37" s="2">
         <f>H37*0.9</f>
-        <v>88.02840450672727</v>
+        <v>132.27244611029164</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>33</v>
@@ -2359,64 +2355,58 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="B38">
-        <v>1959</v>
+        <v>1964</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" t="s">
         <v>22</v>
       </c>
       <c r="E38">
         <f>IF(B38 &gt; 1900, ((B38-1900)*10)+400+C38, ((B38-1730)*2)+C38)+VLOOKUP(D38,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4591</v>
+        <v>4642</v>
       </c>
       <c r="F38">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G38">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H38" s="2">
         <f>SQRT(F38*G38)/$B$1</f>
-        <v>101.54364141151879</v>
+        <v>114.89125293076057</v>
       </c>
       <c r="I38" s="2">
         <f>H38*0.9</f>
-        <v>91.389277270366918</v>
+        <v>103.40212763768452</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K38" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="L38" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M38" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
       <c r="N38" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K38*VLOOKUP(D38,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L38*VLOOKUP(D38,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M38*VLOOKUP(D38,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
+        <v>0x0x0</v>
       </c>
       <c r="O38" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39">
-        <v>1963</v>
+        <v>1965</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2426,21 +2416,21 @@
       </c>
       <c r="E39">
         <f>IF(B39 &gt; 1900, ((B39-1900)*10)+400+C39, ((B39-1730)*2)+C39)+VLOOKUP(D39,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4631</v>
+        <v>4651</v>
       </c>
       <c r="F39">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G39">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="H39" s="2">
         <f>SQRT(F39*G39)/$B$1</f>
-        <v>108.32051206181282</v>
+        <v>150.99668870541501</v>
       </c>
       <c r="I39" s="2">
         <f>H39*0.9</f>
-        <v>97.488460855631544</v>
+        <v>135.8970198348735</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>33</v>
@@ -2458,79 +2448,88 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="B40">
-        <v>1964</v>
+        <v>1965</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40" t="s">
         <v>22</v>
       </c>
       <c r="E40">
         <f>IF(B40 &gt; 1900, ((B40-1900)*10)+400+C40, ((B40-1730)*2)+C40)+VLOOKUP(D40,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4641</v>
+        <v>4652</v>
       </c>
       <c r="F40">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G40">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H40" s="2">
         <f>SQRT(F40*G40)/$B$1</f>
-        <v>146.9693845669907</v>
+        <v>103.27955589886446</v>
       </c>
       <c r="I40" s="2">
         <f>H40*0.9</f>
-        <v>132.27244611029164</v>
+        <v>92.951600308978016</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
+      <c r="K40" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L40" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M40" s="3">
+        <v>2.6</v>
+      </c>
       <c r="N40" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K40*VLOOKUP(D40,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L40*VLOOKUP(D40,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M40*VLOOKUP(D40,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>29x16x13</v>
+      </c>
+      <c r="O40" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B41">
-        <v>1964</v>
+        <v>1965</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E41">
         <f>IF(B41 &gt; 1900, ((B41-1900)*10)+400+C41, ((B41-1730)*2)+C41)+VLOOKUP(D41,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4642</v>
+        <v>7651</v>
       </c>
       <c r="F41">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G41">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="H41" s="2">
         <f>SQRT(F41*G41)/$B$1</f>
-        <v>114.89125293076057</v>
+        <v>76.011695006609202</v>
       </c>
       <c r="I41" s="2">
         <f>H41*0.9</f>
-        <v>103.40212763768452</v>
+        <v>68.410525505948286</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>33</v>
@@ -2545,16 +2544,13 @@
 ROUND(M41*VLOOKUP(D41,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
-      <c r="O41" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="B42">
-        <v>1965</v>
+        <v>1967</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2564,181 +2560,173 @@
       </c>
       <c r="E42">
         <f>IF(B42 &gt; 1900, ((B42-1900)*10)+400+C42, ((B42-1730)*2)+C42)+VLOOKUP(D42,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4651</v>
+        <v>4671</v>
       </c>
       <c r="F42">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G42">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="H42" s="2">
         <f>SQRT(F42*G42)/$B$1</f>
-        <v>150.99668870541501</v>
+        <v>116.99952516522831</v>
       </c>
       <c r="I42" s="2">
         <f>H42*0.9</f>
-        <v>135.8970198348735</v>
+        <v>105.29957264870548</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
+      <c r="K42" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="L42" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M42" s="3">
+        <v>2.8</v>
+      </c>
       <c r="N42" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K42*VLOOKUP(D42,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L42*VLOOKUP(D42,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M42*VLOOKUP(D42,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>40x18x14</v>
+      </c>
+      <c r="O42" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
       <c r="B43">
-        <v>1965</v>
+        <v>1968</v>
       </c>
       <c r="C43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" t="s">
         <v>22</v>
       </c>
       <c r="E43">
         <f>IF(B43 &gt; 1900, ((B43-1900)*10)+400+C43, ((B43-1730)*2)+C43)+VLOOKUP(D43,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4652</v>
+        <v>4681</v>
       </c>
       <c r="F43">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="G43">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="H43" s="2">
         <f>SQRT(F43*G43)/$B$1</f>
-        <v>103.27955589886446</v>
+        <v>164.92422502470643</v>
       </c>
       <c r="I43" s="2">
         <f>H43*0.9</f>
-        <v>92.951600308978016</v>
+        <v>148.43180252223578</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K43" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="L43" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M43" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
       <c r="N43" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K43*VLOOKUP(D43,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L43*VLOOKUP(D43,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M43*VLOOKUP(D43,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
-      </c>
-      <c r="O43" t="s">
-        <v>98</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="B44">
-        <v>1967</v>
+        <v>1972</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E44">
         <f>IF(B44 &gt; 1900, ((B44-1900)*10)+400+C44, ((B44-1730)*2)+C44)+VLOOKUP(D44,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4671</v>
+        <v>1721</v>
       </c>
       <c r="F44">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G44">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="H44" s="2">
         <f>SQRT(F44*G44)/$B$1</f>
-        <v>116.99952516522831</v>
+        <v>183.06040290327977</v>
       </c>
       <c r="I44" s="2">
         <f>H44*0.9</f>
-        <v>105.29957264870548</v>
+        <v>164.75436261295178</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K44" s="3">
-        <v>8.5</v>
+        <v>11.3</v>
       </c>
       <c r="L44" s="3">
         <v>2.5</v>
       </c>
-      <c r="M44" s="3">
-        <v>2.8</v>
-      </c>
+      <c r="M44" s="2"/>
       <c r="N44" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K44*VLOOKUP(D44,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L44*VLOOKUP(D44,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M44*VLOOKUP(D44,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>40x18x14</v>
-      </c>
-      <c r="O44" t="s">
-        <v>31</v>
+        <v>53x18x0</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="B45">
-        <v>1968</v>
+        <v>1974</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E45">
         <f>IF(B45 &gt; 1900, ((B45-1900)*10)+400+C45, ((B45-1730)*2)+C45)+VLOOKUP(D45,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4681</v>
+        <v>10741</v>
       </c>
       <c r="F45">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G45">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="H45" s="2">
         <f>SQRT(F45*G45)/$B$1</f>
-        <v>164.92422502470643</v>
+        <v>74.833147735478832</v>
       </c>
       <c r="I45" s="2">
         <f>H45*0.9</f>
-        <v>148.43180252223578</v>
+        <v>67.349832961930957</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
       <c r="N45" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K45*VLOOKUP(D45,'ID Scheme'!$A$2:$E$5,3),0), "x",
@@ -2749,154 +2737,163 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B46">
-        <v>1980</v>
+        <v>1976</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E46">
         <f>IF(B46 &gt; 1900, ((B46-1900)*10)+400+C46, ((B46-1730)*2)+C46)+VLOOKUP(D46,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4801</v>
+        <v>10761</v>
       </c>
       <c r="F46">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="G46">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="H46" s="2">
         <f>SQRT(F46*G46)/$B$1</f>
-        <v>170.09801096230765</v>
+        <v>63.245553203367592</v>
       </c>
       <c r="I46" s="2">
         <f>H46*0.9</f>
-        <v>153.08820986607688</v>
+        <v>56.920997883030836</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
+      <c r="K46" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L46" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="M46" s="3">
+        <v>1.5</v>
+      </c>
       <c r="N46" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K46*VLOOKUP(D46,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L46*VLOOKUP(D46,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M46*VLOOKUP(D46,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>21x13x7</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="B47">
-        <v>1981</v>
+        <v>1978</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E47">
         <f>IF(B47 &gt; 1900, ((B47-1900)*10)+400+C47, ((B47-1730)*2)+C47)+VLOOKUP(D47,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4811</v>
+        <v>1781</v>
       </c>
       <c r="F47">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G47">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="H47" s="2">
         <f>SQRT(F47*G47)/$B$1</f>
-        <v>116.61903789690601</v>
+        <v>194.65068427541911</v>
       </c>
       <c r="I47" s="2">
         <f>H47*0.9</f>
-        <v>104.95713410721541</v>
+        <v>175.18561584787722</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K47" s="3">
-        <v>6.2</v>
+        <v>12</v>
       </c>
       <c r="L47" s="3">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="M47" s="3">
-        <v>2.6</v>
+        <v>3.3</v>
       </c>
       <c r="N47" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K47*VLOOKUP(D47,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L47*VLOOKUP(D47,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M47*VLOOKUP(D47,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
-      </c>
-      <c r="O47" t="s">
-        <v>97</v>
+        <v>56x18x16</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B48">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E48">
         <f>IF(B48 &gt; 1900, ((B48-1900)*10)+400+C48, ((B48-1730)*2)+C48)+VLOOKUP(D48,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4821</v>
+        <v>1801</v>
       </c>
       <c r="F48">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G48">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="H48" s="2">
         <f>SQRT(F48*G48)/$B$1</f>
-        <v>136.62601021279465</v>
+        <v>195.2491286080996</v>
       </c>
       <c r="I48" s="2">
         <f>H48*0.9</f>
-        <v>122.9634091915152</v>
+        <v>175.72421574728963</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
+      <c r="K48" s="3">
+        <v>12</v>
+      </c>
+      <c r="L48" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M48" s="3">
+        <v>4.2</v>
+      </c>
       <c r="N48" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K48*VLOOKUP(D48,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L48*VLOOKUP(D48,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M48*VLOOKUP(D48,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>56x18x20</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B49">
-        <v>1986</v>
+        <v>1980</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2906,21 +2903,21 @@
       </c>
       <c r="E49">
         <f>IF(B49 &gt; 1900, ((B49-1900)*10)+400+C49, ((B49-1730)*2)+C49)+VLOOKUP(D49,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4861</v>
+        <v>4801</v>
       </c>
       <c r="F49">
         <v>62</v>
       </c>
       <c r="G49">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="H49" s="2">
         <f>SQRT(F49*G49)/$B$1</f>
-        <v>143.75905768565215</v>
+        <v>170.09801096230765</v>
       </c>
       <c r="I49" s="2">
         <f>H49*0.9</f>
-        <v>129.38315191708693</v>
+        <v>153.08820986607688</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>33</v>
@@ -2938,10 +2935,10 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="B50">
-        <v>1987</v>
+        <v>1981</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2951,42 +2948,51 @@
       </c>
       <c r="E50">
         <f>IF(B50 &gt; 1900, ((B50-1900)*10)+400+C50, ((B50-1730)*2)+C50)+VLOOKUP(D50,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4871</v>
+        <v>4811</v>
       </c>
       <c r="F50">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G50">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H50" s="2">
         <f>SQRT(F50*G50)/$B$1</f>
-        <v>178.26322609494585</v>
+        <v>116.61903789690601</v>
       </c>
       <c r="I50" s="2">
         <f>H50*0.9</f>
-        <v>160.43690348545127</v>
+        <v>104.95713410721541</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
+      <c r="K50" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L50" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M50" s="3">
+        <v>2.6</v>
+      </c>
       <c r="N50" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K50*VLOOKUP(D50,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L50*VLOOKUP(D50,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M50*VLOOKUP(D50,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>29x16x13</v>
+      </c>
+      <c r="O50" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="B51">
-        <v>1993</v>
+        <v>1982</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -2996,51 +3002,42 @@
       </c>
       <c r="E51">
         <f>IF(B51 &gt; 1900, ((B51-1900)*10)+400+C51, ((B51-1730)*2)+C51)+VLOOKUP(D51,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4931</v>
+        <v>4821</v>
       </c>
       <c r="F51">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="G51">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H51" s="2">
         <f>SQRT(F51*G51)/$B$1</f>
-        <v>120</v>
+        <v>136.62601021279465</v>
       </c>
       <c r="I51" s="2">
         <f>H51*0.9</f>
-        <v>108</v>
+        <v>122.9634091915152</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K51" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="L51" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M51" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
       <c r="N51" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K51*VLOOKUP(D51,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L51*VLOOKUP(D51,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M51*VLOOKUP(D51,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
-      </c>
-      <c r="O51" t="s">
-        <v>100</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="B52">
-        <v>1995</v>
+        <v>1983</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -3050,42 +3047,51 @@
       </c>
       <c r="E52">
         <f>IF(B52 &gt; 1900, ((B52-1900)*10)+400+C52, ((B52-1730)*2)+C52)+VLOOKUP(D52,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4951</v>
+        <v>4831</v>
       </c>
       <c r="F52">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G52">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="H52" s="2">
         <f>SQRT(F52*G52)/$B$1</f>
-        <v>190.43809142780935</v>
+        <v>125.07775359529147</v>
       </c>
       <c r="I52" s="2">
         <f>H52*0.9</f>
-        <v>171.39428228502842</v>
+        <v>112.56997823576232</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
+      <c r="K52" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="L52" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M52" s="3">
+        <v>2.6</v>
+      </c>
       <c r="N52" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K52*VLOOKUP(D52,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L52*VLOOKUP(D52,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M52*VLOOKUP(D52,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>36x16x13</v>
+      </c>
+      <c r="O52" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B53">
-        <v>1997</v>
+        <v>1986</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -3095,21 +3101,21 @@
       </c>
       <c r="E53">
         <f>IF(B53 &gt; 1900, ((B53-1900)*10)+400+C53, ((B53-1730)*2)+C53)+VLOOKUP(D53,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4971</v>
+        <v>4861</v>
       </c>
       <c r="F53">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G53">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H53" s="2">
         <f>SQRT(F53*G53)/$B$1</f>
-        <v>157.76212754932311</v>
+        <v>143.75905768565215</v>
       </c>
       <c r="I53" s="2">
         <f>H53*0.9</f>
-        <v>141.98591479439079</v>
+        <v>129.38315191708693</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>33</v>
@@ -3127,34 +3133,34 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B54">
-        <v>2004</v>
+        <v>1986</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E54">
         <f>IF(B54 &gt; 1900, ((B54-1900)*10)+400+C54, ((B54-1730)*2)+C54)+VLOOKUP(D54,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>5041</v>
+        <v>7861</v>
       </c>
       <c r="F54">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="G54">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="H54" s="2">
         <f>SQRT(F54*G54)/$B$1</f>
-        <v>207.84609690826528</v>
+        <v>94.28090415820634</v>
       </c>
       <c r="I54" s="2">
         <f>H54*0.9</f>
-        <v>187.06148721743875</v>
+        <v>84.852813742385706</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>33</v>
@@ -3172,88 +3178,79 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="B55">
-        <v>2005</v>
+        <v>1986</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E55">
         <f>IF(B55 &gt; 1900, ((B55-1900)*10)+400+C55, ((B55-1730)*2)+C55)+VLOOKUP(D55,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>5051</v>
+        <v>7862</v>
       </c>
       <c r="F55">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="G55">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="H55" s="2">
         <f>SQRT(F55*G55)/$B$1</f>
-        <v>126.49110640673518</v>
+        <v>53.748384988656994</v>
       </c>
       <c r="I55" s="2">
         <f>H55*0.9</f>
-        <v>113.84199576606167</v>
+        <v>48.373546489791295</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K55" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="L55" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M55" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
       <c r="N55" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K55*VLOOKUP(D55,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L55*VLOOKUP(D55,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M55*VLOOKUP(D55,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
-      </c>
-      <c r="O55" t="s">
-        <v>96</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="B56">
-        <v>1912</v>
+        <v>1987</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E56">
         <f>IF(B56 &gt; 1900, ((B56-1900)*10)+400+C56, ((B56-1730)*2)+C56)+VLOOKUP(D56,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7121</v>
+        <v>4871</v>
       </c>
       <c r="F56">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="G56">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="H56" s="2">
         <f>SQRT(F56*G56)/$B$1</f>
-        <v>42.163702135578397</v>
+        <v>178.26322609494585</v>
       </c>
       <c r="I56" s="2">
         <f>H56*0.9</f>
-        <v>37.94733192202056</v>
+        <v>160.43690348545127</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>33</v>
@@ -3271,116 +3268,131 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B57">
-        <v>1938</v>
+        <v>1989</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E57">
         <f>IF(B57 &gt; 1900, ((B57-1900)*10)+400+C57, ((B57-1730)*2)+C57)+VLOOKUP(D57,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7381</v>
+        <v>1891</v>
       </c>
       <c r="F57">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="G57">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H57" s="2">
         <f>SQRT(F57*G57)/$B$1</f>
-        <v>50</v>
+        <v>176.38342073763937</v>
       </c>
       <c r="I57" s="2">
         <f>H57*0.9</f>
-        <v>45</v>
+        <v>158.74507866387543</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
+      <c r="K57" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="L57" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="M57" s="3">
+        <v>2.7</v>
+      </c>
       <c r="N57" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M57*VLOOKUP(D57,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>48x17x13</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="B58">
-        <v>1957</v>
+        <v>1993</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E58">
         <f>IF(B58 &gt; 1900, ((B58-1900)*10)+400+C58, ((B58-1730)*2)+C58)+VLOOKUP(D58,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7571</v>
+        <v>4931</v>
       </c>
       <c r="F58">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="G58">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H58" s="2">
         <f>SQRT(F58*G58)/$B$1</f>
-        <v>63.245553203367592</v>
+        <v>120</v>
       </c>
       <c r="I58" s="2">
         <f>H58*0.9</f>
-        <v>56.920997883030836</v>
+        <v>108</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
+      <c r="K58" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L58" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M58" s="3">
+        <v>2.6</v>
+      </c>
       <c r="N58" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M58*VLOOKUP(D58,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>29x16x13</v>
+      </c>
+      <c r="O58" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B59">
-        <v>1960</v>
+        <v>1994</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="E59">
         <f>IF(B59 &gt; 1900, ((B59-1900)*10)+400+C59, ((B59-1730)*2)+C59)+VLOOKUP(D59,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7601</v>
+        <v>10941</v>
       </c>
       <c r="F59">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="G59">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H59" s="2">
         <f>SQRT(F59*G59)/$B$1</f>
@@ -3393,47 +3405,53 @@
       <c r="J59" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
+      <c r="K59" s="3">
+        <v>5</v>
+      </c>
+      <c r="L59" s="3">
+        <v>2</v>
+      </c>
+      <c r="M59" s="3">
+        <v>1.5</v>
+      </c>
       <c r="N59" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K59*VLOOKUP(D59,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L59*VLOOKUP(D59,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M59*VLOOKUP(D59,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>23x14x7</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B60">
-        <v>1965</v>
+        <v>1995</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E60">
         <f>IF(B60 &gt; 1900, ((B60-1900)*10)+400+C60, ((B60-1730)*2)+C60)+VLOOKUP(D60,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7651</v>
+        <v>4951</v>
       </c>
       <c r="F60">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G60">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="H60" s="2">
         <f>SQRT(F60*G60)/$B$1</f>
-        <v>76.011695006609202</v>
+        <v>190.43809142780935</v>
       </c>
       <c r="I60" s="2">
         <f>H60*0.9</f>
-        <v>68.410525505948286</v>
+        <v>171.39428228502842</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>33</v>
@@ -3451,34 +3469,34 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B61">
-        <v>1986</v>
+        <v>1997</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E61">
         <f>IF(B61 &gt; 1900, ((B61-1900)*10)+400+C61, ((B61-1730)*2)+C61)+VLOOKUP(D61,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7861</v>
+        <v>4971</v>
       </c>
       <c r="F61">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G61">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H61" s="2">
         <f>SQRT(F61*G61)/$B$1</f>
-        <v>94.28090415820634</v>
+        <v>157.76212754932311</v>
       </c>
       <c r="I61" s="2">
         <f>H61*0.9</f>
-        <v>84.852813742385706</v>
+        <v>141.98591479439079</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>33</v>
@@ -3496,34 +3514,34 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B62">
-        <v>1986</v>
+        <v>1997</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="E62">
         <f>IF(B62 &gt; 1900, ((B62-1900)*10)+400+C62, ((B62-1730)*2)+C62)+VLOOKUP(D62,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7862</v>
+        <v>10971</v>
       </c>
       <c r="F62">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="G62">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H62" s="2">
         <f>SQRT(F62*G62)/$B$1</f>
-        <v>53.748384988656994</v>
+        <v>67.082039324993701</v>
       </c>
       <c r="I62" s="2">
         <f>H62*0.9</f>
-        <v>48.373546489791295</v>
+        <v>60.373835392494335</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>33</v>
@@ -3538,179 +3556,200 @@
 ROUND(M62*VLOOKUP(D62,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
+      <c r="O62" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="B63">
-        <v>2006</v>
+        <v>1998</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E63">
         <f>IF(B63 &gt; 1900, ((B63-1900)*10)+400+C63, ((B63-1730)*2)+C63)+VLOOKUP(D63,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>8061</v>
+        <v>1981</v>
       </c>
       <c r="F63">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="G63">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="H63" s="2">
         <f>SQRT(F63*G63)/$B$1</f>
-        <v>106.45812948447541</v>
+        <v>147.08274315273474</v>
       </c>
       <c r="I63" s="2">
         <f>H63*0.9</f>
-        <v>95.812316536027865</v>
+        <v>132.37446883746128</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K63" s="3"/>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
+      <c r="K63" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="L63" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M63" s="3">
+        <v>2.7</v>
+      </c>
       <c r="N63" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M63*VLOOKUP(D63,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>48x17x13</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B64">
-        <v>2012</v>
+        <v>2001</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E64">
         <f>IF(B64 &gt; 1900, ((B64-1900)*10)+400+C64, ((B64-1730)*2)+C64)+VLOOKUP(D64,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>8121</v>
+        <v>2011</v>
       </c>
       <c r="F64">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="G64">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="H64" s="2">
         <f>SQRT(F64*G64)/$B$1</f>
-        <v>101.10500592068735</v>
+        <v>212.39376429431988</v>
       </c>
       <c r="I64" s="2">
         <f>H64*0.9</f>
-        <v>90.994505328618615</v>
+        <v>191.15438786488789</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K64" s="3"/>
-      <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
+      <c r="K64" s="3">
+        <v>12</v>
+      </c>
+      <c r="L64" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M64" s="3">
+        <v>3.3</v>
+      </c>
       <c r="N64" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K64*VLOOKUP(D64,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L64*VLOOKUP(D64,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M64*VLOOKUP(D64,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>56x18x16</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B65">
-        <v>1958</v>
+        <v>2001</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="E65">
         <f>IF(B65 &gt; 1900, ((B65-1900)*10)+400+C65, ((B65-1730)*2)+C65)+VLOOKUP(D65,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10581</v>
+        <v>2012</v>
       </c>
       <c r="F65">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="G65">
-        <v>4</v>
+        <v>140</v>
       </c>
       <c r="H65" s="2">
         <f>SQRT(F65*G65)/$B$1</f>
-        <v>57.735026918962582</v>
+        <v>292.49881291307071</v>
       </c>
       <c r="I65" s="2">
         <f>H65*0.9</f>
-        <v>51.961524227066327</v>
+        <v>263.24893162176363</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K65" s="3"/>
-      <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
+      <c r="K65" s="3">
+        <v>18</v>
+      </c>
+      <c r="L65" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="M65" s="3">
+        <v>3.2</v>
+      </c>
       <c r="N65" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M65*VLOOKUP(D65,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
-      </c>
-      <c r="O65" t="s">
-        <v>69</v>
+        <v>84x18x15</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B66">
-        <v>1974</v>
+        <v>2001</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="E66">
         <f>IF(B66 &gt; 1900, ((B66-1900)*10)+400+C66, ((B66-1730)*2)+C66)+VLOOKUP(D66,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10741</v>
+        <v>5011</v>
       </c>
       <c r="F66">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G66">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="H66" s="2">
         <f>SQRT(F66*G66)/$B$1</f>
-        <v>74.833147735478832</v>
+        <v>197.20265943665387</v>
       </c>
       <c r="I66" s="2">
         <f>H66*0.9</f>
-        <v>67.349832961930957</v>
+        <v>177.48239349298848</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
       <c r="N66" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K66*VLOOKUP(D66,'ID Scheme'!$A$2:$E$5,3),0), "x",
@@ -3721,61 +3760,55 @@
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="B67">
-        <v>1976</v>
+        <v>2004</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="E67">
         <f>IF(B67 &gt; 1900, ((B67-1900)*10)+400+C67, ((B67-1730)*2)+C67)+VLOOKUP(D67,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10761</v>
+        <v>5041</v>
       </c>
       <c r="F67">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G67">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="H67" s="2">
         <f>SQRT(F67*G67)/$B$1</f>
-        <v>63.245553203367592</v>
+        <v>207.84609690826528</v>
       </c>
       <c r="I67" s="2">
         <f>H67*0.9</f>
-        <v>56.920997883030836</v>
+        <v>187.06148721743875</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K67" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="L67" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="M67" s="3">
-        <v>1.5</v>
-      </c>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
       <c r="N67" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K67*VLOOKUP(D67,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L67*VLOOKUP(D67,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M67*VLOOKUP(D67,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>21x13x7</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B68">
-        <v>1994</v>
+        <v>2004</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -3785,165 +3818,171 @@
       </c>
       <c r="E68">
         <f>IF(B68 &gt; 1900, ((B68-1900)*10)+400+C68, ((B68-1730)*2)+C68)+VLOOKUP(D68,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10941</v>
+        <v>11041</v>
       </c>
       <c r="F68">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="G68">
         <v>4</v>
       </c>
       <c r="H68" s="2">
         <f>SQRT(F68*G68)/$B$1</f>
-        <v>73.029674334022147</v>
+        <v>80.277297191948648</v>
       </c>
       <c r="I68" s="2">
         <f>H68*0.9</f>
-        <v>65.726706900619931</v>
+        <v>72.249567472753782</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K68" s="3">
-        <v>5</v>
-      </c>
-      <c r="L68" s="3">
-        <v>2</v>
-      </c>
-      <c r="M68" s="3">
-        <v>1.5</v>
-      </c>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
       <c r="N68" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K68*VLOOKUP(D68,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L68*VLOOKUP(D68,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M68*VLOOKUP(D68,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>23x14x7</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B69">
-        <v>1997</v>
+        <v>2005</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="E69">
         <f>IF(B69 &gt; 1900, ((B69-1900)*10)+400+C69, ((B69-1730)*2)+C69)+VLOOKUP(D69,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10971</v>
+        <v>2051</v>
       </c>
       <c r="F69">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G69">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="H69" s="2">
         <f>SQRT(F69*G69)/$B$1</f>
-        <v>67.082039324993701</v>
+        <v>244.94897427831785</v>
       </c>
       <c r="I69" s="2">
         <f>H69*0.9</f>
-        <v>60.373835392494335</v>
+        <v>220.45407685048608</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K69" s="3"/>
-      <c r="L69" s="3"/>
-      <c r="M69" s="3"/>
+      <c r="K69" s="3">
+        <v>11.4</v>
+      </c>
+      <c r="L69" s="3">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="M69" s="3">
+        <v>4.2</v>
+      </c>
       <c r="N69" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K69*VLOOKUP(D69,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L69*VLOOKUP(D69,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M69*VLOOKUP(D69,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
-      </c>
-      <c r="O69" t="s">
-        <v>70</v>
+        <v>53x18x20</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B70">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="E70">
         <f>IF(B70 &gt; 1900, ((B70-1900)*10)+400+C70, ((B70-1730)*2)+C70)+VLOOKUP(D70,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>11041</v>
+        <v>5051</v>
       </c>
       <c r="F70">
-        <v>145</v>
+        <v>80</v>
       </c>
       <c r="G70">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H70" s="2">
         <f>SQRT(F70*G70)/$B$1</f>
-        <v>80.277297191948648</v>
+        <v>126.49110640673518</v>
       </c>
       <c r="I70" s="2">
         <f>H70*0.9</f>
-        <v>72.249567472753782</v>
+        <v>113.84199576606167</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K70" s="3"/>
-      <c r="L70" s="3"/>
-      <c r="M70" s="3"/>
+      <c r="K70" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L70" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M70" s="3">
+        <v>2.6</v>
+      </c>
       <c r="N70" s="2" t="str">
         <f>CONCATENATE(
 ROUND(K70*VLOOKUP(D70,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(L70*VLOOKUP(D70,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(M70*VLOOKUP(D70,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>29x16x13</v>
+      </c>
+      <c r="O70" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B71">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E71">
         <f>IF(B71 &gt; 1900, ((B71-1900)*10)+400+C71, ((B71-1730)*2)+C71)+VLOOKUP(D71,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>11091</v>
+        <v>8061</v>
       </c>
       <c r="F71">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="G71">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H71" s="2">
         <f>SQRT(F71*G71)/$B$1</f>
-        <v>70.553368295055762</v>
+        <v>106.45812948447541</v>
       </c>
       <c r="I71" s="2">
         <f>H71*0.9</f>
-        <v>63.498031465550184</v>
+        <v>95.812316536027865</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>33</v>
@@ -3959,9 +3998,195 @@
         <v>0x0x0</v>
       </c>
     </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B72">
+        <v>2009</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>62</v>
+      </c>
+      <c r="E72">
+        <f>IF(B72 &gt; 1900, ((B72-1900)*10)+400+C72, ((B72-1730)*2)+C72)+VLOOKUP(D72,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>11091</v>
+      </c>
+      <c r="F72">
+        <v>112</v>
+      </c>
+      <c r="G72">
+        <v>4</v>
+      </c>
+      <c r="H72" s="2">
+        <f>SQRT(F72*G72)/$B$1</f>
+        <v>70.553368295055762</v>
+      </c>
+      <c r="I72" s="2">
+        <f>H72*0.9</f>
+        <v>63.498031465550184</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3"/>
+      <c r="N72" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K72*VLOOKUP(D72,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(L72*VLOOKUP(D72,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M72*VLOOKUP(D72,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73">
+        <v>2012</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73">
+        <f>IF(B73 &gt; 1900, ((B73-1900)*10)+400+C73, ((B73-1730)*2)+C73)+VLOOKUP(D73,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>2121</v>
+      </c>
+      <c r="F73">
+        <v>50</v>
+      </c>
+      <c r="G73">
+        <v>87</v>
+      </c>
+      <c r="H73" s="2">
+        <f>SQRT(F73*G73)/$B$1</f>
+        <v>219.84843263788198</v>
+      </c>
+      <c r="I73" s="2">
+        <f>H73*0.9</f>
+        <v>197.86358937409378</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K73*VLOOKUP(D73,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(L73*VLOOKUP(D73,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M73*VLOOKUP(D73,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74">
+        <v>2012</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74">
+        <f>IF(B74 &gt; 1900, ((B74-1900)*10)+400+C74, ((B74-1730)*2)+C74)+VLOOKUP(D74,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>2122</v>
+      </c>
+      <c r="F74">
+        <v>60</v>
+      </c>
+      <c r="G74">
+        <v>35</v>
+      </c>
+      <c r="H74" s="2">
+        <f>SQRT(F74*G74)/$B$1</f>
+        <v>152.75252316519467</v>
+      </c>
+      <c r="I74" s="2">
+        <f>H74*0.9</f>
+        <v>137.4772708486752</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K74" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="L74" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M74" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="N74" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K74*VLOOKUP(D74,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(L74*VLOOKUP(D74,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M74*VLOOKUP(D74,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>48x17x13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>54</v>
+      </c>
+      <c r="B75">
+        <v>2012</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" t="s">
+        <v>23</v>
+      </c>
+      <c r="E75">
+        <f>IF(B75 &gt; 1900, ((B75-1900)*10)+400+C75, ((B75-1730)*2)+C75)+VLOOKUP(D75,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>8121</v>
+      </c>
+      <c r="F75">
+        <v>92</v>
+      </c>
+      <c r="G75">
+        <v>10</v>
+      </c>
+      <c r="H75" s="2">
+        <f>SQRT(F75*G75)/$B$1</f>
+        <v>101.10500592068735</v>
+      </c>
+      <c r="I75" s="2">
+        <f>H75*0.9</f>
+        <v>90.994505328618615</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(K75*VLOOKUP(D75,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(L75*VLOOKUP(D75,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(M75*VLOOKUP(D75,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A4:O71">
-    <sortCondition ref="E71"/>
+  <sortState ref="A4:O75">
+    <sortCondition ref="B53"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix height of double deckers
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB317C30-4168-4D0A-A480-C9EF479DE6AF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126EDAC7-D8C5-4E93-85BE-34DAF4BC13CD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8190" windowHeight="2400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="119">
   <si>
     <t>Vehicle</t>
   </si>
@@ -380,6 +380,9 @@
   </si>
   <si>
     <t>249hp</t>
+  </si>
+  <si>
+    <t>Ford Transit Mk3 Minibus</t>
   </si>
 </sst>
 </file>
@@ -435,27 +438,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -816,11 +799,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P81"/>
+  <dimension ref="A1:P82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,11 +903,11 @@
         <v>14</v>
       </c>
       <c r="I4" s="2">
-        <f>SQRT(G4*H4)/$B$1</f>
+        <f t="shared" ref="I4:I35" si="0">SQRT(G4*H4)/$B$1</f>
         <v>52.915026221291818</v>
       </c>
       <c r="J4" s="2">
-        <f>I4*0.9</f>
+        <f t="shared" ref="J4:J35" si="1">I4*0.9</f>
         <v>47.623523599162638</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -949,7 +932,7 @@
         <v>1833</v>
       </c>
       <c r="C5">
-        <f>B5-B4</f>
+        <f t="shared" ref="C5:C36" si="2">B5-B4</f>
         <v>33</v>
       </c>
       <c r="D5">
@@ -969,11 +952,11 @@
         <v>22</v>
       </c>
       <c r="I5" s="2">
-        <f>SQRT(G5*H5)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>66.332495807108003</v>
       </c>
       <c r="J5" s="2">
-        <f>I5*0.9</f>
+        <f t="shared" si="1"/>
         <v>59.699246226397207</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -998,7 +981,7 @@
         <v>1911</v>
       </c>
       <c r="C6">
-        <f>B6-B5</f>
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
       <c r="D6">
@@ -1018,11 +1001,11 @@
         <v>36</v>
       </c>
       <c r="I6" s="2">
-        <f>SQRT(G6*H6)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>89.442719099991592</v>
       </c>
       <c r="J6" s="2">
-        <f>I6*0.9</f>
+        <f t="shared" si="1"/>
         <v>80.498447189992433</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -1047,7 +1030,7 @@
         <v>1920</v>
       </c>
       <c r="C7">
-        <f>B7-B6</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="D7">
@@ -1067,11 +1050,11 @@
         <v>46</v>
       </c>
       <c r="I7" s="2">
-        <f>SQRT(G7*H7)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>113.03883305208781</v>
       </c>
       <c r="J7" s="2">
-        <f>I7*0.9</f>
+        <f t="shared" si="1"/>
         <v>101.73494974687902</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -1096,7 +1079,7 @@
         <v>1924</v>
       </c>
       <c r="C8">
-        <f>B8-B7</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D8">
@@ -1116,11 +1099,11 @@
         <v>32</v>
       </c>
       <c r="I8" s="2">
-        <f>SQRT(G8*H8)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>113.13708498984759</v>
       </c>
       <c r="J8" s="2">
-        <f>I8*0.9</f>
+        <f t="shared" si="1"/>
         <v>101.82337649086284</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -1145,7 +1128,7 @@
         <v>1927</v>
       </c>
       <c r="C9">
-        <f>B9-B8</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="D9">
@@ -1165,11 +1148,11 @@
         <v>35</v>
       </c>
       <c r="I9" s="2">
-        <f>SQRT(G9*H9)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>127.80193008453877</v>
       </c>
       <c r="J9" s="2">
-        <f>I9*0.9</f>
+        <f t="shared" si="1"/>
         <v>115.02173707608489</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -1194,7 +1177,7 @@
         <v>1929</v>
       </c>
       <c r="C10">
-        <f>B10-B9</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="D10">
@@ -1214,11 +1197,11 @@
         <v>50</v>
       </c>
       <c r="I10" s="2">
-        <f>SQRT(G10*H10)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>126.92955176439848</v>
       </c>
       <c r="J10" s="2">
-        <f>I10*0.9</f>
+        <f t="shared" si="1"/>
         <v>114.23659658795863</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -1243,7 +1226,7 @@
         <v>1933</v>
       </c>
       <c r="C11">
-        <f>B11-B10</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D11">
@@ -1263,11 +1246,11 @@
         <v>44</v>
       </c>
       <c r="I11" s="2">
-        <f>SQRT(G11*H11)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>139.84117975602021</v>
       </c>
       <c r="J11" s="2">
-        <f>I11*0.9</f>
+        <f t="shared" si="1"/>
         <v>125.85706178041819</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -1292,7 +1275,7 @@
         <v>1937</v>
       </c>
       <c r="C12">
-        <f>B12-B11</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D12">
@@ -1312,11 +1295,11 @@
         <v>38</v>
       </c>
       <c r="I12" s="2">
-        <f>SQRT(G12*H12)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>136.30032200173915</v>
       </c>
       <c r="J12" s="2">
-        <f>I12*0.9</f>
+        <f t="shared" si="1"/>
         <v>122.67028980156523</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -1347,7 +1330,7 @@
         <v>1945</v>
       </c>
       <c r="C13">
-        <f>B13-B12</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="D13">
@@ -1367,11 +1350,11 @@
         <v>57</v>
       </c>
       <c r="I13" s="2">
-        <f>SQRT(G13*H13)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>155.13435037626795</v>
       </c>
       <c r="J13" s="2">
-        <f>I13*0.9</f>
+        <f t="shared" si="1"/>
         <v>139.62091533864117</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -1396,7 +1379,7 @@
         <v>1949</v>
       </c>
       <c r="C14">
-        <f>B14-B13</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D14">
@@ -1416,11 +1399,11 @@
         <v>58</v>
       </c>
       <c r="I14" s="2">
-        <f>SQRT(G14*H14)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>164.51950239004088</v>
       </c>
       <c r="J14" s="2">
-        <f>I14*0.9</f>
+        <f t="shared" si="1"/>
         <v>148.06755215103681</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -1454,7 +1437,7 @@
         <v>1950</v>
       </c>
       <c r="C15">
-        <f>B15-B14</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D15">
@@ -1474,11 +1457,11 @@
         <v>42</v>
       </c>
       <c r="I15" s="2">
-        <f>SQRT(G15*H15)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>144.91376746189439</v>
       </c>
       <c r="J15" s="2">
-        <f>I15*0.9</f>
+        <f t="shared" si="1"/>
         <v>130.42239071570495</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -1512,7 +1495,7 @@
         <v>1954</v>
       </c>
       <c r="C16">
-        <f>B16-B15</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D16">
@@ -1532,11 +1515,11 @@
         <v>72</v>
       </c>
       <c r="I16" s="2">
-        <f>SQRT(G16*H16)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>178.88543819998318</v>
       </c>
       <c r="J16" s="2">
-        <f>I16*0.9</f>
+        <f t="shared" si="1"/>
         <v>160.99689437998487</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -1561,7 +1544,7 @@
         <v>1958</v>
       </c>
       <c r="C17">
-        <f>B17-B16</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D17">
@@ -1581,11 +1564,11 @@
         <v>34</v>
       </c>
       <c r="I17" s="2">
-        <f>SQRT(G17*H17)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>169.44353369518447</v>
       </c>
       <c r="J17" s="2">
-        <f>I17*0.9</f>
+        <f t="shared" si="1"/>
         <v>152.49918032566603</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -1610,7 +1593,7 @@
         <v>1958</v>
       </c>
       <c r="C18">
-        <f>B18-B17</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D18">
@@ -1630,11 +1613,11 @@
         <v>57</v>
       </c>
       <c r="I18" s="2">
-        <f>SQRT(G18*H18)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>186.63690238892559</v>
       </c>
       <c r="J18" s="2">
-        <f>I18*0.9</f>
+        <f t="shared" si="1"/>
         <v>167.97321215003305</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -1659,7 +1642,7 @@
         <v>1963</v>
       </c>
       <c r="C19">
-        <f>B19-B18</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D19">
@@ -1679,11 +1662,11 @@
         <v>52</v>
       </c>
       <c r="I19" s="2">
-        <f>SQRT(G19*H19)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>178.26322609494585</v>
       </c>
       <c r="J19" s="2">
-        <f>I19*0.9</f>
+        <f t="shared" si="1"/>
         <v>160.43690348545127</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -1712,7 +1695,7 @@
         <v>1972</v>
       </c>
       <c r="C20">
-        <f>B20-B19</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="D20">
@@ -1732,11 +1715,11 @@
         <v>58</v>
       </c>
       <c r="I20" s="2">
-        <f>SQRT(G20*H20)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>183.06040290327977</v>
       </c>
       <c r="J20" s="2">
-        <f>I20*0.9</f>
+        <f t="shared" si="1"/>
         <v>164.75436261295178</v>
       </c>
       <c r="K20" s="2" t="s">
@@ -1765,7 +1748,7 @@
         <v>1977</v>
       </c>
       <c r="C21">
-        <f>B21-B20</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D21">
@@ -1785,11 +1768,11 @@
         <v>71</v>
       </c>
       <c r="I21" s="2">
-        <f>SQRT(G21*H21)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>188.41443681416774</v>
       </c>
       <c r="J21" s="2">
-        <f>I21*0.9</f>
+        <f t="shared" si="1"/>
         <v>169.57299313275098</v>
       </c>
       <c r="K21" s="2" t="s">
@@ -1820,7 +1803,7 @@
         <v>1978</v>
       </c>
       <c r="C22">
-        <f>B22-B21</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D22">
@@ -1840,11 +1823,11 @@
         <v>55</v>
       </c>
       <c r="I22" s="2">
-        <f>SQRT(G22*H22)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>194.65068427541911</v>
       </c>
       <c r="J22" s="2">
-        <f>I22*0.9</f>
+        <f t="shared" si="1"/>
         <v>175.18561584787722</v>
       </c>
       <c r="K22" s="2" t="s">
@@ -1875,7 +1858,7 @@
         <v>1980</v>
       </c>
       <c r="C23">
-        <f>B23-B22</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="D23">
@@ -1895,11 +1878,11 @@
         <v>73</v>
       </c>
       <c r="I23" s="2">
-        <f>SQRT(G23*H23)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>195.2491286080996</v>
       </c>
       <c r="J23" s="2">
-        <f>I23*0.9</f>
+        <f t="shared" si="1"/>
         <v>175.72421574728963</v>
       </c>
       <c r="K23" s="2" t="s">
@@ -1930,7 +1913,7 @@
         <v>1989</v>
       </c>
       <c r="C24">
-        <f>B24-B23</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="D24">
@@ -1950,11 +1933,11 @@
         <v>50</v>
       </c>
       <c r="I24" s="2">
-        <f>SQRT(G24*H24)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>176.38342073763937</v>
       </c>
       <c r="J24" s="2">
-        <f>I24*0.9</f>
+        <f t="shared" si="1"/>
         <v>158.74507866387543</v>
       </c>
       <c r="K24" s="2" t="s">
@@ -1985,7 +1968,7 @@
         <v>1995</v>
       </c>
       <c r="C25">
-        <f>B25-B24</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="D25">
@@ -2005,11 +1988,11 @@
         <v>53</v>
       </c>
       <c r="I25" s="2">
-        <f>SQRT(G25*H25)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>187.97162906495581</v>
       </c>
       <c r="J25" s="2">
-        <f>I25*0.9</f>
+        <f t="shared" si="1"/>
         <v>169.17446615846023</v>
       </c>
       <c r="K25" s="2" t="s">
@@ -2043,7 +2026,7 @@
         <v>1998</v>
       </c>
       <c r="C26">
-        <f>B26-B25</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="D26">
@@ -2063,11 +2046,11 @@
         <v>33</v>
       </c>
       <c r="I26" s="2">
-        <f>SQRT(G26*H26)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>147.08274315273474</v>
       </c>
       <c r="J26" s="2">
-        <f>I26*0.9</f>
+        <f t="shared" si="1"/>
         <v>132.37446883746128</v>
       </c>
       <c r="K26" s="2" t="s">
@@ -2098,7 +2081,7 @@
         <v>2001</v>
       </c>
       <c r="C27">
-        <f>B27-B26</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="D27">
@@ -2118,11 +2101,11 @@
         <v>58</v>
       </c>
       <c r="I27" s="2">
-        <f>SQRT(G27*H27)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>212.39376429431988</v>
       </c>
       <c r="J27" s="2">
-        <f>I27*0.9</f>
+        <f t="shared" si="1"/>
         <v>191.15438786488789</v>
       </c>
       <c r="K27" s="2" t="s">
@@ -2153,7 +2136,7 @@
         <v>2001</v>
       </c>
       <c r="C28">
-        <f>B28-B27</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D28">
@@ -2173,11 +2156,11 @@
         <v>140</v>
       </c>
       <c r="I28" s="2">
-        <f>SQRT(G28*H28)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>292.49881291307071</v>
       </c>
       <c r="J28" s="2">
-        <f>I28*0.9</f>
+        <f t="shared" si="1"/>
         <v>263.24893162176363</v>
       </c>
       <c r="K28" s="2" t="s">
@@ -2208,7 +2191,7 @@
         <v>2005</v>
       </c>
       <c r="C29">
-        <f>B29-B28</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D29">
@@ -2228,11 +2211,11 @@
         <v>90</v>
       </c>
       <c r="I29" s="2">
-        <f>SQRT(G29*H29)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>244.94897427831785</v>
       </c>
       <c r="J29" s="2">
-        <f>I29*0.9</f>
+        <f t="shared" si="1"/>
         <v>220.45407685048608</v>
       </c>
       <c r="K29" s="2" t="s">
@@ -2263,7 +2246,7 @@
         <v>2012</v>
       </c>
       <c r="C30">
-        <f>B30-B29</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="D30">
@@ -2283,11 +2266,11 @@
         <v>87</v>
       </c>
       <c r="I30" s="2">
-        <f>SQRT(G30*H30)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>219.84843263788198</v>
       </c>
       <c r="J30" s="2">
-        <f>I30*0.9</f>
+        <f t="shared" si="1"/>
         <v>197.86358937409378</v>
       </c>
       <c r="K30" s="2" t="s">
@@ -2312,7 +2295,7 @@
         <v>2012</v>
       </c>
       <c r="C31">
-        <f>B31-B30</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D31">
@@ -2332,11 +2315,11 @@
         <v>35</v>
       </c>
       <c r="I31" s="2">
-        <f>SQRT(G31*H31)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>152.75252316519467</v>
       </c>
       <c r="J31" s="2">
-        <f>I31*0.9</f>
+        <f t="shared" si="1"/>
         <v>137.4772708486752</v>
       </c>
       <c r="K31" s="2" t="s">
@@ -2367,7 +2350,7 @@
         <v>1800</v>
       </c>
       <c r="C32">
-        <f>B32-B31</f>
+        <f t="shared" si="2"/>
         <v>-212</v>
       </c>
       <c r="D32">
@@ -2387,11 +2370,11 @@
         <v>12</v>
       </c>
       <c r="I32" s="2">
-        <f>SQRT(G32*H32)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>46.188021535170058</v>
       </c>
       <c r="J32" s="2">
-        <f>I32*0.9</f>
+        <f t="shared" si="1"/>
         <v>41.569219381653056</v>
       </c>
       <c r="K32" s="2" t="s">
@@ -2416,7 +2399,7 @@
         <v>1897</v>
       </c>
       <c r="C33">
-        <f>B33-B32</f>
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
       <c r="D33">
@@ -2436,11 +2419,11 @@
         <v>14</v>
       </c>
       <c r="I33" s="2">
-        <f>SQRT(G33*H33)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>52.915026221291818</v>
       </c>
       <c r="J33" s="2">
-        <f>I33*0.9</f>
+        <f t="shared" si="1"/>
         <v>47.623523599162638</v>
       </c>
       <c r="K33" s="2" t="s">
@@ -2465,7 +2448,7 @@
         <v>1902</v>
       </c>
       <c r="C34">
-        <f>B34-B33</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D34">
@@ -2485,11 +2468,11 @@
         <v>16</v>
       </c>
       <c r="I34" s="2">
-        <f>SQRT(G34*H34)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>56.568542494923797</v>
       </c>
       <c r="J34" s="2">
-        <f>I34*0.9</f>
+        <f t="shared" si="1"/>
         <v>50.911688245431421</v>
       </c>
       <c r="K34" s="2" t="s">
@@ -2514,7 +2497,7 @@
         <v>1907</v>
       </c>
       <c r="C35">
-        <f>B35-B34</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D35">
@@ -2534,11 +2517,11 @@
         <v>18</v>
       </c>
       <c r="I35" s="2">
-        <f>SQRT(G35*H35)/$B$1</f>
+        <f t="shared" si="0"/>
         <v>63.245553203367592</v>
       </c>
       <c r="J35" s="2">
-        <f>I35*0.9</f>
+        <f t="shared" si="1"/>
         <v>56.920997883030836</v>
       </c>
       <c r="K35" s="2" t="s">
@@ -2563,7 +2546,7 @@
         <v>1913</v>
       </c>
       <c r="C36">
-        <f>B36-B35</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="D36">
@@ -2583,11 +2566,11 @@
         <v>18</v>
       </c>
       <c r="I36" s="2">
-        <f>SQRT(G36*H36)/$B$1</f>
+        <f t="shared" ref="I36:I67" si="3">SQRT(G36*H36)/$B$1</f>
         <v>66.332495807108003</v>
       </c>
       <c r="J36" s="2">
-        <f>I36*0.9</f>
+        <f t="shared" ref="J36:J67" si="4">I36*0.9</f>
         <v>59.699246226397207</v>
       </c>
       <c r="K36" s="2" t="s">
@@ -2612,7 +2595,7 @@
         <v>1920</v>
       </c>
       <c r="C37">
-        <f>B37-B36</f>
+        <f t="shared" ref="C37:C68" si="5">B37-B36</f>
         <v>7</v>
       </c>
       <c r="D37">
@@ -2632,11 +2615,11 @@
         <v>28</v>
       </c>
       <c r="I37" s="2">
-        <f>SQRT(G37*H37)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>74.833147735478832</v>
       </c>
       <c r="J37" s="2">
-        <f>I37*0.9</f>
+        <f t="shared" si="4"/>
         <v>67.349832961930957</v>
       </c>
       <c r="K37" s="2" t="s">
@@ -2667,7 +2650,7 @@
         <v>1928</v>
       </c>
       <c r="C38">
-        <f>B38-B37</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="D38">
@@ -2687,11 +2670,11 @@
         <v>15</v>
       </c>
       <c r="I38" s="2">
-        <f>SQRT(G38*H38)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>78.528126595931653</v>
       </c>
       <c r="J38" s="2">
-        <f>I38*0.9</f>
+        <f t="shared" si="4"/>
         <v>70.675313936338483</v>
       </c>
       <c r="K38" s="2" t="s">
@@ -2716,7 +2699,7 @@
         <v>1935</v>
       </c>
       <c r="C39">
-        <f>B39-B38</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="D39">
@@ -2736,11 +2719,11 @@
         <v>24</v>
       </c>
       <c r="I39" s="2">
-        <f>SQRT(G39*H39)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>96.609178307929596</v>
       </c>
       <c r="J39" s="2">
-        <f>I39*0.9</f>
+        <f t="shared" si="4"/>
         <v>86.948260477136643</v>
       </c>
       <c r="K39" s="2" t="s">
@@ -2765,7 +2748,7 @@
         <v>1936</v>
       </c>
       <c r="C40">
-        <f>B40-B39</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D40">
@@ -2785,11 +2768,11 @@
         <v>20</v>
       </c>
       <c r="I40" s="2">
-        <f>SQRT(G40*H40)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>81.649658092772611</v>
       </c>
       <c r="J40" s="2">
-        <f>I40*0.9</f>
+        <f t="shared" si="4"/>
         <v>73.484692283495349</v>
       </c>
       <c r="K40" s="2" t="s">
@@ -2814,7 +2797,7 @@
         <v>1948</v>
       </c>
       <c r="C41">
-        <f>B41-B40</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="D41">
@@ -2834,11 +2817,11 @@
         <v>6</v>
       </c>
       <c r="I41" s="2">
-        <f>SQRT(G41*H41)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>53.541261347363367</v>
       </c>
       <c r="J41" s="2">
-        <f>I41*0.9</f>
+        <f t="shared" si="4"/>
         <v>48.187135212627034</v>
       </c>
       <c r="K41" s="2" t="s">
@@ -2861,7 +2844,7 @@
         <v>1952</v>
       </c>
       <c r="C42">
-        <f>B42-B41</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="D42">
@@ -2881,11 +2864,11 @@
         <v>25</v>
       </c>
       <c r="I42" s="2">
-        <f>SQRT(G42*H42)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>102.74023338281629</v>
       </c>
       <c r="J42" s="2">
-        <f>I42*0.9</f>
+        <f t="shared" si="4"/>
         <v>92.466210044534662</v>
       </c>
       <c r="K42" s="2" t="s">
@@ -2910,7 +2893,7 @@
         <v>1957</v>
       </c>
       <c r="C43">
-        <f>B43-B42</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="D43">
@@ -2930,11 +2913,11 @@
         <v>21</v>
       </c>
       <c r="I43" s="2">
-        <f>SQRT(G43*H43)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>101.32456102380443</v>
       </c>
       <c r="J43" s="2">
-        <f>I43*0.9</f>
+        <f t="shared" si="4"/>
         <v>91.19210492142399</v>
       </c>
       <c r="K43" s="2" t="s">
@@ -2959,7 +2942,7 @@
         <v>1959</v>
       </c>
       <c r="C44">
-        <f>B44-B43</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="D44">
@@ -2979,11 +2962,11 @@
         <v>16</v>
       </c>
       <c r="I44" s="2">
-        <f>SQRT(G44*H44)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>101.54364141151879</v>
       </c>
       <c r="J44" s="2">
-        <f>I44*0.9</f>
+        <f t="shared" si="4"/>
         <v>91.389277270366918</v>
       </c>
       <c r="K44" s="2" t="s">
@@ -3017,7 +3000,7 @@
         <v>1963</v>
       </c>
       <c r="C45">
-        <f>B45-B44</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="D45">
@@ -3037,11 +3020,11 @@
         <v>24</v>
       </c>
       <c r="I45" s="2">
-        <f>SQRT(G45*H45)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>113.13708498984759</v>
       </c>
       <c r="J45" s="2">
-        <f>I45*0.9</f>
+        <f t="shared" si="4"/>
         <v>101.82337649086284</v>
       </c>
       <c r="K45" s="2" t="s">
@@ -3066,7 +3049,7 @@
         <v>1964</v>
       </c>
       <c r="C46">
-        <f>B46-B45</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D46">
@@ -3086,11 +3069,11 @@
         <v>36</v>
       </c>
       <c r="I46" s="2">
-        <f>SQRT(G46*H46)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>146.9693845669907</v>
       </c>
       <c r="J46" s="2">
-        <f>I46*0.9</f>
+        <f t="shared" si="4"/>
         <v>132.27244611029164</v>
       </c>
       <c r="K46" s="2" t="s">
@@ -3115,7 +3098,7 @@
         <v>1964</v>
       </c>
       <c r="C47">
-        <f>B47-B46</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D47">
@@ -3135,11 +3118,11 @@
         <v>22</v>
       </c>
       <c r="I47" s="2">
-        <f>SQRT(G47*H47)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>114.89125293076057</v>
       </c>
       <c r="J47" s="2">
-        <f>I47*0.9</f>
+        <f t="shared" si="4"/>
         <v>103.40212763768452</v>
       </c>
       <c r="K47" s="2" t="s">
@@ -3167,7 +3150,7 @@
         <v>1965</v>
       </c>
       <c r="C48">
-        <f>B48-B47</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D48">
@@ -3187,11 +3170,11 @@
         <v>36</v>
       </c>
       <c r="I48" s="2">
-        <f>SQRT(G48*H48)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>150.99668870541501</v>
       </c>
       <c r="J48" s="2">
-        <f>I48*0.9</f>
+        <f t="shared" si="4"/>
         <v>135.8970198348735</v>
       </c>
       <c r="K48" s="2" t="s">
@@ -3216,7 +3199,7 @@
         <v>1965</v>
       </c>
       <c r="C49">
-        <f>B49-B48</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D49">
@@ -3236,11 +3219,11 @@
         <v>16</v>
       </c>
       <c r="I49" s="2">
-        <f>SQRT(G49*H49)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>103.27955589886446</v>
       </c>
       <c r="J49" s="2">
-        <f>I49*0.9</f>
+        <f t="shared" si="4"/>
         <v>92.951600308978016</v>
       </c>
       <c r="K49" s="2" t="s">
@@ -3274,7 +3257,7 @@
         <v>1967</v>
       </c>
       <c r="C50">
-        <f>B50-B49</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="D50">
@@ -3294,11 +3277,11 @@
         <v>22</v>
       </c>
       <c r="I50" s="2">
-        <f>SQRT(G50*H50)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>116.99952516522831</v>
       </c>
       <c r="J50" s="2">
-        <f>I50*0.9</f>
+        <f t="shared" si="4"/>
         <v>105.29957264870548</v>
       </c>
       <c r="K50" s="2" t="s">
@@ -3332,7 +3315,7 @@
         <v>1968</v>
       </c>
       <c r="C51">
-        <f>B51-B50</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D51">
@@ -3352,11 +3335,11 @@
         <v>36</v>
       </c>
       <c r="I51" s="2">
-        <f>SQRT(G51*H51)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>164.92422502470643</v>
       </c>
       <c r="J51" s="2">
-        <f>I51*0.9</f>
+        <f t="shared" si="4"/>
         <v>148.43180252223578</v>
       </c>
       <c r="K51" s="2" t="s">
@@ -3381,7 +3364,7 @@
         <v>1977</v>
       </c>
       <c r="C52">
-        <f>B52-B51</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="D52">
@@ -3401,11 +3384,11 @@
         <v>40</v>
       </c>
       <c r="I52" s="2">
-        <f>SQRT(G52*H52)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>163.29931618554522</v>
       </c>
       <c r="J52" s="2">
-        <f>I52*0.9</f>
+        <f t="shared" si="4"/>
         <v>146.9693845669907</v>
       </c>
       <c r="K52" s="2" t="s">
@@ -3433,7 +3416,7 @@
         <v>1980</v>
       </c>
       <c r="C53">
-        <f>B53-B52</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="D53">
@@ -3453,11 +3436,11 @@
         <v>42</v>
       </c>
       <c r="I53" s="2">
-        <f>SQRT(G53*H53)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>170.09801096230765</v>
       </c>
       <c r="J53" s="2">
-        <f>I53*0.9</f>
+        <f t="shared" si="4"/>
         <v>153.08820986607688</v>
       </c>
       <c r="K53" s="2" t="s">
@@ -3482,7 +3465,7 @@
         <v>1981</v>
       </c>
       <c r="C54">
-        <f>B54-B53</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D54">
@@ -3502,11 +3485,11 @@
         <v>18</v>
       </c>
       <c r="I54" s="2">
-        <f>SQRT(G54*H54)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>116.61903789690601</v>
       </c>
       <c r="J54" s="2">
-        <f>I54*0.9</f>
+        <f t="shared" si="4"/>
         <v>104.95713410721541</v>
       </c>
       <c r="K54" s="2" t="s">
@@ -3540,7 +3523,7 @@
         <v>1982</v>
       </c>
       <c r="C55">
-        <f>B55-B54</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D55">
@@ -3560,11 +3543,11 @@
         <v>28</v>
       </c>
       <c r="I55" s="2">
-        <f>SQRT(G55*H55)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>136.62601021279465</v>
       </c>
       <c r="J55" s="2">
-        <f>I55*0.9</f>
+        <f t="shared" si="4"/>
         <v>122.9634091915152</v>
       </c>
       <c r="K55" s="2" t="s">
@@ -3589,7 +3572,7 @@
         <v>1983</v>
       </c>
       <c r="C56">
-        <f>B56-B55</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D56">
@@ -3609,11 +3592,11 @@
         <v>22</v>
       </c>
       <c r="I56" s="2">
-        <f>SQRT(G56*H56)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>125.07775359529147</v>
       </c>
       <c r="J56" s="2">
-        <f>I56*0.9</f>
+        <f t="shared" si="4"/>
         <v>112.56997823576232</v>
       </c>
       <c r="K56" s="2" t="s">
@@ -3647,7 +3630,7 @@
         <v>1986</v>
       </c>
       <c r="C57">
-        <f>B57-B56</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="D57">
@@ -3667,11 +3650,11 @@
         <v>30</v>
       </c>
       <c r="I57" s="2">
-        <f>SQRT(G57*H57)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>143.75905768565215</v>
       </c>
       <c r="J57" s="2">
-        <f>I57*0.9</f>
+        <f t="shared" si="4"/>
         <v>129.38315191708693</v>
       </c>
       <c r="K57" s="2" t="s">
@@ -3696,7 +3679,7 @@
         <v>1987</v>
       </c>
       <c r="C58">
-        <f>B58-B57</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D58">
@@ -3716,11 +3699,11 @@
         <v>44</v>
       </c>
       <c r="I58" s="2">
-        <f>SQRT(G58*H58)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>178.26322609494585</v>
       </c>
       <c r="J58" s="2">
-        <f>I58*0.9</f>
+        <f t="shared" si="4"/>
         <v>160.43690348545127</v>
       </c>
       <c r="K58" s="2" t="s">
@@ -3745,7 +3728,7 @@
         <v>1993</v>
       </c>
       <c r="C59">
-        <f>B59-B58</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="D59">
@@ -3765,11 +3748,11 @@
         <v>18</v>
       </c>
       <c r="I59" s="2">
-        <f>SQRT(G59*H59)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="J59" s="2">
-        <f>I59*0.9</f>
+        <f t="shared" si="4"/>
         <v>108</v>
       </c>
       <c r="K59" s="2" t="s">
@@ -3803,7 +3786,7 @@
         <v>1995</v>
       </c>
       <c r="C60">
-        <f>B60-B59</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="D60">
@@ -3823,11 +3806,11 @@
         <v>48</v>
       </c>
       <c r="I60" s="2">
-        <f>SQRT(G60*H60)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>190.43809142780935</v>
       </c>
       <c r="J60" s="2">
-        <f>I60*0.9</f>
+        <f t="shared" si="4"/>
         <v>171.39428228502842</v>
       </c>
       <c r="K60" s="2" t="s">
@@ -3852,7 +3835,7 @@
         <v>1997</v>
       </c>
       <c r="C61">
-        <f>B61-B60</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="D61">
@@ -3872,11 +3855,11 @@
         <v>32</v>
       </c>
       <c r="I61" s="2">
-        <f>SQRT(G61*H61)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>157.76212754932311</v>
       </c>
       <c r="J61" s="2">
-        <f>I61*0.9</f>
+        <f t="shared" si="4"/>
         <v>141.98591479439079</v>
       </c>
       <c r="K61" s="2" t="s">
@@ -3901,7 +3884,7 @@
         <v>2001</v>
       </c>
       <c r="C62">
-        <f>B62-B61</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="D62">
@@ -3921,11 +3904,11 @@
         <v>50</v>
       </c>
       <c r="I62" s="2">
-        <f>SQRT(G62*H62)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>197.20265943665387</v>
       </c>
       <c r="J62" s="2">
-        <f>I62*0.9</f>
+        <f t="shared" si="4"/>
         <v>177.48239349298848</v>
       </c>
       <c r="K62" s="2" t="s">
@@ -3950,7 +3933,7 @@
         <v>2001</v>
       </c>
       <c r="C63">
-        <f>B63-B62</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D63">
@@ -3970,11 +3953,11 @@
         <v>24</v>
       </c>
       <c r="I63" s="2">
-        <f>SQRT(G63*H63)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>141.42135623730951</v>
       </c>
       <c r="J63" s="2">
-        <f>I63*0.9</f>
+        <f t="shared" si="4"/>
         <v>127.27922061357856</v>
       </c>
       <c r="K63" s="2" t="s">
@@ -4008,7 +3991,7 @@
         <v>2004</v>
       </c>
       <c r="C64">
-        <f>B64-B63</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="D64">
@@ -4028,11 +4011,11 @@
         <v>54</v>
       </c>
       <c r="I64" s="2">
-        <f>SQRT(G64*H64)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>207.84609690826528</v>
       </c>
       <c r="J64" s="2">
-        <f>I64*0.9</f>
+        <f t="shared" si="4"/>
         <v>187.06148721743875</v>
       </c>
       <c r="K64" s="2" t="s">
@@ -4057,7 +4040,7 @@
         <v>2005</v>
       </c>
       <c r="C65">
-        <f>B65-B64</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D65">
@@ -4077,11 +4060,11 @@
         <v>18</v>
       </c>
       <c r="I65" s="2">
-        <f>SQRT(G65*H65)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>126.49110640673518</v>
       </c>
       <c r="J65" s="2">
-        <f>I65*0.9</f>
+        <f t="shared" si="4"/>
         <v>113.84199576606167</v>
       </c>
       <c r="K65" s="2" t="s">
@@ -4115,7 +4098,7 @@
         <v>1912</v>
       </c>
       <c r="C66">
-        <f>B66-B65</f>
+        <f t="shared" si="5"/>
         <v>-93</v>
       </c>
       <c r="D66">
@@ -4135,11 +4118,11 @@
         <v>4</v>
       </c>
       <c r="I66" s="2">
-        <f>SQRT(G66*H66)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>42.163702135578397</v>
       </c>
       <c r="J66" s="2">
-        <f>I66*0.9</f>
+        <f t="shared" si="4"/>
         <v>37.94733192202056</v>
       </c>
       <c r="K66" s="2" t="s">
@@ -4164,7 +4147,7 @@
         <v>1938</v>
       </c>
       <c r="C67">
-        <f>B67-B66</f>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="D67">
@@ -4184,11 +4167,11 @@
         <v>5</v>
       </c>
       <c r="I67" s="2">
-        <f>SQRT(G67*H67)/$B$1</f>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="J67" s="2">
-        <f>I67*0.9</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="K67" s="2" t="s">
@@ -4213,7 +4196,7 @@
         <v>1957</v>
       </c>
       <c r="C68">
-        <f>B68-B67</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="D68">
@@ -4233,11 +4216,11 @@
         <v>6</v>
       </c>
       <c r="I68" s="2">
-        <f>SQRT(G68*H68)/$B$1</f>
+        <f t="shared" ref="I68:I82" si="6">SQRT(G68*H68)/$B$1</f>
         <v>63.245553203367592</v>
       </c>
       <c r="J68" s="2">
-        <f>I68*0.9</f>
+        <f t="shared" ref="J68:J82" si="7">I68*0.9</f>
         <v>56.920997883030836</v>
       </c>
       <c r="K68" s="2" t="s">
@@ -4262,7 +4245,7 @@
         <v>1960</v>
       </c>
       <c r="C69">
-        <f>B69-B68</f>
+        <f t="shared" ref="C69:C82" si="8">B69-B68</f>
         <v>3</v>
       </c>
       <c r="D69">
@@ -4282,11 +4265,11 @@
         <v>8</v>
       </c>
       <c r="I69" s="2">
-        <f>SQRT(G69*H69)/$B$1</f>
+        <f t="shared" si="6"/>
         <v>73.029674334022147</v>
       </c>
       <c r="J69" s="2">
-        <f>I69*0.9</f>
+        <f t="shared" si="7"/>
         <v>65.726706900619931</v>
       </c>
       <c r="K69" s="2" t="s">
@@ -4311,7 +4294,7 @@
         <v>1965</v>
       </c>
       <c r="C70">
-        <f>B70-B69</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="D70">
@@ -4331,11 +4314,11 @@
         <v>8</v>
       </c>
       <c r="I70" s="2">
-        <f>SQRT(G70*H70)/$B$1</f>
+        <f t="shared" si="6"/>
         <v>76.011695006609202</v>
       </c>
       <c r="J70" s="2">
-        <f>I70*0.9</f>
+        <f t="shared" si="7"/>
         <v>68.410525505948286</v>
       </c>
       <c r="K70" s="2" t="s">
@@ -4360,7 +4343,7 @@
         <v>1986</v>
       </c>
       <c r="C71">
-        <f>B71-B70</f>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="D71">
@@ -4380,11 +4363,11 @@
         <v>10</v>
       </c>
       <c r="I71" s="2">
-        <f>SQRT(G71*H71)/$B$1</f>
+        <f t="shared" si="6"/>
         <v>94.28090415820634</v>
       </c>
       <c r="J71" s="2">
-        <f>I71*0.9</f>
+        <f t="shared" si="7"/>
         <v>84.852813742385706</v>
       </c>
       <c r="K71" s="2" t="s">
@@ -4409,7 +4392,7 @@
         <v>1986</v>
       </c>
       <c r="C72">
-        <f>B72-B71</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D72">
@@ -4429,11 +4412,11 @@
         <v>4</v>
       </c>
       <c r="I72" s="2">
-        <f>SQRT(G72*H72)/$B$1</f>
+        <f t="shared" si="6"/>
         <v>53.748384988656994</v>
       </c>
       <c r="J72" s="2">
-        <f>I72*0.9</f>
+        <f t="shared" si="7"/>
         <v>48.373546489791295</v>
       </c>
       <c r="K72" s="2" t="s">
@@ -4458,7 +4441,7 @@
         <v>2006</v>
       </c>
       <c r="C73">
-        <f>B73-B72</f>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="D73">
@@ -4478,11 +4461,11 @@
         <v>12</v>
       </c>
       <c r="I73" s="2">
-        <f>SQRT(G73*H73)/$B$1</f>
+        <f t="shared" si="6"/>
         <v>106.45812948447541</v>
       </c>
       <c r="J73" s="2">
-        <f>I73*0.9</f>
+        <f t="shared" si="7"/>
         <v>95.812316536027865</v>
       </c>
       <c r="K73" s="2" t="s">
@@ -4507,7 +4490,7 @@
         <v>2012</v>
       </c>
       <c r="C74">
-        <f>B74-B73</f>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="D74">
@@ -4527,11 +4510,11 @@
         <v>10</v>
       </c>
       <c r="I74" s="2">
-        <f>SQRT(G74*H74)/$B$1</f>
+        <f t="shared" si="6"/>
         <v>101.10500592068735</v>
       </c>
       <c r="J74" s="2">
-        <f>I74*0.9</f>
+        <f t="shared" si="7"/>
         <v>90.994505328618615</v>
       </c>
       <c r="K74" s="2" t="s">
@@ -4556,7 +4539,7 @@
         <v>1958</v>
       </c>
       <c r="C75">
-        <f>B75-B74</f>
+        <f t="shared" si="8"/>
         <v>-54</v>
       </c>
       <c r="D75">
@@ -4576,11 +4559,11 @@
         <v>4</v>
       </c>
       <c r="I75" s="2">
-        <f>SQRT(G75*H75)/$B$1</f>
+        <f t="shared" si="6"/>
         <v>57.735026918962582</v>
       </c>
       <c r="J75" s="2">
-        <f>I75*0.9</f>
+        <f t="shared" si="7"/>
         <v>51.961524227066327</v>
       </c>
       <c r="K75" s="2" t="s">
@@ -4628,11 +4611,11 @@
         <v>8</v>
       </c>
       <c r="I76" s="2">
-        <f>SQRT(G76*H76)/$B$1</f>
+        <f t="shared" si="6"/>
         <v>74.833147735478832</v>
       </c>
       <c r="J76" s="2">
-        <f>I76*0.9</f>
+        <f t="shared" si="7"/>
         <v>67.349832961930957</v>
       </c>
       <c r="K76" s="2" t="s">
@@ -4655,7 +4638,7 @@
         <v>1976</v>
       </c>
       <c r="C77">
-        <f>B77-B76</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="D77">
@@ -4675,11 +4658,11 @@
         <v>4</v>
       </c>
       <c r="I77" s="2">
-        <f>SQRT(G77*H77)/$B$1</f>
+        <f t="shared" si="6"/>
         <v>63.245553203367592</v>
       </c>
       <c r="J77" s="2">
-        <f>I77*0.9</f>
+        <f t="shared" si="7"/>
         <v>56.920997883030836</v>
       </c>
       <c r="K77" s="2" t="s">
@@ -4704,14 +4687,14 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="B78">
-        <v>1994</v>
+        <v>1986</v>
       </c>
       <c r="C78">
-        <f>B78-B77</f>
-        <v>18</v>
+        <f t="shared" si="8"/>
+        <v>10</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -4721,52 +4704,44 @@
       </c>
       <c r="F78">
         <f>IF(B78 &gt; 1900, ((B78-1900)*10)+400+D78, ((B78-1730)*2)+D78)+VLOOKUP(E78,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10941</v>
+        <v>10861</v>
       </c>
       <c r="G78">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="H78">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I78" s="2">
-        <f>SQRT(G78*H78)/$B$1</f>
-        <v>73.029674334022147</v>
+        <f t="shared" ref="I78" si="9">SQRT(G78*H78)/$B$1</f>
+        <v>89.442719099991592</v>
       </c>
       <c r="J78" s="2">
-        <f>I78*0.9</f>
-        <v>65.726706900619931</v>
+        <f t="shared" si="7"/>
+        <v>80.498447189992433</v>
       </c>
       <c r="K78" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L78" s="3">
-        <v>5</v>
-      </c>
-      <c r="M78" s="3">
-        <v>2</v>
-      </c>
-      <c r="N78" s="3">
-        <v>1.5</v>
-      </c>
+      <c r="N78" s="3"/>
       <c r="O78" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L78*VLOOKUP(E78,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M78*VLOOKUP(E78,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N78*VLOOKUP(E78,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>23x14x7</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B79">
-        <v>1997</v>
+        <v>1994</v>
       </c>
       <c r="C79">
-        <f>B79-B78</f>
-        <v>3</v>
+        <f t="shared" si="8"/>
+        <v>8</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -4776,49 +4751,52 @@
       </c>
       <c r="F79">
         <f>IF(B79 &gt; 1900, ((B79-1900)*10)+400+D79, ((B79-1730)*2)+D79)+VLOOKUP(E79,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10971</v>
+        <v>10941</v>
       </c>
       <c r="G79">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="H79">
+        <v>4</v>
+      </c>
+      <c r="I79" s="2">
+        <f t="shared" si="6"/>
+        <v>73.029674334022147</v>
+      </c>
+      <c r="J79" s="2">
+        <f t="shared" si="7"/>
+        <v>65.726706900619931</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L79" s="3">
         <v>5</v>
       </c>
-      <c r="I79" s="2">
-        <f>SQRT(G79*H79)/$B$1</f>
-        <v>67.082039324993701</v>
-      </c>
-      <c r="J79" s="2">
-        <f>I79*0.9</f>
-        <v>60.373835392494335</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L79" s="3"/>
-      <c r="M79" s="3"/>
-      <c r="N79" s="3"/>
+      <c r="M79" s="3">
+        <v>2</v>
+      </c>
+      <c r="N79" s="3">
+        <v>1.5</v>
+      </c>
       <c r="O79" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L79*VLOOKUP(E79,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M79*VLOOKUP(E79,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N79*VLOOKUP(E79,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
-      </c>
-      <c r="P79" t="s">
-        <v>70</v>
+        <v>23x14x7</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B80">
-        <v>2004</v>
+        <v>1997</v>
       </c>
       <c r="C80">
-        <f>B80-B79</f>
-        <v>7</v>
+        <f t="shared" si="8"/>
+        <v>3</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -4828,21 +4806,21 @@
       </c>
       <c r="F80">
         <f>IF(B80 &gt; 1900, ((B80-1900)*10)+400+D80, ((B80-1730)*2)+D80)+VLOOKUP(E80,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>11041</v>
+        <v>10971</v>
       </c>
       <c r="G80">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="H80">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I80" s="2">
-        <f>SQRT(G80*H80)/$B$1</f>
-        <v>80.277297191948648</v>
+        <f t="shared" si="6"/>
+        <v>67.082039324993701</v>
       </c>
       <c r="J80" s="2">
-        <f>I80*0.9</f>
-        <v>72.249567472753782</v>
+        <f t="shared" si="7"/>
+        <v>60.373835392494335</v>
       </c>
       <c r="K80" s="2" t="s">
         <v>33</v>
@@ -4857,17 +4835,20 @@
 ROUND(N80*VLOOKUP(E80,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
+      <c r="P80" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B81">
-        <v>2009</v>
+        <v>2004</v>
       </c>
       <c r="C81">
-        <f>B81-B80</f>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -4877,21 +4858,21 @@
       </c>
       <c r="F81">
         <f>IF(B81 &gt; 1900, ((B81-1900)*10)+400+D81, ((B81-1730)*2)+D81)+VLOOKUP(E81,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>11091</v>
+        <v>11041</v>
       </c>
       <c r="G81">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="H81">
         <v>4</v>
       </c>
       <c r="I81" s="2">
-        <f>SQRT(G81*H81)/$B$1</f>
-        <v>70.553368295055762</v>
+        <f t="shared" si="6"/>
+        <v>80.277297191948648</v>
       </c>
       <c r="J81" s="2">
-        <f>I81*0.9</f>
-        <v>63.498031465550184</v>
+        <f t="shared" si="7"/>
+        <v>72.249567472753782</v>
       </c>
       <c r="K81" s="2" t="s">
         <v>33</v>
@@ -4907,27 +4888,76 @@
         <v>0x0x0</v>
       </c>
     </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B82">
+        <v>2009</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
+        <v>62</v>
+      </c>
+      <c r="F82">
+        <f>IF(B82 &gt; 1900, ((B82-1900)*10)+400+D82, ((B82-1730)*2)+D82)+VLOOKUP(E82,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>11091</v>
+      </c>
+      <c r="G82">
+        <v>112</v>
+      </c>
+      <c r="H82">
+        <v>4</v>
+      </c>
+      <c r="I82" s="2">
+        <f t="shared" si="6"/>
+        <v>70.553368295055762</v>
+      </c>
+      <c r="J82" s="2">
+        <f t="shared" si="7"/>
+        <v>63.498031465550184</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L82" s="3"/>
+      <c r="M82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L82*VLOOKUP(E82,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M82*VLOOKUP(E82,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N82*VLOOKUP(E82,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A4:P81">
+  <sortState ref="A4:P82">
     <sortCondition ref="F20"/>
   </sortState>
-  <conditionalFormatting sqref="C1:C2 C4:C20 C22:C24 C53:C1048576 C26:C51">
+  <conditionalFormatting sqref="C1:C2 C4:C20 C22:C24 C26:C51 C53:C1048576">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+  <conditionalFormatting sqref="C52">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
+  <conditionalFormatting sqref="C25">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Clean up all sprites and add Renault Trafic minibus
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126EDAC7-D8C5-4E93-85BE-34DAF4BC13CD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D364D0E7-0505-4349-8631-60C28BC25939}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8190" windowHeight="2400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="120">
   <si>
     <t>Vehicle</t>
   </si>
@@ -383,6 +383,9 @@
   </si>
   <si>
     <t>Ford Transit Mk3 Minibus</t>
+  </si>
+  <si>
+    <t>Renault Trafic Minibus</t>
   </si>
 </sst>
 </file>
@@ -799,11 +802,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H78" sqref="H78"/>
+      <selection pane="bottomLeft" activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4216,7 +4219,7 @@
         <v>6</v>
       </c>
       <c r="I68" s="2">
-        <f t="shared" ref="I68:I82" si="6">SQRT(G68*H68)/$B$1</f>
+        <f t="shared" ref="I68:I83" si="6">SQRT(G68*H68)/$B$1</f>
         <v>63.245553203367592</v>
       </c>
       <c r="J68" s="2">
@@ -4937,27 +4940,79 @@
         <v>0x0x0</v>
       </c>
     </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>119</v>
+      </c>
+      <c r="B83">
+        <v>2014</v>
+      </c>
+      <c r="C83">
+        <f t="shared" ref="C83" si="10">B83-B82</f>
+        <v>5</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>62</v>
+      </c>
+      <c r="F83">
+        <f>IF(B83 &gt; 1900, ((B83-1900)*10)+400+D83, ((B83-1730)*2)+D83)+VLOOKUP(E83,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>11141</v>
+      </c>
+      <c r="G83">
+        <v>95</v>
+      </c>
+      <c r="H83">
+        <v>9</v>
+      </c>
+      <c r="I83" s="2">
+        <f t="shared" si="6"/>
+        <v>97.467943448089642</v>
+      </c>
+      <c r="J83" s="2">
+        <f t="shared" ref="J83" si="11">I83*0.9</f>
+        <v>87.72114910328068</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N83" s="3"/>
+      <c r="O83" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L83*VLOOKUP(E83,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M83*VLOOKUP(E83,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N83*VLOOKUP(E83,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A4:P82">
     <sortCondition ref="F20"/>
   </sortState>
-  <conditionalFormatting sqref="C1:C2 C4:C20 C22:C24 C26:C51 C53:C1048576">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="C1:C2 C4:C20 C22:C24 C26:C51 C53:C82 C84:C1048576">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C83">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
New vehicles, directory structure improvements and new alignment templates
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D364D0E7-0505-4349-8631-60C28BC25939}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC25AD52-DCE2-4F59-92C7-9B7514F43D60}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8190" windowHeight="2400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8190" windowHeight="2400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="124">
   <si>
     <t>Vehicle</t>
   </si>
@@ -386,6 +386,18 @@
   </si>
   <si>
     <t>Renault Trafic Minibus</t>
+  </si>
+  <si>
+    <t>Dennis Ace</t>
+  </si>
+  <si>
+    <t>Volvo FM9</t>
+  </si>
+  <si>
+    <t>380hp</t>
+  </si>
+  <si>
+    <t>Tram</t>
   </si>
 </sst>
 </file>
@@ -441,7 +453,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -802,11 +824,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G83" sqref="G83"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,69 +1294,61 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B12">
-        <v>1937</v>
+        <v>1933</v>
       </c>
       <c r="C12">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
       </c>
       <c r="F12">
         <f>IF(B12 &gt; 1900, ((B12-1900)*10)+400+D12, ((B12-1730)*2)+D12)+VLOOKUP(E12,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1371</v>
+        <v>1332</v>
       </c>
       <c r="G12">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H12">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="0"/>
-        <v>136.30032200173915</v>
+        <v>103.27955589886446</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="1"/>
-        <v>122.67028980156523</v>
+        <v>92.951600308978016</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="3">
-        <v>8.4</v>
-      </c>
-      <c r="M12" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="N12" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="N12" s="3"/>
       <c r="O12" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L12*VLOOKUP(E12,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M12*VLOOKUP(E12,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N12*VLOOKUP(E12,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>39x17x13</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="B13">
-        <v>1945</v>
+        <v>1937</v>
       </c>
       <c r="C13">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1344,46 +1358,52 @@
       </c>
       <c r="F13">
         <f>IF(B13 &gt; 1900, ((B13-1900)*10)+400+D13, ((B13-1730)*2)+D13)+VLOOKUP(E13,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1451</v>
+        <v>1371</v>
       </c>
       <c r="G13">
+        <v>44</v>
+      </c>
+      <c r="H13">
         <v>38</v>
-      </c>
-      <c r="H13">
-        <v>57</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="0"/>
-        <v>155.13435037626795</v>
+        <v>136.30032200173915</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="1"/>
-        <v>139.62091533864117</v>
+        <v>122.67028980156523</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
+      <c r="L13" s="3">
+        <v>8.4</v>
+      </c>
+      <c r="M13" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="N13" s="3">
+        <v>2.6</v>
+      </c>
       <c r="O13" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L13*VLOOKUP(E13,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M13*VLOOKUP(E13,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N13*VLOOKUP(E13,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>39x17x13</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="B14">
-        <v>1949</v>
+        <v>1945</v>
       </c>
       <c r="C14">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1393,55 +1413,46 @@
       </c>
       <c r="F14">
         <f>IF(B14 &gt; 1900, ((B14-1900)*10)+400+D14, ((B14-1730)*2)+D14)+VLOOKUP(E14,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1491</v>
+        <v>1451</v>
       </c>
       <c r="G14">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H14">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="0"/>
-        <v>164.51950239004088</v>
+        <v>155.13435037626795</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="1"/>
-        <v>148.06755215103681</v>
+        <v>139.62091533864117</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="3">
-        <v>9.1</v>
-      </c>
-      <c r="M14" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="N14" s="3">
-        <v>3.9</v>
-      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
       <c r="O14" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L14*VLOOKUP(E14,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M14*VLOOKUP(E14,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N14*VLOOKUP(E14,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>42x17x19</v>
-      </c>
-      <c r="P14" t="s">
-        <v>105</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B15">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="C15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1451,21 +1462,21 @@
       </c>
       <c r="F15">
         <f>IF(B15 &gt; 1900, ((B15-1900)*10)+400+D15, ((B15-1730)*2)+D15)+VLOOKUP(E15,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1501</v>
+        <v>1491</v>
       </c>
       <c r="G15">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H15">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" si="0"/>
-        <v>144.91376746189439</v>
+        <v>164.51950239004088</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="1"/>
-        <v>130.42239071570495</v>
+        <v>148.06755215103681</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>33</v>
@@ -1477,14 +1488,14 @@
         <v>2.4</v>
       </c>
       <c r="N15" s="3">
-        <v>2.6</v>
+        <v>3.9</v>
       </c>
       <c r="O15" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L15*VLOOKUP(E15,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M15*VLOOKUP(E15,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N15*VLOOKUP(E15,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>42x17x13</v>
+        <v>42x17x19</v>
       </c>
       <c r="P15" t="s">
         <v>105</v>
@@ -1492,14 +1503,14 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="B16">
-        <v>1954</v>
+        <v>1950</v>
       </c>
       <c r="C16">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1509,42 +1520,51 @@
       </c>
       <c r="F16">
         <f>IF(B16 &gt; 1900, ((B16-1900)*10)+400+D16, ((B16-1730)*2)+D16)+VLOOKUP(E16,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1541</v>
+        <v>1501</v>
       </c>
       <c r="G16">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H16">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="0"/>
-        <v>178.88543819998318</v>
+        <v>144.91376746189439</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="1"/>
-        <v>160.99689437998487</v>
+        <v>130.42239071570495</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
+      <c r="L16" s="3">
+        <v>9.1</v>
+      </c>
+      <c r="M16" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="N16" s="3">
+        <v>2.6</v>
+      </c>
       <c r="O16" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L16*VLOOKUP(E16,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M16*VLOOKUP(E16,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N16*VLOOKUP(E16,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>42x17x13</v>
+      </c>
+      <c r="P16" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17">
-        <v>1958</v>
+        <v>1954</v>
       </c>
       <c r="C17">
         <f t="shared" si="2"/>
@@ -1558,21 +1578,21 @@
       </c>
       <c r="F17">
         <f>IF(B17 &gt; 1900, ((B17-1900)*10)+400+D17, ((B17-1730)*2)+D17)+VLOOKUP(E17,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1581</v>
+        <v>1541</v>
       </c>
       <c r="G17">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="H17">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" si="0"/>
-        <v>169.44353369518447</v>
+        <v>178.88543819998318</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="1"/>
-        <v>152.49918032566603</v>
+        <v>160.99689437998487</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>33</v>
@@ -1590,38 +1610,38 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>1958</v>
       </c>
       <c r="C18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>21</v>
       </c>
       <c r="F18">
         <f>IF(B18 &gt; 1900, ((B18-1900)*10)+400+D18, ((B18-1730)*2)+D18)+VLOOKUP(E18,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="G18">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="H18">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="0"/>
-        <v>186.63690238892559</v>
+        <v>169.44353369518447</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="1"/>
-        <v>167.97321215003305</v>
+        <v>152.49918032566603</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>33</v>
@@ -1639,67 +1659,63 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="B19">
-        <v>1963</v>
+        <v>1958</v>
       </c>
       <c r="C19">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
       </c>
       <c r="F19">
         <f>IF(B19 &gt; 1900, ((B19-1900)*10)+400+D19, ((B19-1730)*2)+D19)+VLOOKUP(E19,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1631</v>
+        <v>1582</v>
       </c>
       <c r="G19">
         <v>55</v>
       </c>
       <c r="H19">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="0"/>
-        <v>178.26322609494585</v>
+        <v>186.63690238892559</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="1"/>
-        <v>160.43690348545127</v>
+        <v>167.97321215003305</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L19" s="3">
-        <v>11</v>
-      </c>
-      <c r="M19" s="3">
-        <v>2.5</v>
-      </c>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L19*VLOOKUP(E19,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M19*VLOOKUP(E19,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N19*VLOOKUP(E19,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>51x18x0</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B20">
-        <v>1972</v>
+        <v>1963</v>
       </c>
       <c r="C20">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1709,27 +1725,27 @@
       </c>
       <c r="F20">
         <f>IF(B20 &gt; 1900, ((B20-1900)*10)+400+D20, ((B20-1730)*2)+D20)+VLOOKUP(E20,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1721</v>
+        <v>1631</v>
       </c>
       <c r="G20">
+        <v>55</v>
+      </c>
+      <c r="H20">
         <v>52</v>
-      </c>
-      <c r="H20">
-        <v>58</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" si="0"/>
-        <v>183.06040290327977</v>
+        <v>178.26322609494585</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="1"/>
-        <v>164.75436261295178</v>
+        <v>160.43690348545127</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L20" s="3">
-        <v>11.3</v>
+        <v>11</v>
       </c>
       <c r="M20" s="3">
         <v>2.5</v>
@@ -1740,19 +1756,19 @@
 ROUND(L20*VLOOKUP(E20,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M20*VLOOKUP(E20,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N20*VLOOKUP(E20,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>53x18x0</v>
+        <v>51x18x0</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>113</v>
+        <v>59</v>
       </c>
       <c r="B21">
-        <v>1977</v>
+        <v>1972</v>
       </c>
       <c r="C21">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1762,52 +1778,50 @@
       </c>
       <c r="F21">
         <f>IF(B21 &gt; 1900, ((B21-1900)*10)+400+D21, ((B21-1730)*2)+D21)+VLOOKUP(E21,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1771</v>
+        <v>1721</v>
       </c>
       <c r="G21">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H21">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" si="0"/>
-        <v>188.41443681416774</v>
+        <v>183.06040290327977</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="1"/>
-        <v>169.57299313275098</v>
+        <v>164.75436261295178</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L21" s="3">
-        <v>12</v>
+        <v>11.3</v>
       </c>
       <c r="M21" s="3">
         <v>2.5</v>
       </c>
-      <c r="N21" s="3">
-        <v>4.2</v>
-      </c>
+      <c r="N21" s="3"/>
       <c r="O21" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L21*VLOOKUP(E21,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M21*VLOOKUP(E21,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N21*VLOOKUP(E21,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>56x18x20</v>
+        <v>53x18x0</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="B22">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="C22">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1817,21 +1831,21 @@
       </c>
       <c r="F22">
         <f>IF(B22 &gt; 1900, ((B22-1900)*10)+400+D22, ((B22-1730)*2)+D22)+VLOOKUP(E22,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1781</v>
+        <v>1771</v>
       </c>
       <c r="G22">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="H22">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="0"/>
-        <v>194.65068427541911</v>
+        <v>188.41443681416774</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" si="1"/>
-        <v>175.18561584787722</v>
+        <v>169.57299313275098</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>33</v>
@@ -1843,26 +1857,26 @@
         <v>2.5</v>
       </c>
       <c r="N22" s="3">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="O22" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L22*VLOOKUP(E22,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M22*VLOOKUP(E22,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N22*VLOOKUP(E22,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>56x18x16</v>
+        <v>56x18x20</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B23">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="C23">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1872,21 +1886,21 @@
       </c>
       <c r="F23">
         <f>IF(B23 &gt; 1900, ((B23-1900)*10)+400+D23, ((B23-1730)*2)+D23)+VLOOKUP(E23,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1801</v>
+        <v>1781</v>
       </c>
       <c r="G23">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="H23">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="I23" s="2">
         <f t="shared" si="0"/>
-        <v>195.2491286080996</v>
+        <v>194.65068427541911</v>
       </c>
       <c r="J23" s="2">
         <f t="shared" si="1"/>
-        <v>175.72421574728963</v>
+        <v>175.18561584787722</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>33</v>
@@ -1898,26 +1912,26 @@
         <v>2.5</v>
       </c>
       <c r="N23" s="3">
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="O23" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L23*VLOOKUP(E23,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M23*VLOOKUP(E23,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N23*VLOOKUP(E23,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>56x18x20</v>
+        <v>56x18x16</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B24">
-        <v>1989</v>
+        <v>1980</v>
       </c>
       <c r="C24">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1927,52 +1941,52 @@
       </c>
       <c r="F24">
         <f>IF(B24 &gt; 1900, ((B24-1900)*10)+400+D24, ((B24-1730)*2)+D24)+VLOOKUP(E24,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1891</v>
+        <v>1801</v>
       </c>
       <c r="G24">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H24">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" si="0"/>
-        <v>176.38342073763937</v>
+        <v>195.2491286080996</v>
       </c>
       <c r="J24" s="2">
         <f t="shared" si="1"/>
-        <v>158.74507866387543</v>
+        <v>175.72421574728963</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L24" s="3">
-        <v>10.199999999999999</v>
+        <v>12</v>
       </c>
       <c r="M24" s="3">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="N24" s="3">
-        <v>2.7</v>
+        <v>4.2</v>
       </c>
       <c r="O24" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L24*VLOOKUP(E24,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M24*VLOOKUP(E24,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N24*VLOOKUP(E24,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>48x17x13</v>
+        <v>56x18x20</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="B25">
-        <v>1995</v>
+        <v>1989</v>
       </c>
       <c r="C25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1982,21 +1996,21 @@
       </c>
       <c r="F25">
         <f>IF(B25 &gt; 1900, ((B25-1900)*10)+400+D25, ((B25-1730)*2)+D25)+VLOOKUP(E25,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1951</v>
+        <v>1891</v>
       </c>
       <c r="G25">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H25">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I25" s="2">
         <f t="shared" si="0"/>
-        <v>187.97162906495581</v>
+        <v>176.38342073763937</v>
       </c>
       <c r="J25" s="2">
         <f t="shared" si="1"/>
-        <v>169.17446615846023</v>
+        <v>158.74507866387543</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>33</v>
@@ -2017,20 +2031,17 @@
 ROUND(N25*VLOOKUP(E25,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>48x17x13</v>
       </c>
-      <c r="P25" t="s">
-        <v>117</v>
-      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="B26">
-        <v>1998</v>
+        <v>1995</v>
       </c>
       <c r="C26">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2040,21 +2051,21 @@
       </c>
       <c r="F26">
         <f>IF(B26 &gt; 1900, ((B26-1900)*10)+400+D26, ((B26-1730)*2)+D26)+VLOOKUP(E26,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>1981</v>
+        <v>1951</v>
       </c>
       <c r="G26">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H26">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" si="0"/>
-        <v>147.08274315273474</v>
+        <v>187.97162906495581</v>
       </c>
       <c r="J26" s="2">
         <f t="shared" si="1"/>
-        <v>132.37446883746128</v>
+        <v>169.17446615846023</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>33</v>
@@ -2063,7 +2074,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="M26" s="3">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="N26" s="3">
         <v>2.7</v>
@@ -2075,13 +2086,16 @@
 ROUND(N26*VLOOKUP(E26,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>48x17x13</v>
       </c>
+      <c r="P26" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B27">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="C27">
         <f t="shared" si="2"/>
@@ -2095,162 +2109,162 @@
       </c>
       <c r="F27">
         <f>IF(B27 &gt; 1900, ((B27-1900)*10)+400+D27, ((B27-1730)*2)+D27)+VLOOKUP(E27,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>2011</v>
+        <v>1981</v>
       </c>
       <c r="G27">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="H27">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="I27" s="2">
         <f t="shared" si="0"/>
-        <v>212.39376429431988</v>
+        <v>147.08274315273474</v>
       </c>
       <c r="J27" s="2">
         <f t="shared" si="1"/>
-        <v>191.15438786488789</v>
+        <v>132.37446883746128</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L27" s="3">
-        <v>12</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="M27" s="3">
-        <v>2.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N27" s="3">
-        <v>3.3</v>
+        <v>2.7</v>
       </c>
       <c r="O27" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L27*VLOOKUP(E27,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M27*VLOOKUP(E27,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N27*VLOOKUP(E27,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>56x18x16</v>
+        <v>48x17x13</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="B28">
         <v>2001</v>
       </c>
       <c r="C28">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
         <v>21</v>
       </c>
       <c r="F28">
         <f>IF(B28 &gt; 1900, ((B28-1900)*10)+400+D28, ((B28-1730)*2)+D28)+VLOOKUP(E28,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G28">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="H28">
-        <v>140</v>
+        <v>58</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" si="0"/>
-        <v>292.49881291307071</v>
+        <v>212.39376429431988</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" si="1"/>
-        <v>263.24893162176363</v>
+        <v>191.15438786488789</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L28" s="3">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="M28" s="3">
         <v>2.5</v>
       </c>
       <c r="N28" s="3">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="O28" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L28*VLOOKUP(E28,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M28*VLOOKUP(E28,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N28*VLOOKUP(E28,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>84x18x15</v>
+        <v>56x18x16</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B29">
-        <v>2005</v>
+        <v>2001</v>
       </c>
       <c r="C29">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
         <v>21</v>
       </c>
       <c r="F29">
         <f>IF(B29 &gt; 1900, ((B29-1900)*10)+400+D29, ((B29-1730)*2)+D29)+VLOOKUP(E29,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>2051</v>
+        <v>2012</v>
       </c>
       <c r="G29">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H29">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="I29" s="2">
         <f t="shared" si="0"/>
-        <v>244.94897427831785</v>
+        <v>292.49881291307071</v>
       </c>
       <c r="J29" s="2">
         <f t="shared" si="1"/>
-        <v>220.45407685048608</v>
+        <v>263.24893162176363</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L29" s="3">
-        <v>11.4</v>
+        <v>18</v>
       </c>
       <c r="M29" s="3">
-        <v>2.5499999999999998</v>
+        <v>2.5</v>
       </c>
       <c r="N29" s="3">
-        <v>4.2</v>
+        <v>3.2</v>
       </c>
       <c r="O29" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L29*VLOOKUP(E29,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M29*VLOOKUP(E29,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N29*VLOOKUP(E29,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>53x18x20</v>
+        <v>84x18x15</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="B30">
-        <v>2012</v>
+        <v>2005</v>
       </c>
       <c r="C30">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -2260,150 +2274,156 @@
       </c>
       <c r="F30">
         <f>IF(B30 &gt; 1900, ((B30-1900)*10)+400+D30, ((B30-1730)*2)+D30)+VLOOKUP(E30,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>2121</v>
+        <v>2051</v>
       </c>
       <c r="G30">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H30">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="I30" s="2">
         <f t="shared" si="0"/>
-        <v>219.84843263788198</v>
+        <v>244.94897427831785</v>
       </c>
       <c r="J30" s="2">
         <f t="shared" si="1"/>
-        <v>197.86358937409378</v>
+        <v>220.45407685048608</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
+      <c r="L30" s="3">
+        <v>11.4</v>
+      </c>
+      <c r="M30" s="3">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="N30" s="3">
+        <v>4.2</v>
+      </c>
       <c r="O30" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L30*VLOOKUP(E30,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M30*VLOOKUP(E30,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N30*VLOOKUP(E30,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>53x18x20</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B31">
         <v>2012</v>
       </c>
       <c r="C31">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
         <v>21</v>
       </c>
       <c r="F31">
         <f>IF(B31 &gt; 1900, ((B31-1900)*10)+400+D31, ((B31-1730)*2)+D31)+VLOOKUP(E31,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="G31">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="H31">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" si="0"/>
-        <v>152.75252316519467</v>
+        <v>219.84843263788198</v>
       </c>
       <c r="J31" s="2">
         <f t="shared" si="1"/>
-        <v>137.4772708486752</v>
+        <v>197.86358937409378</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L31" s="3">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="M31" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="N31" s="3">
-        <v>2.7</v>
-      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
       <c r="O31" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L31*VLOOKUP(E31,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M31*VLOOKUP(E31,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N31*VLOOKUP(E31,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>48x17x13</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="B32">
-        <v>1800</v>
+        <v>2012</v>
       </c>
       <c r="C32">
         <f t="shared" si="2"/>
-        <v>-212</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F32">
         <f>IF(B32 &gt; 1900, ((B32-1900)*10)+400+D32, ((B32-1730)*2)+D32)+VLOOKUP(E32,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>3741</v>
+        <v>2122</v>
       </c>
       <c r="G32">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="H32">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" si="0"/>
-        <v>46.188021535170058</v>
+        <v>152.75252316519467</v>
       </c>
       <c r="J32" s="2">
         <f t="shared" si="1"/>
-        <v>41.569219381653056</v>
+        <v>137.4772708486752</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
+      <c r="L32" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="M32" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N32" s="3">
+        <v>2.7</v>
+      </c>
       <c r="O32" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L32*VLOOKUP(E32,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M32*VLOOKUP(E32,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N32*VLOOKUP(E32,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>48x17x13</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B33">
-        <v>1897</v>
+        <v>1800</v>
       </c>
       <c r="C33">
         <f t="shared" si="2"/>
-        <v>97</v>
+        <v>-212</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2413,21 +2433,21 @@
       </c>
       <c r="F33">
         <f>IF(B33 &gt; 1900, ((B33-1900)*10)+400+D33, ((B33-1730)*2)+D33)+VLOOKUP(E33,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>3935</v>
+        <v>3741</v>
       </c>
       <c r="G33">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H33">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" si="0"/>
-        <v>52.915026221291818</v>
+        <v>46.188021535170058</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" si="1"/>
-        <v>47.623523599162638</v>
+        <v>41.569219381653056</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>33</v>
@@ -2445,14 +2465,14 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B34">
-        <v>1902</v>
+        <v>1897</v>
       </c>
       <c r="C34">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -2462,21 +2482,21 @@
       </c>
       <c r="F34">
         <f>IF(B34 &gt; 1900, ((B34-1900)*10)+400+D34, ((B34-1730)*2)+D34)+VLOOKUP(E34,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4021</v>
+        <v>3935</v>
       </c>
       <c r="G34">
         <v>18</v>
       </c>
       <c r="H34">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" si="0"/>
-        <v>56.568542494923797</v>
+        <v>52.915026221291818</v>
       </c>
       <c r="J34" s="2">
         <f t="shared" si="1"/>
-        <v>50.911688245431421</v>
+        <v>47.623523599162638</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>33</v>
@@ -2494,10 +2514,10 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B35">
-        <v>1907</v>
+        <v>1902</v>
       </c>
       <c r="C35">
         <f t="shared" si="2"/>
@@ -2511,21 +2531,21 @@
       </c>
       <c r="F35">
         <f>IF(B35 &gt; 1900, ((B35-1900)*10)+400+D35, ((B35-1730)*2)+D35)+VLOOKUP(E35,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4071</v>
+        <v>4021</v>
       </c>
       <c r="G35">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H35">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" si="0"/>
-        <v>63.245553203367592</v>
+        <v>56.568542494923797</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" si="1"/>
-        <v>56.920997883030836</v>
+        <v>50.911688245431421</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>33</v>
@@ -2543,14 +2563,14 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>1913</v>
+        <v>1907</v>
       </c>
       <c r="C36">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -2560,21 +2580,21 @@
       </c>
       <c r="F36">
         <f>IF(B36 &gt; 1900, ((B36-1900)*10)+400+D36, ((B36-1730)*2)+D36)+VLOOKUP(E36,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4131</v>
+        <v>4071</v>
       </c>
       <c r="G36">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H36">
         <v>18</v>
       </c>
       <c r="I36" s="2">
         <f t="shared" ref="I36:I67" si="3">SQRT(G36*H36)/$B$1</f>
-        <v>66.332495807108003</v>
+        <v>63.245553203367592</v>
       </c>
       <c r="J36" s="2">
         <f t="shared" ref="J36:J67" si="4">I36*0.9</f>
-        <v>59.699246226397207</v>
+        <v>56.920997883030836</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>33</v>
@@ -2592,14 +2612,14 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>2</v>
       </c>
       <c r="B37">
-        <v>1920</v>
+        <v>1913</v>
       </c>
       <c r="C37">
         <f t="shared" ref="C37:C68" si="5">B37-B36</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -2609,52 +2629,46 @@
       </c>
       <c r="F37">
         <f>IF(B37 &gt; 1900, ((B37-1900)*10)+400+D37, ((B37-1730)*2)+D37)+VLOOKUP(E37,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4201</v>
+        <v>4131</v>
       </c>
       <c r="G37">
+        <v>22</v>
+      </c>
+      <c r="H37">
         <v>18</v>
-      </c>
-      <c r="H37">
-        <v>28</v>
       </c>
       <c r="I37" s="2">
         <f t="shared" si="3"/>
-        <v>74.833147735478832</v>
+        <v>66.332495807108003</v>
       </c>
       <c r="J37" s="2">
         <f t="shared" si="4"/>
-        <v>67.349832961930957</v>
+        <v>59.699246226397207</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L37" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="M37" s="3">
-        <v>2</v>
-      </c>
-      <c r="N37" s="3">
-        <v>2.5</v>
-      </c>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
       <c r="O37" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L37*VLOOKUP(E37,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M37*VLOOKUP(E37,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N37*VLOOKUP(E37,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>16x14x12</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B38">
-        <v>1928</v>
+        <v>1920</v>
       </c>
       <c r="C38">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -2664,46 +2678,52 @@
       </c>
       <c r="F38">
         <f>IF(B38 &gt; 1900, ((B38-1900)*10)+400+D38, ((B38-1730)*2)+D38)+VLOOKUP(E38,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4281</v>
+        <v>4201</v>
       </c>
       <c r="G38">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="H38">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I38" s="2">
         <f t="shared" si="3"/>
-        <v>78.528126595931653</v>
+        <v>74.833147735478832</v>
       </c>
       <c r="J38" s="2">
         <f t="shared" si="4"/>
-        <v>70.675313936338483</v>
+        <v>67.349832961930957</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
+      <c r="L38" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="M38" s="3">
+        <v>2</v>
+      </c>
+      <c r="N38" s="3">
+        <v>2.5</v>
+      </c>
       <c r="O38" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L38*VLOOKUP(E38,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M38*VLOOKUP(E38,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N38*VLOOKUP(E38,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>16x14x12</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39">
-        <v>1935</v>
+        <v>1928</v>
       </c>
       <c r="C39">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -2713,21 +2733,21 @@
       </c>
       <c r="F39">
         <f>IF(B39 &gt; 1900, ((B39-1900)*10)+400+D39, ((B39-1730)*2)+D39)+VLOOKUP(E39,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4351</v>
+        <v>4281</v>
       </c>
       <c r="G39">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H39">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="I39" s="2">
         <f t="shared" si="3"/>
-        <v>96.609178307929596</v>
+        <v>78.528126595931653</v>
       </c>
       <c r="J39" s="2">
         <f t="shared" si="4"/>
-        <v>86.948260477136643</v>
+        <v>70.675313936338483</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>33</v>
@@ -2745,14 +2765,14 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="B40">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="C40">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -2762,21 +2782,21 @@
       </c>
       <c r="F40">
         <f>IF(B40 &gt; 1900, ((B40-1900)*10)+400+D40, ((B40-1730)*2)+D40)+VLOOKUP(E40,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4361</v>
+        <v>4351</v>
       </c>
       <c r="G40">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H40">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I40" s="2">
         <f t="shared" si="3"/>
-        <v>81.649658092772611</v>
+        <v>96.609178307929596</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" si="4"/>
-        <v>73.484692283495349</v>
+        <v>86.948260477136643</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>33</v>
@@ -2794,14 +2814,14 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="B41">
-        <v>1948</v>
+        <v>1936</v>
       </c>
       <c r="C41">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2811,25 +2831,27 @@
       </c>
       <c r="F41">
         <f>IF(B41 &gt; 1900, ((B41-1900)*10)+400+D41, ((B41-1730)*2)+D41)+VLOOKUP(E41,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4481</v>
+        <v>4361</v>
       </c>
       <c r="G41">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="H41">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="I41" s="2">
         <f t="shared" si="3"/>
-        <v>53.541261347363367</v>
+        <v>81.649658092772611</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" si="4"/>
-        <v>48.187135212627034</v>
+        <v>73.484692283495349</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="2" t="str">
         <f>CONCATENATE(
@@ -2841,14 +2863,14 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="B42">
-        <v>1952</v>
+        <v>1948</v>
       </c>
       <c r="C42">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -2858,27 +2880,25 @@
       </c>
       <c r="F42">
         <f>IF(B42 &gt; 1900, ((B42-1900)*10)+400+D42, ((B42-1730)*2)+D42)+VLOOKUP(E42,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4521</v>
+        <v>4481</v>
       </c>
       <c r="G42">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H42">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="I42" s="2">
         <f t="shared" si="3"/>
-        <v>102.74023338281629</v>
+        <v>53.541261347363367</v>
       </c>
       <c r="J42" s="2">
         <f t="shared" si="4"/>
-        <v>92.466210044534662</v>
+        <v>48.187135212627034</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="2" t="str">
         <f>CONCATENATE(
@@ -2890,14 +2910,14 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B43">
-        <v>1957</v>
+        <v>1952</v>
       </c>
       <c r="C43">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2907,21 +2927,21 @@
       </c>
       <c r="F43">
         <f>IF(B43 &gt; 1900, ((B43-1900)*10)+400+D43, ((B43-1730)*2)+D43)+VLOOKUP(E43,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4571</v>
+        <v>4521</v>
       </c>
       <c r="G43">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H43">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I43" s="2">
         <f t="shared" si="3"/>
-        <v>101.32456102380443</v>
+        <v>102.74023338281629</v>
       </c>
       <c r="J43" s="2">
         <f t="shared" si="4"/>
-        <v>91.19210492142399</v>
+        <v>92.466210044534662</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>33</v>
@@ -2939,14 +2959,14 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="B44">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="C44">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2956,55 +2976,46 @@
       </c>
       <c r="F44">
         <f>IF(B44 &gt; 1900, ((B44-1900)*10)+400+D44, ((B44-1730)*2)+D44)+VLOOKUP(E44,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4591</v>
+        <v>4571</v>
       </c>
       <c r="G44">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H44">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I44" s="2">
         <f t="shared" si="3"/>
-        <v>101.54364141151879</v>
+        <v>101.32456102380443</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" si="4"/>
-        <v>91.389277270366918</v>
+        <v>91.19210492142399</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L44" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="M44" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N44" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
       <c r="O44" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L44*VLOOKUP(E44,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M44*VLOOKUP(E44,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N44*VLOOKUP(E44,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
-      </c>
-      <c r="P44" t="s">
-        <v>99</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="B45">
-        <v>1963</v>
+        <v>1959</v>
       </c>
       <c r="C45">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -3014,46 +3025,55 @@
       </c>
       <c r="F45">
         <f>IF(B45 &gt; 1900, ((B45-1900)*10)+400+D45, ((B45-1730)*2)+D45)+VLOOKUP(E45,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4631</v>
+        <v>4591</v>
       </c>
       <c r="G45">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="H45">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I45" s="2">
         <f t="shared" si="3"/>
-        <v>113.13708498984759</v>
+        <v>101.54364141151879</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" si="4"/>
-        <v>101.82337649086284</v>
+        <v>91.389277270366918</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
+      <c r="L45" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="M45" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N45" s="3">
+        <v>2.6</v>
+      </c>
       <c r="O45" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L45*VLOOKUP(E45,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M45*VLOOKUP(E45,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N45*VLOOKUP(E45,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>29x16x13</v>
+      </c>
+      <c r="P45" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B46">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="C46">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -3063,21 +3083,21 @@
       </c>
       <c r="F46">
         <f>IF(B46 &gt; 1900, ((B46-1900)*10)+400+D46, ((B46-1730)*2)+D46)+VLOOKUP(E46,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4641</v>
+        <v>4631</v>
       </c>
       <c r="G46">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H46">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="I46" s="2">
         <f t="shared" si="3"/>
-        <v>146.9693845669907</v>
+        <v>113.13708498984759</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" si="4"/>
-        <v>132.27244611029164</v>
+        <v>101.82337649086284</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>33</v>
@@ -3095,38 +3115,38 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B47">
         <v>1964</v>
       </c>
       <c r="C47">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47" t="s">
         <v>22</v>
       </c>
       <c r="F47">
         <f>IF(B47 &gt; 1900, ((B47-1900)*10)+400+D47, ((B47-1730)*2)+D47)+VLOOKUP(E47,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4642</v>
+        <v>4641</v>
       </c>
       <c r="G47">
         <v>54</v>
       </c>
       <c r="H47">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="I47" s="2">
         <f t="shared" si="3"/>
-        <v>114.89125293076057</v>
+        <v>146.9693845669907</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" si="4"/>
-        <v>103.40212763768452</v>
+        <v>132.27244611029164</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>33</v>
@@ -3141,44 +3161,41 @@
 ROUND(N47*VLOOKUP(E47,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
-      <c r="P47" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B48">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="C48">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E48" t="s">
         <v>22</v>
       </c>
       <c r="F48">
         <f>IF(B48 &gt; 1900, ((B48-1900)*10)+400+D48, ((B48-1730)*2)+D48)+VLOOKUP(E48,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4651</v>
+        <v>4642</v>
       </c>
       <c r="G48">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H48">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="I48" s="2">
         <f t="shared" si="3"/>
-        <v>150.99668870541501</v>
+        <v>114.89125293076057</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" si="4"/>
-        <v>135.8970198348735</v>
+        <v>103.40212763768452</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>33</v>
@@ -3193,133 +3210,127 @@
 ROUND(N48*VLOOKUP(E48,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
+      <c r="P48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="B49">
         <v>1965</v>
       </c>
       <c r="C49">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49" t="s">
         <v>22</v>
       </c>
       <c r="F49">
         <f>IF(B49 &gt; 1900, ((B49-1900)*10)+400+D49, ((B49-1730)*2)+D49)+VLOOKUP(E49,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4652</v>
+        <v>4651</v>
       </c>
       <c r="G49">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H49">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="I49" s="2">
         <f t="shared" si="3"/>
-        <v>103.27955589886446</v>
+        <v>150.99668870541501</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" si="4"/>
-        <v>92.951600308978016</v>
+        <v>135.8970198348735</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L49" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="M49" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N49" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
       <c r="O49" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L49*VLOOKUP(E49,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M49*VLOOKUP(E49,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N49*VLOOKUP(E49,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
-      </c>
-      <c r="P49" t="s">
-        <v>98</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B50">
-        <v>1967</v>
+        <v>1965</v>
       </c>
       <c r="C50">
         <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D50">
         <v>2</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
       </c>
       <c r="E50" t="s">
         <v>22</v>
       </c>
       <c r="F50">
         <f>IF(B50 &gt; 1900, ((B50-1900)*10)+400+D50, ((B50-1730)*2)+D50)+VLOOKUP(E50,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4671</v>
+        <v>4652</v>
       </c>
       <c r="G50">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H50">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I50" s="2">
         <f t="shared" si="3"/>
-        <v>116.99952516522831</v>
+        <v>103.27955589886446</v>
       </c>
       <c r="J50" s="2">
         <f t="shared" si="4"/>
-        <v>105.29957264870548</v>
+        <v>92.951600308978016</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L50" s="3">
-        <v>8.5</v>
+        <v>6.2</v>
       </c>
       <c r="M50" s="3">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N50" s="3">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
       <c r="O50" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L50*VLOOKUP(E50,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M50*VLOOKUP(E50,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N50*VLOOKUP(E50,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>40x18x14</v>
+        <v>29x16x13</v>
       </c>
       <c r="P50" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="B51">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="C51">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3329,46 +3340,55 @@
       </c>
       <c r="F51">
         <f>IF(B51 &gt; 1900, ((B51-1900)*10)+400+D51, ((B51-1730)*2)+D51)+VLOOKUP(E51,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4681</v>
+        <v>4671</v>
       </c>
       <c r="G51">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="H51">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="I51" s="2">
         <f t="shared" si="3"/>
-        <v>164.92422502470643</v>
+        <v>116.99952516522831</v>
       </c>
       <c r="J51" s="2">
         <f t="shared" si="4"/>
-        <v>148.43180252223578</v>
+        <v>105.29957264870548</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
+      <c r="L51" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="M51" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="N51" s="3">
+        <v>2.8</v>
+      </c>
       <c r="O51" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L51*VLOOKUP(E51,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M51*VLOOKUP(E51,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N51*VLOOKUP(E51,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>40x18x14</v>
+      </c>
+      <c r="P51" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>8</v>
       </c>
       <c r="B52">
-        <v>1977</v>
+        <v>1968</v>
       </c>
       <c r="C52">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -3378,21 +3398,21 @@
       </c>
       <c r="F52">
         <f>IF(B52 &gt; 1900, ((B52-1900)*10)+400+D52, ((B52-1730)*2)+D52)+VLOOKUP(E52,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4771</v>
+        <v>4681</v>
       </c>
       <c r="G52">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="H52">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I52" s="2">
         <f t="shared" si="3"/>
-        <v>163.29931618554522</v>
+        <v>164.92422502470643</v>
       </c>
       <c r="J52" s="2">
         <f t="shared" si="4"/>
-        <v>146.9693845669907</v>
+        <v>148.43180252223578</v>
       </c>
       <c r="K52" s="2" t="s">
         <v>33</v>
@@ -3407,20 +3427,17 @@
 ROUND(N52*VLOOKUP(E52,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
-      <c r="P52" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="B53">
-        <v>1980</v>
+        <v>1977</v>
       </c>
       <c r="C53">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -3430,21 +3447,21 @@
       </c>
       <c r="F53">
         <f>IF(B53 &gt; 1900, ((B53-1900)*10)+400+D53, ((B53-1730)*2)+D53)+VLOOKUP(E53,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4801</v>
+        <v>4771</v>
       </c>
       <c r="G53">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H53">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I53" s="2">
         <f t="shared" si="3"/>
-        <v>170.09801096230765</v>
+        <v>163.29931618554522</v>
       </c>
       <c r="J53" s="2">
         <f t="shared" si="4"/>
-        <v>153.08820986607688</v>
+        <v>146.9693845669907</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>33</v>
@@ -3459,17 +3476,20 @@
 ROUND(N53*VLOOKUP(E53,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
+      <c r="P53" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>91</v>
+        <v>9</v>
       </c>
       <c r="B54">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="C54">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -3479,51 +3499,42 @@
       </c>
       <c r="F54">
         <f>IF(B54 &gt; 1900, ((B54-1900)*10)+400+D54, ((B54-1730)*2)+D54)+VLOOKUP(E54,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4811</v>
+        <v>4801</v>
       </c>
       <c r="G54">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H54">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="I54" s="2">
         <f t="shared" si="3"/>
-        <v>116.61903789690601</v>
+        <v>170.09801096230765</v>
       </c>
       <c r="J54" s="2">
         <f t="shared" si="4"/>
-        <v>104.95713410721541</v>
+        <v>153.08820986607688</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L54" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="M54" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N54" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
       <c r="O54" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L54*VLOOKUP(E54,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M54*VLOOKUP(E54,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N54*VLOOKUP(E54,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
-      </c>
-      <c r="P54" t="s">
-        <v>97</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B55">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="C55">
         <f t="shared" si="5"/>
@@ -3537,42 +3548,51 @@
       </c>
       <c r="F55">
         <f>IF(B55 &gt; 1900, ((B55-1900)*10)+400+D55, ((B55-1730)*2)+D55)+VLOOKUP(E55,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4821</v>
+        <v>4811</v>
       </c>
       <c r="G55">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="H55">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="I55" s="2">
         <f t="shared" si="3"/>
-        <v>136.62601021279465</v>
+        <v>116.61903789690601</v>
       </c>
       <c r="J55" s="2">
         <f t="shared" si="4"/>
-        <v>122.9634091915152</v>
+        <v>104.95713410721541</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
+      <c r="L55" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="M55" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N55" s="3">
+        <v>2.6</v>
+      </c>
       <c r="O55" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L55*VLOOKUP(E55,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M55*VLOOKUP(E55,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N55*VLOOKUP(E55,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>29x16x13</v>
+      </c>
+      <c r="P55" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="B56">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="C56">
         <f t="shared" si="5"/>
@@ -3586,55 +3606,46 @@
       </c>
       <c r="F56">
         <f>IF(B56 &gt; 1900, ((B56-1900)*10)+400+D56, ((B56-1730)*2)+D56)+VLOOKUP(E56,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4831</v>
+        <v>4821</v>
       </c>
       <c r="G56">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H56">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I56" s="2">
         <f t="shared" si="3"/>
-        <v>125.07775359529147</v>
+        <v>136.62601021279465</v>
       </c>
       <c r="J56" s="2">
         <f t="shared" si="4"/>
-        <v>112.56997823576232</v>
+        <v>122.9634091915152</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L56" s="3">
-        <v>7.7</v>
-      </c>
-      <c r="M56" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N56" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
       <c r="O56" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L56*VLOOKUP(E56,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M56*VLOOKUP(E56,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N56*VLOOKUP(E56,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>36x16x13</v>
-      </c>
-      <c r="P56" t="s">
-        <v>107</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="B57">
-        <v>1986</v>
+        <v>1983</v>
       </c>
       <c r="C57">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -3644,46 +3655,55 @@
       </c>
       <c r="F57">
         <f>IF(B57 &gt; 1900, ((B57-1900)*10)+400+D57, ((B57-1730)*2)+D57)+VLOOKUP(E57,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4861</v>
+        <v>4831</v>
       </c>
       <c r="G57">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H57">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I57" s="2">
         <f t="shared" si="3"/>
-        <v>143.75905768565215</v>
+        <v>125.07775359529147</v>
       </c>
       <c r="J57" s="2">
         <f t="shared" si="4"/>
-        <v>129.38315191708693</v>
+        <v>112.56997823576232</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
+      <c r="L57" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="M57" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N57" s="3">
+        <v>2.6</v>
+      </c>
       <c r="O57" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L57*VLOOKUP(E57,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M57*VLOOKUP(E57,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N57*VLOOKUP(E57,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>36x16x13</v>
+      </c>
+      <c r="P57" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B58">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="C58">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -3693,21 +3713,21 @@
       </c>
       <c r="F58">
         <f>IF(B58 &gt; 1900, ((B58-1900)*10)+400+D58, ((B58-1730)*2)+D58)+VLOOKUP(E58,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4871</v>
+        <v>4861</v>
       </c>
       <c r="G58">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H58">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="I58" s="2">
         <f t="shared" si="3"/>
-        <v>178.26322609494585</v>
+        <v>143.75905768565215</v>
       </c>
       <c r="J58" s="2">
         <f t="shared" si="4"/>
-        <v>160.43690348545127</v>
+        <v>129.38315191708693</v>
       </c>
       <c r="K58" s="2" t="s">
         <v>33</v>
@@ -3725,14 +3745,14 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
       <c r="B59">
-        <v>1993</v>
+        <v>1987</v>
       </c>
       <c r="C59">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -3742,55 +3762,46 @@
       </c>
       <c r="F59">
         <f>IF(B59 &gt; 1900, ((B59-1900)*10)+400+D59, ((B59-1730)*2)+D59)+VLOOKUP(E59,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4931</v>
+        <v>4871</v>
       </c>
       <c r="G59">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H59">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="I59" s="2">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>178.26322609494585</v>
       </c>
       <c r="J59" s="2">
         <f t="shared" si="4"/>
-        <v>108</v>
+        <v>160.43690348545127</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L59" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="M59" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N59" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
       <c r="O59" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L59*VLOOKUP(E59,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M59*VLOOKUP(E59,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N59*VLOOKUP(E59,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
-      </c>
-      <c r="P59" t="s">
-        <v>100</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="B60">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="C60">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -3800,42 +3811,51 @@
       </c>
       <c r="F60">
         <f>IF(B60 &gt; 1900, ((B60-1900)*10)+400+D60, ((B60-1730)*2)+D60)+VLOOKUP(E60,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4951</v>
+        <v>4931</v>
       </c>
       <c r="G60">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="H60">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="I60" s="2">
         <f t="shared" si="3"/>
-        <v>190.43809142780935</v>
+        <v>120</v>
       </c>
       <c r="J60" s="2">
         <f t="shared" si="4"/>
-        <v>171.39428228502842</v>
+        <v>108</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="3"/>
+      <c r="L60" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="M60" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N60" s="3">
+        <v>2.6</v>
+      </c>
       <c r="O60" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L60*VLOOKUP(E60,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M60*VLOOKUP(E60,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N60*VLOOKUP(E60,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>29x16x13</v>
+      </c>
+      <c r="P60" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B61">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="C61">
         <f t="shared" si="5"/>
@@ -3849,21 +3869,21 @@
       </c>
       <c r="F61">
         <f>IF(B61 &gt; 1900, ((B61-1900)*10)+400+D61, ((B61-1730)*2)+D61)+VLOOKUP(E61,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>4971</v>
+        <v>4951</v>
       </c>
       <c r="G61">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H61">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="I61" s="2">
         <f t="shared" si="3"/>
-        <v>157.76212754932311</v>
+        <v>190.43809142780935</v>
       </c>
       <c r="J61" s="2">
         <f t="shared" si="4"/>
-        <v>141.98591479439079</v>
+        <v>171.39428228502842</v>
       </c>
       <c r="K61" s="2" t="s">
         <v>33</v>
@@ -3881,14 +3901,14 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="B62">
-        <v>2001</v>
+        <v>1997</v>
       </c>
       <c r="C62">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -3898,21 +3918,21 @@
       </c>
       <c r="F62">
         <f>IF(B62 &gt; 1900, ((B62-1900)*10)+400+D62, ((B62-1730)*2)+D62)+VLOOKUP(E62,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>5011</v>
+        <v>4971</v>
       </c>
       <c r="G62">
         <v>70</v>
       </c>
       <c r="H62">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="I62" s="2">
         <f t="shared" si="3"/>
-        <v>197.20265943665387</v>
+        <v>157.76212754932311</v>
       </c>
       <c r="J62" s="2">
         <f t="shared" si="4"/>
-        <v>177.48239349298848</v>
+        <v>141.98591479439079</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>33</v>
@@ -3930,121 +3950,121 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B63">
         <v>2001</v>
       </c>
       <c r="C63">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E63" t="s">
         <v>22</v>
       </c>
       <c r="F63">
         <f>IF(B63 &gt; 1900, ((B63-1900)*10)+400+D63, ((B63-1730)*2)+D63)+VLOOKUP(E63,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="G63">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H63">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="I63" s="2">
         <f t="shared" si="3"/>
-        <v>141.42135623730951</v>
+        <v>197.20265943665387</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" si="4"/>
-        <v>127.27922061357856</v>
+        <v>177.48239349298848</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L63" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M63" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N63" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
       <c r="O63" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L63*VLOOKUP(E63,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M63*VLOOKUP(E63,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N63*VLOOKUP(E63,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>40x16x13</v>
-      </c>
-      <c r="P63" t="s">
-        <v>109</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="B64">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="C64">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E64" t="s">
         <v>22</v>
       </c>
       <c r="F64">
         <f>IF(B64 &gt; 1900, ((B64-1900)*10)+400+D64, ((B64-1730)*2)+D64)+VLOOKUP(E64,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>5041</v>
+        <v>5012</v>
       </c>
       <c r="G64">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H64">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="I64" s="2">
         <f t="shared" si="3"/>
-        <v>207.84609690826528</v>
+        <v>141.42135623730951</v>
       </c>
       <c r="J64" s="2">
         <f t="shared" si="4"/>
-        <v>187.06148721743875</v>
+        <v>127.27922061357856</v>
       </c>
       <c r="K64" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
-      <c r="N64" s="3"/>
+      <c r="L64" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="M64" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N64" s="3">
+        <v>2.6</v>
+      </c>
       <c r="O64" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L64*VLOOKUP(E64,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M64*VLOOKUP(E64,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N64*VLOOKUP(E64,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>40x16x13</v>
+      </c>
+      <c r="P64" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>27</v>
       </c>
       <c r="B65">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C65">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -4054,134 +4074,132 @@
       </c>
       <c r="F65">
         <f>IF(B65 &gt; 1900, ((B65-1900)*10)+400+D65, ((B65-1730)*2)+D65)+VLOOKUP(E65,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>5051</v>
+        <v>5041</v>
       </c>
       <c r="G65">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H65">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="I65" s="2">
         <f t="shared" si="3"/>
-        <v>126.49110640673518</v>
+        <v>207.84609690826528</v>
       </c>
       <c r="J65" s="2">
         <f t="shared" si="4"/>
-        <v>113.84199576606167</v>
+        <v>187.06148721743875</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L65" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="M65" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N65" s="3">
-        <v>2.6</v>
-      </c>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
       <c r="O65" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L65*VLOOKUP(E65,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M65*VLOOKUP(E65,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N65*VLOOKUP(E65,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
-      </c>
-      <c r="P65" t="s">
-        <v>96</v>
+        <v>0x0x0</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B66">
-        <v>1912</v>
+        <v>2005</v>
       </c>
       <c r="C66">
         <f t="shared" si="5"/>
-        <v>-93</v>
+        <v>1</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F66">
         <f>IF(B66 &gt; 1900, ((B66-1900)*10)+400+D66, ((B66-1730)*2)+D66)+VLOOKUP(E66,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7121</v>
+        <v>5051</v>
       </c>
       <c r="G66">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="H66">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="I66" s="2">
         <f t="shared" si="3"/>
-        <v>42.163702135578397</v>
+        <v>126.49110640673518</v>
       </c>
       <c r="J66" s="2">
         <f t="shared" si="4"/>
-        <v>37.94733192202056</v>
+        <v>113.84199576606167</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
-      <c r="N66" s="3"/>
+      <c r="L66" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="M66" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N66" s="3">
+        <v>2.6</v>
+      </c>
       <c r="O66" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L66*VLOOKUP(E66,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M66*VLOOKUP(E66,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N66*VLOOKUP(E66,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
+        <v>29x16x13</v>
+      </c>
+      <c r="P66" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>121</v>
       </c>
       <c r="B67">
-        <v>1938</v>
+        <v>2005</v>
       </c>
       <c r="C67">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F67">
         <f>IF(B67 &gt; 1900, ((B67-1900)*10)+400+D67, ((B67-1730)*2)+D67)+VLOOKUP(E67,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7381</v>
+        <v>5052</v>
       </c>
       <c r="G67">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="H67">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="I67" s="2">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>204.93901531919198</v>
       </c>
       <c r="J67" s="2">
         <f t="shared" si="4"/>
-        <v>45</v>
+        <v>184.44511378727279</v>
       </c>
       <c r="K67" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L67" s="3"/>
-      <c r="M67" s="3"/>
       <c r="N67" s="3"/>
       <c r="O67" s="2" t="str">
         <f>CONCATENATE(
@@ -4190,17 +4208,20 @@
 ROUND(N67*VLOOKUP(E67,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
+      <c r="P67" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B68">
-        <v>1957</v>
+        <v>1912</v>
       </c>
       <c r="C68">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>-93</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -4210,21 +4231,21 @@
       </c>
       <c r="F68">
         <f>IF(B68 &gt; 1900, ((B68-1900)*10)+400+D68, ((B68-1730)*2)+D68)+VLOOKUP(E68,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7571</v>
+        <v>7121</v>
       </c>
       <c r="G68">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="H68">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I68" s="2">
-        <f t="shared" ref="I68:I83" si="6">SQRT(G68*H68)/$B$1</f>
-        <v>63.245553203367592</v>
+        <f t="shared" ref="I68:I99" si="6">SQRT(G68*H68)/$B$1</f>
+        <v>42.163702135578397</v>
       </c>
       <c r="J68" s="2">
-        <f t="shared" ref="J68:J82" si="7">I68*0.9</f>
-        <v>56.920997883030836</v>
+        <f t="shared" ref="J68:J99" si="7">I68*0.9</f>
+        <v>37.94733192202056</v>
       </c>
       <c r="K68" s="2" t="s">
         <v>33</v>
@@ -4242,14 +4263,14 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B69">
-        <v>1960</v>
+        <v>1938</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69:C82" si="8">B69-B68</f>
-        <v>3</v>
+        <f t="shared" ref="C69:C100" si="8">B69-B68</f>
+        <v>26</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -4259,21 +4280,21 @@
       </c>
       <c r="F69">
         <f>IF(B69 &gt; 1900, ((B69-1900)*10)+400+D69, ((B69-1730)*2)+D69)+VLOOKUP(E69,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7601</v>
+        <v>7381</v>
       </c>
       <c r="G69">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="H69">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I69" s="2">
         <f t="shared" si="6"/>
-        <v>73.029674334022147</v>
+        <v>50</v>
       </c>
       <c r="J69" s="2">
         <f t="shared" si="7"/>
-        <v>65.726706900619931</v>
+        <v>45</v>
       </c>
       <c r="K69" s="2" t="s">
         <v>33</v>
@@ -4291,14 +4312,14 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B70">
-        <v>1965</v>
+        <v>1957</v>
       </c>
       <c r="C70">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -4308,21 +4329,21 @@
       </c>
       <c r="F70">
         <f>IF(B70 &gt; 1900, ((B70-1900)*10)+400+D70, ((B70-1730)*2)+D70)+VLOOKUP(E70,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7651</v>
+        <v>7571</v>
       </c>
       <c r="G70">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H70">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I70" s="2">
         <f t="shared" si="6"/>
-        <v>76.011695006609202</v>
+        <v>63.245553203367592</v>
       </c>
       <c r="J70" s="2">
         <f t="shared" si="7"/>
-        <v>68.410525505948286</v>
+        <v>56.920997883030836</v>
       </c>
       <c r="K70" s="2" t="s">
         <v>33</v>
@@ -4340,14 +4361,14 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B71">
-        <v>1986</v>
+        <v>1960</v>
       </c>
       <c r="C71">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -4357,21 +4378,21 @@
       </c>
       <c r="F71">
         <f>IF(B71 &gt; 1900, ((B71-1900)*10)+400+D71, ((B71-1730)*2)+D71)+VLOOKUP(E71,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7861</v>
+        <v>7601</v>
       </c>
       <c r="G71">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="H71">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I71" s="2">
         <f t="shared" si="6"/>
-        <v>94.28090415820634</v>
+        <v>73.029674334022147</v>
       </c>
       <c r="J71" s="2">
         <f t="shared" si="7"/>
-        <v>84.852813742385706</v>
+        <v>65.726706900619931</v>
       </c>
       <c r="K71" s="2" t="s">
         <v>33</v>
@@ -4389,38 +4410,38 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B72">
-        <v>1986</v>
+        <v>1965</v>
       </c>
       <c r="C72">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E72" t="s">
         <v>23</v>
       </c>
       <c r="F72">
         <f>IF(B72 &gt; 1900, ((B72-1900)*10)+400+D72, ((B72-1730)*2)+D72)+VLOOKUP(E72,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>7862</v>
+        <v>7651</v>
       </c>
       <c r="G72">
         <v>65</v>
       </c>
       <c r="H72">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I72" s="2">
         <f t="shared" si="6"/>
-        <v>53.748384988656994</v>
+        <v>76.011695006609202</v>
       </c>
       <c r="J72" s="2">
         <f t="shared" si="7"/>
-        <v>48.373546489791295</v>
+        <v>68.410525505948286</v>
       </c>
       <c r="K72" s="2" t="s">
         <v>33</v>
@@ -4438,14 +4459,14 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B73">
-        <v>2006</v>
+        <v>1986</v>
       </c>
       <c r="C73">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -4455,21 +4476,21 @@
       </c>
       <c r="F73">
         <f>IF(B73 &gt; 1900, ((B73-1900)*10)+400+D73, ((B73-1730)*2)+D73)+VLOOKUP(E73,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>8061</v>
+        <v>7861</v>
       </c>
       <c r="G73">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H73">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I73" s="2">
         <f t="shared" si="6"/>
-        <v>106.45812948447541</v>
+        <v>94.28090415820634</v>
       </c>
       <c r="J73" s="2">
         <f t="shared" si="7"/>
-        <v>95.812316536027865</v>
+        <v>84.852813742385706</v>
       </c>
       <c r="K73" s="2" t="s">
         <v>33</v>
@@ -4487,38 +4508,38 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B74">
-        <v>2012</v>
+        <v>1986</v>
       </c>
       <c r="C74">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E74" t="s">
         <v>23</v>
       </c>
       <c r="F74">
         <f>IF(B74 &gt; 1900, ((B74-1900)*10)+400+D74, ((B74-1730)*2)+D74)+VLOOKUP(E74,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>8121</v>
+        <v>7862</v>
       </c>
       <c r="G74">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="H74">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I74" s="2">
         <f t="shared" si="6"/>
-        <v>101.10500592068735</v>
+        <v>53.748384988656994</v>
       </c>
       <c r="J74" s="2">
         <f t="shared" si="7"/>
-        <v>90.994505328618615</v>
+        <v>48.373546489791295</v>
       </c>
       <c r="K74" s="2" t="s">
         <v>33</v>
@@ -4536,38 +4557,38 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B75">
-        <v>1958</v>
+        <v>2006</v>
       </c>
       <c r="C75">
         <f t="shared" si="8"/>
-        <v>-54</v>
+        <v>20</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="F75">
         <f>IF(B75 &gt; 1900, ((B75-1900)*10)+400+D75, ((B75-1730)*2)+D75)+VLOOKUP(E75,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10581</v>
+        <v>8061</v>
       </c>
       <c r="G75">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H75">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I75" s="2">
         <f t="shared" si="6"/>
-        <v>57.735026918962582</v>
+        <v>106.45812948447541</v>
       </c>
       <c r="J75" s="2">
         <f t="shared" si="7"/>
-        <v>51.961524227066327</v>
+        <v>95.812316536027865</v>
       </c>
       <c r="K75" s="2" t="s">
         <v>33</v>
@@ -4582,48 +4603,47 @@
 ROUND(N75*VLOOKUP(E75,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
-      <c r="P75" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="B76">
-        <v>1974</v>
+        <v>2012</v>
       </c>
       <c r="C76">
-        <f>B76-B75</f>
-        <v>16</v>
+        <f t="shared" si="8"/>
+        <v>6</v>
       </c>
       <c r="D76">
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="F76">
         <f>IF(B76 &gt; 1900, ((B76-1900)*10)+400+D76, ((B76-1730)*2)+D76)+VLOOKUP(E76,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10741</v>
+        <v>8121</v>
       </c>
       <c r="G76">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="H76">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I76" s="2">
         <f t="shared" si="6"/>
-        <v>74.833147735478832</v>
+        <v>101.10500592068735</v>
       </c>
       <c r="J76" s="2">
         <f t="shared" si="7"/>
-        <v>67.349832961930957</v>
+        <v>90.994505328618615</v>
       </c>
       <c r="K76" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
       <c r="N76" s="3"/>
       <c r="O76" s="2" t="str">
         <f>CONCATENATE(
@@ -4635,14 +4655,14 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B77">
-        <v>1976</v>
+        <v>1958</v>
       </c>
       <c r="C77">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>-54</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -4652,52 +4672,49 @@
       </c>
       <c r="F77">
         <f>IF(B77 &gt; 1900, ((B77-1900)*10)+400+D77, ((B77-1730)*2)+D77)+VLOOKUP(E77,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10761</v>
+        <v>10581</v>
       </c>
       <c r="G77">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="H77">
         <v>4</v>
       </c>
       <c r="I77" s="2">
         <f t="shared" si="6"/>
-        <v>63.245553203367592</v>
+        <v>57.735026918962582</v>
       </c>
       <c r="J77" s="2">
         <f t="shared" si="7"/>
-        <v>56.920997883030836</v>
+        <v>51.961524227066327</v>
       </c>
       <c r="K77" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L77" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="M77" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="N77" s="3">
-        <v>1.5</v>
-      </c>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
       <c r="O77" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L77*VLOOKUP(E77,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M77*VLOOKUP(E77,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N77*VLOOKUP(E77,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>21x13x7</v>
+        <v>0x0x0</v>
+      </c>
+      <c r="P77" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="B78">
-        <v>1986</v>
+        <v>1974</v>
       </c>
       <c r="C78">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -4707,21 +4724,21 @@
       </c>
       <c r="F78">
         <f>IF(B78 &gt; 1900, ((B78-1900)*10)+400+D78, ((B78-1730)*2)+D78)+VLOOKUP(E78,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10861</v>
+        <v>10741</v>
       </c>
       <c r="G78">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="H78">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I78" s="2">
-        <f t="shared" ref="I78" si="9">SQRT(G78*H78)/$B$1</f>
-        <v>89.442719099991592</v>
+        <f t="shared" si="6"/>
+        <v>74.833147735478832</v>
       </c>
       <c r="J78" s="2">
         <f t="shared" si="7"/>
-        <v>80.498447189992433</v>
+        <v>67.349832961930957</v>
       </c>
       <c r="K78" s="2" t="s">
         <v>33</v>
@@ -4737,14 +4754,14 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B79">
-        <v>1994</v>
+        <v>1976</v>
       </c>
       <c r="C79">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -4754,30 +4771,30 @@
       </c>
       <c r="F79">
         <f>IF(B79 &gt; 1900, ((B79-1900)*10)+400+D79, ((B79-1730)*2)+D79)+VLOOKUP(E79,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10941</v>
+        <v>10761</v>
       </c>
       <c r="G79">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="H79">
         <v>4</v>
       </c>
       <c r="I79" s="2">
         <f t="shared" si="6"/>
-        <v>73.029674334022147</v>
+        <v>63.245553203367592</v>
       </c>
       <c r="J79" s="2">
         <f t="shared" si="7"/>
-        <v>65.726706900619931</v>
+        <v>56.920997883030836</v>
       </c>
       <c r="K79" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L79" s="3">
-        <v>5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="M79" s="3">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="N79" s="3">
         <v>1.5</v>
@@ -4787,19 +4804,19 @@
 ROUND(L79*VLOOKUP(E79,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M79*VLOOKUP(E79,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N79*VLOOKUP(E79,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>23x14x7</v>
+        <v>21x13x7</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="B80">
-        <v>1997</v>
+        <v>1986</v>
       </c>
       <c r="C80">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -4809,27 +4826,25 @@
       </c>
       <c r="F80">
         <f>IF(B80 &gt; 1900, ((B80-1900)*10)+400+D80, ((B80-1730)*2)+D80)+VLOOKUP(E80,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>10971</v>
+        <v>10861</v>
       </c>
       <c r="G80">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H80">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I80" s="2">
         <f t="shared" si="6"/>
-        <v>67.082039324993701</v>
+        <v>89.442719099991592</v>
       </c>
       <c r="J80" s="2">
         <f t="shared" si="7"/>
-        <v>60.373835392494335</v>
+        <v>80.498447189992433</v>
       </c>
       <c r="K80" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
       <c r="N80" s="3"/>
       <c r="O80" s="2" t="str">
         <f>CONCATENATE(
@@ -4838,20 +4853,17 @@
 ROUND(N80*VLOOKUP(E80,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
-      <c r="P80" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B81">
-        <v>2004</v>
+        <v>1994</v>
       </c>
       <c r="C81">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -4861,46 +4873,52 @@
       </c>
       <c r="F81">
         <f>IF(B81 &gt; 1900, ((B81-1900)*10)+400+D81, ((B81-1730)*2)+D81)+VLOOKUP(E81,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>11041</v>
+        <v>10941</v>
       </c>
       <c r="G81">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="H81">
         <v>4</v>
       </c>
       <c r="I81" s="2">
         <f t="shared" si="6"/>
-        <v>80.277297191948648</v>
+        <v>73.029674334022147</v>
       </c>
       <c r="J81" s="2">
         <f t="shared" si="7"/>
-        <v>72.249567472753782</v>
+        <v>65.726706900619931</v>
       </c>
       <c r="K81" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L81" s="3"/>
-      <c r="M81" s="3"/>
-      <c r="N81" s="3"/>
+      <c r="L81" s="3">
+        <v>5</v>
+      </c>
+      <c r="M81" s="3">
+        <v>2</v>
+      </c>
+      <c r="N81" s="3">
+        <v>1.5</v>
+      </c>
       <c r="O81" s="2" t="str">
         <f>CONCATENATE(
 ROUND(L81*VLOOKUP(E81,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M81*VLOOKUP(E81,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N81*VLOOKUP(E81,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>0x0x0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+        <v>23x14x7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B82">
-        <v>2009</v>
+        <v>1997</v>
       </c>
       <c r="C82">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -4910,21 +4928,21 @@
       </c>
       <c r="F82">
         <f>IF(B82 &gt; 1900, ((B82-1900)*10)+400+D82, ((B82-1730)*2)+D82)+VLOOKUP(E82,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>11091</v>
+        <v>10971</v>
       </c>
       <c r="G82">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="H82">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I82" s="2">
         <f t="shared" si="6"/>
-        <v>70.553368295055762</v>
+        <v>67.082039324993701</v>
       </c>
       <c r="J82" s="2">
         <f t="shared" si="7"/>
-        <v>63.498031465550184</v>
+        <v>60.373835392494335</v>
       </c>
       <c r="K82" s="2" t="s">
         <v>33</v>
@@ -4939,17 +4957,20 @@
 ROUND(N82*VLOOKUP(E82,'ID Scheme'!$A$2:$E$5,4),0))</f>
         <v>0x0x0</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P82" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="B83">
-        <v>2014</v>
+        <v>2004</v>
       </c>
       <c r="C83">
-        <f t="shared" ref="C83" si="10">B83-B82</f>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -4959,25 +4980,27 @@
       </c>
       <c r="F83">
         <f>IF(B83 &gt; 1900, ((B83-1900)*10)+400+D83, ((B83-1730)*2)+D83)+VLOOKUP(E83,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
-        <v>11141</v>
+        <v>11041</v>
       </c>
       <c r="G83">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="H83">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I83" s="2">
         <f t="shared" si="6"/>
-        <v>97.467943448089642</v>
+        <v>80.277297191948648</v>
       </c>
       <c r="J83" s="2">
-        <f t="shared" ref="J83" si="11">I83*0.9</f>
-        <v>87.72114910328068</v>
+        <f t="shared" si="7"/>
+        <v>72.249567472753782</v>
       </c>
       <c r="K83" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="L83" s="3"/>
+      <c r="M83" s="3"/>
       <c r="N83" s="3"/>
       <c r="O83" s="2" t="str">
         <f>CONCATENATE(
@@ -4987,31 +5010,132 @@
         <v>0x0x0</v>
       </c>
     </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>67</v>
+      </c>
+      <c r="B84">
+        <v>2009</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84" t="s">
+        <v>62</v>
+      </c>
+      <c r="F84">
+        <f>IF(B84 &gt; 1900, ((B84-1900)*10)+400+D84, ((B84-1730)*2)+D84)+VLOOKUP(E84,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>11091</v>
+      </c>
+      <c r="G84">
+        <v>112</v>
+      </c>
+      <c r="H84">
+        <v>4</v>
+      </c>
+      <c r="I84" s="2">
+        <f t="shared" si="6"/>
+        <v>70.553368295055762</v>
+      </c>
+      <c r="J84" s="2">
+        <f t="shared" si="7"/>
+        <v>63.498031465550184</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L84" s="3"/>
+      <c r="M84" s="3"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L84*VLOOKUP(E84,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M84*VLOOKUP(E84,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N84*VLOOKUP(E84,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>119</v>
+      </c>
+      <c r="B85">
+        <v>2014</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>62</v>
+      </c>
+      <c r="F85">
+        <f>IF(B85 &gt; 1900, ((B85-1900)*10)+400+D85, ((B85-1730)*2)+D85)+VLOOKUP(E85,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>11141</v>
+      </c>
+      <c r="G85">
+        <v>95</v>
+      </c>
+      <c r="H85">
+        <v>9</v>
+      </c>
+      <c r="I85" s="2">
+        <f t="shared" si="6"/>
+        <v>97.467943448089642</v>
+      </c>
+      <c r="J85" s="2">
+        <f t="shared" si="7"/>
+        <v>87.72114910328068</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N85" s="3"/>
+      <c r="O85" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L85*VLOOKUP(E85,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M85*VLOOKUP(E85,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N85*VLOOKUP(E85,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A4:P82">
-    <sortCondition ref="F20"/>
+  <sortState ref="A4:P85">
+    <sortCondition ref="F65"/>
   </sortState>
-  <conditionalFormatting sqref="C1:C2 C4:C20 C22:C24 C26:C51 C53:C82 C84:C1048576">
+  <conditionalFormatting sqref="C1:C2 C22:C24 C26:C51 C53:C82 C84 C4:C20 C86:C1048576">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
     <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+  <conditionalFormatting sqref="C52">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
+  <conditionalFormatting sqref="C25">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="C83">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C83">
+  <conditionalFormatting sqref="C85">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
@@ -5035,9 +5159,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5132,6 +5256,23 @@
         <v>7.2</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6">
+        <v>12600</v>
+      </c>
+      <c r="C6">
+        <v>4.67</v>
+      </c>
+      <c r="D6">
+        <v>4.84</v>
+      </c>
+      <c r="E6">
+        <v>7.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Grantham steam tram
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC25AD52-DCE2-4F59-92C7-9B7514F43D60}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC037EF-B2BD-49A0-ADC9-4696D5FFE5B4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8190" windowHeight="2400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8190" windowHeight="2400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ID Scheme" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="145">
   <si>
     <t>Vehicle</t>
   </si>
@@ -398,6 +398,69 @@
   </si>
   <si>
     <t>Tram</t>
+  </si>
+  <si>
+    <t>Horse-Drawn Tram</t>
+  </si>
+  <si>
+    <t>Grantham's Steam Tram</t>
+  </si>
+  <si>
+    <t>Progress TwinSet</t>
+  </si>
+  <si>
+    <t>Coronation Tram</t>
+  </si>
+  <si>
+    <t>Conduit Car</t>
+  </si>
+  <si>
+    <t>Marton Box Car</t>
+  </si>
+  <si>
+    <t>Standard Car</t>
+  </si>
+  <si>
+    <t>Fleetwood Box Car</t>
+  </si>
+  <si>
+    <t>Jubilee Tram</t>
+  </si>
+  <si>
+    <t>Centenary Tram</t>
+  </si>
+  <si>
+    <t>CR4000</t>
+  </si>
+  <si>
+    <t>CAF Urbos 3</t>
+  </si>
+  <si>
+    <t>LHB P86 Stock</t>
+  </si>
+  <si>
+    <t>Bombardier B07 Stock</t>
+  </si>
+  <si>
+    <t>MER Tunnel Car</t>
+  </si>
+  <si>
+    <t>MER Winter Saloon</t>
+  </si>
+  <si>
+    <t>80hp</t>
+  </si>
+  <si>
+    <t>UEC Blackpool "Toastrack"</t>
+  </si>
+  <si>
+    <t>English Electric Balloon</t>
+  </si>
+  <si>
+    <t>114hp</t>
+  </si>
+  <si>
+    <t>56+66 pax, 114hp</t>
   </si>
 </sst>
 </file>
@@ -824,11 +887,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:P103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1391,7 +1454,7 @@
 ROUND(L13*VLOOKUP(E13,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M13*VLOOKUP(E13,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N13*VLOOKUP(E13,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>39x17x13</v>
+        <v>78x35x25</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1495,7 +1558,7 @@
 ROUND(L15*VLOOKUP(E15,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M15*VLOOKUP(E15,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N15*VLOOKUP(E15,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>42x17x19</v>
+        <v>85x35x38</v>
       </c>
       <c r="P15" t="s">
         <v>105</v>
@@ -1553,7 +1616,7 @@
 ROUND(L16*VLOOKUP(E16,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M16*VLOOKUP(E16,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N16*VLOOKUP(E16,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>42x17x13</v>
+        <v>85x35x25</v>
       </c>
       <c r="P16" t="s">
         <v>105</v>
@@ -1756,7 +1819,7 @@
 ROUND(L20*VLOOKUP(E20,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M20*VLOOKUP(E20,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N20*VLOOKUP(E20,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>51x18x0</v>
+        <v>103x36x0</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1809,7 +1872,7 @@
 ROUND(L21*VLOOKUP(E21,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M21*VLOOKUP(E21,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N21*VLOOKUP(E21,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>53x18x0</v>
+        <v>106x36x0</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1864,7 +1927,7 @@
 ROUND(L22*VLOOKUP(E22,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M22*VLOOKUP(E22,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N22*VLOOKUP(E22,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>56x18x20</v>
+        <v>112x36x41</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -1919,7 +1982,7 @@
 ROUND(L23*VLOOKUP(E23,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M23*VLOOKUP(E23,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N23*VLOOKUP(E23,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>56x18x16</v>
+        <v>112x36x32</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -1974,7 +2037,7 @@
 ROUND(L24*VLOOKUP(E24,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M24*VLOOKUP(E24,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N24*VLOOKUP(E24,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>56x18x20</v>
+        <v>112x36x41</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -2029,7 +2092,7 @@
 ROUND(L25*VLOOKUP(E25,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M25*VLOOKUP(E25,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N25*VLOOKUP(E25,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>48x17x13</v>
+        <v>95x35x26</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -2084,7 +2147,7 @@
 ROUND(L26*VLOOKUP(E26,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M26*VLOOKUP(E26,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N26*VLOOKUP(E26,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>48x17x13</v>
+        <v>95x35x26</v>
       </c>
       <c r="P26" t="s">
         <v>117</v>
@@ -2142,7 +2205,7 @@
 ROUND(L27*VLOOKUP(E27,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M27*VLOOKUP(E27,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N27*VLOOKUP(E27,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>48x17x13</v>
+        <v>95x33x26</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -2197,7 +2260,7 @@
 ROUND(L28*VLOOKUP(E28,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M28*VLOOKUP(E28,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N28*VLOOKUP(E28,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>56x18x16</v>
+        <v>112x36x32</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -2252,7 +2315,7 @@
 ROUND(L29*VLOOKUP(E29,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M29*VLOOKUP(E29,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N29*VLOOKUP(E29,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>84x18x15</v>
+        <v>168x36x31</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -2307,7 +2370,7 @@
 ROUND(L30*VLOOKUP(E30,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M30*VLOOKUP(E30,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N30*VLOOKUP(E30,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>53x18x20</v>
+        <v>106x37x41</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2411,7 +2474,7 @@
 ROUND(L32*VLOOKUP(E32,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M32*VLOOKUP(E32,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N32*VLOOKUP(E32,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>48x17x13</v>
+        <v>95x33x26</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -2711,7 +2774,7 @@
 ROUND(L38*VLOOKUP(E38,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M38*VLOOKUP(E38,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N38*VLOOKUP(E38,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>16x14x12</v>
+        <v>32x29x24</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -3058,7 +3121,7 @@
 ROUND(L45*VLOOKUP(E45,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M45*VLOOKUP(E45,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N45*VLOOKUP(E45,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
+        <v>58x32x25</v>
       </c>
       <c r="P45" t="s">
         <v>99</v>
@@ -3315,7 +3378,7 @@
 ROUND(L50*VLOOKUP(E50,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M50*VLOOKUP(E50,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N50*VLOOKUP(E50,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
+        <v>58x32x25</v>
       </c>
       <c r="P50" t="s">
         <v>98</v>
@@ -3373,7 +3436,7 @@
 ROUND(L51*VLOOKUP(E51,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M51*VLOOKUP(E51,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N51*VLOOKUP(E51,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>40x18x14</v>
+        <v>79x36x27</v>
       </c>
       <c r="P51" t="s">
         <v>31</v>
@@ -3581,7 +3644,7 @@
 ROUND(L55*VLOOKUP(E55,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M55*VLOOKUP(E55,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N55*VLOOKUP(E55,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
+        <v>58x32x25</v>
       </c>
       <c r="P55" t="s">
         <v>97</v>
@@ -3688,7 +3751,7 @@
 ROUND(L57*VLOOKUP(E57,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M57*VLOOKUP(E57,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N57*VLOOKUP(E57,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>36x16x13</v>
+        <v>72x32x25</v>
       </c>
       <c r="P57" t="s">
         <v>107</v>
@@ -3844,7 +3907,7 @@
 ROUND(L60*VLOOKUP(E60,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M60*VLOOKUP(E60,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N60*VLOOKUP(E60,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
+        <v>58x32x25</v>
       </c>
       <c r="P60" t="s">
         <v>100</v>
@@ -4049,7 +4112,7 @@
 ROUND(L64*VLOOKUP(E64,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M64*VLOOKUP(E64,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N64*VLOOKUP(E64,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>40x16x13</v>
+        <v>79x32x25</v>
       </c>
       <c r="P64" t="s">
         <v>109</v>
@@ -4156,7 +4219,7 @@
 ROUND(L66*VLOOKUP(E66,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M66*VLOOKUP(E66,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N66*VLOOKUP(E66,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>29x16x13</v>
+        <v>58x32x25</v>
       </c>
       <c r="P66" t="s">
         <v>96</v>
@@ -4240,11 +4303,11 @@
         <v>4</v>
       </c>
       <c r="I68" s="2">
-        <f t="shared" ref="I68:I99" si="6">SQRT(G68*H68)/$B$1</f>
+        <f t="shared" ref="I68:I85" si="6">SQRT(G68*H68)/$B$1</f>
         <v>42.163702135578397</v>
       </c>
       <c r="J68" s="2">
-        <f t="shared" ref="J68:J99" si="7">I68*0.9</f>
+        <f t="shared" ref="J68:J85" si="7">I68*0.9</f>
         <v>37.94733192202056</v>
       </c>
       <c r="K68" s="2" t="s">
@@ -4269,7 +4332,7 @@
         <v>1938</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69:C100" si="8">B69-B68</f>
+        <f t="shared" ref="C69:C85" si="8">B69-B68</f>
         <v>26</v>
       </c>
       <c r="D69">
@@ -4804,7 +4867,7 @@
 ROUND(L79*VLOOKUP(E79,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M79*VLOOKUP(E79,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N79*VLOOKUP(E79,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>21x13x7</v>
+        <v>41x26x15</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -4906,7 +4969,7 @@
 ROUND(L81*VLOOKUP(E81,'ID Scheme'!$A$2:$E$5,3),0), "x",
 ROUND(M81*VLOOKUP(E81,'ID Scheme'!$A$2:$E$5,5),0), "x",
 ROUND(N81*VLOOKUP(E81,'ID Scheme'!$A$2:$E$5,4),0))</f>
-        <v>23x14x7</v>
+        <v>47x29x15</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
@@ -5106,11 +5169,742 @@
         <v>0x0x0</v>
       </c>
     </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>124</v>
+      </c>
+      <c r="B86">
+        <v>1860</v>
+      </c>
+      <c r="C86">
+        <f t="shared" ref="C86" si="9">B86-B85</f>
+        <v>-154</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>123</v>
+      </c>
+      <c r="F86">
+        <f>IF(B86 &gt; 1900, ((B86-1900)*10)+400+D86, ((B86-1730)*2)+D86)+VLOOKUP(E86,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>12861</v>
+      </c>
+      <c r="G86">
+        <v>18</v>
+      </c>
+      <c r="H86">
+        <v>60</v>
+      </c>
+      <c r="I86" s="2">
+        <f t="shared" ref="I86" si="10">SQRT(G86*H86)/$B$1</f>
+        <v>109.54451150103323</v>
+      </c>
+      <c r="J86" s="2">
+        <f t="shared" ref="J86" si="11">I86*0.9</f>
+        <v>98.590060350929903</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N86" s="3"/>
+      <c r="O86" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L86*VLOOKUP(E86,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M86*VLOOKUP(E86,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N86*VLOOKUP(E86,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>125</v>
+      </c>
+      <c r="B87">
+        <v>1873</v>
+      </c>
+      <c r="C87">
+        <f t="shared" ref="C87" si="12">B87-B86</f>
+        <v>13</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>123</v>
+      </c>
+      <c r="F87">
+        <f>IF(B87 &gt; 1900, ((B87-1900)*10)+400+D87, ((B87-1730)*2)+D87)+VLOOKUP(E87,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>12887</v>
+      </c>
+      <c r="G87">
+        <v>20</v>
+      </c>
+      <c r="H87">
+        <v>50</v>
+      </c>
+      <c r="I87" s="2">
+        <f t="shared" ref="I87" si="13">SQRT(G87*H87)/$B$1</f>
+        <v>105.40925533894598</v>
+      </c>
+      <c r="J87" s="2">
+        <f t="shared" ref="J87" si="14">I87*0.9</f>
+        <v>94.868329805051388</v>
+      </c>
+      <c r="K87" s="2"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L87*VLOOKUP(E87,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M87*VLOOKUP(E87,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N87*VLOOKUP(E87,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>138</v>
+      </c>
+      <c r="B88">
+        <v>1894</v>
+      </c>
+      <c r="C88">
+        <f t="shared" ref="C88:C103" si="15">B88-B87</f>
+        <v>21</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88" t="s">
+        <v>123</v>
+      </c>
+      <c r="F88">
+        <f>IF(B88 &gt; 1900, ((B88-1900)*10)+400+D88, ((B88-1730)*2)+D88)+VLOOKUP(E88,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>12929</v>
+      </c>
+      <c r="G88">
+        <v>22</v>
+      </c>
+      <c r="H88">
+        <v>44</v>
+      </c>
+      <c r="I88" s="2">
+        <f t="shared" ref="I88:I103" si="16">SQRT(G88*H88)/$B$1</f>
+        <v>103.70899457402697</v>
+      </c>
+      <c r="J88" s="2">
+        <f t="shared" ref="J88:J103" si="17">I88*0.9</f>
+        <v>93.338095116624274</v>
+      </c>
+      <c r="K88" s="2"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L88*VLOOKUP(E88,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M88*VLOOKUP(E88,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N88*VLOOKUP(E88,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+      <c r="P88" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>139</v>
+      </c>
+      <c r="B89">
+        <v>1899</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89" t="s">
+        <v>123</v>
+      </c>
+      <c r="F89">
+        <f>IF(B89 &gt; 1900, ((B89-1900)*10)+400+D89, ((B89-1730)*2)+D89)+VLOOKUP(E89,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>12939</v>
+      </c>
+      <c r="G89">
+        <v>24</v>
+      </c>
+      <c r="H89">
+        <v>48</v>
+      </c>
+      <c r="I89" s="2">
+        <f t="shared" si="16"/>
+        <v>113.13708498984759</v>
+      </c>
+      <c r="J89" s="2">
+        <f t="shared" si="17"/>
+        <v>101.82337649086284</v>
+      </c>
+      <c r="K89" s="2"/>
+      <c r="N89" s="3"/>
+      <c r="O89" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L89*VLOOKUP(E89,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M89*VLOOKUP(E89,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N89*VLOOKUP(E89,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+      <c r="P89" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>141</v>
+      </c>
+      <c r="B90">
+        <v>1911</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="15"/>
+        <v>12</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90" t="s">
+        <v>123</v>
+      </c>
+      <c r="F90">
+        <f>IF(B90 &gt; 1900, ((B90-1900)*10)+400+D90, ((B90-1730)*2)+D90)+VLOOKUP(E90,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>13111</v>
+      </c>
+      <c r="G90">
+        <v>22</v>
+      </c>
+      <c r="H90">
+        <v>69</v>
+      </c>
+      <c r="I90" s="2">
+        <f t="shared" si="16"/>
+        <v>129.8717315918544</v>
+      </c>
+      <c r="J90" s="2">
+        <f t="shared" si="17"/>
+        <v>116.88455843266897</v>
+      </c>
+      <c r="K90" s="2"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L90*VLOOKUP(E90,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M90*VLOOKUP(E90,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N90*VLOOKUP(E90,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+      <c r="P90" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>142</v>
+      </c>
+      <c r="B91">
+        <v>1934</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="15"/>
+        <v>23</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91" t="s">
+        <v>123</v>
+      </c>
+      <c r="F91">
+        <f>IF(B91 &gt; 1900, ((B91-1900)*10)+400+D91, ((B91-1730)*2)+D91)+VLOOKUP(E91,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>13341</v>
+      </c>
+      <c r="G91">
+        <v>43</v>
+      </c>
+      <c r="H91">
+        <v>84</v>
+      </c>
+      <c r="I91" s="2">
+        <f t="shared" si="16"/>
+        <v>200.33305601755626</v>
+      </c>
+      <c r="J91" s="2">
+        <f t="shared" si="17"/>
+        <v>180.29975041580064</v>
+      </c>
+      <c r="K91" s="2"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L91*VLOOKUP(E91,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M91*VLOOKUP(E91,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N91*VLOOKUP(E91,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+      <c r="P91" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>126</v>
+      </c>
+      <c r="B92">
+        <v>1960</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="15"/>
+        <v>26</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92" t="s">
+        <v>123</v>
+      </c>
+      <c r="F92">
+        <f>IF(B92 &gt; 1900, ((B92-1900)*10)+400+D92, ((B92-1730)*2)+D92)+VLOOKUP(E92,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>13601</v>
+      </c>
+      <c r="G92">
+        <v>40</v>
+      </c>
+      <c r="H92">
+        <v>122</v>
+      </c>
+      <c r="I92" s="2">
+        <f t="shared" si="16"/>
+        <v>232.8566559543064</v>
+      </c>
+      <c r="J92" s="2">
+        <f t="shared" si="17"/>
+        <v>209.57099035887578</v>
+      </c>
+      <c r="K92" s="2"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L92*VLOOKUP(E92,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M92*VLOOKUP(E92,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N92*VLOOKUP(E92,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+      <c r="P92" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>127</v>
+      </c>
+      <c r="B93">
+        <v>1952</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="15"/>
+        <v>-8</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93" t="s">
+        <v>123</v>
+      </c>
+      <c r="F93">
+        <f>IF(B93 &gt; 1900, ((B93-1900)*10)+400+D93, ((B93-1730)*2)+D93)+VLOOKUP(E93,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>13521</v>
+      </c>
+      <c r="I93" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J93" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K93" s="2"/>
+      <c r="N93" s="3"/>
+      <c r="O93" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L93*VLOOKUP(E93,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M93*VLOOKUP(E93,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N93*VLOOKUP(E93,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>128</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="15"/>
+        <v>-1952</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94" t="s">
+        <v>123</v>
+      </c>
+      <c r="F94">
+        <f>IF(B94 &gt; 1900, ((B94-1900)*10)+400+D94, ((B94-1730)*2)+D94)+VLOOKUP(E94,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>9141</v>
+      </c>
+      <c r="I94" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J94" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K94" s="2"/>
+      <c r="N94" s="3"/>
+      <c r="O94" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L94*VLOOKUP(E94,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M94*VLOOKUP(E94,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N94*VLOOKUP(E94,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>129</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95" t="s">
+        <v>123</v>
+      </c>
+      <c r="F95">
+        <f>IF(B95 &gt; 1900, ((B95-1900)*10)+400+D95, ((B95-1730)*2)+D95)+VLOOKUP(E95,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>9141</v>
+      </c>
+      <c r="I95" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J95" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K95" s="2"/>
+      <c r="N95" s="3"/>
+      <c r="O95" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L95*VLOOKUP(E95,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M95*VLOOKUP(E95,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N95*VLOOKUP(E95,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>130</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96" t="s">
+        <v>123</v>
+      </c>
+      <c r="F96">
+        <f>IF(B96 &gt; 1900, ((B96-1900)*10)+400+D96, ((B96-1730)*2)+D96)+VLOOKUP(E96,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>9141</v>
+      </c>
+      <c r="I96" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J96" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K96" s="2"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L96*VLOOKUP(E96,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M96*VLOOKUP(E96,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N96*VLOOKUP(E96,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>131</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97" t="s">
+        <v>123</v>
+      </c>
+      <c r="F97">
+        <f>IF(B97 &gt; 1900, ((B97-1900)*10)+400+D97, ((B97-1730)*2)+D97)+VLOOKUP(E97,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>9141</v>
+      </c>
+      <c r="I97" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J97" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K97" s="2"/>
+      <c r="N97" s="3"/>
+      <c r="O97" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L97*VLOOKUP(E97,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M97*VLOOKUP(E97,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N97*VLOOKUP(E97,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>132</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98" t="s">
+        <v>123</v>
+      </c>
+      <c r="F98">
+        <f>IF(B98 &gt; 1900, ((B98-1900)*10)+400+D98, ((B98-1730)*2)+D98)+VLOOKUP(E98,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>9141</v>
+      </c>
+      <c r="I98" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J98" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K98" s="2"/>
+      <c r="N98" s="3"/>
+      <c r="O98" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L98*VLOOKUP(E98,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M98*VLOOKUP(E98,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N98*VLOOKUP(E98,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>133</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99" t="s">
+        <v>123</v>
+      </c>
+      <c r="F99">
+        <f>IF(B99 &gt; 1900, ((B99-1900)*10)+400+D99, ((B99-1730)*2)+D99)+VLOOKUP(E99,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>9141</v>
+      </c>
+      <c r="I99" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J99" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K99" s="2"/>
+      <c r="N99" s="3"/>
+      <c r="O99" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L99*VLOOKUP(E99,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M99*VLOOKUP(E99,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N99*VLOOKUP(E99,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>134</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100" t="s">
+        <v>123</v>
+      </c>
+      <c r="F100">
+        <f>IF(B100 &gt; 1900, ((B100-1900)*10)+400+D100, ((B100-1730)*2)+D100)+VLOOKUP(E100,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>9141</v>
+      </c>
+      <c r="I100" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J100" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K100" s="2"/>
+      <c r="N100" s="3"/>
+      <c r="O100" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L100*VLOOKUP(E100,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M100*VLOOKUP(E100,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N100*VLOOKUP(E100,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>135</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101" t="s">
+        <v>123</v>
+      </c>
+      <c r="F101">
+        <f>IF(B101 &gt; 1900, ((B101-1900)*10)+400+D101, ((B101-1730)*2)+D101)+VLOOKUP(E101,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>9141</v>
+      </c>
+      <c r="I101" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J101" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K101" s="2"/>
+      <c r="N101" s="3"/>
+      <c r="O101" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L101*VLOOKUP(E101,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M101*VLOOKUP(E101,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N101*VLOOKUP(E101,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>136</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102" t="s">
+        <v>123</v>
+      </c>
+      <c r="F102">
+        <f>IF(B102 &gt; 1900, ((B102-1900)*10)+400+D102, ((B102-1730)*2)+D102)+VLOOKUP(E102,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>9141</v>
+      </c>
+      <c r="I102" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J102" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K102" s="2"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L102*VLOOKUP(E102,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M102*VLOOKUP(E102,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N102*VLOOKUP(E102,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>137</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103" t="s">
+        <v>123</v>
+      </c>
+      <c r="F103">
+        <f>IF(B103 &gt; 1900, ((B103-1900)*10)+400+D103, ((B103-1730)*2)+D103)+VLOOKUP(E103,'ID Scheme'!$A$2:$B$6,2, FALSE)</f>
+        <v>9141</v>
+      </c>
+      <c r="I103" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J103" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K103" s="2"/>
+      <c r="N103" s="3"/>
+      <c r="O103" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(L103*VLOOKUP(E103,'ID Scheme'!$A$2:$E$5,3),0), "x",
+ROUND(M103*VLOOKUP(E103,'ID Scheme'!$A$2:$E$5,5),0), "x",
+ROUND(N103*VLOOKUP(E103,'ID Scheme'!$A$2:$E$5,4),0))</f>
+        <v>0x0x0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A4:P85">
     <sortCondition ref="F65"/>
   </sortState>
-  <conditionalFormatting sqref="C1:C2 C22:C24 C26:C51 C53:C82 C84 C4:C20 C86:C1048576">
+  <conditionalFormatting sqref="C1:C2 C22:C24 C26:C51 C53:C82 C84 C4:C20 C104:C1048576">
     <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
@@ -5135,7 +5929,7 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85">
+  <conditionalFormatting sqref="C85:C103">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
@@ -5147,7 +5941,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
-            <xm:f>'ID Scheme'!$A$2:$A$5</xm:f>
+            <xm:f>'ID Scheme'!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
@@ -5161,7 +5955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5196,13 +5990,13 @@
         <v>600</v>
       </c>
       <c r="C2">
-        <v>4.67</v>
+        <v>9.34</v>
       </c>
       <c r="D2">
-        <v>4.84</v>
+        <v>9.68</v>
       </c>
       <c r="E2">
-        <v>7.2</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5213,13 +6007,13 @@
         <v>3600</v>
       </c>
       <c r="C3">
-        <v>4.67</v>
+        <v>9.34</v>
       </c>
       <c r="D3">
-        <v>4.84</v>
+        <v>9.68</v>
       </c>
       <c r="E3">
-        <v>7.2</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5230,13 +6024,13 @@
         <v>6600</v>
       </c>
       <c r="C4">
-        <v>4.67</v>
+        <v>9.34</v>
       </c>
       <c r="D4">
-        <v>4.84</v>
+        <v>9.68</v>
       </c>
       <c r="E4">
-        <v>7.2</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5247,13 +6041,13 @@
         <v>9600</v>
       </c>
       <c r="C5">
-        <v>4.67</v>
+        <v>9.34</v>
       </c>
       <c r="D5">
-        <v>4.84</v>
+        <v>9.68</v>
       </c>
       <c r="E5">
-        <v>7.2</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -5264,13 +6058,13 @@
         <v>12600</v>
       </c>
       <c r="C6">
-        <v>4.67</v>
+        <v>9.34</v>
       </c>
       <c r="D6">
-        <v>4.84</v>
+        <v>9.68</v>
       </c>
       <c r="E6">
-        <v>7.2</v>
+        <v>14.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add y10 and Drewry
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054FD170-58F7-4FD2-94CA-356F5761083B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF017DE9-CDDF-4D59-88B1-6C847465014C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8190" windowHeight="2400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,17 +19,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="166">
   <si>
     <t>Vehicle</t>
   </si>
@@ -521,6 +516,12 @@
   </si>
   <si>
     <t>Y6 0-4-0</t>
+  </si>
+  <si>
+    <t>Y10 "Super Sentinel"</t>
+  </si>
+  <si>
+    <t>Drewry Shunter</t>
   </si>
 </sst>
 </file>
@@ -576,7 +577,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -897,11 +918,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R110"/>
+  <dimension ref="A1:R112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H109" sqref="H109"/>
+      <pane ySplit="3" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7062,10 +7083,10 @@
         <v>16031</v>
       </c>
       <c r="G110">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H110">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="I110">
         <v>30</v>
@@ -7075,11 +7096,11 @@
       </c>
       <c r="K110" s="2">
         <f>SQRT(G110*H110)*POWER((MIN(I110,20)+SQRT(MAX(I110-20,0))),0.9)*$B$1</f>
-        <v>43.061647353748292</v>
+        <v>46.094739623279715</v>
       </c>
       <c r="L110" s="2">
         <f>POWER((G110*G110*H110), 0.33)*LOG10(J110)*10*$B$1</f>
-        <v>38.97435985704201</v>
+        <v>39.61127712007552</v>
       </c>
       <c r="M110" s="2" t="s">
         <v>33</v>
@@ -7094,6 +7115,116 @@
 ROUND(O110*VLOOKUP(E110,'ID Scheme'!$A$2:$E$7,5),0), "x",
 ROUND(P110*VLOOKUP(E110,'ID Scheme'!$A$2:$E$7,4),0))</f>
         <v>56x0x0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>164</v>
+      </c>
+      <c r="B111">
+        <v>1930</v>
+      </c>
+      <c r="C111">
+        <f>B111-B110</f>
+        <v>27</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111" t="s">
+        <v>160</v>
+      </c>
+      <c r="F111">
+        <v>16041</v>
+      </c>
+      <c r="G111">
+        <v>24</v>
+      </c>
+      <c r="H111">
+        <v>60</v>
+      </c>
+      <c r="I111">
+        <v>26</v>
+      </c>
+      <c r="J111">
+        <v>200</v>
+      </c>
+      <c r="K111" s="2">
+        <f>SQRT(G111*H111)*POWER((MIN(I111,20)+SQRT(MAX(I111-20,0))),0.9)*$B$1</f>
+        <v>46.808889320396581</v>
+      </c>
+      <c r="L111" s="2">
+        <f>POWER((G111*G111*H111), 0.33)*LOG10(J111)*10*$B$1</f>
+        <v>54.289129200123334</v>
+      </c>
+      <c r="M111" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N111">
+        <v>7</v>
+      </c>
+      <c r="P111" s="3"/>
+      <c r="Q111" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(N111*VLOOKUP(E111,'ID Scheme'!$A$2:$E$7,3),0), "x",
+ROUND(O111*VLOOKUP(E111,'ID Scheme'!$A$2:$E$7,5),0), "x",
+ROUND(P111*VLOOKUP(E111,'ID Scheme'!$A$2:$E$7,4),0))</f>
+        <v>65x0x0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>165</v>
+      </c>
+      <c r="B112">
+        <v>1952</v>
+      </c>
+      <c r="C112">
+        <f>B112-B111</f>
+        <v>22</v>
+      </c>
+      <c r="D112">
+        <v>2</v>
+      </c>
+      <c r="E112" t="s">
+        <v>160</v>
+      </c>
+      <c r="F112">
+        <v>16051</v>
+      </c>
+      <c r="G112">
+        <v>27</v>
+      </c>
+      <c r="H112">
+        <v>60</v>
+      </c>
+      <c r="I112">
+        <v>26</v>
+      </c>
+      <c r="J112">
+        <v>152</v>
+      </c>
+      <c r="K112" s="2">
+        <f>SQRT(G112*H112)*POWER((MIN(I112,20)+SQRT(MAX(I112-20,0))),0.9)*$B$1</f>
+        <v>49.648324587394477</v>
+      </c>
+      <c r="L112" s="2">
+        <f>POWER((G112*G112*H112), 0.33)*LOG10(J112)*10*$B$1</f>
+        <v>55.638430948840913</v>
+      </c>
+      <c r="M112" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N112">
+        <v>7</v>
+      </c>
+      <c r="P112" s="3"/>
+      <c r="Q112" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(N112*VLOOKUP(E112,'ID Scheme'!$A$2:$E$7,3),0), "x",
+ROUND(O112*VLOOKUP(E112,'ID Scheme'!$A$2:$E$7,5),0), "x",
+ROUND(P112*VLOOKUP(E112,'ID Scheme'!$A$2:$E$7,4),0))</f>
+        <v>65x0x0</v>
       </c>
     </row>
   </sheetData>
@@ -7105,8 +7236,18 @@
   <sortState ref="A4:R106">
     <sortCondition ref="A10"/>
   </sortState>
-  <conditionalFormatting sqref="C1:C2 C4:C1048576">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="greaterThan">
+  <conditionalFormatting sqref="C1:C2 C4:C110 C113:C1048576">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C111">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C112">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Re-rendered sprites for better contrast
</commit_message>
<xml_diff>
--- a/Tracking Table.xlsx
+++ b/Tracking Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF017DE9-CDDF-4D59-88B1-6C847465014C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106CDDE1-AA6C-4268-AE84-44BA9F6CAAC1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8190" windowHeight="2400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,12 +19,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="167">
   <si>
     <t>Vehicle</t>
   </si>
@@ -522,6 +527,9 @@
   </si>
   <si>
     <t>Drewry Shunter</t>
+  </si>
+  <si>
+    <t>FC Hibberd Planet</t>
   </si>
 </sst>
 </file>
@@ -918,11 +926,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R112"/>
+  <dimension ref="A1:R113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F111" sqref="F111"/>
+      <pane ySplit="3" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J110" sqref="J110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6627,7 +6635,9 @@
         <f t="shared" si="10"/>
         <v>124.02429472574501</v>
       </c>
-      <c r="M102" s="2"/>
+      <c r="M102" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="N102">
         <v>28</v>
       </c>
@@ -6734,20 +6744,28 @@
         <v>14081</v>
       </c>
       <c r="G104">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="H104">
         <v>284</v>
       </c>
+      <c r="I104">
+        <v>25</v>
+      </c>
+      <c r="J104">
+        <v>375</v>
+      </c>
       <c r="K104" s="2">
         <f t="shared" si="9"/>
-        <v>118.48883383446805</v>
-      </c>
-      <c r="L104" s="2" t="e">
+        <v>162.28129769016738</v>
+      </c>
+      <c r="L104" s="2">
         <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="M104" s="2"/>
+        <v>189.77921627665754</v>
+      </c>
+      <c r="M104" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="N104">
         <v>32</v>
       </c>
@@ -7174,49 +7192,49 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B112">
-        <v>1952</v>
+        <v>1948</v>
       </c>
       <c r="C112">
-        <f>B112-B111</f>
-        <v>22</v>
+        <f t="shared" ref="C112:C113" si="12">B112-B111</f>
+        <v>18</v>
       </c>
       <c r="D112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E112" t="s">
         <v>160</v>
       </c>
       <c r="F112">
-        <v>16051</v>
+        <v>16046</v>
       </c>
       <c r="G112">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H112">
         <v>60</v>
       </c>
       <c r="I112">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J112">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="K112" s="2">
         <f>SQRT(G112*H112)*POWER((MIN(I112,20)+SQRT(MAX(I112-20,0))),0.9)*$B$1</f>
-        <v>49.648324587394477</v>
+        <v>49.137157539542891</v>
       </c>
       <c r="L112" s="2">
         <f>POWER((G112*G112*H112), 0.33)*LOG10(J112)*10*$B$1</f>
-        <v>55.638430948840913</v>
+        <v>50.654513648978117</v>
       </c>
       <c r="M112" s="2" t="s">
         <v>33</v>
       </c>
       <c r="N112">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P112" s="3"/>
       <c r="Q112" s="2" t="str">
@@ -7224,6 +7242,61 @@
 ROUND(N112*VLOOKUP(E112,'ID Scheme'!$A$2:$E$7,3),0), "x",
 ROUND(O112*VLOOKUP(E112,'ID Scheme'!$A$2:$E$7,5),0), "x",
 ROUND(P112*VLOOKUP(E112,'ID Scheme'!$A$2:$E$7,4),0))</f>
+        <v>56x0x0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>165</v>
+      </c>
+      <c r="B113">
+        <v>1952</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="D113">
+        <v>2</v>
+      </c>
+      <c r="E113" t="s">
+        <v>160</v>
+      </c>
+      <c r="F113">
+        <v>16051</v>
+      </c>
+      <c r="G113">
+        <v>27</v>
+      </c>
+      <c r="H113">
+        <v>60</v>
+      </c>
+      <c r="I113">
+        <v>26</v>
+      </c>
+      <c r="J113">
+        <v>152</v>
+      </c>
+      <c r="K113" s="2">
+        <f>SQRT(G113*H113)*POWER((MIN(I113,20)+SQRT(MAX(I113-20,0))),0.9)*$B$1</f>
+        <v>49.648324587394477</v>
+      </c>
+      <c r="L113" s="2">
+        <f>POWER((G113*G113*H113), 0.33)*LOG10(J113)*10*$B$1</f>
+        <v>55.638430948840913</v>
+      </c>
+      <c r="M113" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N113">
+        <v>7</v>
+      </c>
+      <c r="P113" s="3"/>
+      <c r="Q113" s="2" t="str">
+        <f>CONCATENATE(
+ROUND(N113*VLOOKUP(E113,'ID Scheme'!$A$2:$E$7,3),0), "x",
+ROUND(O113*VLOOKUP(E113,'ID Scheme'!$A$2:$E$7,5),0), "x",
+ROUND(P113*VLOOKUP(E113,'ID Scheme'!$A$2:$E$7,4),0))</f>
         <v>65x0x0</v>
       </c>
     </row>
@@ -7236,18 +7309,13 @@
   <sortState ref="A4:R106">
     <sortCondition ref="A10"/>
   </sortState>
-  <conditionalFormatting sqref="C1:C2 C4:C110 C113:C1048576">
+  <conditionalFormatting sqref="C1:C2 C4:C110 C114:C1048576">
     <cfRule type="cellIs" dxfId="2" priority="10" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C111">
+  <conditionalFormatting sqref="C111:C113">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C112">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>